<commit_message>
Remove code of moveTOelemt and replace with java script
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -1271,7 +1271,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4916666666667" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1522,7 +1522,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 D2:E2 D3:E3 D6:E6 D4:E5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 D4:E6 D2:E3">
       <formula1>"Yes"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update in cucumber steps text
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -50,7 +50,7 @@
     <t>login.feature</t>
   </si>
   <si>
-    <t>verify_login_with_valid_email</t>
+    <t>User verify login with valid credentials</t>
   </si>
   <si>
     <t>Yes</t>
@@ -68,16 +68,16 @@
     <t>AddClient.feature</t>
   </si>
   <si>
-    <t>validate the functionality for creating a new client</t>
+    <t>Validate the functionality for creating a new client</t>
   </si>
   <si>
     <t>TC_004</t>
   </si>
   <si>
-    <t>validate the functionality for updating a client</t>
-  </si>
-  <si>
-    <t>validate the functionality for deleting a client</t>
+    <t>Validate the functionality for updating a client</t>
+  </si>
+  <si>
+    <t>Validate the functionality for deleting a client</t>
   </si>
 </sst>
 </file>
@@ -1271,7 +1271,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4916666666667" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1522,7 +1522,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 D4:E6 D2:E3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 D2:E3 D4:E6">
       <formula1>"Yes"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Change in Steps and refector some code
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -53,22 +53,22 @@
     <t>User verify login with valid credentials</t>
   </si>
   <si>
+    <t>TC_002</t>
+  </si>
+  <si>
+    <t>User tries to log in with invalid credentials</t>
+  </si>
+  <si>
+    <t>TC_003</t>
+  </si>
+  <si>
+    <t>AddClient.feature</t>
+  </si>
+  <si>
+    <t>Validate the functionality for creating a new client</t>
+  </si>
+  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_002</t>
-  </si>
-  <si>
-    <t>User tries to log in with invalid credentials</t>
-  </si>
-  <si>
-    <t>TC_003</t>
-  </si>
-  <si>
-    <t>AddClient.feature</t>
-  </si>
-  <si>
-    <t>Validate the functionality for creating a new client</t>
   </si>
   <si>
     <t>TC_004</t>
@@ -1271,7 +1271,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4916666666667" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1309,45 +1309,37 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1355,16 +1347,16 @@
         <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1372,16 +1364,16 @@
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1522,7 +1514,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 D2:E3 D4:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 D2:E4 D5:E6">
       <formula1>"Yes"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update test data for login
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -53,6 +53,9 @@
     <t>User verify login with valid credentials</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_002</t>
   </si>
   <si>
@@ -66,9 +69,6 @@
   </si>
   <si>
     <t>Validate the functionality for creating a new client</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>TC_004</t>
@@ -1271,7 +1271,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4916666666667" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1309,37 +1309,45 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1347,16 +1355,16 @@
         <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1364,16 +1372,16 @@
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1514,7 +1522,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 D2:E4 D5:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 D4:E6 D2:E3">
       <formula1>"Yes"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
merged new test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="48">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -49,9 +49,6 @@
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC_002</t>
   </si>
   <si>
@@ -82,25 +79,85 @@
     <t xml:space="preserve">TC_006</t>
   </si>
   <si>
+    <t xml:space="preserve">Validate the functionality for client is searched successfully.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the functionality for client details are correctly displayed in the client list.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the functionality for selected client is successfully Activated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the functionality for update the client invalid data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the functionality for creating a new client with invalid data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_011</t>
+  </si>
+  <si>
     <t xml:space="preserve">AddClientContact.feature</t>
   </si>
   <si>
     <t xml:space="preserve">Validate the functionality for creating a new client Contact</t>
   </si>
   <si>
-    <t xml:space="preserve">TC_007</t>
+    <t xml:space="preserve">TC_012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the functionality for updating a client Contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the functionality for updating a client Contact with Invalid Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the functionality for creating a new client Contact with invalid data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the functionality for deleting a client contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the functionality for report associated with the client are displayed on the Report tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_017</t>
   </si>
   <si>
     <t xml:space="preserve">Validate the functionality for campaigns associated with the client are displayed on the Campaign tab</t>
   </si>
   <si>
-    <t xml:space="preserve">TC_008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validate the functionality for report associated with the client are displayed on the Report tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_009</t>
+    <t xml:space="preserve">TC_018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the functionality for proposal associated with the client are displayed on the proposal tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_019</t>
   </si>
   <si>
     <t xml:space="preserve">Campaigns.feature</t>
@@ -116,7 +173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -166,6 +223,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -224,7 +288,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -246,6 +310,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -502,16 +570,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="81.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.9"/>
   </cols>
@@ -547,196 +615,361 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="B12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="A13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="A14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+    </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E1" type="list">
       <formula1>"Yes"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D1:D10 E2:E10" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D1" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:E20" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
added test case for Login with valid credentials
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>ID</t>
   </si>
@@ -53,169 +53,7 @@
     <t>User verify login with valid credentials</t>
   </si>
   <si>
-    <t>TC_002</t>
-  </si>
-  <si>
-    <t>User tries to log in with invalid credentials</t>
-  </si>
-  <si>
-    <t>TC_003</t>
-  </si>
-  <si>
-    <t>AddClient.feature</t>
-  </si>
-  <si>
-    <t>Validate the functionality for creating a new client</t>
-  </si>
-  <si>
-    <t>TC_004</t>
-  </si>
-  <si>
-    <t>Validate the functionality for updating a client</t>
-  </si>
-  <si>
-    <t>TC_005</t>
-  </si>
-  <si>
-    <t>Validate the functionality for deleting a client</t>
-  </si>
-  <si>
-    <t>TC_006</t>
-  </si>
-  <si>
-    <t>Validate the functionality for client is searched successfully.</t>
-  </si>
-  <si>
-    <t>TC_007</t>
-  </si>
-  <si>
-    <t>Validate the functionality for client details are correctly displayed in the client list.</t>
-  </si>
-  <si>
-    <t>TC_008</t>
-  </si>
-  <si>
-    <t>Validate the functionality for selected client is successfully Activated</t>
-  </si>
-  <si>
-    <t>TC_009</t>
-  </si>
-  <si>
-    <t>Validate the functionality for update the client invalid data</t>
-  </si>
-  <si>
-    <t>TC_010</t>
-  </si>
-  <si>
-    <t>Validate the functionality for creating a new client with invalid data</t>
-  </si>
-  <si>
-    <t>TC_011</t>
-  </si>
-  <si>
-    <t>AddClientContact.feature</t>
-  </si>
-  <si>
-    <t>Validate the functionality for creating a new client Contact</t>
-  </si>
-  <si>
-    <t>TC_012</t>
-  </si>
-  <si>
-    <t>Validate the functionality for updating a client Contact</t>
-  </si>
-  <si>
-    <t>TC_013</t>
-  </si>
-  <si>
-    <t>Validate the functionality for updating a client Contact with Invalid Data</t>
-  </si>
-  <si>
-    <t>TC_014</t>
-  </si>
-  <si>
-    <t>Validate the functionality for creating a new client Contact with invalid data</t>
-  </si>
-  <si>
-    <t>TC_015</t>
-  </si>
-  <si>
-    <t>Validate the functionality for deleting a client contact</t>
-  </si>
-  <si>
-    <t>TC_016</t>
-  </si>
-  <si>
-    <t>Validate the functionality for report associated with the client are displayed on the Report tab</t>
-  </si>
-  <si>
-    <t>TC_017</t>
-  </si>
-  <si>
-    <t>Validate the functionality for campaigns associated with the client are displayed on the Campaign tab</t>
-  </si>
-  <si>
-    <t>TC_018</t>
-  </si>
-  <si>
-    <t>Validate the functionality for proposal associated with the client are displayed on the proposal tab</t>
-  </si>
-  <si>
-    <t>TC_019</t>
-  </si>
-  <si>
-    <t>Campaigns.feature</t>
-  </si>
-  <si>
-    <t>Validate the functionality for creating a new Campaign page</t>
-  </si>
-  <si>
-    <t>TC_020</t>
-  </si>
-  <si>
-    <t>CampaignsNew.feature</t>
-  </si>
-  <si>
-    <t>Verify whether user is able to select the campaign from the menu bar</t>
-  </si>
-  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_021</t>
-  </si>
-  <si>
-    <t>Verify whether a user is able to select the All Date Ranges</t>
-  </si>
-  <si>
-    <t>TC_022</t>
-  </si>
-  <si>
-    <t>Verify whether a user is able to select the All Statuses option</t>
-  </si>
-  <si>
-    <t>TC_023</t>
-  </si>
-  <si>
-    <t>Verify whether a user is able to select the Organization</t>
-  </si>
-  <si>
-    <t>TC_024</t>
-  </si>
-  <si>
-    <t>User searches for a client or campaign name using the search field</t>
-  </si>
-  <si>
-    <t>TC_025</t>
-  </si>
-  <si>
-    <t>Validate user able to click on New Campaign button</t>
-  </si>
-  <si>
-    <t>TC_026</t>
-  </si>
-  <si>
-    <t>Validate the Overview Field input functionality for creating a new Campaign page</t>
   </si>
 </sst>
 </file>
@@ -1416,8 +1254,8 @@
   <sheetPr/>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25:E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1455,361 +1293,187 @@
       <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="A18" s="3"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="A20" s="3"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8"/>

</xml_diff>

<commit_message>
Added Test Cases for verifying error messages
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -54,6 +54,24 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>TC_002</t>
+  </si>
+  <si>
+    <t>User verify validation message is thrown for incorrect email-id</t>
+  </si>
+  <si>
+    <t>TC_003</t>
+  </si>
+  <si>
+    <t>User verify login using invalid credentials</t>
+  </si>
+  <si>
+    <t>TC_004</t>
+  </si>
+  <si>
+    <t>User verify if user is able to login without entering username</t>
   </si>
 </sst>
 </file>
@@ -1255,7 +1273,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1301,25 +1319,55 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="3"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="3"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3"/>
@@ -1330,17 +1378,17 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3"/>
-      <c r="B7" s="5"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3"/>
-      <c r="B8" s="5"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3"/>
@@ -1484,11 +1532,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2:E3 D12:E20">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D3 E2:E3 D7:E8 D12:E20">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
login test cases run successfully
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>User verify if user is able to login without entering username</t>
+  </si>
+  <si>
+    <t>TC_005</t>
+  </si>
+  <si>
+    <t>User verify if user is able to login without entering password</t>
+  </si>
+  <si>
+    <t>TC_006</t>
+  </si>
+  <si>
+    <t>User verify that password is visible on clicking eye icon</t>
   </si>
 </sst>
 </file>
@@ -1270,10 +1282,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1370,18 +1382,38 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3"/>
@@ -1392,10 +1424,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3"/>
-      <c r="B9" s="5"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3"/>
@@ -1415,8 +1447,8 @@
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3"/>
@@ -1475,11 +1507,11 @@
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="5"/>
+      <c r="A21" s="3"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="5"/>
@@ -1498,14 +1530,14 @@
     <row r="24" spans="1:5">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="7"/>
+      <c r="C24" s="6"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="C25" s="7"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
@@ -1524,18 +1556,25 @@
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D3 E2:E3 D7:E8 D12:E20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D3 E2:E3 D8:E9 D13:E21">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
checked the login code
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -53,7 +53,7 @@
     <t>User verify login with valid credentials</t>
   </si>
   <si>
-    <t>Yes</t>
+    <t>No</t>
   </si>
   <si>
     <t>TC_002</t>
@@ -1285,7 +1285,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1357,10 +1357,10 @@
       <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1374,10 +1374,10 @@
       <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1391,10 +1391,10 @@
       <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1408,10 +1408,10 @@
       <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1571,11 +1571,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2:D7 E2:E7 D8:E9 D13:E21">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D3 E2:E3 D8:E9 D13:E21">
-      <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added test case scenario to verify user type
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>User verify login with valid credentials</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
   <si>
     <t>No</t>
@@ -1285,7 +1288,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1327,92 +1330,92 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1571,11 +1574,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2:D7 E2:E7 D8:E9 D13:E21">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D7 E2:E7 D8:E9 D13:E21">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
firm creation new feature added
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>User verify user landed on login page after click on Back to Login link</t>
+  </si>
+  <si>
+    <t>TC_011</t>
+  </si>
+  <si>
+    <t>User verify that the logged-in user is admin or support staff</t>
   </si>
 </sst>
 </file>
@@ -1312,7 +1318,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1368,7 +1374,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>9</v>
@@ -1385,7 +1391,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>9</v>
@@ -1402,7 +1408,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>9</v>
@@ -1419,7 +1425,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>9</v>
@@ -1436,7 +1442,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>9</v>
@@ -1453,7 +1459,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>9</v>
@@ -1470,7 +1476,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>9</v>
@@ -1487,7 +1493,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>9</v>
@@ -1504,18 +1510,28 @@
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="3"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3"/>
@@ -1638,11 +1654,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 E11 D2:D11 E2:E10 D13:E21">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2 D3:D8 D9:D14 E2:E11 E13:E14 D15:E21">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Global contact creation code for review
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -53,9 +53,6 @@
     <t>User verify login with valid credentials</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -113,10 +110,25 @@
     <t>User verify user landed on login page after click on Back to Login link</t>
   </si>
   <si>
+    <t>TC_000</t>
+  </si>
+  <si>
+    <t>User verify that the logged-in user is admin or support staff</t>
+  </si>
+  <si>
     <t>TC_011</t>
   </si>
   <si>
-    <t>User verify that the logged-in user is admin or support staff</t>
+    <t>globalContact.feature</t>
+  </si>
+  <si>
+    <t>Launch Browser and go to application</t>
+  </si>
+  <si>
+    <t>TC_012</t>
+  </si>
+  <si>
+    <t>Verify user enters first and last name then clicks Create Individual Contact and lands on the Individual Contact page with pre-filled fields</t>
   </si>
 </sst>
 </file>
@@ -1318,7 +1330,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1360,192 +1372,212 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="3"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="B13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="3"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="A14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3"/>
@@ -1657,7 +1689,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2 D3:D8 D9:D14 E2:E11 E13:E14 D15:E21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D14 E2:E11 E13:E14 D15:E21">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
code merge with gaurav
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -221,7 +221,7 @@
     <t>TC_026</t>
   </si>
   <si>
-    <t>Verify, new individual contact can be created</t>
+    <t>Verify new individual contact can be created</t>
   </si>
 </sst>
 </file>
@@ -1451,8 +1451,8 @@
   <sheetPr/>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1716,7 +1716,7 @@
         <v>36</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>37</v>
@@ -1948,7 +1948,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11:F11 D1:D28 E2:E10 E15:E28 E13:F14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11:F11 D1:D28 E2:E10 E15:E23 E24:E28 E13:F14">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
code change for estate contacts according to new ui
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -1451,8 +1451,8 @@
   <sheetPr/>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:E28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A15" sqref="$A15:$XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1948,7 +1948,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11:F11 D1:D28 E2:E10 E15:E23 E24:E28 E13:F14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11:F11 D1:D28 E2:E10 E15:E28 E13:F14">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
global contact auto-save TC added
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" tabRatio="500"/>
+    <workbookView windowWidth="19200" windowHeight="6350" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioMapping" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -119,16 +119,61 @@
     <t>TC_011</t>
   </si>
   <si>
-    <t>globalContact.feature</t>
-  </si>
-  <si>
-    <t>Launch Browser and go to application</t>
+    <t>globalContacts.feature</t>
+  </si>
+  <si>
+    <t>SETUP: Launch Browser and go to application</t>
   </si>
   <si>
     <t>TC_012</t>
   </si>
   <si>
-    <t>Verify user enters first and last name then clicks Create Individual Contact and lands on the Individual Contact page with pre-filled fields</t>
+    <t>User verify user is on the Global Contact Creation page</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>TC_013</t>
+  </si>
+  <si>
+    <t>Create and then Edit the same contact for Individual Global Contact</t>
+  </si>
+  <si>
+    <t>TC_014</t>
+  </si>
+  <si>
+    <t>Create the contact for Entity Global Contact</t>
+  </si>
+  <si>
+    <t>TC_015</t>
+  </si>
+  <si>
+    <t>Attempt to create a duplicate entity contact with the same EIN</t>
+  </si>
+  <si>
+    <t>TC_016</t>
+  </si>
+  <si>
+    <t>Verify Select &amp; Proceed button is enabled after selecting a radio button</t>
+  </si>
+  <si>
+    <t>TC_017</t>
+  </si>
+  <si>
+    <t>Verify that the system trims leading and trailing spaces from text input fields</t>
+  </si>
+  <si>
+    <t>TC_018</t>
+  </si>
+  <si>
+    <t>Verify display result on entity name</t>
+  </si>
+  <si>
+    <t>TC_019</t>
+  </si>
+  <si>
+    <t>verify user authorization for "View Only" user</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1375,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1576,57 +1621,127 @@
         <v>8</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="3"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="A16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="A17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="A18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="3"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="A19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="3"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="A20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="3"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="A21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="5"/>

</xml_diff>

<commit_message>
code ready for jenkins job
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6350" tabRatio="500"/>
+    <workbookView windowWidth="19200" windowHeight="6800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioMapping" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -47,190 +47,151 @@
     <t>TC_001</t>
   </si>
   <si>
-    <t>login.feature</t>
-  </si>
-  <si>
-    <t>User verify login with valid credentials</t>
+    <t>globalContacts.feature</t>
+  </si>
+  <si>
+    <t>User verify user is on the Global Contact Creation page</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_002</t>
   </si>
   <si>
-    <t>User verify validation message is thrown for incorrect email-id</t>
+    <t>Create and then Edit the same contact for Individual Global Contact</t>
   </si>
   <si>
     <t>TC_003</t>
   </si>
   <si>
-    <t>User verify login using invalid credentials</t>
+    <t>Create the contact for Entity Global Contact</t>
   </si>
   <si>
     <t>TC_004</t>
   </si>
   <si>
-    <t>User verify if user is able to login without entering username</t>
+    <t>Attempt to create a duplicate entity contact with the same EIN</t>
   </si>
   <si>
     <t>TC_005</t>
   </si>
   <si>
-    <t>User verify if user is able to login without entering password</t>
+    <t>Verify Select &amp; Proceed button is enabled after selecting a radio button</t>
   </si>
   <si>
     <t>TC_006</t>
   </si>
   <si>
-    <t>User verify that password is visible on clicking eye icon</t>
+    <t>Verify that the system trims leading and trailing spaces from text input fields</t>
   </si>
   <si>
     <t>TC_007</t>
   </si>
   <si>
-    <t>User verify Remember me checkbox available on the login page</t>
+    <t>Verify display result on entity name</t>
   </si>
   <si>
     <t>TC_008</t>
   </si>
   <si>
-    <t>User verify Remember me checkbox is clickable</t>
+    <t>Verify user authorization for "View Only" user</t>
   </si>
   <si>
     <t>TC_009</t>
   </si>
   <si>
-    <t>User verify Forgot password page open after click on forgot password link</t>
+    <t>estateCreation.feature</t>
+  </si>
+  <si>
+    <t>User verify after filling decedent information clicking on next button other details are opened</t>
   </si>
   <si>
     <t>TC_010</t>
   </si>
   <si>
-    <t>User verify user landed on login page after click on Back to Login link</t>
-  </si>
-  <si>
-    <t>TC_000</t>
-  </si>
-  <si>
-    <t>User verify that the logged-in user is admin or support staff</t>
+    <t>Verify validations for all the fields under last address/domicile</t>
   </si>
   <si>
     <t>TC_011</t>
   </si>
   <si>
-    <t>globalContact.feature</t>
-  </si>
-  <si>
-    <t>Launch Browser and go to application</t>
+    <t>Verify Life Details fields, validations, and behaviors</t>
   </si>
   <si>
     <t>TC_012</t>
   </si>
   <si>
-    <t>Verify user enters first and last name then clicks Create Individual Contact and lands on the Individual Contact page with pre-filled fields</t>
+    <t>Verify validations for place of deaths</t>
   </si>
   <si>
     <t>TC_013</t>
   </si>
   <si>
-    <t>estateCreation.feature</t>
-  </si>
-  <si>
-    <t>user verify after filling decedent information clicking on next button other details are opened</t>
-  </si>
-  <si>
-    <t>Yes</t>
+    <t>Verify for Codicil Date picker open and values stored in correct format</t>
   </si>
   <si>
     <t>TC_014</t>
   </si>
   <si>
-    <t>Verify validations for all the fields under last address/domicile</t>
+    <t>Verify only one address can be selected at a time</t>
   </si>
   <si>
     <t>TC_015</t>
   </si>
   <si>
-    <t>Verify Life Details fields, validations, and behaviors</t>
-  </si>
-  <si>
     <t>TC_016</t>
   </si>
   <si>
-    <t>Verify validations for place of deaths</t>
+    <t>Verify created estate can be archived</t>
   </si>
   <si>
     <t>TC_017</t>
   </si>
   <si>
-    <t>Verify for Codicil Date picker open and values stored in correct format</t>
-  </si>
-  <si>
     <t>TC_018</t>
   </si>
   <si>
-    <t>Verify only one address can be selected at a time</t>
+    <t>estateContacts.feature</t>
+  </si>
+  <si>
+    <t>Verify add estate contact appears on clicking add button</t>
   </si>
   <si>
     <t>TC_019</t>
   </si>
   <si>
-    <t>Verify an estate is saved with all the fields</t>
+    <t>Verify existing individual type of contact can be added</t>
   </si>
   <si>
     <t>TC_020</t>
   </si>
   <si>
-    <t>Verify created estate can be archived</t>
+    <t>Verify existing entity type of contact can be added</t>
   </si>
   <si>
     <t>TC_021</t>
   </si>
   <si>
-    <t>Verify user authorization for "View Only" user</t>
+    <t>Verify new entity contact can be created</t>
   </si>
   <si>
     <t>TC_022</t>
   </si>
   <si>
-    <t>estateContacts.feature</t>
-  </si>
-  <si>
-    <t>Verify add estate contact appears on clicking add button</t>
+    <t>Verify contact can be saved without selecting any role</t>
   </si>
   <si>
     <t>TC_023</t>
   </si>
   <si>
-    <t>Verify existing individual type of contact can be added</t>
+    <t>Verify new individual contact can be created</t>
   </si>
   <si>
     <t>TC_024</t>
-  </si>
-  <si>
-    <t>Verify existing entity type of contact can be added</t>
-  </si>
-  <si>
-    <t>TC_025</t>
-  </si>
-  <si>
-    <t>Verify new entity contact can be created</t>
-  </si>
-  <si>
-    <t>TC_026</t>
-  </si>
-  <si>
-    <t>Verify contact can be saved without selecting any role</t>
-  </si>
-  <si>
-    <t>TC_027</t>
-  </si>
-  <si>
-    <t>Verify new individual contact can be created</t>
-  </si>
-  <si>
-    <t>TC_028</t>
   </si>
   <si>
     <t>Verify notification is displayed on removing the role</t>
@@ -268,12 +229,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
@@ -281,6 +236,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
@@ -435,7 +395,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,6 +410,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -635,7 +601,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -656,19 +622,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -796,7 +749,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -808,119 +761,119 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -930,19 +883,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1462,10 +1412,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1493,501 +1443,414 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
+      <c r="C4" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>22</v>
+      <c r="C9" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="B10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="3" t="s">
+      <c r="E10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6">
+        <v>29</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="8"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1995,7 +1858,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11:F11 D1:D23 D24:D30 E2:E10 E15:E21 E22:E30 E13:F14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D25 E2:E8 E9:E18 E19:E25 F2:F3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added 1 more TC
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" tabRatio="500"/>
+    <workbookView windowWidth="19200" windowHeight="6350" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioMapping" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>TC_015</t>
+  </si>
+  <si>
+    <t>Verify an estate is saved with all fields</t>
   </si>
   <si>
     <t>TC_016</t>
@@ -1414,8 +1417,8 @@
   <sheetPr/>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1691,7 +1694,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
@@ -1702,13 +1705,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>8</v>
@@ -1719,7 +1722,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>25</v>
@@ -1736,13 +1739,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>8</v>
@@ -1753,13 +1756,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>8</v>
@@ -1770,13 +1773,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>8</v>
@@ -1787,13 +1790,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>8</v>
@@ -1804,13 +1807,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>8</v>
@@ -1821,13 +1824,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>8</v>
@@ -1838,13 +1841,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>8</v>
@@ -1858,7 +1861,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D25 E2:E8 E9:E18 E19:E25 F2:F3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D25 E2:E22 E23:E25 F2:F3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
resolved TC failure issue in estateContacts
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" tabRatio="500"/>
+    <workbookView windowWidth="19200" windowHeight="6350" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioMapping" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>TC_015</t>
+  </si>
+  <si>
+    <t>Verify an estate is saved with all fields</t>
   </si>
   <si>
     <t>TC_016</t>
@@ -222,19 +225,19 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF263238"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF263238"/>
       <name val="Arial"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <name val="Arial"/>
       <charset val="1"/>
     </font>
@@ -882,14 +885,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1415,7 +1418,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1691,7 +1694,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
@@ -1702,13 +1705,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>8</v>
@@ -1719,7 +1722,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>25</v>
@@ -1736,13 +1739,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>8</v>
@@ -1753,13 +1756,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>8</v>
@@ -1770,13 +1773,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>8</v>
@@ -1787,13 +1790,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>8</v>
@@ -1804,13 +1807,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>8</v>
@@ -1821,13 +1824,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>8</v>
@@ -1838,13 +1841,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>8</v>
@@ -1858,7 +1861,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D25 E2:E8 E9:E18 E19:E25 F2:F3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D25 E2:E25 F2:F3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
resolved TC failure issue
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6350" tabRatio="500"/>
+    <workbookView windowWidth="19200" windowHeight="6800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioMapping" sheetId="1" r:id="rId1"/>
@@ -876,7 +876,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -892,7 +892,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1418,7 +1417,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1489,7 +1488,7 @@
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1506,7 +1505,7 @@
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -1517,13 +1516,13 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -1540,7 +1539,7 @@
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1557,7 +1556,7 @@
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -1574,7 +1573,7 @@
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -1602,7 +1601,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1642,7 +1641,7 @@
       <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1659,7 +1658,7 @@
       <c r="B14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1676,7 +1675,7 @@
       <c r="B15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1693,7 +1692,7 @@
       <c r="B16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1710,7 +1709,7 @@
       <c r="B17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1727,7 +1726,7 @@
       <c r="B18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -1741,10 +1740,10 @@
       <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -1758,10 +1757,10 @@
       <c r="A20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -1775,10 +1774,10 @@
       <c r="A21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -1792,10 +1791,10 @@
       <c r="A22" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -1809,10 +1808,10 @@
       <c r="A23" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D23" s="5" t="s">
@@ -1826,10 +1825,10 @@
       <c r="A24" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -1843,10 +1842,10 @@
       <c r="A25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D25" s="5" t="s">
@@ -1861,7 +1860,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D25 E2:E25 F2:F3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D25 E2:E8 E9:E25 F2:F3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
RW01 probate form all TCs done
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="68">
   <si>
     <t>ID</t>
   </si>
@@ -56,148 +56,181 @@
     <t>No</t>
   </si>
   <si>
+    <t>TC_002</t>
+  </si>
+  <si>
+    <t>Create and then Edit the same contact for Individual Global Contact</t>
+  </si>
+  <si>
+    <t>TC_003</t>
+  </si>
+  <si>
+    <t>Create the contact for Entity Global Contact</t>
+  </si>
+  <si>
+    <t>TC_004</t>
+  </si>
+  <si>
+    <t>Attempt to create a duplicate entity contact with the same EIN</t>
+  </si>
+  <si>
+    <t>TC_005</t>
+  </si>
+  <si>
+    <t>Verify Select &amp; Proceed button is enabled after selecting a radio button</t>
+  </si>
+  <si>
+    <t>TC_006</t>
+  </si>
+  <si>
+    <t>Verify that the system trims leading and trailing spaces from text input fields</t>
+  </si>
+  <si>
+    <t>TC_007</t>
+  </si>
+  <si>
+    <t>Verify display result on entity name</t>
+  </si>
+  <si>
+    <t>TC_008</t>
+  </si>
+  <si>
+    <t>Verify user authorization for "View Only" user</t>
+  </si>
+  <si>
+    <t>TC_009</t>
+  </si>
+  <si>
+    <t>estateCreation.feature</t>
+  </si>
+  <si>
+    <t>User verify after filling decedent information clicking on next button other details are opened</t>
+  </si>
+  <si>
+    <t>TC_010</t>
+  </si>
+  <si>
+    <t>Verify validations for all the fields under last address/domicile</t>
+  </si>
+  <si>
+    <t>TC_011</t>
+  </si>
+  <si>
+    <t>Verify Life Details fields, validations, and behaviors</t>
+  </si>
+  <si>
+    <t>TC_012</t>
+  </si>
+  <si>
+    <t>Verify validations for place of deaths</t>
+  </si>
+  <si>
+    <t>TC_013</t>
+  </si>
+  <si>
+    <t>Verify for Codicil Date picker open and values stored in correct format</t>
+  </si>
+  <si>
+    <t>TC_014</t>
+  </si>
+  <si>
+    <t>Verify only one address can be selected at a time</t>
+  </si>
+  <si>
+    <t>TC_015</t>
+  </si>
+  <si>
+    <t>Verify an estate is saved with all fields</t>
+  </si>
+  <si>
+    <t>TC_016</t>
+  </si>
+  <si>
+    <t>Verify created estate can be archived</t>
+  </si>
+  <si>
+    <t>TC_017</t>
+  </si>
+  <si>
+    <t>TC_018</t>
+  </si>
+  <si>
+    <t>estateContacts.feature</t>
+  </si>
+  <si>
+    <t>Verify add estate contact appears on clicking add button</t>
+  </si>
+  <si>
+    <t>TC_019</t>
+  </si>
+  <si>
+    <t>Verify existing individual type of contact can be added</t>
+  </si>
+  <si>
+    <t>TC_020</t>
+  </si>
+  <si>
+    <t>Verify existing entity type of contact can be added</t>
+  </si>
+  <si>
+    <t>TC_021</t>
+  </si>
+  <si>
+    <t>Verify new entity contact can be created</t>
+  </si>
+  <si>
+    <t>TC_022</t>
+  </si>
+  <si>
+    <t>Verify contact can be saved without selecting any role</t>
+  </si>
+  <si>
+    <t>TC_023</t>
+  </si>
+  <si>
+    <t>Verify new individual contact can be created</t>
+  </si>
+  <si>
+    <t>TC_024</t>
+  </si>
+  <si>
+    <t>Verify notification is displayed on removing the role</t>
+  </si>
+  <si>
+    <t>TC_025</t>
+  </si>
+  <si>
+    <t>probateFormsRW03.feature</t>
+  </si>
+  <si>
+    <t>User Creates an Estate</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>TC_002</t>
-  </si>
-  <si>
-    <t>Create and then Edit the same contact for Individual Global Contact</t>
-  </si>
-  <si>
-    <t>TC_003</t>
-  </si>
-  <si>
-    <t>Create the contact for Entity Global Contact</t>
-  </si>
-  <si>
-    <t>TC_004</t>
-  </si>
-  <si>
-    <t>Attempt to create a duplicate entity contact with the same EIN</t>
-  </si>
-  <si>
-    <t>TC_005</t>
-  </si>
-  <si>
-    <t>Verify Select &amp; Proceed button is enabled after selecting a radio button</t>
-  </si>
-  <si>
-    <t>TC_006</t>
-  </si>
-  <si>
-    <t>Verify that the system trims leading and trailing spaces from text input fields</t>
-  </si>
-  <si>
-    <t>TC_007</t>
-  </si>
-  <si>
-    <t>Verify display result on entity name</t>
-  </si>
-  <si>
-    <t>TC_008</t>
-  </si>
-  <si>
-    <t>Verify user authorization for "View Only" user</t>
-  </si>
-  <si>
-    <t>TC_009</t>
-  </si>
-  <si>
-    <t>estateCreation.feature</t>
-  </si>
-  <si>
-    <t>User verify after filling decedent information clicking on next button other details are opened</t>
-  </si>
-  <si>
-    <t>TC_010</t>
-  </si>
-  <si>
-    <t>Verify validations for all the fields under last address/domicile</t>
-  </si>
-  <si>
-    <t>TC_011</t>
-  </si>
-  <si>
-    <t>Verify Life Details fields, validations, and behaviors</t>
-  </si>
-  <si>
-    <t>TC_012</t>
-  </si>
-  <si>
-    <t>Verify validations for place of deaths</t>
-  </si>
-  <si>
-    <t>TC_013</t>
-  </si>
-  <si>
-    <t>Verify for Codicil Date picker open and values stored in correct format</t>
-  </si>
-  <si>
-    <t>TC_014</t>
-  </si>
-  <si>
-    <t>Verify only one address can be selected at a time</t>
-  </si>
-  <si>
-    <t>TC_015</t>
-  </si>
-  <si>
-    <t>Verify an estate is saved with all fields</t>
-  </si>
-  <si>
-    <t>TC_016</t>
-  </si>
-  <si>
-    <t>Verify created estate can be archived</t>
-  </si>
-  <si>
-    <t>TC_017</t>
-  </si>
-  <si>
-    <t>TC_018</t>
-  </si>
-  <si>
-    <t>estateContacts.feature</t>
-  </si>
-  <si>
-    <t>Verify add estate contact appears on clicking add button</t>
-  </si>
-  <si>
-    <t>TC_019</t>
-  </si>
-  <si>
-    <t>Verify existing individual type of contact can be added</t>
-  </si>
-  <si>
-    <t>TC_020</t>
-  </si>
-  <si>
-    <t>Verify existing entity type of contact can be added</t>
-  </si>
-  <si>
-    <t>TC_021</t>
-  </si>
-  <si>
-    <t>Verify new entity contact can be created</t>
-  </si>
-  <si>
-    <t>TC_022</t>
-  </si>
-  <si>
-    <t>Verify contact can be saved without selecting any role</t>
-  </si>
-  <si>
-    <t>TC_023</t>
-  </si>
-  <si>
-    <t>Verify new individual contact can be created</t>
-  </si>
-  <si>
-    <t>TC_024</t>
-  </si>
-  <si>
-    <t>Verify notification is displayed on removing the role</t>
+    <t>TC_026</t>
+  </si>
+  <si>
+    <t>Verify county, estate and aka names are auto-populated on the form</t>
+  </si>
+  <si>
+    <t>TC_027</t>
+  </si>
+  <si>
+    <t>probateFormsRW01.feature</t>
+  </si>
+  <si>
+    <t>TC_028</t>
+  </si>
+  <si>
+    <t>User adds Estate Contacts</t>
+  </si>
+  <si>
+    <t>TC_029</t>
+  </si>
+  <si>
+    <t>Verify RW01 form</t>
   </si>
 </sst>
 </file>
@@ -604,7 +637,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -631,6 +664,17 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="thin">
         <color auto="1"/>
@@ -752,7 +796,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -764,34 +808,34 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -876,7 +920,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -893,6 +937,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1414,16 +1466,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="7.30833333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7833333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.4166666666667" style="1" customWidth="1"/>
     <col min="3" max="3" width="81.1" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.9" style="1" customWidth="1"/>
   </cols>
@@ -1459,408 +1511,508 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="D17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="D19" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="D20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="D21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="D22" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="D23" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="D24" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="B26" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="11"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="11"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="11"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="11"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D25 E2:E25 F2:F3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D27 E2:E27 F2:F3 D28:E30">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added TCs for RW02 probate form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -206,31 +206,46 @@
     <t>User Creates an Estate</t>
   </si>
   <si>
+    <t>TC_026</t>
+  </si>
+  <si>
+    <t>Verify county, estate and aka names are auto-populated on the form</t>
+  </si>
+  <si>
+    <t>TC_027</t>
+  </si>
+  <si>
+    <t>probateFormsRW01.feature</t>
+  </si>
+  <si>
+    <t>TC_028</t>
+  </si>
+  <si>
+    <t>User adds Estate Contacts</t>
+  </si>
+  <si>
+    <t>TC_029</t>
+  </si>
+  <si>
+    <t>Verify RW01 form</t>
+  </si>
+  <si>
+    <t>TC_030</t>
+  </si>
+  <si>
+    <t>probateFormsRW02.feature</t>
+  </si>
+  <si>
+    <t>Open Estate</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>TC_026</t>
-  </si>
-  <si>
-    <t>Verify county, estate and aka names are auto-populated on the form</t>
-  </si>
-  <si>
-    <t>TC_027</t>
-  </si>
-  <si>
-    <t>probateFormsRW01.feature</t>
-  </si>
-  <si>
-    <t>TC_028</t>
-  </si>
-  <si>
-    <t>User adds Estate Contacts</t>
-  </si>
-  <si>
-    <t>TC_029</t>
-  </si>
-  <si>
-    <t>Verify RW01 form</t>
+    <t>TC_031</t>
+  </si>
+  <si>
+    <t>Verify RW02 form</t>
   </si>
 </sst>
 </file>
@@ -243,7 +258,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -271,6 +286,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="1"/>
     </font>
@@ -785,21 +806,18 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -808,119 +826,122 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -944,6 +965,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1469,7 +1492,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1921,32 +1944,32 @@
         <v>8</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>58</v>
@@ -1955,64 +1978,92 @@
         <v>8</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="D29" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="D30" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="11"/>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="11"/>
+      <c r="B31" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="11"/>
+      <c r="A33" s="13"/>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="11"/>
+      <c r="A34" s="13"/>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="11"/>
+      <c r="A35" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D27 E2:E27 F2:F3 D28:E30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D28 D1:D27 D29:D32 E2:E22 E23:E30 E31:E32 F2:F3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
made changes in RW01, RW02 and RW03 codes
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="93">
   <si>
     <t>ID</t>
   </si>
@@ -200,52 +200,112 @@
     <t>TC_025</t>
   </si>
   <si>
+    <t>probateFormsRW01.feature</t>
+  </si>
+  <si>
+    <t>Open Estate</t>
+  </si>
+  <si>
+    <t>TC_026</t>
+  </si>
+  <si>
+    <t>Verify RW01 form</t>
+  </si>
+  <si>
+    <t>TC_027</t>
+  </si>
+  <si>
+    <t>Reset the RW01 form</t>
+  </si>
+  <si>
+    <t>TC_028</t>
+  </si>
+  <si>
+    <t>probateFormsRW02.feature</t>
+  </si>
+  <si>
+    <t>TC_029</t>
+  </si>
+  <si>
+    <t>Verify RW02 form</t>
+  </si>
+  <si>
+    <t>TC_030</t>
+  </si>
+  <si>
+    <t>Reset the RW02 form</t>
+  </si>
+  <si>
+    <t>TC_031</t>
+  </si>
+  <si>
     <t>probateFormsRW03.feature</t>
   </si>
   <si>
-    <t>User Creates an Estate</t>
-  </si>
-  <si>
-    <t>TC_026</t>
-  </si>
-  <si>
-    <t>Verify county, estate and aka names are auto-populated on the form</t>
-  </si>
-  <si>
-    <t>TC_027</t>
-  </si>
-  <si>
-    <t>probateFormsRW01.feature</t>
-  </si>
-  <si>
-    <t>TC_028</t>
-  </si>
-  <si>
-    <t>User adds Estate Contacts</t>
-  </si>
-  <si>
-    <t>TC_029</t>
-  </si>
-  <si>
-    <t>Verify RW01 form</t>
-  </si>
-  <si>
-    <t>TC_030</t>
-  </si>
-  <si>
-    <t>probateFormsRW02.feature</t>
-  </si>
-  <si>
-    <t>Open Estate</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_031</t>
-  </si>
-  <si>
-    <t>Verify RW02 form</t>
+    <t>TC_032</t>
+  </si>
+  <si>
+    <t>Verify RW03 form</t>
+  </si>
+  <si>
+    <t>TC_033</t>
+  </si>
+  <si>
+    <t>Reset the RW03 form</t>
+  </si>
+  <si>
+    <t>TC_034</t>
+  </si>
+  <si>
+    <t>probateFormsRW04.feature</t>
+  </si>
+  <si>
+    <t>TC_035</t>
+  </si>
+  <si>
+    <t>Verify RW04 form</t>
+  </si>
+  <si>
+    <t>TC_036</t>
+  </si>
+  <si>
+    <t>Reset the RW04 form</t>
+  </si>
+  <si>
+    <t>TC_037</t>
+  </si>
+  <si>
+    <t>probateFormsRW05.feature</t>
+  </si>
+  <si>
+    <t>TC_038</t>
+  </si>
+  <si>
+    <t>Verify RW05 form</t>
+  </si>
+  <si>
+    <t>TC_039</t>
+  </si>
+  <si>
+    <t>Reset the RW05 form</t>
+  </si>
+  <si>
+    <t>TC_040</t>
+  </si>
+  <si>
+    <t>probateFormsRWxx.feature</t>
+  </si>
+  <si>
+    <t>TC_041</t>
+  </si>
+  <si>
+    <t>Verify RWxx form</t>
+  </si>
+  <si>
+    <t>TC_042</t>
+  </si>
+  <si>
+    <t>Reset the RWxx form</t>
   </si>
 </sst>
 </file>
@@ -941,7 +1001,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -965,7 +1025,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1489,10 +1548,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1969,10 +2028,10 @@
         <v>61</v>
       </c>
       <c r="B28" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>8</v>
@@ -1986,10 +2045,10 @@
         <v>63</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>8</v>
@@ -2003,7 +2062,7 @@
         <v>65</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>66</v>
@@ -2019,51 +2078,250 @@
       <c r="A31" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>69</v>
-      </c>
       <c r="D31" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="12" t="s">
+      <c r="B33" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="D33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="13"/>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="13"/>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="13"/>
+      <c r="C34" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="12"/>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="12"/>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="12"/>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="12"/>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="12"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="12"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="12"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D28 D1:D27 D29:D32 E2:E22 E23:E30 E31:E32 F2:F3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D43 E2:E43 F2:F3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
working on RW02 PDF
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="97">
   <si>
     <t>ID</t>
   </si>
@@ -206,6 +206,9 @@
     <t>Open Estate</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_026</t>
   </si>
   <si>
@@ -233,76 +236,85 @@
     <t>TC_030</t>
   </si>
   <si>
+    <t>Verify form can be printed in pdf</t>
+  </si>
+  <si>
+    <t>TC_031</t>
+  </si>
+  <si>
     <t>Reset the RW02 form</t>
   </si>
   <si>
-    <t>TC_031</t>
+    <t>TC_032</t>
   </si>
   <si>
     <t>probateFormsRW03.feature</t>
   </si>
   <si>
-    <t>TC_032</t>
+    <t>TC_033</t>
   </si>
   <si>
     <t>Verify RW03 form</t>
   </si>
   <si>
-    <t>TC_033</t>
+    <t>TC_034</t>
+  </si>
+  <si>
+    <t>TC_035</t>
   </si>
   <si>
     <t>Reset the RW03 form</t>
   </si>
   <si>
-    <t>TC_034</t>
+    <t>TC_036</t>
   </si>
   <si>
     <t>probateFormsRW04.feature</t>
   </si>
   <si>
-    <t>TC_035</t>
+    <t>TC_037</t>
   </si>
   <si>
     <t>Verify RW04 form</t>
   </si>
   <si>
-    <t>TC_036</t>
+    <t>TC_038</t>
   </si>
   <si>
     <t>Reset the RW04 form</t>
   </si>
   <si>
-    <t>TC_037</t>
+    <t>TC_039</t>
   </si>
   <si>
     <t>probateFormsRW05.feature</t>
   </si>
   <si>
-    <t>TC_038</t>
+    <t>TC_040</t>
   </si>
   <si>
     <t>Verify RW05 form</t>
   </si>
   <si>
-    <t>TC_039</t>
+    <t>TC_041</t>
   </si>
   <si>
     <t>Reset the RW05 form</t>
   </si>
   <si>
-    <t>TC_040</t>
+    <t>TC_042</t>
   </si>
   <si>
     <t>probateFormsRWxx.feature</t>
   </si>
   <si>
-    <t>TC_041</t>
+    <t>TC_043</t>
   </si>
   <si>
     <t>Verify RWxx form</t>
   </si>
   <si>
-    <t>TC_042</t>
+    <t>TC_044</t>
   </si>
   <si>
     <t>Reset the RWxx form</t>
@@ -1548,10 +1560,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2000,7 +2012,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>8</v>
@@ -2008,16 +2020,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>8</v>
@@ -2025,16 +2037,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>8</v>
@@ -2042,16 +2054,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>8</v>
@@ -2059,16 +2071,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>64</v>
-      </c>
       <c r="C30" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>8</v>
@@ -2076,16 +2088,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>8</v>
+        <v>65</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>8</v>
@@ -2093,16 +2105,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>8</v>
+        <v>71</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>8</v>
@@ -2110,16 +2122,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>8</v>
+        <v>73</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>8</v>
@@ -2127,16 +2139,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>70</v>
-      </c>
       <c r="C34" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>8</v>
+        <v>75</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>8</v>
@@ -2144,16 +2156,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>8</v>
+        <v>69</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>8</v>
@@ -2164,13 +2176,13 @@
         <v>77</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>8</v>
+      <c r="D36" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>8</v>
@@ -2181,10 +2193,10 @@
         <v>79</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>8</v>
@@ -2198,10 +2210,10 @@
         <v>81</v>
       </c>
       <c r="B38" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>8</v>
@@ -2215,7 +2227,7 @@
         <v>83</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>84</v>
@@ -2232,10 +2244,10 @@
         <v>85</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>8</v>
@@ -2249,10 +2261,10 @@
         <v>87</v>
       </c>
       <c r="B41" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>8</v>
@@ -2266,7 +2278,7 @@
         <v>89</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>90</v>
@@ -2283,23 +2295,51 @@
         <v>91</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C43" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="12"/>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="12"/>
+      <c r="C44" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="12"/>
@@ -2315,13 +2355,19 @@
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="12"/>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="12"/>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="12"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D43 E2:E43 F2:F3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D31 E31 D35 E35 D1:D30 D32:D34 D36:D45 E2:E30 E32:E34 E36:E45 F2:F3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated feature files of RW01, RW02 and RW03
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="176">
   <si>
     <t>ID</t>
   </si>
@@ -206,106 +206,355 @@
     <t>Open Estate</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_026</t>
   </si>
   <si>
-    <t>Verify RW01 form</t>
+    <t>Verify, file no. is displayed at the top of the form.</t>
   </si>
   <si>
     <t>TC_027</t>
   </si>
   <si>
+    <t>Verify, decedent information is displayed in section1 of the form.</t>
+  </si>
+  <si>
+    <t>TC_028</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 2 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_029</t>
+  </si>
+  <si>
+    <t>Verify, in section 2 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_030</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 3 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_031</t>
+  </si>
+  <si>
+    <t>Verify, in section 3 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_032</t>
+  </si>
+  <si>
+    <t>Verify, on clicking other checkbox, text area is enabled.</t>
+  </si>
+  <si>
+    <t>TC_033</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 4 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_034</t>
+  </si>
+  <si>
+    <t>Verify, on clicking last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_035</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_036</t>
+  </si>
+  <si>
+    <t>Verify, on selecting the contact its information is displayed in section 4.</t>
+  </si>
+  <si>
+    <t>TC_037</t>
+  </si>
+  <si>
+    <t>Verify, on clicking executor last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_038</t>
+  </si>
+  <si>
+    <t>Verify, 3 types of selection is available.</t>
+  </si>
+  <si>
+    <t>TC_039</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be dragged and dropped in a each of the type.</t>
+  </si>
+  <si>
+    <t>TC_040</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 5 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_041</t>
+  </si>
+  <si>
+    <t>Verify the selected contacts are displayed under executor, co executor and secondary co executor.</t>
+  </si>
+  <si>
+    <t>TC_042</t>
+  </si>
+  <si>
     <t>Reset the RW01 form</t>
   </si>
   <si>
-    <t>TC_028</t>
+    <t>TC_043</t>
   </si>
   <si>
     <t>probateFormsRW02.feature</t>
   </si>
   <si>
-    <t>TC_029</t>
-  </si>
-  <si>
-    <t>Verify RW02 form</t>
-  </si>
-  <si>
-    <t>TC_030</t>
+    <t>TC_044</t>
+  </si>
+  <si>
+    <t>Verify, correct county name is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_045</t>
+  </si>
+  <si>
+    <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
+  </si>
+  <si>
+    <t>TC_046</t>
+  </si>
+  <si>
+    <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
+  </si>
+  <si>
+    <t>TC_047</t>
+  </si>
+  <si>
+    <t>Verify, county, estate and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_048</t>
+  </si>
+  <si>
+    <t>Verify, the auto populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_049</t>
+  </si>
+  <si>
+    <t>Verify, names can be added in aka fields.</t>
+  </si>
+  <si>
+    <t>TC_050</t>
+  </si>
+  <si>
+    <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
+  </si>
+  <si>
+    <t>TC_051</t>
+  </si>
+  <si>
+    <t>Verify, amount can be entered in the input fields.</t>
+  </si>
+  <si>
+    <t>TC_052</t>
+  </si>
+  <si>
+    <t>Verify, total estimated value should display total of 1st and last field only.</t>
+  </si>
+  <si>
+    <t>TC_053</t>
+  </si>
+  <si>
+    <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_054</t>
+  </si>
+  <si>
+    <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_055</t>
+  </si>
+  <si>
+    <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
+  </si>
+  <si>
+    <t>TC_056</t>
+  </si>
+  <si>
+    <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
+  </si>
+  <si>
+    <t>TC_057</t>
+  </si>
+  <si>
+    <t>Verify that selecting option A keeps it selected without affecting option B.</t>
+  </si>
+  <si>
+    <t>TC_058</t>
+  </si>
+  <si>
+    <t>Verify, decedent died date is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_059</t>
+  </si>
+  <si>
+    <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
+  </si>
+  <si>
+    <t>TC_060</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
+  </si>
+  <si>
+    <t>TC_061</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B keeps it selected without affecting option A.</t>
+  </si>
+  <si>
+    <t>TC_062</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
+  </si>
+  <si>
+    <t>TC_063</t>
+  </si>
+  <si>
+    <t>Verify, multiple beneficiaries can be selected.</t>
+  </si>
+  <si>
+    <t>TC_064</t>
+  </si>
+  <si>
+    <t>Verify, bene contacts in the table.</t>
+  </si>
+  <si>
+    <t>TC_065</t>
+  </si>
+  <si>
+    <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
+  </si>
+  <si>
+    <t>TC_066</t>
+  </si>
+  <si>
+    <t>Verify, on checking "Display all heirs on attachment".</t>
+  </si>
+  <si>
+    <t>TC_067</t>
+  </si>
+  <si>
+    <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
+  </si>
+  <si>
+    <t>TC_068</t>
+  </si>
+  <si>
+    <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
+  </si>
+  <si>
+    <t>TC_069</t>
+  </si>
+  <si>
+    <t>Verify fees section.</t>
+  </si>
+  <si>
+    <t>TC_070</t>
+  </si>
+  <si>
+    <t>Verify, attorney can be selected.</t>
+  </si>
+  <si>
+    <t>TC_071</t>
+  </si>
+  <si>
+    <t>Verify, information in decree of the register.</t>
+  </si>
+  <si>
+    <t>TC_072</t>
   </si>
   <si>
     <t>Reset the RW02 form</t>
   </si>
   <si>
-    <t>TC_031</t>
+    <t>TC_073</t>
   </si>
   <si>
     <t>probateFormsRW03.feature</t>
   </si>
   <si>
-    <t>TC_032</t>
-  </si>
-  <si>
-    <t>Verify RW03 form</t>
-  </si>
-  <si>
-    <t>TC_033</t>
+    <t>TC_074</t>
+  </si>
+  <si>
+    <t>Verify county, estate and aka names are auto-populated on the form</t>
+  </si>
+  <si>
+    <t>TC_075</t>
+  </si>
+  <si>
+    <t>Verify, the auto-populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_076</t>
+  </si>
+  <si>
+    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
+  </si>
+  <si>
+    <t>TC_077</t>
+  </si>
+  <si>
+    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
+  </si>
+  <si>
+    <t>TC_078</t>
+  </si>
+  <si>
+    <t>Verify, names can be entered in witness fields.</t>
+  </si>
+  <si>
+    <t>TC_079</t>
+  </si>
+  <si>
+    <t>Verify, names updated from signature are reflected in witness names fields.</t>
+  </si>
+  <si>
+    <t>TC_080</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered in address, city, zip fields.</t>
+  </si>
+  <si>
+    <t>TC_081</t>
+  </si>
+  <si>
+    <t>Verify, form is auto saved.</t>
+  </si>
+  <si>
+    <t>TC_082</t>
+  </si>
+  <si>
+    <t>Verify form can be printed in pdf</t>
+  </si>
+  <si>
+    <t>TC_083</t>
   </si>
   <si>
     <t>Reset the RW03 form</t>
-  </si>
-  <si>
-    <t>TC_034</t>
-  </si>
-  <si>
-    <t>probateFormsRW04.feature</t>
-  </si>
-  <si>
-    <t>TC_035</t>
-  </si>
-  <si>
-    <t>Verify RW04 form</t>
-  </si>
-  <si>
-    <t>TC_036</t>
-  </si>
-  <si>
-    <t>Reset the RW04 form</t>
-  </si>
-  <si>
-    <t>TC_037</t>
-  </si>
-  <si>
-    <t>probateFormsRW05.feature</t>
-  </si>
-  <si>
-    <t>TC_038</t>
-  </si>
-  <si>
-    <t>Verify RW05 form</t>
-  </si>
-  <si>
-    <t>TC_039</t>
-  </si>
-  <si>
-    <t>Reset the RW05 form</t>
-  </si>
-  <si>
-    <t>TC_040</t>
-  </si>
-  <si>
-    <t>probateFormsRWxx.feature</t>
-  </si>
-  <si>
-    <t>TC_041</t>
-  </si>
-  <si>
-    <t>Verify RWxx form</t>
-  </si>
-  <si>
-    <t>TC_042</t>
-  </si>
-  <si>
-    <t>Reset the RWxx form</t>
   </si>
 </sst>
 </file>
@@ -318,7 +567,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -346,12 +595,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <charset val="1"/>
     </font>
@@ -718,7 +961,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -745,17 +988,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color auto="1"/>
@@ -866,18 +1098,21 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -886,122 +1121,119 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1021,13 +1253,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1548,10 +1775,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1999,329 +2226,1005 @@
       <c r="C26" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="10" t="s">
+      <c r="C27" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="10" t="s">
+      <c r="C28" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D29" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>68</v>
+        <v>57</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>72</v>
+        <v>57</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>74</v>
+        <v>57</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>77</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>78</v>
+        <v>57</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>84</v>
+        <v>57</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>86</v>
+        <v>57</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>87</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>90</v>
+        <v>57</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>92</v>
+        <v>57</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="12"/>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="12"/>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="12"/>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="12"/>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="12"/>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="12"/>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="12"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" ht="28" spans="1:5">
+      <c r="A51" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" ht="28" spans="1:5">
+      <c r="A54" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" ht="28" spans="1:5">
+      <c r="A57" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" ht="28" spans="1:5">
+      <c r="A61" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D43 E2:E43 F2:F3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D84 E2:E41 E42:E84 F2:F3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated RW03 page code
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -206,295 +206,295 @@
     <t>Open Estate</t>
   </si>
   <si>
+    <t>TC_026</t>
+  </si>
+  <si>
+    <t>Verify, file no. is displayed at the top of the form.</t>
+  </si>
+  <si>
+    <t>TC_027</t>
+  </si>
+  <si>
+    <t>Verify, decedent information is displayed in section1 of the form.</t>
+  </si>
+  <si>
+    <t>TC_028</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 2 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_029</t>
+  </si>
+  <si>
+    <t>Verify, in section 2 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_030</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 3 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_031</t>
+  </si>
+  <si>
+    <t>Verify, in section 3 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_032</t>
+  </si>
+  <si>
+    <t>Verify, on clicking other checkbox, text area is enabled.</t>
+  </si>
+  <si>
+    <t>TC_033</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 4 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_034</t>
+  </si>
+  <si>
+    <t>Verify, on clicking last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_035</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_036</t>
+  </si>
+  <si>
+    <t>Verify, on selecting the contact its information is displayed in section 4.</t>
+  </si>
+  <si>
+    <t>TC_037</t>
+  </si>
+  <si>
+    <t>Verify, on clicking executor last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_038</t>
+  </si>
+  <si>
+    <t>Verify, 3 types of selection is available.</t>
+  </si>
+  <si>
+    <t>TC_039</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be dragged and dropped in a each of the type.</t>
+  </si>
+  <si>
+    <t>TC_040</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 5 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_041</t>
+  </si>
+  <si>
+    <t>Verify the selected contacts are displayed under executor, co executor and secondary co executor.</t>
+  </si>
+  <si>
+    <t>TC_042</t>
+  </si>
+  <si>
+    <t>Reset the RW01 form</t>
+  </si>
+  <si>
+    <t>TC_043</t>
+  </si>
+  <si>
+    <t>probateFormsRW02.feature</t>
+  </si>
+  <si>
+    <t>TC_044</t>
+  </si>
+  <si>
+    <t>Verify, correct county name is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_045</t>
+  </si>
+  <si>
+    <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
+  </si>
+  <si>
+    <t>TC_046</t>
+  </si>
+  <si>
+    <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
+  </si>
+  <si>
+    <t>TC_047</t>
+  </si>
+  <si>
+    <t>Verify, county, estate and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_048</t>
+  </si>
+  <si>
+    <t>Verify, the auto populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_049</t>
+  </si>
+  <si>
+    <t>Verify, names can be added in aka fields.</t>
+  </si>
+  <si>
+    <t>TC_050</t>
+  </si>
+  <si>
+    <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
+  </si>
+  <si>
+    <t>TC_051</t>
+  </si>
+  <si>
+    <t>Verify, amount can be entered in the input fields.</t>
+  </si>
+  <si>
+    <t>TC_052</t>
+  </si>
+  <si>
+    <t>Verify, total estimated value should display total of 1st and last field only.</t>
+  </si>
+  <si>
+    <t>TC_053</t>
+  </si>
+  <si>
+    <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_054</t>
+  </si>
+  <si>
+    <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_055</t>
+  </si>
+  <si>
+    <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
+  </si>
+  <si>
+    <t>TC_056</t>
+  </si>
+  <si>
+    <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
+  </si>
+  <si>
+    <t>TC_057</t>
+  </si>
+  <si>
+    <t>Verify that selecting option A keeps it selected without affecting option B.</t>
+  </si>
+  <si>
+    <t>TC_058</t>
+  </si>
+  <si>
+    <t>Verify, decedent died date is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_059</t>
+  </si>
+  <si>
+    <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
+  </si>
+  <si>
+    <t>TC_060</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
+  </si>
+  <si>
+    <t>TC_061</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B keeps it selected without affecting option A.</t>
+  </si>
+  <si>
+    <t>TC_062</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
+  </si>
+  <si>
+    <t>TC_063</t>
+  </si>
+  <si>
+    <t>Verify, multiple beneficiaries can be selected.</t>
+  </si>
+  <si>
+    <t>TC_064</t>
+  </si>
+  <si>
+    <t>Verify, bene contacts in the table.</t>
+  </si>
+  <si>
+    <t>TC_065</t>
+  </si>
+  <si>
+    <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
+  </si>
+  <si>
+    <t>TC_066</t>
+  </si>
+  <si>
+    <t>Verify, on checking "Display all heirs on attachment".</t>
+  </si>
+  <si>
+    <t>TC_067</t>
+  </si>
+  <si>
+    <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
+  </si>
+  <si>
+    <t>TC_068</t>
+  </si>
+  <si>
+    <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
+  </si>
+  <si>
+    <t>TC_069</t>
+  </si>
+  <si>
+    <t>Verify fees section.</t>
+  </si>
+  <si>
+    <t>TC_070</t>
+  </si>
+  <si>
+    <t>Verify, attorney can be selected.</t>
+  </si>
+  <si>
+    <t>TC_071</t>
+  </si>
+  <si>
+    <t>Verify, information in decree of the register.</t>
+  </si>
+  <si>
+    <t>TC_072</t>
+  </si>
+  <si>
+    <t>Reset the RW02 form</t>
+  </si>
+  <si>
+    <t>TC_073</t>
+  </si>
+  <si>
+    <t>probateFormsRW03.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_026</t>
-  </si>
-  <si>
-    <t>Verify, file no. is displayed at the top of the form.</t>
-  </si>
-  <si>
-    <t>TC_027</t>
-  </si>
-  <si>
-    <t>Verify, decedent information is displayed in section1 of the form.</t>
-  </si>
-  <si>
-    <t>TC_028</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 2 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_029</t>
-  </si>
-  <si>
-    <t>Verify, in section 2 only 1 checkbox can be checked.</t>
-  </si>
-  <si>
-    <t>TC_030</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 3 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_031</t>
-  </si>
-  <si>
-    <t>Verify, in section 3 only 1 checkbox can be checked.</t>
-  </si>
-  <si>
-    <t>TC_032</t>
-  </si>
-  <si>
-    <t>Verify, on clicking other checkbox, text area is enabled.</t>
-  </si>
-  <si>
-    <t>TC_033</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 4 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_034</t>
-  </si>
-  <si>
-    <t>Verify, on clicking last name, a side bar is displayed.</t>
-  </si>
-  <si>
-    <t>TC_035</t>
-  </si>
-  <si>
-    <t>Verify, only 1 contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_036</t>
-  </si>
-  <si>
-    <t>Verify, on selecting the contact its information is displayed in section 4.</t>
-  </si>
-  <si>
-    <t>TC_037</t>
-  </si>
-  <si>
-    <t>Verify, on clicking executor last name, a side bar is displayed.</t>
-  </si>
-  <si>
-    <t>TC_038</t>
-  </si>
-  <si>
-    <t>Verify, 3 types of selection is available.</t>
-  </si>
-  <si>
-    <t>TC_039</t>
-  </si>
-  <si>
-    <t>Verify, only 1 contact can be dragged and dropped in a each of the type.</t>
-  </si>
-  <si>
-    <t>TC_040</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 5 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_041</t>
-  </si>
-  <si>
-    <t>Verify the selected contacts are displayed under executor, co executor and secondary co executor.</t>
-  </si>
-  <si>
-    <t>TC_042</t>
-  </si>
-  <si>
-    <t>Reset the RW01 form</t>
-  </si>
-  <si>
-    <t>TC_043</t>
-  </si>
-  <si>
-    <t>probateFormsRW02.feature</t>
-  </si>
-  <si>
-    <t>TC_044</t>
-  </si>
-  <si>
-    <t>Verify, correct county name is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_045</t>
-  </si>
-  <si>
-    <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
-  </si>
-  <si>
-    <t>TC_046</t>
-  </si>
-  <si>
-    <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
-  </si>
-  <si>
-    <t>TC_047</t>
-  </si>
-  <si>
-    <t>Verify, county, estate and aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_048</t>
-  </si>
-  <si>
-    <t>Verify, the auto populated fields are not editable.</t>
-  </si>
-  <si>
-    <t>TC_049</t>
-  </si>
-  <si>
-    <t>Verify, names can be added in aka fields.</t>
-  </si>
-  <si>
-    <t>TC_050</t>
-  </si>
-  <si>
-    <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
-  </si>
-  <si>
-    <t>TC_051</t>
-  </si>
-  <si>
-    <t>Verify, amount can be entered in the input fields.</t>
-  </si>
-  <si>
-    <t>TC_052</t>
-  </si>
-  <si>
-    <t>Verify, total estimated value should display total of 1st and last field only.</t>
-  </si>
-  <si>
-    <t>TC_053</t>
-  </si>
-  <si>
-    <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
-  </si>
-  <si>
-    <t>TC_054</t>
-  </si>
-  <si>
-    <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
-  </si>
-  <si>
-    <t>TC_055</t>
-  </si>
-  <si>
-    <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
-  </si>
-  <si>
-    <t>TC_056</t>
-  </si>
-  <si>
-    <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
-  </si>
-  <si>
-    <t>TC_057</t>
-  </si>
-  <si>
-    <t>Verify that selecting option A keeps it selected without affecting option B.</t>
-  </si>
-  <si>
-    <t>TC_058</t>
-  </si>
-  <si>
-    <t>Verify, decedent died date is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_059</t>
-  </si>
-  <si>
-    <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
-  </si>
-  <si>
-    <t>TC_060</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
-  </si>
-  <si>
-    <t>TC_061</t>
-  </si>
-  <si>
-    <t>Verify that selecting option B keeps it selected without affecting option A.</t>
-  </si>
-  <si>
-    <t>TC_062</t>
-  </si>
-  <si>
-    <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
-  </si>
-  <si>
-    <t>TC_063</t>
-  </si>
-  <si>
-    <t>Verify, multiple beneficiaries can be selected.</t>
-  </si>
-  <si>
-    <t>TC_064</t>
-  </si>
-  <si>
-    <t>Verify, bene contacts in the table.</t>
-  </si>
-  <si>
-    <t>TC_065</t>
-  </si>
-  <si>
-    <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
-  </si>
-  <si>
-    <t>TC_066</t>
-  </si>
-  <si>
-    <t>Verify, on checking "Display all heirs on attachment".</t>
-  </si>
-  <si>
-    <t>TC_067</t>
-  </si>
-  <si>
-    <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
-  </si>
-  <si>
-    <t>TC_068</t>
-  </si>
-  <si>
-    <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
-  </si>
-  <si>
-    <t>TC_069</t>
-  </si>
-  <si>
-    <t>Verify fees section.</t>
-  </si>
-  <si>
-    <t>TC_070</t>
-  </si>
-  <si>
-    <t>Verify, attorney can be selected.</t>
-  </si>
-  <si>
-    <t>TC_071</t>
-  </si>
-  <si>
-    <t>Verify, information in decree of the register.</t>
-  </si>
-  <si>
-    <t>TC_072</t>
-  </si>
-  <si>
-    <t>Reset the RW02 form</t>
-  </si>
-  <si>
-    <t>TC_073</t>
-  </si>
-  <si>
-    <t>probateFormsRW03.feature</t>
   </si>
   <si>
     <t>TC_074</t>
@@ -1777,8 +1777,8 @@
   <sheetPr/>
   <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2230,304 +2230,304 @@
         <v>8</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>58</v>
@@ -2536,508 +2536,508 @@
         <v>8</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>97</v>
-      </c>
       <c r="D45" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>99</v>
-      </c>
       <c r="D46" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>101</v>
-      </c>
       <c r="D47" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>103</v>
-      </c>
       <c r="D48" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B49" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>105</v>
-      </c>
       <c r="D49" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B50" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>107</v>
-      </c>
       <c r="D50" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" ht="28" spans="1:5">
       <c r="A51" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B51" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>109</v>
-      </c>
       <c r="D51" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B52" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>111</v>
-      </c>
       <c r="D52" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>113</v>
-      </c>
       <c r="D53" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" ht="28" spans="1:5">
       <c r="A54" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>115</v>
-      </c>
       <c r="D54" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B55" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>117</v>
-      </c>
       <c r="D55" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>119</v>
-      </c>
       <c r="D56" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" ht="28" spans="1:5">
       <c r="A57" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B57" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>121</v>
-      </c>
       <c r="D57" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B58" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>123</v>
-      </c>
       <c r="D58" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>125</v>
-      </c>
       <c r="D59" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>127</v>
-      </c>
       <c r="D60" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" ht="28" spans="1:5">
       <c r="A61" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B61" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>129</v>
-      </c>
       <c r="D61" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B62" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>131</v>
-      </c>
       <c r="D62" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C63" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="B63" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>133</v>
-      </c>
       <c r="D63" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="B64" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>135</v>
-      </c>
       <c r="D64" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C65" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B65" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>137</v>
-      </c>
       <c r="D65" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B66" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>139</v>
-      </c>
       <c r="D66" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>141</v>
-      </c>
       <c r="D67" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="B68" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>143</v>
-      </c>
       <c r="D68" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="B69" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>145</v>
-      </c>
       <c r="D69" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B70" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>147</v>
-      </c>
       <c r="D70" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C71" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B71" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>149</v>
-      </c>
       <c r="D71" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B72" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>151</v>
-      </c>
       <c r="D72" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C73" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="B73" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>153</v>
-      </c>
       <c r="D73" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" s="8" t="s">
         <v>154</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>155</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>58</v>
@@ -3046,7 +3046,7 @@
         <v>8</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -3054,7 +3054,7 @@
         <v>156</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C75" s="9" t="s">
         <v>157</v>
@@ -3063,7 +3063,7 @@
         <v>8</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -3071,7 +3071,7 @@
         <v>158</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>159</v>
@@ -3080,7 +3080,7 @@
         <v>8</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -3088,7 +3088,7 @@
         <v>160</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C77" s="9" t="s">
         <v>161</v>
@@ -3097,7 +3097,7 @@
         <v>8</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -3105,7 +3105,7 @@
         <v>162</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C78" s="9" t="s">
         <v>163</v>
@@ -3114,7 +3114,7 @@
         <v>8</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -3122,7 +3122,7 @@
         <v>164</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C79" s="9" t="s">
         <v>165</v>
@@ -3131,7 +3131,7 @@
         <v>8</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -3139,7 +3139,7 @@
         <v>166</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C80" s="9" t="s">
         <v>167</v>
@@ -3148,7 +3148,7 @@
         <v>8</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -3156,7 +3156,7 @@
         <v>168</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C81" s="9" t="s">
         <v>169</v>
@@ -3165,7 +3165,7 @@
         <v>8</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -3173,7 +3173,7 @@
         <v>170</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C82" s="9" t="s">
         <v>171</v>
@@ -3182,7 +3182,7 @@
         <v>8</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -3190,7 +3190,7 @@
         <v>172</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>173</v>
@@ -3199,7 +3199,7 @@
         <v>8</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -3207,7 +3207,7 @@
         <v>174</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C84" s="9" t="s">
         <v>175</v>
@@ -3216,7 +3216,7 @@
         <v>8</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3224,7 +3224,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D84 E2:E41 E42:E84 F2:F3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D84 E2:E23 E24:E71 E72:E84 F2:F3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
TCs added for RW04 probate form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="187">
   <si>
     <t>ID</t>
   </si>
@@ -494,67 +494,100 @@
     <t>probateFormsRW03.feature</t>
   </si>
   <si>
+    <t>TC_074</t>
+  </si>
+  <si>
+    <t>Verify county, estate and aka names are auto-populated on the form</t>
+  </si>
+  <si>
+    <t>TC_075</t>
+  </si>
+  <si>
+    <t>Verify, the auto-populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_076</t>
+  </si>
+  <si>
+    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
+  </si>
+  <si>
+    <t>TC_077</t>
+  </si>
+  <si>
+    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
+  </si>
+  <si>
+    <t>TC_078</t>
+  </si>
+  <si>
+    <t>Verify, names can be entered in witness fields.</t>
+  </si>
+  <si>
+    <t>TC_079</t>
+  </si>
+  <si>
+    <t>Verify, names updated from signature are reflected in witness names fields.</t>
+  </si>
+  <si>
+    <t>TC_080</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered in address, city, zip fields.</t>
+  </si>
+  <si>
+    <t>TC_081</t>
+  </si>
+  <si>
+    <t>Verify, form is auto saved.</t>
+  </si>
+  <si>
+    <t>TC_082</t>
+  </si>
+  <si>
+    <t>Verify form can be printed in pdf</t>
+  </si>
+  <si>
+    <t>TC_083</t>
+  </si>
+  <si>
+    <t>Reset the RW03 form</t>
+  </si>
+  <si>
+    <t>TC_084</t>
+  </si>
+  <si>
+    <t>probateFormsRW04.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>TC_074</t>
-  </si>
-  <si>
-    <t>Verify county, estate and aka names are auto-populated on the form</t>
-  </si>
-  <si>
-    <t>TC_075</t>
-  </si>
-  <si>
-    <t>Verify, the auto-populated fields are not editable.</t>
-  </si>
-  <si>
-    <t>TC_076</t>
-  </si>
-  <si>
-    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
-  </si>
-  <si>
-    <t>TC_077</t>
-  </si>
-  <si>
-    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
-  </si>
-  <si>
-    <t>TC_078</t>
-  </si>
-  <si>
-    <t>Verify, names can be entered in witness fields.</t>
-  </si>
-  <si>
-    <t>TC_079</t>
-  </si>
-  <si>
-    <t>Verify, names updated from signature are reflected in witness names fields.</t>
-  </si>
-  <si>
-    <t>TC_080</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered in address, city, zip fields.</t>
-  </si>
-  <si>
-    <t>TC_081</t>
-  </si>
-  <si>
-    <t>Verify, form is auto saved.</t>
-  </si>
-  <si>
-    <t>TC_082</t>
-  </si>
-  <si>
-    <t>Verify form can be printed in pdf</t>
-  </si>
-  <si>
-    <t>TC_083</t>
-  </si>
-  <si>
-    <t>Reset the RW03 form</t>
+    <t>TC_085</t>
+  </si>
+  <si>
+    <t>Verify, correct title is displayed on the form's header.</t>
+  </si>
+  <si>
+    <t>TC_086</t>
+  </si>
+  <si>
+    <t>Verify, county, and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_087</t>
+  </si>
+  <si>
+    <t>Verify, correct estate's name is displayed on the form.</t>
+  </si>
+  <si>
+    <t>TC_088</t>
+  </si>
+  <si>
+    <t>Verify, name of the decedent should be auto populated from the form.</t>
+  </si>
+  <si>
+    <t>TC_089</t>
   </si>
 </sst>
 </file>
@@ -1233,7 +1266,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1256,6 +1289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1775,10 +1809,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3046,177 +3080,279 @@
         <v>8</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>155</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>154</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>155</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>154</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>155</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>154</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>155</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>154</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>155</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>154</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>155</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>154</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>155</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>154</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>155</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>154</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>155</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>154</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>155</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>154</v>
       </c>
       <c r="C84" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>155</v>
+      <c r="B85" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C90" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -3224,7 +3360,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D84 E2:E23 E24:E71 E72:E84 F2:F3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D81 D82:D84 D85:D90 E2:E72 E73:E81 E82:E90 F2:F3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated code of global contacts, estate creation, RW01 and added TCs for RW04 form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="193">
   <si>
     <t>ID</t>
   </si>
@@ -107,6 +107,9 @@
     <t>User verify after filling decedent information clicking on next button other details are opened</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_010</t>
   </si>
   <si>
@@ -560,9 +563,6 @@
     <t>probateFormsRW04.feature</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>TC_085</t>
   </si>
   <si>
@@ -588,6 +588,24 @@
   </si>
   <si>
     <t>TC_089</t>
+  </si>
+  <si>
+    <t>TC_090</t>
+  </si>
+  <si>
+    <t>TC_091</t>
+  </si>
+  <si>
+    <t>TC_092</t>
+  </si>
+  <si>
+    <t>TC_093</t>
+  </si>
+  <si>
+    <t>TC_094</t>
+  </si>
+  <si>
+    <t>Reset the RW04 form</t>
   </si>
 </sst>
 </file>
@@ -1266,7 +1284,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1289,7 +1307,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1809,10 +1826,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1886,7 +1903,7 @@
       <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1989,7 +2006,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>8</v>
@@ -1997,16 +2014,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>8</v>
@@ -2014,16 +2031,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>8</v>
@@ -2031,16 +2048,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>8</v>
@@ -2048,16 +2065,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>8</v>
@@ -2065,16 +2082,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>8</v>
@@ -2082,16 +2099,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>8</v>
@@ -2099,16 +2116,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>8</v>
@@ -2116,7 +2133,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>24</v>
@@ -2133,13 +2150,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>8</v>
@@ -2150,13 +2167,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>8</v>
@@ -2167,13 +2184,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>8</v>
@@ -2184,13 +2201,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>8</v>
@@ -2201,13 +2218,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>8</v>
@@ -2218,13 +2235,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>8</v>
@@ -2235,13 +2252,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>8</v>
@@ -2252,15 +2269,15 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -2269,15 +2286,15 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -2286,15 +2303,15 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -2303,15 +2320,15 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -2320,15 +2337,15 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -2337,15 +2354,15 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -2354,15 +2371,15 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -2371,15 +2388,15 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D33" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="3" t="s">
@@ -2388,15 +2405,15 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="3" t="s">
@@ -2405,15 +2422,15 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D35" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -2422,15 +2439,15 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D36" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -2439,15 +2456,15 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -2456,15 +2473,15 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D38" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -2473,15 +2490,15 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D39" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -2490,15 +2507,15 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D40" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -2507,15 +2524,15 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D41" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -2524,15 +2541,15 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D42" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="3" t="s">
@@ -2541,15 +2558,15 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -2558,13 +2575,13 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>8</v>
@@ -2575,13 +2592,13 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>94</v>
-      </c>
       <c r="C45" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>8</v>
@@ -2592,13 +2609,13 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>8</v>
@@ -2609,13 +2626,13 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>8</v>
@@ -2626,13 +2643,13 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>8</v>
@@ -2643,13 +2660,13 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>8</v>
@@ -2660,13 +2677,13 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>8</v>
@@ -2677,13 +2694,13 @@
     </row>
     <row r="51" ht="28" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>8</v>
@@ -2694,13 +2711,13 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>8</v>
@@ -2711,13 +2728,13 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>8</v>
@@ -2728,13 +2745,13 @@
     </row>
     <row r="54" ht="28" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>8</v>
@@ -2745,13 +2762,13 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>8</v>
@@ -2762,13 +2779,13 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>8</v>
@@ -2779,13 +2796,13 @@
     </row>
     <row r="57" ht="28" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>8</v>
@@ -2796,13 +2813,13 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>8</v>
@@ -2813,13 +2830,13 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>8</v>
@@ -2830,13 +2847,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>8</v>
@@ -2847,13 +2864,13 @@
     </row>
     <row r="61" ht="28" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>8</v>
@@ -2864,13 +2881,13 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>8</v>
@@ -2881,13 +2898,13 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>8</v>
@@ -2898,13 +2915,13 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>8</v>
@@ -2915,13 +2932,13 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>8</v>
@@ -2932,13 +2949,13 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>8</v>
@@ -2949,13 +2966,13 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>8</v>
@@ -2966,13 +2983,13 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>8</v>
@@ -2983,13 +3000,13 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>8</v>
@@ -3000,13 +3017,13 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>8</v>
@@ -3017,13 +3034,13 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>8</v>
@@ -3034,13 +3051,13 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>8</v>
@@ -3051,13 +3068,13 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>8</v>
@@ -3068,13 +3085,13 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>8</v>
@@ -3085,13 +3102,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B75" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="C75" s="9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>8</v>
@@ -3102,13 +3119,13 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>8</v>
@@ -3119,13 +3136,13 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>8</v>
@@ -3136,13 +3153,13 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>8</v>
@@ -3153,13 +3170,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>8</v>
@@ -3170,13 +3187,13 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>8</v>
@@ -3187,13 +3204,13 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>8</v>
@@ -3204,13 +3221,13 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>8</v>
@@ -3221,13 +3238,13 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>8</v>
@@ -3238,13 +3255,13 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>8</v>
@@ -3255,16 +3272,16 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C85" s="10" t="s">
-        <v>58</v>
+        <v>177</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>8</v>
@@ -3275,13 +3292,13 @@
         <v>178</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C86" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C86" s="8" t="s">
         <v>179</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>8</v>
@@ -3292,13 +3309,13 @@
         <v>180</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C87" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C87" s="8" t="s">
         <v>181</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>8</v>
@@ -3309,13 +3326,13 @@
         <v>182</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C88" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C88" s="8" t="s">
         <v>183</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>8</v>
@@ -3326,13 +3343,13 @@
         <v>184</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C89" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C89" s="8" t="s">
         <v>185</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>8</v>
@@ -3343,25 +3360,110 @@
         <v>186</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C90" s="10" t="s">
-        <v>162</v>
+        <v>177</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>163</v>
       </c>
       <c r="D90" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B91" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="E90" s="3" t="s">
+      <c r="C91" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" s="3" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D9 D2:D8 D10:D16 D17:D95 E2:E95 F2:F3">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D81 D82:D84 D85:D90 E2:E72 E73:E81 E82:E90 F2:F3">
-      <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
added common step definitions in CommonSteps file
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -107,460 +107,460 @@
     <t>User verify after filling decedent information clicking on next button other details are opened</t>
   </si>
   <si>
+    <t>TC_010</t>
+  </si>
+  <si>
+    <t>Verify validations for all the fields under last address/domicile</t>
+  </si>
+  <si>
+    <t>TC_011</t>
+  </si>
+  <si>
+    <t>Verify Life Details fields, validations, and behaviors</t>
+  </si>
+  <si>
+    <t>TC_012</t>
+  </si>
+  <si>
+    <t>Verify validations for place of deaths</t>
+  </si>
+  <si>
+    <t>TC_013</t>
+  </si>
+  <si>
+    <t>Verify for Codicil Date picker open and values stored in correct format</t>
+  </si>
+  <si>
+    <t>TC_014</t>
+  </si>
+  <si>
+    <t>Verify only one address can be selected at a time</t>
+  </si>
+  <si>
+    <t>TC_015</t>
+  </si>
+  <si>
+    <t>Verify an estate is saved with all fields</t>
+  </si>
+  <si>
+    <t>TC_016</t>
+  </si>
+  <si>
+    <t>Verify created estate can be archived</t>
+  </si>
+  <si>
+    <t>TC_017</t>
+  </si>
+  <si>
+    <t>TC_018</t>
+  </si>
+  <si>
+    <t>estateContacts.feature</t>
+  </si>
+  <si>
+    <t>Verify add estate contact appears on clicking add button</t>
+  </si>
+  <si>
+    <t>TC_019</t>
+  </si>
+  <si>
+    <t>Verify existing individual type of contact can be added</t>
+  </si>
+  <si>
+    <t>TC_020</t>
+  </si>
+  <si>
+    <t>Verify existing entity type of contact can be added</t>
+  </si>
+  <si>
+    <t>TC_021</t>
+  </si>
+  <si>
+    <t>Verify new entity contact can be created</t>
+  </si>
+  <si>
+    <t>TC_022</t>
+  </si>
+  <si>
+    <t>Verify contact can be saved without selecting any role</t>
+  </si>
+  <si>
+    <t>TC_023</t>
+  </si>
+  <si>
+    <t>Verify new individual contact can be created</t>
+  </si>
+  <si>
+    <t>TC_024</t>
+  </si>
+  <si>
+    <t>Verify notification is displayed on removing the role</t>
+  </si>
+  <si>
+    <t>TC_025</t>
+  </si>
+  <si>
+    <t>probateFormsRW01.feature</t>
+  </si>
+  <si>
+    <t>Open Estate</t>
+  </si>
+  <si>
+    <t>TC_026</t>
+  </si>
+  <si>
+    <t>Verify, file no. is displayed at the top of the form.</t>
+  </si>
+  <si>
+    <t>TC_027</t>
+  </si>
+  <si>
+    <t>Verify, decedent information is displayed in section1 of the form.</t>
+  </si>
+  <si>
+    <t>TC_028</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 2 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_029</t>
+  </si>
+  <si>
+    <t>Verify, in section 2 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_030</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 3 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_031</t>
+  </si>
+  <si>
+    <t>Verify, in section 3 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_032</t>
+  </si>
+  <si>
+    <t>Verify, on clicking other checkbox, text area is enabled.</t>
+  </si>
+  <si>
+    <t>TC_033</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 4 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_034</t>
+  </si>
+  <si>
+    <t>Verify, on clicking last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_035</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_036</t>
+  </si>
+  <si>
+    <t>Verify, on selecting the contact its information is displayed in section 4.</t>
+  </si>
+  <si>
+    <t>TC_037</t>
+  </si>
+  <si>
+    <t>Verify, on clicking executor last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_038</t>
+  </si>
+  <si>
+    <t>Verify, 3 types of selection is available.</t>
+  </si>
+  <si>
+    <t>TC_039</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be dragged and dropped in a each of the type.</t>
+  </si>
+  <si>
+    <t>TC_040</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 5 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_041</t>
+  </si>
+  <si>
+    <t>Verify the selected contacts are displayed under executor, co executor and secondary co executor.</t>
+  </si>
+  <si>
+    <t>TC_042</t>
+  </si>
+  <si>
+    <t>Reset the RW01 form</t>
+  </si>
+  <si>
+    <t>TC_043</t>
+  </si>
+  <si>
+    <t>probateFormsRW02.feature</t>
+  </si>
+  <si>
+    <t>TC_044</t>
+  </si>
+  <si>
+    <t>Verify, correct county name is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_045</t>
+  </si>
+  <si>
+    <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
+  </si>
+  <si>
+    <t>TC_046</t>
+  </si>
+  <si>
+    <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
+  </si>
+  <si>
+    <t>TC_047</t>
+  </si>
+  <si>
+    <t>Verify, county, estate and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_048</t>
+  </si>
+  <si>
+    <t>Verify, the auto populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_049</t>
+  </si>
+  <si>
+    <t>Verify, names can be added in aka fields.</t>
+  </si>
+  <si>
+    <t>TC_050</t>
+  </si>
+  <si>
+    <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
+  </si>
+  <si>
+    <t>TC_051</t>
+  </si>
+  <si>
+    <t>Verify, amount can be entered in the input fields.</t>
+  </si>
+  <si>
+    <t>TC_052</t>
+  </si>
+  <si>
+    <t>Verify, total estimated value should display total of 1st and last field only.</t>
+  </si>
+  <si>
+    <t>TC_053</t>
+  </si>
+  <si>
+    <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_054</t>
+  </si>
+  <si>
+    <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_055</t>
+  </si>
+  <si>
+    <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
+  </si>
+  <si>
+    <t>TC_056</t>
+  </si>
+  <si>
+    <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
+  </si>
+  <si>
+    <t>TC_057</t>
+  </si>
+  <si>
+    <t>Verify that selecting option A keeps it selected without affecting option B.</t>
+  </si>
+  <si>
+    <t>TC_058</t>
+  </si>
+  <si>
+    <t>Verify, decedent died date is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_059</t>
+  </si>
+  <si>
+    <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
+  </si>
+  <si>
+    <t>TC_060</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
+  </si>
+  <si>
+    <t>TC_061</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B keeps it selected without affecting option A.</t>
+  </si>
+  <si>
+    <t>TC_062</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
+  </si>
+  <si>
+    <t>TC_063</t>
+  </si>
+  <si>
+    <t>Verify, multiple beneficiaries can be selected.</t>
+  </si>
+  <si>
+    <t>TC_064</t>
+  </si>
+  <si>
+    <t>Verify, bene contacts in the table.</t>
+  </si>
+  <si>
+    <t>TC_065</t>
+  </si>
+  <si>
+    <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
+  </si>
+  <si>
+    <t>TC_066</t>
+  </si>
+  <si>
+    <t>Verify, on checking "Display all heirs on attachment".</t>
+  </si>
+  <si>
+    <t>TC_067</t>
+  </si>
+  <si>
+    <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
+  </si>
+  <si>
+    <t>TC_068</t>
+  </si>
+  <si>
+    <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
+  </si>
+  <si>
+    <t>TC_069</t>
+  </si>
+  <si>
+    <t>Verify fees section.</t>
+  </si>
+  <si>
+    <t>TC_070</t>
+  </si>
+  <si>
+    <t>Verify, attorney can be selected.</t>
+  </si>
+  <si>
+    <t>TC_071</t>
+  </si>
+  <si>
+    <t>Verify, information in decree of the register.</t>
+  </si>
+  <si>
+    <t>TC_072</t>
+  </si>
+  <si>
+    <t>Reset the RW02 form</t>
+  </si>
+  <si>
+    <t>TC_073</t>
+  </si>
+  <si>
+    <t>probateFormsRW03.feature</t>
+  </si>
+  <si>
+    <t>TC_074</t>
+  </si>
+  <si>
+    <t>Verify county, estate and aka names are auto-populated on the form</t>
+  </si>
+  <si>
+    <t>TC_075</t>
+  </si>
+  <si>
+    <t>Verify, the auto-populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_076</t>
+  </si>
+  <si>
+    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
+  </si>
+  <si>
+    <t>TC_077</t>
+  </si>
+  <si>
+    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
+  </si>
+  <si>
+    <t>TC_078</t>
+  </si>
+  <si>
+    <t>Verify, names can be entered in witness fields.</t>
+  </si>
+  <si>
+    <t>TC_079</t>
+  </si>
+  <si>
+    <t>Verify, names updated from signature are reflected in witness names fields.</t>
+  </si>
+  <si>
+    <t>TC_080</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered in address, city, zip fields.</t>
+  </si>
+  <si>
+    <t>TC_081</t>
+  </si>
+  <si>
+    <t>Verify, form is auto saved.</t>
+  </si>
+  <si>
+    <t>TC_082</t>
+  </si>
+  <si>
+    <t>Verify form can be printed in pdf</t>
+  </si>
+  <si>
+    <t>TC_083</t>
+  </si>
+  <si>
+    <t>Reset the RW03 form</t>
+  </si>
+  <si>
+    <t>TC_084</t>
+  </si>
+  <si>
+    <t>probateFormsRW04.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_010</t>
-  </si>
-  <si>
-    <t>Verify validations for all the fields under last address/domicile</t>
-  </si>
-  <si>
-    <t>TC_011</t>
-  </si>
-  <si>
-    <t>Verify Life Details fields, validations, and behaviors</t>
-  </si>
-  <si>
-    <t>TC_012</t>
-  </si>
-  <si>
-    <t>Verify validations for place of deaths</t>
-  </si>
-  <si>
-    <t>TC_013</t>
-  </si>
-  <si>
-    <t>Verify for Codicil Date picker open and values stored in correct format</t>
-  </si>
-  <si>
-    <t>TC_014</t>
-  </si>
-  <si>
-    <t>Verify only one address can be selected at a time</t>
-  </si>
-  <si>
-    <t>TC_015</t>
-  </si>
-  <si>
-    <t>Verify an estate is saved with all fields</t>
-  </si>
-  <si>
-    <t>TC_016</t>
-  </si>
-  <si>
-    <t>Verify created estate can be archived</t>
-  </si>
-  <si>
-    <t>TC_017</t>
-  </si>
-  <si>
-    <t>TC_018</t>
-  </si>
-  <si>
-    <t>estateContacts.feature</t>
-  </si>
-  <si>
-    <t>Verify add estate contact appears on clicking add button</t>
-  </si>
-  <si>
-    <t>TC_019</t>
-  </si>
-  <si>
-    <t>Verify existing individual type of contact can be added</t>
-  </si>
-  <si>
-    <t>TC_020</t>
-  </si>
-  <si>
-    <t>Verify existing entity type of contact can be added</t>
-  </si>
-  <si>
-    <t>TC_021</t>
-  </si>
-  <si>
-    <t>Verify new entity contact can be created</t>
-  </si>
-  <si>
-    <t>TC_022</t>
-  </si>
-  <si>
-    <t>Verify contact can be saved without selecting any role</t>
-  </si>
-  <si>
-    <t>TC_023</t>
-  </si>
-  <si>
-    <t>Verify new individual contact can be created</t>
-  </si>
-  <si>
-    <t>TC_024</t>
-  </si>
-  <si>
-    <t>Verify notification is displayed on removing the role</t>
-  </si>
-  <si>
-    <t>TC_025</t>
-  </si>
-  <si>
-    <t>probateFormsRW01.feature</t>
-  </si>
-  <si>
-    <t>Open Estate</t>
-  </si>
-  <si>
-    <t>TC_026</t>
-  </si>
-  <si>
-    <t>Verify, file no. is displayed at the top of the form.</t>
-  </si>
-  <si>
-    <t>TC_027</t>
-  </si>
-  <si>
-    <t>Verify, decedent information is displayed in section1 of the form.</t>
-  </si>
-  <si>
-    <t>TC_028</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 2 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_029</t>
-  </si>
-  <si>
-    <t>Verify, in section 2 only 1 checkbox can be checked.</t>
-  </si>
-  <si>
-    <t>TC_030</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 3 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_031</t>
-  </si>
-  <si>
-    <t>Verify, in section 3 only 1 checkbox can be checked.</t>
-  </si>
-  <si>
-    <t>TC_032</t>
-  </si>
-  <si>
-    <t>Verify, on clicking other checkbox, text area is enabled.</t>
-  </si>
-  <si>
-    <t>TC_033</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 4 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_034</t>
-  </si>
-  <si>
-    <t>Verify, on clicking last name, a side bar is displayed.</t>
-  </si>
-  <si>
-    <t>TC_035</t>
-  </si>
-  <si>
-    <t>Verify, only 1 contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_036</t>
-  </si>
-  <si>
-    <t>Verify, on selecting the contact its information is displayed in section 4.</t>
-  </si>
-  <si>
-    <t>TC_037</t>
-  </si>
-  <si>
-    <t>Verify, on clicking executor last name, a side bar is displayed.</t>
-  </si>
-  <si>
-    <t>TC_038</t>
-  </si>
-  <si>
-    <t>Verify, 3 types of selection is available.</t>
-  </si>
-  <si>
-    <t>TC_039</t>
-  </si>
-  <si>
-    <t>Verify, only 1 contact can be dragged and dropped in a each of the type.</t>
-  </si>
-  <si>
-    <t>TC_040</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 5 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_041</t>
-  </si>
-  <si>
-    <t>Verify the selected contacts are displayed under executor, co executor and secondary co executor.</t>
-  </si>
-  <si>
-    <t>TC_042</t>
-  </si>
-  <si>
-    <t>Reset the RW01 form</t>
-  </si>
-  <si>
-    <t>TC_043</t>
-  </si>
-  <si>
-    <t>probateFormsRW02.feature</t>
-  </si>
-  <si>
-    <t>TC_044</t>
-  </si>
-  <si>
-    <t>Verify, correct county name is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_045</t>
-  </si>
-  <si>
-    <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
-  </si>
-  <si>
-    <t>TC_046</t>
-  </si>
-  <si>
-    <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
-  </si>
-  <si>
-    <t>TC_047</t>
-  </si>
-  <si>
-    <t>Verify, county, estate and aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_048</t>
-  </si>
-  <si>
-    <t>Verify, the auto populated fields are not editable.</t>
-  </si>
-  <si>
-    <t>TC_049</t>
-  </si>
-  <si>
-    <t>Verify, names can be added in aka fields.</t>
-  </si>
-  <si>
-    <t>TC_050</t>
-  </si>
-  <si>
-    <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
-  </si>
-  <si>
-    <t>TC_051</t>
-  </si>
-  <si>
-    <t>Verify, amount can be entered in the input fields.</t>
-  </si>
-  <si>
-    <t>TC_052</t>
-  </si>
-  <si>
-    <t>Verify, total estimated value should display total of 1st and last field only.</t>
-  </si>
-  <si>
-    <t>TC_053</t>
-  </si>
-  <si>
-    <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
-  </si>
-  <si>
-    <t>TC_054</t>
-  </si>
-  <si>
-    <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
-  </si>
-  <si>
-    <t>TC_055</t>
-  </si>
-  <si>
-    <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
-  </si>
-  <si>
-    <t>TC_056</t>
-  </si>
-  <si>
-    <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
-  </si>
-  <si>
-    <t>TC_057</t>
-  </si>
-  <si>
-    <t>Verify that selecting option A keeps it selected without affecting option B.</t>
-  </si>
-  <si>
-    <t>TC_058</t>
-  </si>
-  <si>
-    <t>Verify, decedent died date is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_059</t>
-  </si>
-  <si>
-    <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
-  </si>
-  <si>
-    <t>TC_060</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
-  </si>
-  <si>
-    <t>TC_061</t>
-  </si>
-  <si>
-    <t>Verify that selecting option B keeps it selected without affecting option A.</t>
-  </si>
-  <si>
-    <t>TC_062</t>
-  </si>
-  <si>
-    <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
-  </si>
-  <si>
-    <t>TC_063</t>
-  </si>
-  <si>
-    <t>Verify, multiple beneficiaries can be selected.</t>
-  </si>
-  <si>
-    <t>TC_064</t>
-  </si>
-  <si>
-    <t>Verify, bene contacts in the table.</t>
-  </si>
-  <si>
-    <t>TC_065</t>
-  </si>
-  <si>
-    <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
-  </si>
-  <si>
-    <t>TC_066</t>
-  </si>
-  <si>
-    <t>Verify, on checking "Display all heirs on attachment".</t>
-  </si>
-  <si>
-    <t>TC_067</t>
-  </si>
-  <si>
-    <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
-  </si>
-  <si>
-    <t>TC_068</t>
-  </si>
-  <si>
-    <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
-  </si>
-  <si>
-    <t>TC_069</t>
-  </si>
-  <si>
-    <t>Verify fees section.</t>
-  </si>
-  <si>
-    <t>TC_070</t>
-  </si>
-  <si>
-    <t>Verify, attorney can be selected.</t>
-  </si>
-  <si>
-    <t>TC_071</t>
-  </si>
-  <si>
-    <t>Verify, information in decree of the register.</t>
-  </si>
-  <si>
-    <t>TC_072</t>
-  </si>
-  <si>
-    <t>Reset the RW02 form</t>
-  </si>
-  <si>
-    <t>TC_073</t>
-  </si>
-  <si>
-    <t>probateFormsRW03.feature</t>
-  </si>
-  <si>
-    <t>TC_074</t>
-  </si>
-  <si>
-    <t>Verify county, estate and aka names are auto-populated on the form</t>
-  </si>
-  <si>
-    <t>TC_075</t>
-  </si>
-  <si>
-    <t>Verify, the auto-populated fields are not editable.</t>
-  </si>
-  <si>
-    <t>TC_076</t>
-  </si>
-  <si>
-    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
-  </si>
-  <si>
-    <t>TC_077</t>
-  </si>
-  <si>
-    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
-  </si>
-  <si>
-    <t>TC_078</t>
-  </si>
-  <si>
-    <t>Verify, names can be entered in witness fields.</t>
-  </si>
-  <si>
-    <t>TC_079</t>
-  </si>
-  <si>
-    <t>Verify, names updated from signature are reflected in witness names fields.</t>
-  </si>
-  <si>
-    <t>TC_080</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered in address, city, zip fields.</t>
-  </si>
-  <si>
-    <t>TC_081</t>
-  </si>
-  <si>
-    <t>Verify, form is auto saved.</t>
-  </si>
-  <si>
-    <t>TC_082</t>
-  </si>
-  <si>
-    <t>Verify form can be printed in pdf</t>
-  </si>
-  <si>
-    <t>TC_083</t>
-  </si>
-  <si>
-    <t>Reset the RW03 form</t>
-  </si>
-  <si>
-    <t>TC_084</t>
-  </si>
-  <si>
-    <t>probateFormsRW04.feature</t>
   </si>
   <si>
     <t>TC_085</t>
@@ -1828,8 +1828,8 @@
   <sheetPr/>
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85:D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2006,7 +2006,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>8</v>
@@ -2014,16 +2014,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>8</v>
@@ -2031,16 +2031,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>8</v>
@@ -2048,16 +2048,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>8</v>
@@ -2065,16 +2065,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>8</v>
@@ -2082,16 +2082,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>8</v>
@@ -2099,16 +2099,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>8</v>
@@ -2116,16 +2116,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>8</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>24</v>
@@ -2150,13 +2150,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>8</v>
@@ -2167,13 +2167,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>8</v>
@@ -2184,13 +2184,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>8</v>
@@ -2201,13 +2201,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>8</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>8</v>
@@ -2235,13 +2235,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>8</v>
@@ -2252,13 +2252,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>8</v>
@@ -2269,13 +2269,13 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>8</v>
@@ -2286,13 +2286,13 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>8</v>
@@ -2303,13 +2303,13 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>8</v>
@@ -2320,13 +2320,13 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>65</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>8</v>
@@ -2337,13 +2337,13 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>8</v>
@@ -2354,13 +2354,13 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>8</v>
@@ -2371,13 +2371,13 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>8</v>
@@ -2388,13 +2388,13 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>73</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>8</v>
@@ -2405,13 +2405,13 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>8</v>
@@ -2422,13 +2422,13 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>8</v>
@@ -2439,13 +2439,13 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>8</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>8</v>
@@ -2473,13 +2473,13 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>83</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>8</v>
@@ -2490,13 +2490,13 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>85</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>8</v>
@@ -2507,13 +2507,13 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>87</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>8</v>
@@ -2524,13 +2524,13 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>89</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>8</v>
@@ -2541,13 +2541,13 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>8</v>
@@ -2558,13 +2558,13 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>93</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>8</v>
@@ -2575,13 +2575,13 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>95</v>
-      </c>
       <c r="C44" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>8</v>
@@ -2592,13 +2592,13 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>97</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>8</v>
@@ -2609,13 +2609,13 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>99</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>8</v>
@@ -2626,13 +2626,13 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>101</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>8</v>
@@ -2643,13 +2643,13 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>103</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>8</v>
@@ -2660,13 +2660,13 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>8</v>
@@ -2677,13 +2677,13 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>8</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="51" ht="28" spans="1:5">
       <c r="A51" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>108</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>109</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>8</v>
@@ -2711,13 +2711,13 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>8</v>
@@ -2728,13 +2728,13 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>113</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>8</v>
@@ -2745,13 +2745,13 @@
     </row>
     <row r="54" ht="28" spans="1:5">
       <c r="A54" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>8</v>
@@ -2762,13 +2762,13 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>8</v>
@@ -2779,13 +2779,13 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>119</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>8</v>
@@ -2796,13 +2796,13 @@
     </row>
     <row r="57" ht="28" spans="1:5">
       <c r="A57" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>121</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>8</v>
@@ -2813,13 +2813,13 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>123</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>8</v>
@@ -2830,13 +2830,13 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>8</v>
@@ -2847,13 +2847,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>8</v>
@@ -2864,13 +2864,13 @@
     </row>
     <row r="61" ht="28" spans="1:5">
       <c r="A61" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>129</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>8</v>
@@ -2881,13 +2881,13 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="9" t="s">
         <v>130</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>131</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>8</v>
@@ -2898,13 +2898,13 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C63" s="9" t="s">
         <v>132</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>133</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>8</v>
@@ -2915,13 +2915,13 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" s="9" t="s">
         <v>134</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>135</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>8</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C65" s="9" t="s">
         <v>136</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>137</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>8</v>
@@ -2949,13 +2949,13 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>138</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>139</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>8</v>
@@ -2966,13 +2966,13 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>140</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>141</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>8</v>
@@ -2983,13 +2983,13 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>142</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>143</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>8</v>
@@ -3000,13 +3000,13 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>144</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>145</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>8</v>
@@ -3017,13 +3017,13 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>146</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>147</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>8</v>
@@ -3034,13 +3034,13 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C71" s="9" t="s">
         <v>148</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>149</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>8</v>
@@ -3051,13 +3051,13 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>150</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>151</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>8</v>
@@ -3068,13 +3068,13 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C73" s="9" t="s">
         <v>152</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>153</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>8</v>
@@ -3085,13 +3085,13 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B74" s="8" t="s">
-        <v>155</v>
-      </c>
       <c r="C74" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>8</v>
@@ -3102,13 +3102,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C75" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>157</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>8</v>
@@ -3119,13 +3119,13 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C76" s="9" t="s">
         <v>158</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>159</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>8</v>
@@ -3136,13 +3136,13 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C77" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>161</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>8</v>
@@ -3153,13 +3153,13 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C78" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>8</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>8</v>
@@ -3187,13 +3187,13 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C80" s="9" t="s">
         <v>166</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>167</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>8</v>
@@ -3204,13 +3204,13 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C81" s="9" t="s">
         <v>168</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>169</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>8</v>
@@ -3221,13 +3221,13 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C82" s="9" t="s">
         <v>170</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>171</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>8</v>
@@ -3238,13 +3238,13 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C83" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>173</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>8</v>
@@ -3255,13 +3255,13 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C84" s="9" t="s">
         <v>174</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>175</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>8</v>
@@ -3272,16 +3272,16 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B85" s="8" t="s">
+      <c r="C85" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D85" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>8</v>
@@ -3292,13 +3292,13 @@
         <v>178</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>179</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>8</v>
@@ -3309,13 +3309,13 @@
         <v>180</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>181</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>8</v>
@@ -3326,13 +3326,13 @@
         <v>182</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>183</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>8</v>
@@ -3343,13 +3343,13 @@
         <v>184</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>185</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>8</v>
@@ -3360,13 +3360,13 @@
         <v>186</v>
       </c>
       <c r="B90" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D90" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>8</v>
@@ -3377,13 +3377,13 @@
         <v>187</v>
       </c>
       <c r="B91" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D91" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>8</v>
@@ -3394,13 +3394,13 @@
         <v>188</v>
       </c>
       <c r="B92" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D92" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>8</v>
@@ -3411,13 +3411,13 @@
         <v>189</v>
       </c>
       <c r="B93" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D93" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>8</v>
@@ -3428,13 +3428,13 @@
         <v>190</v>
       </c>
       <c r="B94" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D94" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>8</v>
@@ -3445,13 +3445,13 @@
         <v>191</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C95" s="8" t="s">
         <v>192</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>8</v>
@@ -3459,7 +3459,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D9 D2:D8 D10:D16 D17:D95 E2:E95 F2:F3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 E25 E43 E85 D25:D43 D85:D95 E26:E42 E86:E95 F2:F3 D2:E24 D73:E84 D44:E72">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">

</xml_diff>

<commit_message>
added TCs for RW05 probate form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="207">
   <si>
     <t>ID</t>
   </si>
@@ -560,52 +560,94 @@
     <t>probateFormsRW04.feature</t>
   </si>
   <si>
+    <t>TC_085</t>
+  </si>
+  <si>
+    <t>Verify, correct title is displayed on the form's header.</t>
+  </si>
+  <si>
+    <t>TC_086</t>
+  </si>
+  <si>
+    <t>Verify, county, and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_087</t>
+  </si>
+  <si>
+    <t>Verify, correct estate's name is displayed on the form.</t>
+  </si>
+  <si>
+    <t>TC_088</t>
+  </si>
+  <si>
+    <t>Verify, name of the decedent should be auto populated from the form.</t>
+  </si>
+  <si>
+    <t>TC_089</t>
+  </si>
+  <si>
+    <t>TC_090</t>
+  </si>
+  <si>
+    <t>TC_091</t>
+  </si>
+  <si>
+    <t>TC_092</t>
+  </si>
+  <si>
+    <t>TC_093</t>
+  </si>
+  <si>
+    <t>TC_094</t>
+  </si>
+  <si>
+    <t>Reset the RW04 form</t>
+  </si>
+  <si>
+    <t>TC_095</t>
+  </si>
+  <si>
+    <t>probateFormsRW05.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>TC_085</t>
-  </si>
-  <si>
-    <t>Verify, correct title is displayed on the form's header.</t>
-  </si>
-  <si>
-    <t>TC_086</t>
-  </si>
-  <si>
-    <t>Verify, county, and aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_087</t>
-  </si>
-  <si>
-    <t>Verify, correct estate's name is displayed on the form.</t>
-  </si>
-  <si>
-    <t>TC_088</t>
-  </si>
-  <si>
-    <t>Verify, name of the decedent should be auto populated from the form.</t>
-  </si>
-  <si>
-    <t>TC_089</t>
-  </si>
-  <si>
-    <t>TC_090</t>
-  </si>
-  <si>
-    <t>TC_091</t>
-  </si>
-  <si>
-    <t>TC_092</t>
-  </si>
-  <si>
-    <t>TC_093</t>
-  </si>
-  <si>
-    <t>TC_094</t>
-  </si>
-  <si>
-    <t>Reset the RW04 form</t>
+    <t>TC_096</t>
+  </si>
+  <si>
+    <t>TC_097</t>
+  </si>
+  <si>
+    <t>TC_098</t>
+  </si>
+  <si>
+    <t>TC_099</t>
+  </si>
+  <si>
+    <t>TC_100</t>
+  </si>
+  <si>
+    <t>TC_101</t>
+  </si>
+  <si>
+    <t>TC_102</t>
+  </si>
+  <si>
+    <t>TC_103</t>
+  </si>
+  <si>
+    <t>Verify, on checking notary checkbox, notary section displays.</t>
+  </si>
+  <si>
+    <t>TC_104</t>
+  </si>
+  <si>
+    <t>TC_105</t>
+  </si>
+  <si>
+    <t>Reset the RW05 form</t>
   </si>
 </sst>
 </file>
@@ -1284,7 +1326,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1307,6 +1349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1826,10 +1869,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F95"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85:D95"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2583,7 +2626,7 @@
       <c r="C44" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -2600,7 +2643,7 @@
       <c r="C45" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -2617,7 +2660,7 @@
       <c r="C46" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E46" s="3" t="s">
@@ -2634,7 +2677,7 @@
       <c r="C47" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -2651,7 +2694,7 @@
       <c r="C48" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E48" s="3" t="s">
@@ -2668,7 +2711,7 @@
       <c r="C49" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E49" s="3" t="s">
@@ -2685,7 +2728,7 @@
       <c r="C50" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E50" s="3" t="s">
@@ -2702,7 +2745,7 @@
       <c r="C51" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E51" s="3" t="s">
@@ -2719,7 +2762,7 @@
       <c r="C52" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E52" s="3" t="s">
@@ -2736,7 +2779,7 @@
       <c r="C53" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E53" s="3" t="s">
@@ -2753,7 +2796,7 @@
       <c r="C54" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E54" s="3" t="s">
@@ -2770,7 +2813,7 @@
       <c r="C55" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E55" s="3" t="s">
@@ -2787,7 +2830,7 @@
       <c r="C56" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E56" s="3" t="s">
@@ -2804,7 +2847,7 @@
       <c r="C57" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E57" s="3" t="s">
@@ -2821,7 +2864,7 @@
       <c r="C58" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E58" s="3" t="s">
@@ -2838,7 +2881,7 @@
       <c r="C59" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E59" s="3" t="s">
@@ -2855,7 +2898,7 @@
       <c r="C60" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E60" s="3" t="s">
@@ -2872,7 +2915,7 @@
       <c r="C61" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E61" s="3" t="s">
@@ -2889,7 +2932,7 @@
       <c r="C62" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E62" s="3" t="s">
@@ -2906,7 +2949,7 @@
       <c r="C63" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E63" s="3" t="s">
@@ -2923,7 +2966,7 @@
       <c r="C64" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E64" s="3" t="s">
@@ -2940,7 +2983,7 @@
       <c r="C65" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E65" s="3" t="s">
@@ -2957,7 +3000,7 @@
       <c r="C66" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -2974,7 +3017,7 @@
       <c r="C67" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E67" s="3" t="s">
@@ -2991,7 +3034,7 @@
       <c r="C68" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E68" s="3" t="s">
@@ -3008,7 +3051,7 @@
       <c r="C69" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E69" s="3" t="s">
@@ -3025,7 +3068,7 @@
       <c r="C70" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E70" s="3" t="s">
@@ -3042,7 +3085,7 @@
       <c r="C71" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E71" s="3" t="s">
@@ -3059,7 +3102,7 @@
       <c r="C72" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D72" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E72" s="3" t="s">
@@ -3076,7 +3119,7 @@
       <c r="C73" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D73" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E73" s="3" t="s">
@@ -3281,7 +3324,7 @@
         <v>58</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>8</v>
@@ -3289,16 +3332,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>8</v>
@@ -3306,16 +3349,16 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>8</v>
@@ -3323,16 +3366,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>8</v>
@@ -3340,16 +3383,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>8</v>
@@ -3357,7 +3400,7 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>176</v>
@@ -3366,7 +3409,7 @@
         <v>162</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>8</v>
@@ -3374,7 +3417,7 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>176</v>
@@ -3383,7 +3426,7 @@
         <v>164</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>8</v>
@@ -3391,7 +3434,7 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>176</v>
@@ -3400,7 +3443,7 @@
         <v>166</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>8</v>
@@ -3408,7 +3451,7 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>176</v>
@@ -3417,7 +3460,7 @@
         <v>168</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>8</v>
@@ -3425,7 +3468,7 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>176</v>
@@ -3434,7 +3477,7 @@
         <v>170</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>8</v>
@@ -3442,24 +3485,211 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C95" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D95" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="E95" s="3" t="s">
+      <c r="B96" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C100" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C101" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C102" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C104" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C105" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C106" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E106" s="3" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 E25 E43 E85 D25:D43 D85:D95 E26:E42 E86:E95 F2:F3 D2:E24 D73:E84 D44:E72">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 E84 D84:D94 D95:D106 E85:E94 E95:E106 F2:F3 D25:E43 D44:E83 D2:E24">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">

</xml_diff>

<commit_message>
updated code of RW01 probate form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -206,6 +206,9 @@
     <t>Open Estate</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_026</t>
   </si>
   <si>
@@ -609,9 +612,6 @@
   </si>
   <si>
     <t>probateFormsRW05.feature</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>TC_096</t>
@@ -1326,7 +1326,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1349,7 +1349,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1871,8 +1870,8 @@
   <sheetPr/>
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="G92" sqref="G92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2201,7 +2200,7 @@
       <c r="C19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -2218,7 +2217,7 @@
       <c r="C20" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -2252,7 +2251,7 @@
       <c r="C22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -2269,7 +2268,7 @@
       <c r="C23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -2286,7 +2285,7 @@
       <c r="C24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -2303,7 +2302,7 @@
       <c r="C25" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -2321,7 +2320,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>8</v>
@@ -2329,16 +2328,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>8</v>
@@ -2346,16 +2345,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>8</v>
@@ -2363,16 +2362,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>8</v>
@@ -2380,16 +2379,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>8</v>
@@ -2397,16 +2396,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>8</v>
@@ -2414,16 +2413,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>8</v>
@@ -2431,16 +2430,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>8</v>
@@ -2448,16 +2447,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>8</v>
@@ -2465,16 +2464,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>8</v>
@@ -2482,16 +2481,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>8</v>
@@ -2499,16 +2498,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>8</v>
@@ -2516,16 +2515,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>8</v>
@@ -2533,16 +2532,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>8</v>
@@ -2550,16 +2549,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>8</v>
@@ -2567,16 +2566,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>8</v>
@@ -2584,16 +2583,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>8</v>
@@ -2601,16 +2600,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>8</v>
@@ -2618,10 +2617,10 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>58</v>
@@ -2635,13 +2634,13 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>94</v>
-      </c>
       <c r="C45" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>8</v>
@@ -2652,13 +2651,13 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>8</v>
@@ -2669,13 +2668,13 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>8</v>
@@ -2686,13 +2685,13 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>8</v>
@@ -2703,13 +2702,13 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>8</v>
@@ -2720,13 +2719,13 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>8</v>
@@ -2737,13 +2736,13 @@
     </row>
     <row r="51" ht="28" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>8</v>
@@ -2754,13 +2753,13 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>8</v>
@@ -2771,13 +2770,13 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>8</v>
@@ -2788,13 +2787,13 @@
     </row>
     <row r="54" ht="28" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>8</v>
@@ -2805,13 +2804,13 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>8</v>
@@ -2822,13 +2821,13 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>8</v>
@@ -2839,13 +2838,13 @@
     </row>
     <row r="57" ht="28" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>8</v>
@@ -2856,13 +2855,13 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>8</v>
@@ -2873,13 +2872,13 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>8</v>
@@ -2890,13 +2889,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>8</v>
@@ -2907,13 +2906,13 @@
     </row>
     <row r="61" ht="28" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>8</v>
@@ -2924,13 +2923,13 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>8</v>
@@ -2941,13 +2940,13 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>8</v>
@@ -2958,13 +2957,13 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>8</v>
@@ -2975,13 +2974,13 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>8</v>
@@ -2992,13 +2991,13 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>8</v>
@@ -3009,13 +3008,13 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>8</v>
@@ -3026,13 +3025,13 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>8</v>
@@ -3043,13 +3042,13 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>8</v>
@@ -3060,13 +3059,13 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>8</v>
@@ -3077,13 +3076,13 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>8</v>
@@ -3094,13 +3093,13 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>8</v>
@@ -3111,13 +3110,13 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>8</v>
@@ -3128,15 +3127,15 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D74" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E74" s="3" t="s">
@@ -3145,15 +3144,15 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B75" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="C75" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D75" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D75" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E75" s="3" t="s">
@@ -3162,15 +3161,15 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="D76" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D76" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E76" s="3" t="s">
@@ -3179,15 +3178,15 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D77" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D77" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E77" s="3" t="s">
@@ -3196,15 +3195,15 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="D78" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D78" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E78" s="3" t="s">
@@ -3213,15 +3212,15 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D79" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D79" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E79" s="3" t="s">
@@ -3230,15 +3229,15 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D80" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E80" s="3" t="s">
@@ -3247,15 +3246,15 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="D81" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D81" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E81" s="3" t="s">
@@ -3264,15 +3263,15 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="D82" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D82" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E82" s="3" t="s">
@@ -3281,15 +3280,15 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="D83" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E83" s="3" t="s">
@@ -3298,15 +3297,15 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="D84" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D84" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E84" s="3" t="s">
@@ -3315,10 +3314,10 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>58</v>
@@ -3332,13 +3331,13 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B86" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B86" s="8" t="s">
-        <v>176</v>
-      </c>
       <c r="C86" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>8</v>
@@ -3349,13 +3348,13 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>8</v>
@@ -3366,13 +3365,13 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>8</v>
@@ -3383,13 +3382,13 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>8</v>
@@ -3400,13 +3399,13 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>8</v>
@@ -3417,13 +3416,13 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>8</v>
@@ -3434,13 +3433,13 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>8</v>
@@ -3451,13 +3450,13 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>8</v>
@@ -3468,13 +3467,13 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>8</v>
@@ -3485,13 +3484,13 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>8</v>
@@ -3502,16 +3501,16 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C96" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C96" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>194</v>
+        <v>8</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>8</v>
@@ -3522,13 +3521,13 @@
         <v>195</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C97" s="10" t="s">
-        <v>102</v>
+        <v>194</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>194</v>
+        <v>8</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -3539,13 +3538,13 @@
         <v>196</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C98" s="10" t="s">
-        <v>158</v>
+        <v>194</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>194</v>
+        <v>8</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -3556,13 +3555,13 @@
         <v>197</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C99" s="10" t="s">
-        <v>160</v>
+        <v>194</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>161</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>194</v>
+        <v>8</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -3573,13 +3572,13 @@
         <v>198</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C100" s="10" t="s">
-        <v>162</v>
+        <v>194</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>163</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>194</v>
+        <v>8</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -3590,13 +3589,13 @@
         <v>199</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C101" s="10" t="s">
-        <v>164</v>
+        <v>194</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>165</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>194</v>
+        <v>8</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -3607,13 +3606,13 @@
         <v>200</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C102" s="10" t="s">
-        <v>166</v>
+        <v>194</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>167</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>194</v>
+        <v>8</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -3624,13 +3623,13 @@
         <v>201</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C103" s="10" t="s">
-        <v>168</v>
+        <v>194</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>194</v>
+        <v>8</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -3641,13 +3640,13 @@
         <v>202</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C104" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C104" s="8" t="s">
         <v>203</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>194</v>
+        <v>8</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -3658,13 +3657,13 @@
         <v>204</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C105" s="10" t="s">
-        <v>170</v>
+        <v>194</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>171</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>194</v>
+        <v>8</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -3675,13 +3674,13 @@
         <v>205</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C106" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C106" s="8" t="s">
         <v>206</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>194</v>
+        <v>8</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -3689,11 +3688,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 E84 D84:D94 D95:D106 E85:E94 E95:E106 F2:F3 D25:E43 D44:E83 D2:E24">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E18 E25 E26 D1:D8 D18:D25 D26:D42 E2:E8 E19:E24 E27:E42 F2:F3 D9:E17 D43:E106">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
added TCs for RW06 probate form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="226">
   <si>
     <t>ID</t>
   </si>
@@ -206,448 +206,505 @@
     <t>Open Estate</t>
   </si>
   <si>
+    <t>TC_026</t>
+  </si>
+  <si>
+    <t>Verify, file no. is displayed at the top of the form.</t>
+  </si>
+  <si>
+    <t>TC_027</t>
+  </si>
+  <si>
+    <t>Verify, decedent information is displayed in section1 of the form.</t>
+  </si>
+  <si>
+    <t>TC_028</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 2 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_029</t>
+  </si>
+  <si>
+    <t>Verify, in section 2 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_030</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 3 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_031</t>
+  </si>
+  <si>
+    <t>Verify, in section 3 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_032</t>
+  </si>
+  <si>
+    <t>Verify, on clicking other checkbox, text area is enabled.</t>
+  </si>
+  <si>
+    <t>TC_033</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 4 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_034</t>
+  </si>
+  <si>
+    <t>Verify, on clicking last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_035</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_036</t>
+  </si>
+  <si>
+    <t>Verify, on selecting the contact its information is displayed in section 4.</t>
+  </si>
+  <si>
+    <t>TC_037</t>
+  </si>
+  <si>
+    <t>Verify, on clicking executor last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_038</t>
+  </si>
+  <si>
+    <t>Verify, 3 types of selection is available.</t>
+  </si>
+  <si>
+    <t>TC_039</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be dragged and dropped in a each of the type.</t>
+  </si>
+  <si>
+    <t>TC_040</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 5 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_041</t>
+  </si>
+  <si>
+    <t>Verify the selected contacts are displayed under executor, co executor and secondary co executor.</t>
+  </si>
+  <si>
+    <t>TC_042</t>
+  </si>
+  <si>
+    <t>Reset the RW01 form</t>
+  </si>
+  <si>
+    <t>TC_043</t>
+  </si>
+  <si>
+    <t>probateFormsRW02.feature</t>
+  </si>
+  <si>
+    <t>TC_044</t>
+  </si>
+  <si>
+    <t>Verify, correct county name is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_045</t>
+  </si>
+  <si>
+    <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
+  </si>
+  <si>
+    <t>TC_046</t>
+  </si>
+  <si>
+    <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
+  </si>
+  <si>
+    <t>TC_047</t>
+  </si>
+  <si>
+    <t>Verify, county, estate and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_048</t>
+  </si>
+  <si>
+    <t>Verify, the auto populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_049</t>
+  </si>
+  <si>
+    <t>Verify, names can be added in aka fields.</t>
+  </si>
+  <si>
+    <t>TC_050</t>
+  </si>
+  <si>
+    <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
+  </si>
+  <si>
+    <t>TC_051</t>
+  </si>
+  <si>
+    <t>Verify, amount can be entered in the input fields.</t>
+  </si>
+  <si>
+    <t>TC_052</t>
+  </si>
+  <si>
+    <t>Verify, total estimated value should display total of 1st and last field only.</t>
+  </si>
+  <si>
+    <t>TC_053</t>
+  </si>
+  <si>
+    <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_054</t>
+  </si>
+  <si>
+    <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_055</t>
+  </si>
+  <si>
+    <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
+  </si>
+  <si>
+    <t>TC_056</t>
+  </si>
+  <si>
+    <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
+  </si>
+  <si>
+    <t>TC_057</t>
+  </si>
+  <si>
+    <t>Verify that selecting option A keeps it selected without affecting option B.</t>
+  </si>
+  <si>
+    <t>TC_058</t>
+  </si>
+  <si>
+    <t>Verify, decedent died date is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_059</t>
+  </si>
+  <si>
+    <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
+  </si>
+  <si>
+    <t>TC_060</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
+  </si>
+  <si>
+    <t>TC_061</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B keeps it selected without affecting option A.</t>
+  </si>
+  <si>
+    <t>TC_062</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
+  </si>
+  <si>
+    <t>TC_063</t>
+  </si>
+  <si>
+    <t>Verify, multiple beneficiaries can be selected.</t>
+  </si>
+  <si>
+    <t>TC_064</t>
+  </si>
+  <si>
+    <t>Verify, bene contacts in the table.</t>
+  </si>
+  <si>
+    <t>TC_065</t>
+  </si>
+  <si>
+    <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
+  </si>
+  <si>
+    <t>TC_066</t>
+  </si>
+  <si>
+    <t>Verify, on checking "Display all heirs on attachment".</t>
+  </si>
+  <si>
+    <t>TC_067</t>
+  </si>
+  <si>
+    <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
+  </si>
+  <si>
+    <t>TC_068</t>
+  </si>
+  <si>
+    <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
+  </si>
+  <si>
+    <t>TC_069</t>
+  </si>
+  <si>
+    <t>Verify fees section.</t>
+  </si>
+  <si>
+    <t>TC_070</t>
+  </si>
+  <si>
+    <t>Verify, attorney can be selected.</t>
+  </si>
+  <si>
+    <t>TC_071</t>
+  </si>
+  <si>
+    <t>Verify, information in decree of the register.</t>
+  </si>
+  <si>
+    <t>TC_072</t>
+  </si>
+  <si>
+    <t>Reset the RW02 form</t>
+  </si>
+  <si>
+    <t>TC_073</t>
+  </si>
+  <si>
+    <t>probateFormsRW03.feature</t>
+  </si>
+  <si>
+    <t>TC_074</t>
+  </si>
+  <si>
+    <t>Verify county, estate and aka names are auto-populated on the form</t>
+  </si>
+  <si>
+    <t>TC_075</t>
+  </si>
+  <si>
+    <t>Verify, the auto-populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_076</t>
+  </si>
+  <si>
+    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
+  </si>
+  <si>
+    <t>TC_077</t>
+  </si>
+  <si>
+    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
+  </si>
+  <si>
+    <t>TC_078</t>
+  </si>
+  <si>
+    <t>Verify, names can be entered in witness fields.</t>
+  </si>
+  <si>
+    <t>TC_079</t>
+  </si>
+  <si>
+    <t>Verify, names updated from signature are reflected in witness names fields.</t>
+  </si>
+  <si>
+    <t>TC_080</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered in address, city, zip fields.</t>
+  </si>
+  <si>
+    <t>TC_081</t>
+  </si>
+  <si>
+    <t>Verify, form is auto saved.</t>
+  </si>
+  <si>
+    <t>TC_082</t>
+  </si>
+  <si>
+    <t>Verify form can be printed in pdf</t>
+  </si>
+  <si>
+    <t>TC_083</t>
+  </si>
+  <si>
+    <t>Reset the RW03 form</t>
+  </si>
+  <si>
+    <t>TC_084</t>
+  </si>
+  <si>
+    <t>probateFormsRW04.feature</t>
+  </si>
+  <si>
+    <t>TC_085</t>
+  </si>
+  <si>
+    <t>Verify, correct title is displayed on the form's header.</t>
+  </si>
+  <si>
+    <t>TC_086</t>
+  </si>
+  <si>
+    <t>Verify, county, and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_087</t>
+  </si>
+  <si>
+    <t>Verify, correct estate's name is displayed on the form.</t>
+  </si>
+  <si>
+    <t>TC_088</t>
+  </si>
+  <si>
+    <t>Verify, name of the decedent should be auto populated from the form.</t>
+  </si>
+  <si>
+    <t>TC_089</t>
+  </si>
+  <si>
+    <t>TC_090</t>
+  </si>
+  <si>
+    <t>TC_091</t>
+  </si>
+  <si>
+    <t>TC_092</t>
+  </si>
+  <si>
+    <t>TC_093</t>
+  </si>
+  <si>
+    <t>TC_094</t>
+  </si>
+  <si>
+    <t>Reset the RW04 form</t>
+  </si>
+  <si>
+    <t>TC_095</t>
+  </si>
+  <si>
+    <t>probateFormsRW05.feature</t>
+  </si>
+  <si>
+    <t>TC_096</t>
+  </si>
+  <si>
+    <t>TC_097</t>
+  </si>
+  <si>
+    <t>TC_098</t>
+  </si>
+  <si>
+    <t>TC_099</t>
+  </si>
+  <si>
+    <t>TC_100</t>
+  </si>
+  <si>
+    <t>TC_101</t>
+  </si>
+  <si>
+    <t>TC_102</t>
+  </si>
+  <si>
+    <t>TC_103</t>
+  </si>
+  <si>
+    <t>Verify, on checking notary checkbox, notary section displays.</t>
+  </si>
+  <si>
+    <t>TC_104</t>
+  </si>
+  <si>
+    <t>TC_105</t>
+  </si>
+  <si>
+    <t>Reset the RW05 form</t>
+  </si>
+  <si>
+    <t>TC_106</t>
+  </si>
+  <si>
+    <t>probateFormsRW06.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>TC_026</t>
-  </si>
-  <si>
-    <t>Verify, file no. is displayed at the top of the form.</t>
-  </si>
-  <si>
-    <t>TC_027</t>
-  </si>
-  <si>
-    <t>Verify, decedent information is displayed in section1 of the form.</t>
-  </si>
-  <si>
-    <t>TC_028</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 2 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_029</t>
-  </si>
-  <si>
-    <t>Verify, in section 2 only 1 checkbox can be checked.</t>
-  </si>
-  <si>
-    <t>TC_030</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 3 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_031</t>
-  </si>
-  <si>
-    <t>Verify, in section 3 only 1 checkbox can be checked.</t>
-  </si>
-  <si>
-    <t>TC_032</t>
-  </si>
-  <si>
-    <t>Verify, on clicking other checkbox, text area is enabled.</t>
-  </si>
-  <si>
-    <t>TC_033</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 4 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_034</t>
-  </si>
-  <si>
-    <t>Verify, on clicking last name, a side bar is displayed.</t>
-  </si>
-  <si>
-    <t>TC_035</t>
-  </si>
-  <si>
-    <t>Verify, only 1 contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_036</t>
-  </si>
-  <si>
-    <t>Verify, on selecting the contact its information is displayed in section 4.</t>
-  </si>
-  <si>
-    <t>TC_037</t>
-  </si>
-  <si>
-    <t>Verify, on clicking executor last name, a side bar is displayed.</t>
-  </si>
-  <si>
-    <t>TC_038</t>
-  </si>
-  <si>
-    <t>Verify, 3 types of selection is available.</t>
-  </si>
-  <si>
-    <t>TC_039</t>
-  </si>
-  <si>
-    <t>Verify, only 1 contact can be dragged and dropped in a each of the type.</t>
-  </si>
-  <si>
-    <t>TC_040</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 5 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_041</t>
-  </si>
-  <si>
-    <t>Verify the selected contacts are displayed under executor, co executor and secondary co executor.</t>
-  </si>
-  <si>
-    <t>TC_042</t>
-  </si>
-  <si>
-    <t>Reset the RW01 form</t>
-  </si>
-  <si>
-    <t>TC_043</t>
-  </si>
-  <si>
-    <t>probateFormsRW02.feature</t>
-  </si>
-  <si>
-    <t>TC_044</t>
-  </si>
-  <si>
-    <t>Verify, correct county name is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_045</t>
-  </si>
-  <si>
-    <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
-  </si>
-  <si>
-    <t>TC_046</t>
-  </si>
-  <si>
-    <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
-  </si>
-  <si>
-    <t>TC_047</t>
-  </si>
-  <si>
-    <t>Verify, county, estate and aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_048</t>
-  </si>
-  <si>
-    <t>Verify, the auto populated fields are not editable.</t>
-  </si>
-  <si>
-    <t>TC_049</t>
-  </si>
-  <si>
-    <t>Verify, names can be added in aka fields.</t>
-  </si>
-  <si>
-    <t>TC_050</t>
-  </si>
-  <si>
-    <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
-  </si>
-  <si>
-    <t>TC_051</t>
-  </si>
-  <si>
-    <t>Verify, amount can be entered in the input fields.</t>
-  </si>
-  <si>
-    <t>TC_052</t>
-  </si>
-  <si>
-    <t>Verify, total estimated value should display total of 1st and last field only.</t>
-  </si>
-  <si>
-    <t>TC_053</t>
-  </si>
-  <si>
-    <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
-  </si>
-  <si>
-    <t>TC_054</t>
-  </si>
-  <si>
-    <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
-  </si>
-  <si>
-    <t>TC_055</t>
-  </si>
-  <si>
-    <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
-  </si>
-  <si>
-    <t>TC_056</t>
-  </si>
-  <si>
-    <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
-  </si>
-  <si>
-    <t>TC_057</t>
-  </si>
-  <si>
-    <t>Verify that selecting option A keeps it selected without affecting option B.</t>
-  </si>
-  <si>
-    <t>TC_058</t>
-  </si>
-  <si>
-    <t>Verify, decedent died date is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_059</t>
-  </si>
-  <si>
-    <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
-  </si>
-  <si>
-    <t>TC_060</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
-  </si>
-  <si>
-    <t>TC_061</t>
-  </si>
-  <si>
-    <t>Verify that selecting option B keeps it selected without affecting option A.</t>
-  </si>
-  <si>
-    <t>TC_062</t>
-  </si>
-  <si>
-    <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
-  </si>
-  <si>
-    <t>TC_063</t>
-  </si>
-  <si>
-    <t>Verify, multiple beneficiaries can be selected.</t>
-  </si>
-  <si>
-    <t>TC_064</t>
-  </si>
-  <si>
-    <t>Verify, bene contacts in the table.</t>
-  </si>
-  <si>
-    <t>TC_065</t>
-  </si>
-  <si>
-    <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
-  </si>
-  <si>
-    <t>TC_066</t>
-  </si>
-  <si>
-    <t>Verify, on checking "Display all heirs on attachment".</t>
-  </si>
-  <si>
-    <t>TC_067</t>
-  </si>
-  <si>
-    <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
-  </si>
-  <si>
-    <t>TC_068</t>
-  </si>
-  <si>
-    <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
-  </si>
-  <si>
-    <t>TC_069</t>
-  </si>
-  <si>
-    <t>Verify fees section.</t>
-  </si>
-  <si>
-    <t>TC_070</t>
-  </si>
-  <si>
-    <t>Verify, attorney can be selected.</t>
-  </si>
-  <si>
-    <t>TC_071</t>
-  </si>
-  <si>
-    <t>Verify, information in decree of the register.</t>
-  </si>
-  <si>
-    <t>TC_072</t>
-  </si>
-  <si>
-    <t>Reset the RW02 form</t>
-  </si>
-  <si>
-    <t>TC_073</t>
-  </si>
-  <si>
-    <t>probateFormsRW03.feature</t>
-  </si>
-  <si>
-    <t>TC_074</t>
-  </si>
-  <si>
-    <t>Verify county, estate and aka names are auto-populated on the form</t>
-  </si>
-  <si>
-    <t>TC_075</t>
-  </si>
-  <si>
-    <t>Verify, the auto-populated fields are not editable.</t>
-  </si>
-  <si>
-    <t>TC_076</t>
-  </si>
-  <si>
-    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
-  </si>
-  <si>
-    <t>TC_077</t>
-  </si>
-  <si>
-    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
-  </si>
-  <si>
-    <t>TC_078</t>
-  </si>
-  <si>
-    <t>Verify, names can be entered in witness fields.</t>
-  </si>
-  <si>
-    <t>TC_079</t>
-  </si>
-  <si>
-    <t>Verify, names updated from signature are reflected in witness names fields.</t>
-  </si>
-  <si>
-    <t>TC_080</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered in address, city, zip fields.</t>
-  </si>
-  <si>
-    <t>TC_081</t>
-  </si>
-  <si>
-    <t>Verify, form is auto saved.</t>
-  </si>
-  <si>
-    <t>TC_082</t>
-  </si>
-  <si>
-    <t>Verify form can be printed in pdf</t>
-  </si>
-  <si>
-    <t>TC_083</t>
-  </si>
-  <si>
-    <t>Reset the RW03 form</t>
-  </si>
-  <si>
-    <t>TC_084</t>
-  </si>
-  <si>
-    <t>probateFormsRW04.feature</t>
-  </si>
-  <si>
-    <t>TC_085</t>
-  </si>
-  <si>
-    <t>Verify, correct title is displayed on the form's header.</t>
-  </si>
-  <si>
-    <t>TC_086</t>
-  </si>
-  <si>
-    <t>Verify, county, and aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_087</t>
-  </si>
-  <si>
-    <t>Verify, correct estate's name is displayed on the form.</t>
-  </si>
-  <si>
-    <t>TC_088</t>
-  </si>
-  <si>
-    <t>Verify, name of the decedent should be auto populated from the form.</t>
-  </si>
-  <si>
-    <t>TC_089</t>
-  </si>
-  <si>
-    <t>TC_090</t>
-  </si>
-  <si>
-    <t>TC_091</t>
-  </si>
-  <si>
-    <t>TC_092</t>
-  </si>
-  <si>
-    <t>TC_093</t>
-  </si>
-  <si>
-    <t>TC_094</t>
-  </si>
-  <si>
-    <t>Reset the RW04 form</t>
-  </si>
-  <si>
-    <t>TC_095</t>
-  </si>
-  <si>
-    <t>probateFormsRW05.feature</t>
-  </si>
-  <si>
-    <t>TC_096</t>
-  </si>
-  <si>
-    <t>TC_097</t>
-  </si>
-  <si>
-    <t>TC_098</t>
-  </si>
-  <si>
-    <t>TC_099</t>
-  </si>
-  <si>
-    <t>TC_100</t>
-  </si>
-  <si>
-    <t>TC_101</t>
-  </si>
-  <si>
-    <t>TC_102</t>
-  </si>
-  <si>
-    <t>TC_103</t>
-  </si>
-  <si>
-    <t>Verify, on checking notary checkbox, notary section displays.</t>
-  </si>
-  <si>
-    <t>TC_104</t>
-  </si>
-  <si>
-    <t>TC_105</t>
-  </si>
-  <si>
-    <t>Reset the RW05 form</t>
+    <t>TC_107</t>
+  </si>
+  <si>
+    <t>TC_108</t>
+  </si>
+  <si>
+    <t>TC_109</t>
+  </si>
+  <si>
+    <t>Verify, form is repeated based on the number of contacts selected.</t>
+  </si>
+  <si>
+    <t>TC_110</t>
+  </si>
+  <si>
+    <t>Verify, corporate fiduciary selected is reflected in the corporate name field.</t>
+  </si>
+  <si>
+    <t>TC_111</t>
+  </si>
+  <si>
+    <t>Verify, details of the selected contact's is displayed in the block under it.</t>
+  </si>
+  <si>
+    <t>TC_112</t>
+  </si>
+  <si>
+    <t>Verify, on clicking signature of person, beneficiary contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_113</t>
+  </si>
+  <si>
+    <t>TC_114</t>
+  </si>
+  <si>
+    <t>Verify, contact details are correctly displayed on each page.</t>
+  </si>
+  <si>
+    <t>TC_115</t>
+  </si>
+  <si>
+    <t>Verify, Relationship, date and reason text box fields are not same for each field.</t>
+  </si>
+  <si>
+    <t>TC_116</t>
+  </si>
+  <si>
+    <t>Reset the RW06 form</t>
   </si>
 </sst>
 </file>
@@ -1326,7 +1383,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1349,6 +1406,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1868,10 +1926,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2319,8 +2377,8 @@
       <c r="C26" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>59</v>
+      <c r="D26" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>8</v>
@@ -2328,16 +2386,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>8</v>
@@ -2345,16 +2403,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>8</v>
@@ -2362,16 +2420,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>59</v>
+        <v>64</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>8</v>
@@ -2379,16 +2437,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>59</v>
+        <v>66</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>8</v>
@@ -2396,16 +2454,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>59</v>
+        <v>68</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>8</v>
@@ -2413,16 +2471,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>59</v>
+        <v>70</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>8</v>
@@ -2430,16 +2488,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>59</v>
+        <v>72</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>8</v>
@@ -2447,16 +2505,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>59</v>
+        <v>74</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>8</v>
@@ -2464,16 +2522,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>59</v>
+        <v>76</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>8</v>
@@ -2481,16 +2539,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>59</v>
+        <v>78</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>8</v>
@@ -2498,16 +2556,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>59</v>
+        <v>80</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>8</v>
@@ -2515,16 +2573,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>59</v>
+        <v>82</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>8</v>
@@ -2532,16 +2590,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>59</v>
+        <v>84</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>8</v>
@@ -2549,16 +2607,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>59</v>
+        <v>86</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>8</v>
@@ -2566,16 +2624,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>59</v>
+        <v>88</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>8</v>
@@ -2583,16 +2641,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>59</v>
+        <v>90</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>8</v>
@@ -2600,16 +2658,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>59</v>
+        <v>92</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>8</v>
@@ -2617,15 +2675,15 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -2634,13 +2692,13 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>97</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>8</v>
@@ -2651,13 +2709,13 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>99</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>8</v>
@@ -2668,13 +2726,13 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>101</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>8</v>
@@ -2685,13 +2743,13 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>103</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>8</v>
@@ -2702,13 +2760,13 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>8</v>
@@ -2719,13 +2777,13 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>8</v>
@@ -2736,13 +2794,13 @@
     </row>
     <row r="51" ht="28" spans="1:5">
       <c r="A51" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>108</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>109</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>8</v>
@@ -2753,13 +2811,13 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>8</v>
@@ -2770,13 +2828,13 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>113</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>8</v>
@@ -2787,13 +2845,13 @@
     </row>
     <row r="54" ht="28" spans="1:5">
       <c r="A54" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>8</v>
@@ -2804,13 +2862,13 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>8</v>
@@ -2821,13 +2879,13 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>119</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>8</v>
@@ -2838,13 +2896,13 @@
     </row>
     <row r="57" ht="28" spans="1:5">
       <c r="A57" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>121</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>8</v>
@@ -2855,13 +2913,13 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>123</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>8</v>
@@ -2872,13 +2930,13 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>8</v>
@@ -2889,13 +2947,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>8</v>
@@ -2906,13 +2964,13 @@
     </row>
     <row r="61" ht="28" spans="1:5">
       <c r="A61" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>129</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>8</v>
@@ -2923,13 +2981,13 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="9" t="s">
         <v>130</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>131</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>8</v>
@@ -2940,13 +2998,13 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C63" s="9" t="s">
         <v>132</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>133</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>8</v>
@@ -2957,13 +3015,13 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" s="9" t="s">
         <v>134</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>135</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>8</v>
@@ -2974,13 +3032,13 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C65" s="9" t="s">
         <v>136</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>137</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>8</v>
@@ -2991,13 +3049,13 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>138</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>139</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>8</v>
@@ -3008,13 +3066,13 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>140</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>141</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>8</v>
@@ -3025,13 +3083,13 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>142</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>143</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>8</v>
@@ -3042,13 +3100,13 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>144</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>145</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>8</v>
@@ -3059,13 +3117,13 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>146</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>147</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>8</v>
@@ -3076,13 +3134,13 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C71" s="9" t="s">
         <v>148</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>149</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>8</v>
@@ -3093,13 +3151,13 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>150</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>151</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>8</v>
@@ -3110,13 +3168,13 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C73" s="9" t="s">
         <v>152</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>153</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>8</v>
@@ -3127,10 +3185,10 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" s="8" t="s">
         <v>154</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>155</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>58</v>
@@ -3144,13 +3202,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C75" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>157</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>8</v>
@@ -3161,13 +3219,13 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C76" s="9" t="s">
         <v>158</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>159</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>8</v>
@@ -3178,13 +3236,13 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C77" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>161</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>8</v>
@@ -3195,13 +3253,13 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C78" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>8</v>
@@ -3212,13 +3270,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>8</v>
@@ -3229,13 +3287,13 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C80" s="9" t="s">
         <v>166</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>167</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>8</v>
@@ -3246,13 +3304,13 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C81" s="9" t="s">
         <v>168</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>169</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>8</v>
@@ -3263,13 +3321,13 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C82" s="9" t="s">
         <v>170</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>171</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>8</v>
@@ -3280,13 +3338,13 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C83" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>173</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>8</v>
@@ -3297,13 +3355,13 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C84" s="9" t="s">
         <v>174</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>175</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>8</v>
@@ -3314,10 +3372,10 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>176</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>177</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>58</v>
@@ -3331,13 +3389,13 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86" s="8" t="s">
         <v>178</v>
-      </c>
-      <c r="B86" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>179</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>8</v>
@@ -3348,13 +3406,13 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C87" s="8" t="s">
         <v>180</v>
-      </c>
-      <c r="B87" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>181</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>8</v>
@@ -3365,13 +3423,13 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C88" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="B88" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>8</v>
@@ -3382,13 +3440,13 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C89" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>185</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>8</v>
@@ -3399,13 +3457,13 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>8</v>
@@ -3416,13 +3474,13 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>8</v>
@@ -3433,13 +3491,13 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>8</v>
@@ -3450,13 +3508,13 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>8</v>
@@ -3467,13 +3525,13 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>8</v>
@@ -3484,13 +3542,13 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C95" s="8" t="s">
         <v>191</v>
-      </c>
-      <c r="B95" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>192</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>8</v>
@@ -3501,10 +3559,10 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B96" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="B96" s="8" t="s">
-        <v>194</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>58</v>
@@ -3518,13 +3576,13 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>8</v>
@@ -3535,13 +3593,13 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>8</v>
@@ -3552,13 +3610,13 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>8</v>
@@ -3569,13 +3627,13 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>8</v>
@@ -3586,13 +3644,13 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>8</v>
@@ -3603,13 +3661,13 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>8</v>
@@ -3620,13 +3678,13 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>8</v>
@@ -3637,13 +3695,13 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C104" s="8" t="s">
         <v>202</v>
-      </c>
-      <c r="B104" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>203</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>8</v>
@@ -3654,13 +3712,13 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>8</v>
@@ -3671,18 +3729,205 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C106" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="B106" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C106" s="8" t="s">
+      <c r="D106" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D106" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E106" s="3" t="s">
+      <c r="B107" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C107" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C108" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C109" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C110" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C111" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C112" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C113" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C114" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C115" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C116" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C117" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E117" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3691,7 +3936,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E18 E25 E26 D1:D8 D18:D25 D26:D42 E2:E8 E19:E24 E27:E42 F2:F3 D9:E17 D43:E106">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E25 D1:D8 D25:D44 D105:D106 D107:D117 E2:E8 E26:E42 E43:E44 E105:E117 F2:F3 D18:E24 D9:E17 D45:E104">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
resolved issues in  code of RW04, RW05 and RW06 probate form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -611,6 +611,9 @@
     <t>probateFormsRW05.feature</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_096</t>
   </si>
   <si>
@@ -653,9 +656,6 @@
     <t>probateFormsRW06.feature</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>TC_107</t>
   </si>
   <si>
@@ -698,7 +698,7 @@
     <t>TC_115</t>
   </si>
   <si>
-    <t>Verify, Relationship, date and reason text box fields are not same for each field.</t>
+    <t>Verify, date and reason text box fields are not same for each field.</t>
   </si>
   <si>
     <t>TC_116</t>
@@ -1383,7 +1383,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1406,7 +1406,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1928,8 +1927,8 @@
   <sheetPr/>
   <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3380,7 +3379,7 @@
       <c r="C85" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D85" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E85" s="3" t="s">
@@ -3397,7 +3396,7 @@
       <c r="C86" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="D86" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E86" s="3" t="s">
@@ -3414,7 +3413,7 @@
       <c r="C87" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="D87" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E87" s="3" t="s">
@@ -3431,7 +3430,7 @@
       <c r="C88" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="D88" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E88" s="3" t="s">
@@ -3448,7 +3447,7 @@
       <c r="C89" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="D89" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E89" s="3" t="s">
@@ -3465,7 +3464,7 @@
       <c r="C90" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="D90" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E90" s="3" t="s">
@@ -3482,7 +3481,7 @@
       <c r="C91" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="D91" s="3" t="s">
+      <c r="D91" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E91" s="3" t="s">
@@ -3499,7 +3498,7 @@
       <c r="C92" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="D92" s="3" t="s">
+      <c r="D92" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E92" s="3" t="s">
@@ -3516,7 +3515,7 @@
       <c r="C93" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D93" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E93" s="3" t="s">
@@ -3533,7 +3532,7 @@
       <c r="C94" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D94" s="3" t="s">
+      <c r="D94" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E94" s="3" t="s">
@@ -3550,7 +3549,7 @@
       <c r="C95" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D95" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E95" s="3" t="s">
@@ -3568,7 +3567,7 @@
         <v>58</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>8</v>
@@ -3576,7 +3575,7 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>193</v>
@@ -3585,7 +3584,7 @@
         <v>102</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -3593,7 +3592,7 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>193</v>
@@ -3602,7 +3601,7 @@
         <v>158</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -3610,7 +3609,7 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>193</v>
@@ -3619,7 +3618,7 @@
         <v>160</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -3627,7 +3626,7 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>193</v>
@@ -3636,7 +3635,7 @@
         <v>162</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -3644,7 +3643,7 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>193</v>
@@ -3653,7 +3652,7 @@
         <v>164</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -3661,7 +3660,7 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>193</v>
@@ -3670,7 +3669,7 @@
         <v>166</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -3678,7 +3677,7 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>193</v>
@@ -3687,7 +3686,7 @@
         <v>168</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -3695,16 +3694,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>193</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -3712,7 +3711,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>193</v>
@@ -3721,7 +3720,7 @@
         <v>170</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -3729,16 +3728,16 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B106" s="8" t="s">
         <v>193</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -3746,16 +3745,16 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C107" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C107" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -3766,13 +3765,13 @@
         <v>209</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C108" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C108" s="8" t="s">
         <v>156</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -3783,13 +3782,13 @@
         <v>210</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C109" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C109" s="8" t="s">
         <v>158</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -3800,13 +3799,13 @@
         <v>211</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C110" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C110" s="8" t="s">
         <v>212</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -3817,13 +3816,13 @@
         <v>213</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C111" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C111" s="8" t="s">
         <v>214</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -3834,13 +3833,13 @@
         <v>215</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C112" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C112" s="8" t="s">
         <v>216</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -3851,13 +3850,13 @@
         <v>217</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C113" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C113" s="8" t="s">
         <v>218</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -3868,13 +3867,13 @@
         <v>219</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C114" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C114" s="8" t="s">
         <v>212</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -3885,13 +3884,13 @@
         <v>220</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C115" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C115" s="8" t="s">
         <v>221</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -3902,13 +3901,13 @@
         <v>222</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C116" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C116" s="8" t="s">
         <v>223</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -3919,13 +3918,13 @@
         <v>224</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C117" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C117" s="8" t="s">
         <v>225</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -3936,7 +3935,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E25 D1:D8 D25:D44 D105:D106 D107:D117 E2:E8 E26:E42 E43:E44 E105:E117 F2:F3 D18:E24 D9:E17 D45:E104">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E84 E95 D96:E96 E97 D1:D8 D84:D95 D97:D105 E2:E8 E85:E94 E98:E105 F2:F3 D9:E83 D106:E117">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
resolved issues in code of RW06 probate form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -611,49 +611,49 @@
     <t>probateFormsRW05.feature</t>
   </si>
   <si>
+    <t>TC_096</t>
+  </si>
+  <si>
+    <t>TC_097</t>
+  </si>
+  <si>
+    <t>TC_098</t>
+  </si>
+  <si>
+    <t>TC_099</t>
+  </si>
+  <si>
+    <t>TC_100</t>
+  </si>
+  <si>
+    <t>TC_101</t>
+  </si>
+  <si>
+    <t>TC_102</t>
+  </si>
+  <si>
+    <t>TC_103</t>
+  </si>
+  <si>
+    <t>Verify, on checking notary checkbox, notary section displays.</t>
+  </si>
+  <si>
+    <t>TC_104</t>
+  </si>
+  <si>
+    <t>TC_105</t>
+  </si>
+  <si>
+    <t>Reset the RW05 form</t>
+  </si>
+  <si>
+    <t>TC_106</t>
+  </si>
+  <si>
+    <t>probateFormsRW06.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_096</t>
-  </si>
-  <si>
-    <t>TC_097</t>
-  </si>
-  <si>
-    <t>TC_098</t>
-  </si>
-  <si>
-    <t>TC_099</t>
-  </si>
-  <si>
-    <t>TC_100</t>
-  </si>
-  <si>
-    <t>TC_101</t>
-  </si>
-  <si>
-    <t>TC_102</t>
-  </si>
-  <si>
-    <t>TC_103</t>
-  </si>
-  <si>
-    <t>Verify, on checking notary checkbox, notary section displays.</t>
-  </si>
-  <si>
-    <t>TC_104</t>
-  </si>
-  <si>
-    <t>TC_105</t>
-  </si>
-  <si>
-    <t>Reset the RW05 form</t>
-  </si>
-  <si>
-    <t>TC_106</t>
-  </si>
-  <si>
-    <t>probateFormsRW06.feature</t>
   </si>
   <si>
     <t>TC_107</t>
@@ -1927,8 +1927,8 @@
   <sheetPr/>
   <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E101" sqref="E101"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="E114" sqref="E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3566,8 +3566,8 @@
       <c r="C96" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D96" s="3" t="s">
-        <v>194</v>
+      <c r="D96" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>8</v>
@@ -3575,7 +3575,7 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>193</v>
@@ -3583,8 +3583,8 @@
       <c r="C97" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D97" s="3" t="s">
-        <v>194</v>
+      <c r="D97" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -3592,7 +3592,7 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>193</v>
@@ -3600,8 +3600,8 @@
       <c r="C98" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D98" s="3" t="s">
-        <v>194</v>
+      <c r="D98" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -3609,7 +3609,7 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>193</v>
@@ -3617,8 +3617,8 @@
       <c r="C99" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>194</v>
+      <c r="D99" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -3626,7 +3626,7 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>193</v>
@@ -3634,8 +3634,8 @@
       <c r="C100" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="D100" s="3" t="s">
-        <v>194</v>
+      <c r="D100" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -3643,7 +3643,7 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>193</v>
@@ -3651,8 +3651,8 @@
       <c r="C101" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="D101" s="3" t="s">
-        <v>194</v>
+      <c r="D101" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -3660,7 +3660,7 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>193</v>
@@ -3668,8 +3668,8 @@
       <c r="C102" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="D102" s="3" t="s">
-        <v>194</v>
+      <c r="D102" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -3677,7 +3677,7 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>193</v>
@@ -3685,8 +3685,8 @@
       <c r="C103" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="D103" s="3" t="s">
-        <v>194</v>
+      <c r="D103" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -3694,16 +3694,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>193</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>194</v>
+        <v>202</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -3711,7 +3711,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>193</v>
@@ -3719,8 +3719,8 @@
       <c r="C105" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D105" s="3" t="s">
-        <v>194</v>
+      <c r="D105" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -3728,16 +3728,16 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B106" s="8" t="s">
         <v>193</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>194</v>
+        <v>205</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -3745,16 +3745,16 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B107" s="8" t="s">
         <v>207</v>
-      </c>
-      <c r="B107" s="8" t="s">
-        <v>208</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -3765,13 +3765,13 @@
         <v>209</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>156</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -3782,13 +3782,13 @@
         <v>210</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>158</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -3799,13 +3799,13 @@
         <v>211</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>212</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -3816,13 +3816,13 @@
         <v>213</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C111" s="8" t="s">
         <v>214</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -3833,13 +3833,13 @@
         <v>215</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>216</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -3850,13 +3850,13 @@
         <v>217</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C113" s="8" t="s">
         <v>218</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -3867,13 +3867,13 @@
         <v>219</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C114" s="8" t="s">
         <v>212</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -3884,13 +3884,13 @@
         <v>220</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C115" s="8" t="s">
         <v>221</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -3901,13 +3901,13 @@
         <v>222</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C116" s="8" t="s">
         <v>223</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -3918,13 +3918,13 @@
         <v>224</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C117" s="8" t="s">
         <v>225</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -3935,7 +3935,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E84 E95 D96:E96 E97 D1:D8 D84:D95 D97:D105 E2:E8 E85:E94 E98:E105 F2:F3 D9:E83 D106:E117">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E95 E96 E106 D1:D8 D95:D106 D107:D117 E2:E8 E97:E105 E107:E108 E109:E117 F2:F3 D84:E94 D9:E83">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added some more TCs
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="228">
   <si>
     <t>ID</t>
   </si>
@@ -560,63 +560,63 @@
     <t>probateFormsRW04.feature</t>
   </si>
   <si>
+    <t>TC_085</t>
+  </si>
+  <si>
+    <t>Verify, correct title is displayed on the form's header.</t>
+  </si>
+  <si>
+    <t>TC_086</t>
+  </si>
+  <si>
+    <t>Verify, county, and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_087</t>
+  </si>
+  <si>
+    <t>Verify, correct estate's name is displayed on the form.</t>
+  </si>
+  <si>
+    <t>TC_088</t>
+  </si>
+  <si>
+    <t>Verify, name of the decedent should be auto populated from the form.</t>
+  </si>
+  <si>
+    <t>TC_089</t>
+  </si>
+  <si>
+    <t>TC_090</t>
+  </si>
+  <si>
+    <t>TC_091</t>
+  </si>
+  <si>
+    <t>TC_092</t>
+  </si>
+  <si>
+    <t>TC_093</t>
+  </si>
+  <si>
+    <t>TC_094</t>
+  </si>
+  <si>
+    <t>TC_095</t>
+  </si>
+  <si>
+    <t>Reset the RW04 form</t>
+  </si>
+  <si>
+    <t>TC_096</t>
+  </si>
+  <si>
+    <t>probateFormsRW05.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>TC_085</t>
-  </si>
-  <si>
-    <t>Verify, correct title is displayed on the form's header.</t>
-  </si>
-  <si>
-    <t>TC_086</t>
-  </si>
-  <si>
-    <t>Verify, county, and aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_087</t>
-  </si>
-  <si>
-    <t>Verify, correct estate's name is displayed on the form.</t>
-  </si>
-  <si>
-    <t>TC_088</t>
-  </si>
-  <si>
-    <t>Verify, name of the decedent should be auto populated from the form.</t>
-  </si>
-  <si>
-    <t>TC_089</t>
-  </si>
-  <si>
-    <t>TC_090</t>
-  </si>
-  <si>
-    <t>TC_091</t>
-  </si>
-  <si>
-    <t>TC_092</t>
-  </si>
-  <si>
-    <t>TC_093</t>
-  </si>
-  <si>
-    <t>TC_094</t>
-  </si>
-  <si>
-    <t>TC_095</t>
-  </si>
-  <si>
-    <t>Reset the RW04 form</t>
-  </si>
-  <si>
-    <t>TC_096</t>
-  </si>
-  <si>
-    <t>probateFormsRW05.feature</t>
-  </si>
-  <si>
     <t>TC_097</t>
   </si>
   <si>
@@ -650,61 +650,64 @@
     <t>TC_106</t>
   </si>
   <si>
+    <t>TC_107</t>
+  </si>
+  <si>
     <t>Reset the RW05 form</t>
   </si>
   <si>
-    <t>TC_107</t>
+    <t>TC_108</t>
   </si>
   <si>
     <t>probateFormsRW06.feature</t>
   </si>
   <si>
-    <t>TC_108</t>
-  </si>
-  <si>
     <t>TC_109</t>
   </si>
   <si>
     <t>TC_110</t>
   </si>
   <si>
+    <t>TC_111</t>
+  </si>
+  <si>
     <t>Verify, form is repeated based on the number of contacts selected.</t>
   </si>
   <si>
-    <t>TC_111</t>
+    <t>TC_112</t>
   </si>
   <si>
     <t>Verify, corporate fiduciary selected is reflected in the corporate name field.</t>
   </si>
   <si>
-    <t>TC_112</t>
+    <t>TC_113</t>
   </si>
   <si>
     <t>Verify, details of the selected contact's is displayed in the block under it.</t>
   </si>
   <si>
-    <t>TC_113</t>
+    <t>TC_114</t>
   </si>
   <si>
     <t>Verify, on clicking signature of person, beneficiary contact can be selected.</t>
   </si>
   <si>
-    <t>TC_114</t>
-  </si>
-  <si>
     <t>TC_115</t>
   </si>
   <si>
+    <t>TC_116</t>
+  </si>
+  <si>
     <t>Verify, contact details are correctly displayed on each page.</t>
   </si>
   <si>
-    <t>TC_116</t>
+    <t>TC_117</t>
   </si>
   <si>
     <t>Verify, date and reason text box fields are not same for each field.</t>
   </si>
   <si>
-    <t>TC_117</t>
+    <t>TC_118</t>
   </si>
   <si>
     <t>Reset the RW06 form</t>
@@ -1928,10 +1931,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F118"/>
+  <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3383,7 +3386,7 @@
         <v>58</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>8</v>
@@ -3391,16 +3394,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>8</v>
@@ -3408,16 +3411,16 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>8</v>
@@ -3425,16 +3428,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>8</v>
@@ -3442,16 +3445,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>8</v>
@@ -3459,7 +3462,7 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>176</v>
@@ -3468,7 +3471,7 @@
         <v>162</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>8</v>
@@ -3476,7 +3479,7 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>176</v>
@@ -3485,7 +3488,7 @@
         <v>164</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>8</v>
@@ -3493,7 +3496,7 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>176</v>
@@ -3502,7 +3505,7 @@
         <v>166</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>8</v>
@@ -3510,7 +3513,7 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>176</v>
@@ -3519,7 +3522,7 @@
         <v>168</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>8</v>
@@ -3527,7 +3530,7 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>176</v>
@@ -3536,7 +3539,7 @@
         <v>170</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>8</v>
@@ -3544,7 +3547,7 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>176</v>
@@ -3553,7 +3556,7 @@
         <v>172</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>8</v>
@@ -3561,16 +3564,16 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>8</v>
@@ -3578,16 +3581,16 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B97" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>195</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -3598,13 +3601,13 @@
         <v>196</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>102</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -3615,13 +3618,13 @@
         <v>197</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>158</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -3632,13 +3635,13 @@
         <v>198</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>160</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -3649,13 +3652,13 @@
         <v>199</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C101" s="8" t="s">
         <v>162</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -3666,13 +3669,13 @@
         <v>200</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>164</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -3683,13 +3686,13 @@
         <v>201</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>166</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -3700,13 +3703,13 @@
         <v>202</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>168</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -3717,13 +3720,13 @@
         <v>203</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C105" s="8" t="s">
         <v>204</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -3734,13 +3737,13 @@
         <v>205</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -3751,13 +3754,13 @@
         <v>206</v>
       </c>
       <c r="B107" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D107" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="C107" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -3765,16 +3768,16 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C108" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="B108" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C108" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>8</v>
+      <c r="D108" s="5" t="s">
+        <v>195</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -3782,13 +3785,13 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B109" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="B109" s="8" t="s">
-        <v>209</v>
-      </c>
       <c r="C109" s="8" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>8</v>
@@ -3802,10 +3805,10 @@
         <v>211</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>8</v>
@@ -3819,10 +3822,10 @@
         <v>212</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>213</v>
+        <v>158</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>8</v>
@@ -3833,13 +3836,13 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C112" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="B112" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C112" s="8" t="s">
-        <v>215</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>8</v>
@@ -3850,13 +3853,13 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C113" s="8" t="s">
         <v>216</v>
-      </c>
-      <c r="B113" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C113" s="8" t="s">
-        <v>217</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>8</v>
@@ -3867,13 +3870,13 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C114" s="8" t="s">
         <v>218</v>
-      </c>
-      <c r="B114" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C114" s="8" t="s">
-        <v>219</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>8</v>
@@ -3884,13 +3887,13 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C115" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="B115" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C115" s="8" t="s">
-        <v>213</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>8</v>
@@ -3904,10 +3907,10 @@
         <v>221</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>8</v>
@@ -3918,13 +3921,13 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C117" s="8" t="s">
         <v>223</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C117" s="8" t="s">
-        <v>224</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>8</v>
@@ -3935,18 +3938,35 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C118" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="B118" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C118" s="8" t="s">
+      <c r="D118" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="D118" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E118" s="3" t="s">
+      <c r="B119" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E119" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3955,7 +3975,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 E2:E8 F2:F3 D9:E118">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 E2:E8 F2:F3 D9:E119">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added some more TCs for Rw form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="229">
   <si>
     <t>ID</t>
   </si>
@@ -314,6 +314,9 @@
     <t>probateFormsRW02.feature</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_044</t>
   </si>
   <si>
@@ -614,9 +617,6 @@
     <t>probateFormsRW05.feature</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>TC_097</t>
   </si>
   <si>
@@ -708,6 +708,9 @@
   </si>
   <si>
     <t>TC_118</t>
+  </si>
+  <si>
+    <t>TC_119</t>
   </si>
   <si>
     <t>Reset the RW06 form</t>
@@ -1931,10 +1934,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F119"/>
+  <dimension ref="A1:F120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44:D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2689,7 +2692,7 @@
         <v>58</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>8</v>
@@ -2697,16 +2700,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -2714,16 +2717,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>8</v>
+        <v>99</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -2731,16 +2734,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -2748,16 +2751,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>8</v>
+        <v>103</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -2765,16 +2768,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -2782,16 +2785,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>8</v>
+        <v>107</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -2799,16 +2802,16 @@
     </row>
     <row r="51" ht="28" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -2816,16 +2819,16 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>8</v>
+        <v>111</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -2833,16 +2836,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -2850,16 +2853,16 @@
     </row>
     <row r="54" ht="28" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>8</v>
+        <v>115</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -2867,16 +2870,16 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -2884,16 +2887,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>8</v>
+        <v>119</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -2901,16 +2904,16 @@
     </row>
     <row r="57" ht="28" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -2918,16 +2921,16 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>8</v>
+        <v>123</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -2935,16 +2938,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -2952,16 +2955,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>8</v>
+        <v>127</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -2969,16 +2972,16 @@
     </row>
     <row r="61" ht="28" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -2986,16 +2989,16 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>8</v>
+        <v>131</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3003,16 +3006,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3020,16 +3023,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>8</v>
+        <v>135</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3037,16 +3040,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3054,16 +3057,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>8</v>
+        <v>139</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3071,16 +3074,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3088,16 +3091,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>8</v>
+        <v>143</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3105,16 +3108,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3122,16 +3125,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3139,16 +3142,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3156,16 +3159,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>8</v>
+        <v>151</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3173,16 +3176,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3190,10 +3193,10 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>58</v>
@@ -3207,13 +3210,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B75" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="C75" s="9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>8</v>
@@ -3224,13 +3227,13 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>8</v>
@@ -3241,13 +3244,13 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>8</v>
@@ -3258,13 +3261,13 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>8</v>
@@ -3275,13 +3278,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>8</v>
@@ -3292,13 +3295,13 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>8</v>
@@ -3309,13 +3312,13 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>8</v>
@@ -3326,13 +3329,13 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>8</v>
@@ -3343,13 +3346,13 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>8</v>
@@ -3360,13 +3363,13 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>8</v>
@@ -3377,10 +3380,10 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>58</v>
@@ -3394,13 +3397,13 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B86" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B86" s="8" t="s">
-        <v>176</v>
-      </c>
       <c r="C86" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>8</v>
@@ -3411,13 +3414,13 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>8</v>
@@ -3428,13 +3431,13 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>8</v>
@@ -3445,13 +3448,13 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>8</v>
@@ -3462,13 +3465,13 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>8</v>
@@ -3479,13 +3482,13 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>8</v>
@@ -3496,13 +3499,13 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>8</v>
@@ -3513,13 +3516,13 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>8</v>
@@ -3530,13 +3533,13 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>8</v>
@@ -3547,13 +3550,13 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>8</v>
@@ -3564,13 +3567,13 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>8</v>
@@ -3581,16 +3584,16 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>195</v>
+        <v>8</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -3601,13 +3604,13 @@
         <v>196</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>195</v>
+        <v>8</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -3618,13 +3621,13 @@
         <v>197</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>195</v>
+        <v>8</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -3635,13 +3638,13 @@
         <v>198</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>195</v>
+        <v>8</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -3652,13 +3655,13 @@
         <v>199</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>195</v>
+        <v>8</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -3669,13 +3672,13 @@
         <v>200</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>195</v>
+        <v>8</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -3686,13 +3689,13 @@
         <v>201</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>195</v>
+        <v>8</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -3703,13 +3706,13 @@
         <v>202</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>195</v>
+        <v>8</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -3720,13 +3723,13 @@
         <v>203</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C105" s="8" t="s">
         <v>204</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>195</v>
+        <v>8</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -3737,13 +3740,13 @@
         <v>205</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>195</v>
+        <v>8</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -3754,13 +3757,13 @@
         <v>206</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>195</v>
+        <v>8</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -3771,13 +3774,13 @@
         <v>207</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>208</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>195</v>
+        <v>8</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -3793,7 +3796,7 @@
       <c r="C109" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D109" s="3" t="s">
+      <c r="D109" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E109" s="3" t="s">
@@ -3808,9 +3811,9 @@
         <v>210</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D110" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D110" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E110" s="3" t="s">
@@ -3825,9 +3828,9 @@
         <v>210</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="D111" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D111" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E111" s="3" t="s">
@@ -3844,7 +3847,7 @@
       <c r="C112" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="D112" s="3" t="s">
+      <c r="D112" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E112" s="3" t="s">
@@ -3861,7 +3864,7 @@
       <c r="C113" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="D113" s="3" t="s">
+      <c r="D113" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E113" s="3" t="s">
@@ -3878,7 +3881,7 @@
       <c r="C114" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="D114" s="3" t="s">
+      <c r="D114" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E114" s="3" t="s">
@@ -3895,7 +3898,7 @@
       <c r="C115" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="D115" s="3" t="s">
+      <c r="D115" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E115" s="3" t="s">
@@ -3912,7 +3915,7 @@
       <c r="C116" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="D116" s="3" t="s">
+      <c r="D116" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E116" s="3" t="s">
@@ -3929,7 +3932,7 @@
       <c r="C117" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="D117" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E117" s="3" t="s">
@@ -3946,7 +3949,7 @@
       <c r="C118" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D118" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E118" s="3" t="s">
@@ -3961,12 +3964,29 @@
         <v>210</v>
       </c>
       <c r="C119" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="D119" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E119" s="3" t="s">
+      <c r="B120" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C120" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E120" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3975,7 +3995,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 E2:E8 F2:F3 D9:E119">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D44:D73 D106:D120 E2:E8 E44:E45 E46:E73 E106:E108 E109:E120 F2:F3 D95:E105 D9:E43 D74:E94">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added TCs for RWxx probate form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="238">
   <si>
     <t>ID</t>
   </si>
@@ -653,58 +653,94 @@
     <t>probateFormsRW06.feature</t>
   </si>
   <si>
+    <t>TC_107</t>
+  </si>
+  <si>
+    <t>TC_108</t>
+  </si>
+  <si>
+    <t>TC_109</t>
+  </si>
+  <si>
+    <t>Verify, form is repeated based on the number of contacts selected.</t>
+  </si>
+  <si>
+    <t>TC_110</t>
+  </si>
+  <si>
+    <t>Verify, corporate fiduciary selected is reflected in the corporate name field.</t>
+  </si>
+  <si>
+    <t>TC_111</t>
+  </si>
+  <si>
+    <t>Verify, details of the selected contact's is displayed in the block under it.</t>
+  </si>
+  <si>
+    <t>TC_112</t>
+  </si>
+  <si>
+    <t>Verify, on clicking signature of person, beneficiary contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_113</t>
+  </si>
+  <si>
+    <t>TC_114</t>
+  </si>
+  <si>
+    <t>Verify, contact details are correctly displayed on each page.</t>
+  </si>
+  <si>
+    <t>TC_115</t>
+  </si>
+  <si>
+    <t>Verify, date and reason text box fields are not same for each field.</t>
+  </si>
+  <si>
+    <t>TC_116</t>
+  </si>
+  <si>
+    <t>Reset the RW06 form</t>
+  </si>
+  <si>
+    <t>TC_117</t>
+  </si>
+  <si>
+    <t>probateFormsRWxx.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>TC_107</t>
-  </si>
-  <si>
-    <t>TC_108</t>
-  </si>
-  <si>
-    <t>TC_109</t>
-  </si>
-  <si>
-    <t>Verify, form is repeated based on the number of contacts selected.</t>
-  </si>
-  <si>
-    <t>TC_110</t>
-  </si>
-  <si>
-    <t>Verify, corporate fiduciary selected is reflected in the corporate name field.</t>
-  </si>
-  <si>
-    <t>TC_111</t>
-  </si>
-  <si>
-    <t>Verify, details of the selected contact's is displayed in the block under it.</t>
-  </si>
-  <si>
-    <t>TC_112</t>
-  </si>
-  <si>
-    <t>Verify, on clicking signature of person, beneficiary contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_113</t>
-  </si>
-  <si>
-    <t>TC_114</t>
-  </si>
-  <si>
-    <t>Verify, contact details are correctly displayed on each page.</t>
-  </si>
-  <si>
-    <t>TC_115</t>
-  </si>
-  <si>
-    <t>Verify, date and reason text box fields are not same for each field.</t>
-  </si>
-  <si>
-    <t>TC_116</t>
-  </si>
-  <si>
-    <t>Reset the RW06 form</t>
+    <t>TC_118</t>
+  </si>
+  <si>
+    <t>Verify that the county, estate name, and "Also Known As" (AKA) values are auto-populated from the selected estate.</t>
+  </si>
+  <si>
+    <t>TC_119</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered in all the text areas.</t>
+  </si>
+  <si>
+    <t>TC_120</t>
+  </si>
+  <si>
+    <t>Verify, the name entered in 1st text area is reflected in the signature.</t>
+  </si>
+  <si>
+    <t>TC_121</t>
+  </si>
+  <si>
+    <t>Verify that changes in the witness name field are reflected under the signature line and vice-versa.</t>
+  </si>
+  <si>
+    <t>TC_122</t>
+  </si>
+  <si>
+    <t>Reset the RWxx form</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1138,6 +1174,17 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="thin">
         <color auto="1"/>
@@ -1259,7 +1306,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1271,34 +1318,34 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1383,7 +1430,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1404,6 +1451,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1925,10 +1979,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F117"/>
+  <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="E114" sqref="E114"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3753,8 +3807,8 @@
       <c r="C107" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D107" s="3" t="s">
-        <v>208</v>
+      <c r="D107" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -3762,7 +3816,7 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B108" s="8" t="s">
         <v>207</v>
@@ -3770,8 +3824,8 @@
       <c r="C108" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D108" s="3" t="s">
-        <v>208</v>
+      <c r="D108" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -3779,7 +3833,7 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B109" s="8" t="s">
         <v>207</v>
@@ -3787,8 +3841,8 @@
       <c r="C109" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D109" s="3" t="s">
-        <v>208</v>
+      <c r="D109" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -3796,16 +3850,16 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B110" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>208</v>
+        <v>211</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -3813,16 +3867,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B111" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>208</v>
+        <v>213</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -3830,16 +3884,16 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B112" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>208</v>
+        <v>215</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -3847,16 +3901,16 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B113" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>208</v>
+        <v>217</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -3864,16 +3918,16 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B114" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>208</v>
+        <v>211</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -3881,16 +3935,16 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B115" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>208</v>
+        <v>220</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -3898,16 +3952,16 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>208</v>
+        <v>222</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -3915,18 +3969,120 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B117" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C117" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D117" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E117" s="3" t="s">
+      <c r="B118" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C118" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D118" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" ht="28" spans="1:5">
+      <c r="A119" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C119" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="D119" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C120" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D120" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C121" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D121" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C122" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="D122" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C123" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="D123" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E123" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3935,7 +4091,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E95 E96 E106 D1:D8 D95:D106 D107:D117 E2:E8 E97:E105 E107:E108 E109:E117 F2:F3 D84:E94 D9:E83">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E106 D1:D8 D106:D114 D115:D117 D118:D123 E2:E8 E107:E113 E114:E121 E122:E123 F2:F3 D9:E94 D95:E105">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
resolved the issues of RW06 and RWxx probate form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -653,6 +653,9 @@
     <t>probateFormsRW06.feature</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_107</t>
   </si>
   <si>
@@ -708,9 +711,6 @@
   </si>
   <si>
     <t>probateFormsRWxx.feature</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>TC_118</t>
@@ -1147,7 +1147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1174,17 +1174,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color auto="1"/>
@@ -1306,7 +1295,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1318,34 +1307,34 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1430,7 +1419,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1452,10 +1441,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -1981,8 +1966,8 @@
   <sheetPr/>
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3808,7 +3793,7 @@
         <v>58</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -3816,7 +3801,7 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B108" s="8" t="s">
         <v>207</v>
@@ -3825,7 +3810,7 @@
         <v>156</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -3833,7 +3818,7 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B109" s="8" t="s">
         <v>207</v>
@@ -3842,7 +3827,7 @@
         <v>158</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -3850,16 +3835,16 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B110" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -3867,16 +3852,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B111" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -3884,16 +3869,16 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B112" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -3901,16 +3886,16 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B113" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -3918,16 +3903,16 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B114" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -3935,16 +3920,16 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B115" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -3952,16 +3937,16 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -3969,16 +3954,16 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B117" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -3986,16 +3971,16 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C118" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C118" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D118" s="11" t="s">
-        <v>227</v>
+      <c r="D118" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -4006,13 +3991,13 @@
         <v>228</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C119" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="C119" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="D119" s="11" t="s">
-        <v>227</v>
+      <c r="D119" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4023,13 +4008,13 @@
         <v>230</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C120" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C120" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="D120" s="11" t="s">
-        <v>227</v>
+      <c r="D120" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4040,13 +4025,13 @@
         <v>232</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C121" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C121" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="D121" s="11" t="s">
-        <v>227</v>
+      <c r="D121" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4057,13 +4042,13 @@
         <v>234</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C122" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C122" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="D122" s="11" t="s">
-        <v>227</v>
+      <c r="D122" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4074,13 +4059,13 @@
         <v>236</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C123" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C123" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="D123" s="11" t="s">
-        <v>227</v>
+      <c r="D123" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>8</v>
@@ -4091,7 +4076,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E106 D1:D8 D106:D114 D115:D117 D118:D123 E2:E8 E107:E113 E114:E121 E122:E123 F2:F3 D9:E94 D95:E105">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D106:E106 E107 E117 D1:D8 D107:D116 D117:D123 E2:E8 E108:E116 E118:E123 F2:F3 D9:E105">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
works on some fix
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -653,67 +653,67 @@
     <t>probateFormsRW06.feature</t>
   </si>
   <si>
+    <t>TC_107</t>
+  </si>
+  <si>
+    <t>TC_108</t>
+  </si>
+  <si>
+    <t>TC_109</t>
+  </si>
+  <si>
+    <t>Verify, form is repeated based on the number of contacts selected.</t>
+  </si>
+  <si>
+    <t>TC_110</t>
+  </si>
+  <si>
+    <t>Verify, corporate fiduciary selected is reflected in the corporate name field.</t>
+  </si>
+  <si>
+    <t>TC_111</t>
+  </si>
+  <si>
+    <t>Verify, details of the selected contact's is displayed in the block under it.</t>
+  </si>
+  <si>
+    <t>TC_112</t>
+  </si>
+  <si>
+    <t>Verify, on clicking signature of person, beneficiary contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_113</t>
+  </si>
+  <si>
+    <t>TC_114</t>
+  </si>
+  <si>
+    <t>Verify, contact details are correctly displayed on each page.</t>
+  </si>
+  <si>
+    <t>TC_115</t>
+  </si>
+  <si>
+    <t>Verify, date and reason text box fields are not same for each field.</t>
+  </si>
+  <si>
+    <t>TC_116</t>
+  </si>
+  <si>
+    <t>TC_117</t>
+  </si>
+  <si>
+    <t>Reset the RW06 form</t>
+  </si>
+  <si>
+    <t>TC_118</t>
+  </si>
+  <si>
+    <t>probateFormsRWxx.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_107</t>
-  </si>
-  <si>
-    <t>TC_108</t>
-  </si>
-  <si>
-    <t>TC_109</t>
-  </si>
-  <si>
-    <t>Verify, form is repeated based on the number of contacts selected.</t>
-  </si>
-  <si>
-    <t>TC_110</t>
-  </si>
-  <si>
-    <t>Verify, corporate fiduciary selected is reflected in the corporate name field.</t>
-  </si>
-  <si>
-    <t>TC_111</t>
-  </si>
-  <si>
-    <t>Verify, details of the selected contact's is displayed in the block under it.</t>
-  </si>
-  <si>
-    <t>TC_112</t>
-  </si>
-  <si>
-    <t>Verify, on clicking signature of person, beneficiary contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_113</t>
-  </si>
-  <si>
-    <t>TC_114</t>
-  </si>
-  <si>
-    <t>Verify, contact details are correctly displayed on each page.</t>
-  </si>
-  <si>
-    <t>TC_115</t>
-  </si>
-  <si>
-    <t>Verify, date and reason text box fields are not same for each field.</t>
-  </si>
-  <si>
-    <t>TC_116</t>
-  </si>
-  <si>
-    <t>TC_117</t>
-  </si>
-  <si>
-    <t>Reset the RW06 form</t>
-  </si>
-  <si>
-    <t>TC_118</t>
-  </si>
-  <si>
-    <t>probateFormsRWxx.feature</t>
   </si>
   <si>
     <t>TC_119</t>
@@ -1969,8 +1969,8 @@
   <sheetPr/>
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="E126" sqref="E126"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3796,7 +3796,7 @@
         <v>58</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -3804,7 +3804,7 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B108" s="8" t="s">
         <v>207</v>
@@ -3813,7 +3813,7 @@
         <v>156</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B109" s="8" t="s">
         <v>207</v>
@@ -3830,7 +3830,7 @@
         <v>158</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -3838,16 +3838,16 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B110" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -3855,16 +3855,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B111" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -3872,16 +3872,16 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B112" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -3889,16 +3889,16 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B113" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -3906,16 +3906,16 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B114" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -3923,16 +3923,16 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B115" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -3940,16 +3940,16 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -3957,7 +3957,7 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B117" s="8" t="s">
         <v>207</v>
@@ -3966,7 +3966,7 @@
         <v>172</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -3974,16 +3974,16 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -3991,16 +3991,16 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B119" s="8" t="s">
         <v>227</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>228</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>8</v>
+        <v>228</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4011,13 +4011,13 @@
         <v>229</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C120" s="10" t="s">
         <v>230</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>8</v>
+        <v>228</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4028,13 +4028,13 @@
         <v>231</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>232</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>8</v>
+        <v>228</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4045,13 +4045,13 @@
         <v>233</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C122" s="8" t="s">
         <v>234</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>8</v>
+        <v>228</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4062,13 +4062,13 @@
         <v>235</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C123" s="8" t="s">
         <v>236</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>8</v>
+        <v>228</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>8</v>
@@ -4079,13 +4079,13 @@
         <v>237</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C124" s="8" t="s">
         <v>238</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>8</v>
+        <v>228</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>8</v>
@@ -4096,7 +4096,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D107:D118 D119:D124 E2:E8 E107:E112 E113:E118 E119:E120 E121:E124 F2:F3 D9:E106">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D101:D118 D119:D124 E2:E8 E101:E102 E103:E106 E107:E115 E116:E117 E118:E124 F2:F3 D9:E100">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
modified the code of RW02 probate form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -314,6 +314,9 @@
     <t>probateFormsRW02.feature</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_044</t>
   </si>
   <si>
@@ -744,9 +747,6 @@
   </si>
   <si>
     <t>probateFormsRW07.feature</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>TC_124</t>
@@ -2119,8 +2119,8 @@
   <sheetPr/>
   <dimension ref="A1:F152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2875,7 +2875,7 @@
         <v>58</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>8</v>
@@ -2883,16 +2883,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>8</v>
+        <v>97</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -2900,16 +2900,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>8</v>
+        <v>99</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -2917,16 +2917,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>8</v>
+        <v>101</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -2934,16 +2934,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>8</v>
+        <v>103</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -2951,16 +2951,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>8</v>
+        <v>105</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -2968,16 +2968,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>8</v>
+        <v>107</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -2985,16 +2985,16 @@
     </row>
     <row r="51" ht="28" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>8</v>
+        <v>109</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -3002,16 +3002,16 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>8</v>
+        <v>111</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -3019,16 +3019,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>8</v>
+        <v>113</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -3036,16 +3036,16 @@
     </row>
     <row r="54" ht="28" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>8</v>
+        <v>115</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -3053,16 +3053,16 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>8</v>
+        <v>117</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -3070,16 +3070,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>8</v>
+        <v>119</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -3087,16 +3087,16 @@
     </row>
     <row r="57" ht="28" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>8</v>
+        <v>121</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -3104,16 +3104,16 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>8</v>
+        <v>123</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -3121,16 +3121,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>8</v>
+        <v>125</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -3138,16 +3138,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>8</v>
+        <v>127</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -3155,16 +3155,16 @@
     </row>
     <row r="61" ht="28" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>8</v>
+        <v>129</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -3172,16 +3172,16 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>8</v>
+        <v>131</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3189,16 +3189,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>8</v>
+        <v>133</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3206,16 +3206,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>8</v>
+        <v>135</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3223,16 +3223,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>8</v>
+        <v>137</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3240,16 +3240,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>8</v>
+        <v>139</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3257,16 +3257,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>8</v>
+        <v>141</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3274,16 +3274,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>8</v>
+        <v>143</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3291,16 +3291,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>8</v>
+        <v>145</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3308,16 +3308,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3325,16 +3325,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>8</v>
+        <v>149</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3342,16 +3342,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>8</v>
+        <v>151</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3359,16 +3359,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>8</v>
+        <v>153</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3376,10 +3376,10 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>58</v>
@@ -3393,13 +3393,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B75" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="C75" s="9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>8</v>
@@ -3410,13 +3410,13 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>8</v>
@@ -3427,13 +3427,13 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>8</v>
@@ -3444,13 +3444,13 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>8</v>
@@ -3461,13 +3461,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>8</v>
@@ -3478,13 +3478,13 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>8</v>
@@ -3495,13 +3495,13 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>8</v>
@@ -3512,13 +3512,13 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>8</v>
@@ -3529,13 +3529,13 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>8</v>
@@ -3546,13 +3546,13 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>8</v>
@@ -3563,10 +3563,10 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>58</v>
@@ -3580,13 +3580,13 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B86" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B86" s="8" t="s">
-        <v>176</v>
-      </c>
       <c r="C86" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>8</v>
@@ -3597,13 +3597,13 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>8</v>
@@ -3614,13 +3614,13 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>8</v>
@@ -3631,13 +3631,13 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>8</v>
@@ -3648,13 +3648,13 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>8</v>
@@ -3665,13 +3665,13 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>8</v>
@@ -3682,13 +3682,13 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>8</v>
@@ -3699,13 +3699,13 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>8</v>
@@ -3716,13 +3716,13 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>8</v>
@@ -3733,13 +3733,13 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>8</v>
@@ -3750,10 +3750,10 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>58</v>
@@ -3767,13 +3767,13 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B97" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="B97" s="8" t="s">
-        <v>193</v>
-      </c>
       <c r="C97" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>8</v>
@@ -3784,13 +3784,13 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>8</v>
@@ -3801,13 +3801,13 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>8</v>
@@ -3818,13 +3818,13 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>8</v>
@@ -3835,13 +3835,13 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>8</v>
@@ -3852,13 +3852,13 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>8</v>
@@ -3869,13 +3869,13 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>8</v>
@@ -3886,13 +3886,13 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>8</v>
@@ -3903,13 +3903,13 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>8</v>
@@ -3920,13 +3920,13 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>8</v>
@@ -3937,10 +3937,10 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>58</v>
@@ -3954,13 +3954,13 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B108" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="B108" s="8" t="s">
-        <v>207</v>
-      </c>
       <c r="C108" s="8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>8</v>
@@ -3971,13 +3971,13 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>8</v>
@@ -3988,13 +3988,13 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>8</v>
@@ -4005,13 +4005,13 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>8</v>
@@ -4022,13 +4022,13 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>8</v>
@@ -4039,13 +4039,13 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>8</v>
@@ -4056,13 +4056,13 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>8</v>
@@ -4073,13 +4073,13 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>8</v>
@@ -4090,13 +4090,13 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>8</v>
@@ -4107,13 +4107,13 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>8</v>
@@ -4124,10 +4124,10 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C118" s="8" t="s">
         <v>58</v>
@@ -4141,13 +4141,13 @@
     </row>
     <row r="119" ht="28" spans="1:5">
       <c r="A119" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B119" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="B119" s="8" t="s">
-        <v>226</v>
-      </c>
       <c r="C119" s="10" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>8</v>
@@ -4158,13 +4158,13 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>8</v>
@@ -4175,13 +4175,13 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>8</v>
@@ -4192,13 +4192,13 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>8</v>
@@ -4209,13 +4209,13 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D123" s="5" t="s">
         <v>8</v>
@@ -4226,16 +4226,16 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C124" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>8</v>
@@ -4246,13 +4246,13 @@
         <v>240</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C125" s="8" t="s">
         <v>241</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>8</v>
@@ -4263,13 +4263,13 @@
         <v>242</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>8</v>
@@ -4280,13 +4280,13 @@
         <v>243</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C127" s="8" t="s">
         <v>244</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>8</v>
@@ -4297,13 +4297,13 @@
         <v>245</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C128" s="8" t="s">
         <v>246</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>8</v>
@@ -4314,13 +4314,13 @@
         <v>247</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C129" s="8" t="s">
         <v>248</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>8</v>
@@ -4331,13 +4331,13 @@
         <v>249</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C130" s="8" t="s">
         <v>250</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>8</v>
@@ -4348,13 +4348,13 @@
         <v>251</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C131" s="8" t="s">
         <v>252</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -4365,13 +4365,13 @@
         <v>253</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C132" s="8" t="s">
         <v>254</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>8</v>
@@ -4382,13 +4382,13 @@
         <v>255</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C133" s="8" t="s">
         <v>256</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>8</v>
@@ -4399,13 +4399,13 @@
         <v>257</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C134" s="8" t="s">
         <v>258</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -4416,13 +4416,13 @@
         <v>259</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C135" s="8" t="s">
         <v>260</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -4433,13 +4433,13 @@
         <v>261</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C136" s="8" t="s">
         <v>262</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -4450,13 +4450,13 @@
         <v>263</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C137" s="8" t="s">
         <v>264</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -4467,13 +4467,13 @@
         <v>265</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C138" s="8" t="s">
         <v>266</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>8</v>
@@ -4521,7 +4521,7 @@
         <v>268</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D141" s="5" t="s">
         <v>8</v>
@@ -4572,7 +4572,7 @@
         <v>268</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D144" s="5" t="s">
         <v>8</v>
@@ -4722,7 +4722,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E124 E138 D1:D8 D124:D137 D138:D152 E2:E8 E125:E137 E139:E152 F2:F3 D106:E117 D118:E121 D9:E105 D122:E123">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E44 E138 E139 D1:D8 D44:D72 D138:D152 E2:E8 E45:E72 E140:E152 F2:F3 D123:E137 D9:E43 D73:E122">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
works on RW PDF
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="291">
   <si>
     <t>ID</t>
   </si>
@@ -701,196 +701,202 @@
     <t>TC_116</t>
   </si>
   <si>
+    <t>TC_117</t>
+  </si>
+  <si>
     <t>Reset the RW06 form</t>
   </si>
   <si>
-    <t>TC_117</t>
+    <t>TC_118</t>
   </si>
   <si>
     <t>probateFormsRWxx.feature</t>
   </si>
   <si>
-    <t>TC_118</t>
+    <t>TC_119</t>
   </si>
   <si>
     <t>Verify that the county, estate name, and "Also Known As" (AKA) values are auto-populated from the selected estate.</t>
   </si>
   <si>
-    <t>TC_119</t>
+    <t>TC_120</t>
   </si>
   <si>
     <t>Verify, text can be entered in all the text areas.</t>
   </si>
   <si>
-    <t>TC_120</t>
+    <t>TC_121</t>
   </si>
   <si>
     <t>Verify, the name entered in 1st text area is reflected in the signature.</t>
   </si>
   <si>
-    <t>TC_121</t>
+    <t>TC_122</t>
   </si>
   <si>
     <t>Verify that changes in the witness name field are reflected under the signature line and vice-versa.</t>
   </si>
   <si>
-    <t>TC_122</t>
+    <t>TC_123</t>
   </si>
   <si>
     <t>Reset the RWxx form</t>
   </si>
   <si>
-    <t>TC_123</t>
+    <t>TC_124</t>
   </si>
   <si>
     <t>probateFormsRW07.feature</t>
   </si>
   <si>
+    <t>TC_125</t>
+  </si>
+  <si>
+    <t>Verify, county, estate and file number aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_126</t>
+  </si>
+  <si>
+    <t>TC_127</t>
+  </si>
+  <si>
+    <t>Verify, on checking use 4 digit checkbox, changes in file number</t>
+  </si>
+  <si>
+    <t>TC_128</t>
+  </si>
+  <si>
+    <t>Verify, on clicking bene address field, multiple beneficiaries can be selected.</t>
+  </si>
+  <si>
+    <t>TC_129</t>
+  </si>
+  <si>
+    <t>Verify, beneficiary name and address should be displayed in the form.</t>
+  </si>
+  <si>
+    <t>TC_130</t>
+  </si>
+  <si>
+    <t>Verify, decedent died and county is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_131</t>
+  </si>
+  <si>
+    <t>Verify, on clicking name fiduciary contact list is displayed and multiple users can be selected.</t>
+  </si>
+  <si>
+    <t>TC_132</t>
+  </si>
+  <si>
+    <t>Verify, these contacts are common for all the forms.</t>
+  </si>
+  <si>
+    <t>TC_133</t>
+  </si>
+  <si>
+    <t>Verify, date can be entered.</t>
+  </si>
+  <si>
+    <t>TC_134</t>
+  </si>
+  <si>
+    <t>Verify, registrars address is auto fetched and is editable.</t>
+  </si>
+  <si>
+    <t>TC_135</t>
+  </si>
+  <si>
+    <t>Verify, corporate fiduciary type of contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_136</t>
+  </si>
+  <si>
+    <t>Verify, based on capacity contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_137</t>
+  </si>
+  <si>
+    <t>Verify, selection is cleared on clicking clear selection button.</t>
+  </si>
+  <si>
+    <t>TC_138</t>
+  </si>
+  <si>
+    <t>Reset the RW07 form</t>
+  </si>
+  <si>
+    <t>TC_139</t>
+  </si>
+  <si>
+    <t>probateFormsRW08.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>TC_124</t>
-  </si>
-  <si>
-    <t>Verify, county, estate and file number aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_125</t>
-  </si>
-  <si>
-    <t>TC_126</t>
-  </si>
-  <si>
-    <t>Verify, on checking use 4 digit checkbox, changes in file number</t>
-  </si>
-  <si>
-    <t>TC_127</t>
-  </si>
-  <si>
-    <t>Verify, on clicking bene address field, multiple beneficiaries can be selected.</t>
-  </si>
-  <si>
-    <t>TC_128</t>
-  </si>
-  <si>
-    <t>Verify, beneficiary name and address should be displayed in the form.</t>
-  </si>
-  <si>
-    <t>TC_129</t>
-  </si>
-  <si>
-    <t>Verify, decedent died and county is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_130</t>
-  </si>
-  <si>
-    <t>Verify, on clicking name fiduciary contact list is displayed and multiple users can be selected.</t>
-  </si>
-  <si>
-    <t>TC_131</t>
-  </si>
-  <si>
-    <t>Verify, these contacts are common for all the forms.</t>
-  </si>
-  <si>
-    <t>TC_132</t>
-  </si>
-  <si>
-    <t>Verify, date can be entered.</t>
-  </si>
-  <si>
-    <t>TC_133</t>
-  </si>
-  <si>
-    <t>Verify, registrars address is auto fetched and is editable.</t>
-  </si>
-  <si>
-    <t>TC_134</t>
-  </si>
-  <si>
-    <t>Verify, corporate fiduciary type of contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_135</t>
-  </si>
-  <si>
-    <t>Verify, based on capacity contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_136</t>
-  </si>
-  <si>
-    <t>Verify, selection is cleared on clicking clear selection button.</t>
-  </si>
-  <si>
-    <t>TC_137</t>
-  </si>
-  <si>
-    <t>Reset the RW07 form</t>
-  </si>
-  <si>
-    <t>TC_138</t>
-  </si>
-  <si>
-    <t>probateFormsRW08.feature</t>
-  </si>
-  <si>
-    <t>TC_139</t>
-  </si>
-  <si>
     <t>TC_140</t>
   </si>
   <si>
     <t>TC_141</t>
   </si>
   <si>
+    <t>TC_142</t>
+  </si>
+  <si>
     <t>Verify, Will number and other dates can be entered in correct format.</t>
   </si>
   <si>
-    <t>TC_142</t>
+    <t>TC_143</t>
   </si>
   <si>
     <t>Verify, checkboxes for file no field.</t>
   </si>
   <si>
-    <t>TC_143</t>
-  </si>
-  <si>
     <t>TC_144</t>
   </si>
   <si>
+    <t>TC_145</t>
+  </si>
+  <si>
     <t>Verify, the beneficiaries selected beyond 6 are displayed on the attachment.</t>
   </si>
   <si>
-    <t>TC_145</t>
+    <t>TC_146</t>
   </si>
   <si>
     <t>Verify, count is correctly displayed.</t>
   </si>
   <si>
-    <t>TC_146</t>
+    <t>TC_147</t>
   </si>
   <si>
     <t>Verify, on clicking "Display ALL beneficiary on attachment" checkbox all the contacts are transferred on attachment.</t>
   </si>
   <si>
-    <t>TC_147</t>
-  </si>
-  <si>
     <t>TC_148</t>
   </si>
   <si>
     <t>TC_149</t>
   </si>
   <si>
+    <t>TC_150</t>
+  </si>
+  <si>
     <t>Verify, these 2 sections are common for RW07, RW08 and anything updated is reflected in all the forms.</t>
   </si>
   <si>
-    <t>TC_150</t>
-  </si>
-  <si>
     <t>TC_151</t>
+  </si>
+  <si>
+    <t>TC_152</t>
+  </si>
+  <si>
+    <t>TC_153</t>
   </si>
   <si>
     <t>Reset the RW08 form</t>
@@ -2117,10 +2123,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F152"/>
+  <dimension ref="A1:F155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="C152" sqref="C152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -4112,8 +4118,8 @@
       <c r="B117" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="C117" s="8" t="s">
-        <v>224</v>
+      <c r="C117" s="9" t="s">
+        <v>172</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>8</v>
@@ -4124,47 +4130,47 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C118" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="B118" s="8" t="s">
+      <c r="D118" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C118" s="8" t="s">
+      <c r="B119" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C119" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D118" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E118" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="119" ht="28" spans="1:5">
-      <c r="A119" s="3" t="s">
+      <c r="D119" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" ht="28" spans="1:5">
+      <c r="A120" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B120" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="B119" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C119" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="D119" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E119" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5">
-      <c r="A120" s="3" t="s">
+      <c r="C120" s="10" t="s">
         <v>229</v>
-      </c>
-      <c r="B120" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C120" s="8" t="s">
-        <v>230</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>8</v>
@@ -4175,13 +4181,13 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C121" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="B121" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C121" s="8" t="s">
-        <v>232</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>8</v>
@@ -4192,13 +4198,13 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C122" s="8" t="s">
         <v>233</v>
-      </c>
-      <c r="B122" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C122" s="8" t="s">
-        <v>234</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>8</v>
@@ -4209,13 +4215,13 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C123" s="8" t="s">
         <v>235</v>
-      </c>
-      <c r="B123" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C123" s="8" t="s">
-        <v>236</v>
       </c>
       <c r="D123" s="5" t="s">
         <v>8</v>
@@ -4226,16 +4232,16 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="C124" s="8" t="s">
-        <v>58</v>
+        <v>227</v>
+      </c>
+      <c r="C124" s="9" t="s">
+        <v>172</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>8</v>
@@ -4243,16 +4249,16 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>8</v>
@@ -4260,16 +4266,16 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>8</v>
@@ -4277,16 +4283,16 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>8</v>
@@ -4294,16 +4300,16 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>246</v>
+        <v>104</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>8</v>
@@ -4311,16 +4317,16 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>8</v>
@@ -4328,16 +4334,16 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>8</v>
@@ -4345,16 +4351,16 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -4362,16 +4368,16 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>8</v>
@@ -4379,16 +4385,16 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>8</v>
@@ -4396,16 +4402,16 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="3" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -4413,16 +4419,16 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -4430,16 +4436,16 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -4447,16 +4453,16 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -4464,16 +4470,16 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>8</v>
@@ -4481,13 +4487,13 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>268</v>
+        <v>239</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>58</v>
+        <v>264</v>
       </c>
       <c r="D139" s="5" t="s">
         <v>8</v>
@@ -4498,13 +4504,13 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>268</v>
+        <v>239</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="D140" s="5" t="s">
         <v>8</v>
@@ -4515,16 +4521,16 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B141" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>8</v>
+        <v>269</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -4532,16 +4538,16 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B142" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>272</v>
+        <v>241</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>8</v>
+        <v>269</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -4549,16 +4555,16 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B143" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>274</v>
+        <v>104</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>8</v>
+        <v>269</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -4566,16 +4572,16 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B144" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>134</v>
+        <v>273</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>8</v>
+        <v>269</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>8</v>
@@ -4583,16 +4589,16 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B145" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>8</v>
+        <v>269</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>8</v>
@@ -4600,33 +4606,33 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B146" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>279</v>
+        <v>134</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>8</v>
+        <v>269</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="147" ht="28" spans="1:5">
+    <row r="147" spans="1:5">
       <c r="A147" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B147" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="C147" s="10" t="s">
-        <v>281</v>
+      <c r="C147" s="8" t="s">
+        <v>278</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>8</v>
+        <v>269</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>8</v>
@@ -4634,50 +4640,50 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B148" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>8</v>
+        <v>269</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" ht="28" spans="1:5">
       <c r="A149" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B149" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="C149" s="8" t="s">
-        <v>262</v>
+      <c r="C149" s="10" t="s">
+        <v>282</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>8</v>
+        <v>269</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="150" ht="28" spans="1:5">
+    <row r="150" spans="1:5">
       <c r="A150" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B150" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="C150" s="10" t="s">
-        <v>285</v>
+      <c r="C150" s="8" t="s">
+        <v>260</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>8</v>
+        <v>269</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>8</v>
@@ -4685,35 +4691,86 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B151" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>8</v>
+        <v>269</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" ht="28" spans="1:5">
       <c r="A152" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B152" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="C152" s="8" t="s">
+      <c r="C152" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="D152" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="C153" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D153" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="D152" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E152" s="3" t="s">
+      <c r="B154" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="C154" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D154" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="C155" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="D155" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="E155" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4722,7 +4779,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E124 E138 D1:D8 D124:D137 D138:D152 E2:E8 E125:E137 E139:E152 F2:F3 D106:E117 D118:E121 D9:E105 D122:E123">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D155:E155 D1:D8 E2:E8 F2:F3 D9:E100 D101:E119 D120:E152 D153:E154">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added TCs of RW10 probate form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="290">
   <si>
     <t>ID</t>
   </si>
@@ -314,528 +314,528 @@
     <t>probateFormsRW02.feature</t>
   </si>
   <si>
+    <t>TC_044</t>
+  </si>
+  <si>
+    <t>Verify, correct county name is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_045</t>
+  </si>
+  <si>
+    <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
+  </si>
+  <si>
+    <t>TC_046</t>
+  </si>
+  <si>
+    <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
+  </si>
+  <si>
+    <t>TC_047</t>
+  </si>
+  <si>
+    <t>Verify, county, estate and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_048</t>
+  </si>
+  <si>
+    <t>Verify, the auto populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_049</t>
+  </si>
+  <si>
+    <t>Verify, names can be added in aka fields.</t>
+  </si>
+  <si>
+    <t>TC_050</t>
+  </si>
+  <si>
+    <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
+  </si>
+  <si>
+    <t>TC_051</t>
+  </si>
+  <si>
+    <t>Verify, amount can be entered in the input fields.</t>
+  </si>
+  <si>
+    <t>TC_052</t>
+  </si>
+  <si>
+    <t>Verify, total estimated value should display total of 1st and last field only.</t>
+  </si>
+  <si>
+    <t>TC_053</t>
+  </si>
+  <si>
+    <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_054</t>
+  </si>
+  <si>
+    <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_055</t>
+  </si>
+  <si>
+    <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
+  </si>
+  <si>
+    <t>TC_056</t>
+  </si>
+  <si>
+    <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
+  </si>
+  <si>
+    <t>TC_057</t>
+  </si>
+  <si>
+    <t>Verify that selecting option A keeps it selected without affecting option B.</t>
+  </si>
+  <si>
+    <t>TC_058</t>
+  </si>
+  <si>
+    <t>Verify, decedent died date is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_059</t>
+  </si>
+  <si>
+    <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
+  </si>
+  <si>
+    <t>TC_060</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
+  </si>
+  <si>
+    <t>TC_061</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B keeps it selected without affecting option A.</t>
+  </si>
+  <si>
+    <t>TC_062</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
+  </si>
+  <si>
+    <t>TC_063</t>
+  </si>
+  <si>
+    <t>Verify, multiple beneficiaries can be selected.</t>
+  </si>
+  <si>
+    <t>TC_064</t>
+  </si>
+  <si>
+    <t>Verify, bene contacts in the table.</t>
+  </si>
+  <si>
+    <t>TC_065</t>
+  </si>
+  <si>
+    <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
+  </si>
+  <si>
+    <t>TC_066</t>
+  </si>
+  <si>
+    <t>Verify, on checking "Display all heirs on attachment".</t>
+  </si>
+  <si>
+    <t>TC_067</t>
+  </si>
+  <si>
+    <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
+  </si>
+  <si>
+    <t>TC_068</t>
+  </si>
+  <si>
+    <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
+  </si>
+  <si>
+    <t>TC_069</t>
+  </si>
+  <si>
+    <t>Verify fees section.</t>
+  </si>
+  <si>
+    <t>TC_070</t>
+  </si>
+  <si>
+    <t>Verify, attorney can be selected.</t>
+  </si>
+  <si>
+    <t>TC_071</t>
+  </si>
+  <si>
+    <t>Verify, information in decree of the register.</t>
+  </si>
+  <si>
+    <t>TC_072</t>
+  </si>
+  <si>
+    <t>Reset the RW02 form</t>
+  </si>
+  <si>
+    <t>TC_073</t>
+  </si>
+  <si>
+    <t>probateFormsRW03.feature</t>
+  </si>
+  <si>
+    <t>TC_074</t>
+  </si>
+  <si>
+    <t>Verify county, estate and aka names are auto-populated on the form</t>
+  </si>
+  <si>
+    <t>TC_075</t>
+  </si>
+  <si>
+    <t>Verify, the auto-populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_076</t>
+  </si>
+  <si>
+    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
+  </si>
+  <si>
+    <t>TC_077</t>
+  </si>
+  <si>
+    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
+  </si>
+  <si>
+    <t>TC_078</t>
+  </si>
+  <si>
+    <t>Verify, names can be entered in witness fields.</t>
+  </si>
+  <si>
+    <t>TC_079</t>
+  </si>
+  <si>
+    <t>Verify, names updated from signature are reflected in witness names fields.</t>
+  </si>
+  <si>
+    <t>TC_080</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered in address, city, zip fields.</t>
+  </si>
+  <si>
+    <t>TC_081</t>
+  </si>
+  <si>
+    <t>Verify, form is auto saved.</t>
+  </si>
+  <si>
+    <t>TC_082</t>
+  </si>
+  <si>
+    <t>Verify form can be printed in pdf</t>
+  </si>
+  <si>
+    <t>TC_083</t>
+  </si>
+  <si>
+    <t>Reset the RW03 form</t>
+  </si>
+  <si>
+    <t>TC_084</t>
+  </si>
+  <si>
+    <t>probateFormsRW04.feature</t>
+  </si>
+  <si>
+    <t>TC_085</t>
+  </si>
+  <si>
+    <t>Verify, correct title is displayed on the form's header.</t>
+  </si>
+  <si>
+    <t>TC_086</t>
+  </si>
+  <si>
+    <t>Verify, county, and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_087</t>
+  </si>
+  <si>
+    <t>Verify, correct estate's name is displayed on the form.</t>
+  </si>
+  <si>
+    <t>TC_088</t>
+  </si>
+  <si>
+    <t>Verify, name of the decedent should be auto populated from the form.</t>
+  </si>
+  <si>
+    <t>TC_089</t>
+  </si>
+  <si>
+    <t>TC_090</t>
+  </si>
+  <si>
+    <t>TC_091</t>
+  </si>
+  <si>
+    <t>TC_092</t>
+  </si>
+  <si>
+    <t>TC_093</t>
+  </si>
+  <si>
+    <t>TC_094</t>
+  </si>
+  <si>
+    <t>Reset the RW04 form</t>
+  </si>
+  <si>
+    <t>TC_095</t>
+  </si>
+  <si>
+    <t>probateFormsRW05.feature</t>
+  </si>
+  <si>
+    <t>TC_096</t>
+  </si>
+  <si>
+    <t>TC_097</t>
+  </si>
+  <si>
+    <t>TC_098</t>
+  </si>
+  <si>
+    <t>TC_099</t>
+  </si>
+  <si>
+    <t>TC_100</t>
+  </si>
+  <si>
+    <t>TC_101</t>
+  </si>
+  <si>
+    <t>TC_102</t>
+  </si>
+  <si>
+    <t>TC_103</t>
+  </si>
+  <si>
+    <t>Verify, on checking notary checkbox, notary section displays.</t>
+  </si>
+  <si>
+    <t>TC_104</t>
+  </si>
+  <si>
+    <t>TC_105</t>
+  </si>
+  <si>
+    <t>Reset the RW05 form</t>
+  </si>
+  <si>
+    <t>TC_106</t>
+  </si>
+  <si>
+    <t>probateFormsRW06.feature</t>
+  </si>
+  <si>
+    <t>TC_107</t>
+  </si>
+  <si>
+    <t>TC_108</t>
+  </si>
+  <si>
+    <t>TC_109</t>
+  </si>
+  <si>
+    <t>Verify, form is repeated based on the number of contacts selected.</t>
+  </si>
+  <si>
+    <t>TC_110</t>
+  </si>
+  <si>
+    <t>Verify, corporate fiduciary selected is reflected in the corporate name field.</t>
+  </si>
+  <si>
+    <t>TC_111</t>
+  </si>
+  <si>
+    <t>Verify, details of the selected contact's is displayed in the block under it.</t>
+  </si>
+  <si>
+    <t>TC_112</t>
+  </si>
+  <si>
+    <t>Verify, on clicking signature of person, beneficiary contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_113</t>
+  </si>
+  <si>
+    <t>TC_114</t>
+  </si>
+  <si>
+    <t>Verify, contact details are correctly displayed on each page.</t>
+  </si>
+  <si>
+    <t>TC_115</t>
+  </si>
+  <si>
+    <t>Verify, date and reason text box fields are not same for each field.</t>
+  </si>
+  <si>
+    <t>TC_116</t>
+  </si>
+  <si>
+    <t>Reset the RW06 form</t>
+  </si>
+  <si>
+    <t>TC_117</t>
+  </si>
+  <si>
+    <t>probateFormsRWxx.feature</t>
+  </si>
+  <si>
+    <t>TC_118</t>
+  </si>
+  <si>
+    <t>Verify that the county, estate name, and "Also Known As" (AKA) values are auto-populated from the selected estate.</t>
+  </si>
+  <si>
+    <t>TC_119</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered in all the text areas.</t>
+  </si>
+  <si>
+    <t>TC_120</t>
+  </si>
+  <si>
+    <t>Verify, the name entered in 1st text area is reflected in the signature.</t>
+  </si>
+  <si>
+    <t>TC_121</t>
+  </si>
+  <si>
+    <t>Verify that changes in the witness name field are reflected under the signature line and vice-versa.</t>
+  </si>
+  <si>
+    <t>TC_122</t>
+  </si>
+  <si>
+    <t>Reset the RWxx form</t>
+  </si>
+  <si>
+    <t>TC_123</t>
+  </si>
+  <si>
+    <t>probateFormsRW07.feature</t>
+  </si>
+  <si>
+    <t>TC_124</t>
+  </si>
+  <si>
+    <t>Verify, county, estate and file number aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_125</t>
+  </si>
+  <si>
+    <t>TC_126</t>
+  </si>
+  <si>
+    <t>Verify, on checking use 4 digit checkbox, changes in file number</t>
+  </si>
+  <si>
+    <t>TC_127</t>
+  </si>
+  <si>
+    <t>Verify, on clicking bene address field, multiple beneficiaries can be selected.</t>
+  </si>
+  <si>
+    <t>TC_128</t>
+  </si>
+  <si>
+    <t>Verify, beneficiary name and address should be displayed in the form.</t>
+  </si>
+  <si>
+    <t>TC_129</t>
+  </si>
+  <si>
+    <t>Verify, decedent died and county is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_130</t>
+  </si>
+  <si>
+    <t>Verify, on clicking name fiduciary contact list is displayed and multiple users can be selected.</t>
+  </si>
+  <si>
+    <t>TC_131</t>
+  </si>
+  <si>
+    <t>Verify, these contacts are common for all the forms.</t>
+  </si>
+  <si>
+    <t>TC_132</t>
+  </si>
+  <si>
+    <t>Verify, date can be entered.</t>
+  </si>
+  <si>
+    <t>TC_133</t>
+  </si>
+  <si>
+    <t>Verify, registrars address is auto fetched and is editable.</t>
+  </si>
+  <si>
+    <t>TC_134</t>
+  </si>
+  <si>
+    <t>Verify, corporate fiduciary type of contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_135</t>
+  </si>
+  <si>
+    <t>Verify, based on capacity contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_136</t>
+  </si>
+  <si>
+    <t>Verify, selection is cleared on clicking clear selection button.</t>
+  </si>
+  <si>
+    <t>TC_137</t>
+  </si>
+  <si>
+    <t>Reset the RW07 form</t>
+  </si>
+  <si>
+    <t>TC_138</t>
+  </si>
+  <si>
+    <t>probateFormsRW08.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>TC_044</t>
-  </si>
-  <si>
-    <t>Verify, correct county name is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_045</t>
-  </si>
-  <si>
-    <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
-  </si>
-  <si>
-    <t>TC_046</t>
-  </si>
-  <si>
-    <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
-  </si>
-  <si>
-    <t>TC_047</t>
-  </si>
-  <si>
-    <t>Verify, county, estate and aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_048</t>
-  </si>
-  <si>
-    <t>Verify, the auto populated fields are not editable.</t>
-  </si>
-  <si>
-    <t>TC_049</t>
-  </si>
-  <si>
-    <t>Verify, names can be added in aka fields.</t>
-  </si>
-  <si>
-    <t>TC_050</t>
-  </si>
-  <si>
-    <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
-  </si>
-  <si>
-    <t>TC_051</t>
-  </si>
-  <si>
-    <t>Verify, amount can be entered in the input fields.</t>
-  </si>
-  <si>
-    <t>TC_052</t>
-  </si>
-  <si>
-    <t>Verify, total estimated value should display total of 1st and last field only.</t>
-  </si>
-  <si>
-    <t>TC_053</t>
-  </si>
-  <si>
-    <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
-  </si>
-  <si>
-    <t>TC_054</t>
-  </si>
-  <si>
-    <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
-  </si>
-  <si>
-    <t>TC_055</t>
-  </si>
-  <si>
-    <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
-  </si>
-  <si>
-    <t>TC_056</t>
-  </si>
-  <si>
-    <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
-  </si>
-  <si>
-    <t>TC_057</t>
-  </si>
-  <si>
-    <t>Verify that selecting option A keeps it selected without affecting option B.</t>
-  </si>
-  <si>
-    <t>TC_058</t>
-  </si>
-  <si>
-    <t>Verify, decedent died date is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_059</t>
-  </si>
-  <si>
-    <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
-  </si>
-  <si>
-    <t>TC_060</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
-  </si>
-  <si>
-    <t>TC_061</t>
-  </si>
-  <si>
-    <t>Verify that selecting option B keeps it selected without affecting option A.</t>
-  </si>
-  <si>
-    <t>TC_062</t>
-  </si>
-  <si>
-    <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
-  </si>
-  <si>
-    <t>TC_063</t>
-  </si>
-  <si>
-    <t>Verify, multiple beneficiaries can be selected.</t>
-  </si>
-  <si>
-    <t>TC_064</t>
-  </si>
-  <si>
-    <t>Verify, bene contacts in the table.</t>
-  </si>
-  <si>
-    <t>TC_065</t>
-  </si>
-  <si>
-    <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
-  </si>
-  <si>
-    <t>TC_066</t>
-  </si>
-  <si>
-    <t>Verify, on checking "Display all heirs on attachment".</t>
-  </si>
-  <si>
-    <t>TC_067</t>
-  </si>
-  <si>
-    <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
-  </si>
-  <si>
-    <t>TC_068</t>
-  </si>
-  <si>
-    <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
-  </si>
-  <si>
-    <t>TC_069</t>
-  </si>
-  <si>
-    <t>Verify fees section.</t>
-  </si>
-  <si>
-    <t>TC_070</t>
-  </si>
-  <si>
-    <t>Verify, attorney can be selected.</t>
-  </si>
-  <si>
-    <t>TC_071</t>
-  </si>
-  <si>
-    <t>Verify, information in decree of the register.</t>
-  </si>
-  <si>
-    <t>TC_072</t>
-  </si>
-  <si>
-    <t>Reset the RW02 form</t>
-  </si>
-  <si>
-    <t>TC_073</t>
-  </si>
-  <si>
-    <t>probateFormsRW03.feature</t>
-  </si>
-  <si>
-    <t>TC_074</t>
-  </si>
-  <si>
-    <t>Verify county, estate and aka names are auto-populated on the form</t>
-  </si>
-  <si>
-    <t>TC_075</t>
-  </si>
-  <si>
-    <t>Verify, the auto-populated fields are not editable.</t>
-  </si>
-  <si>
-    <t>TC_076</t>
-  </si>
-  <si>
-    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
-  </si>
-  <si>
-    <t>TC_077</t>
-  </si>
-  <si>
-    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
-  </si>
-  <si>
-    <t>TC_078</t>
-  </si>
-  <si>
-    <t>Verify, names can be entered in witness fields.</t>
-  </si>
-  <si>
-    <t>TC_079</t>
-  </si>
-  <si>
-    <t>Verify, names updated from signature are reflected in witness names fields.</t>
-  </si>
-  <si>
-    <t>TC_080</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered in address, city, zip fields.</t>
-  </si>
-  <si>
-    <t>TC_081</t>
-  </si>
-  <si>
-    <t>Verify, form is auto saved.</t>
-  </si>
-  <si>
-    <t>TC_082</t>
-  </si>
-  <si>
-    <t>Verify form can be printed in pdf</t>
-  </si>
-  <si>
-    <t>TC_083</t>
-  </si>
-  <si>
-    <t>Reset the RW03 form</t>
-  </si>
-  <si>
-    <t>TC_084</t>
-  </si>
-  <si>
-    <t>probateFormsRW04.feature</t>
-  </si>
-  <si>
-    <t>TC_085</t>
-  </si>
-  <si>
-    <t>Verify, correct title is displayed on the form's header.</t>
-  </si>
-  <si>
-    <t>TC_086</t>
-  </si>
-  <si>
-    <t>Verify, county, and aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_087</t>
-  </si>
-  <si>
-    <t>Verify, correct estate's name is displayed on the form.</t>
-  </si>
-  <si>
-    <t>TC_088</t>
-  </si>
-  <si>
-    <t>Verify, name of the decedent should be auto populated from the form.</t>
-  </si>
-  <si>
-    <t>TC_089</t>
-  </si>
-  <si>
-    <t>TC_090</t>
-  </si>
-  <si>
-    <t>TC_091</t>
-  </si>
-  <si>
-    <t>TC_092</t>
-  </si>
-  <si>
-    <t>TC_093</t>
-  </si>
-  <si>
-    <t>TC_094</t>
-  </si>
-  <si>
-    <t>Reset the RW04 form</t>
-  </si>
-  <si>
-    <t>TC_095</t>
-  </si>
-  <si>
-    <t>probateFormsRW05.feature</t>
-  </si>
-  <si>
-    <t>TC_096</t>
-  </si>
-  <si>
-    <t>TC_097</t>
-  </si>
-  <si>
-    <t>TC_098</t>
-  </si>
-  <si>
-    <t>TC_099</t>
-  </si>
-  <si>
-    <t>TC_100</t>
-  </si>
-  <si>
-    <t>TC_101</t>
-  </si>
-  <si>
-    <t>TC_102</t>
-  </si>
-  <si>
-    <t>TC_103</t>
-  </si>
-  <si>
-    <t>Verify, on checking notary checkbox, notary section displays.</t>
-  </si>
-  <si>
-    <t>TC_104</t>
-  </si>
-  <si>
-    <t>TC_105</t>
-  </si>
-  <si>
-    <t>Reset the RW05 form</t>
-  </si>
-  <si>
-    <t>TC_106</t>
-  </si>
-  <si>
-    <t>probateFormsRW06.feature</t>
-  </si>
-  <si>
-    <t>TC_107</t>
-  </si>
-  <si>
-    <t>TC_108</t>
-  </si>
-  <si>
-    <t>TC_109</t>
-  </si>
-  <si>
-    <t>Verify, form is repeated based on the number of contacts selected.</t>
-  </si>
-  <si>
-    <t>TC_110</t>
-  </si>
-  <si>
-    <t>Verify, corporate fiduciary selected is reflected in the corporate name field.</t>
-  </si>
-  <si>
-    <t>TC_111</t>
-  </si>
-  <si>
-    <t>Verify, details of the selected contact's is displayed in the block under it.</t>
-  </si>
-  <si>
-    <t>TC_112</t>
-  </si>
-  <si>
-    <t>Verify, on clicking signature of person, beneficiary contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_113</t>
-  </si>
-  <si>
-    <t>TC_114</t>
-  </si>
-  <si>
-    <t>Verify, contact details are correctly displayed on each page.</t>
-  </si>
-  <si>
-    <t>TC_115</t>
-  </si>
-  <si>
-    <t>Verify, date and reason text box fields are not same for each field.</t>
-  </si>
-  <si>
-    <t>TC_116</t>
-  </si>
-  <si>
-    <t>Reset the RW06 form</t>
-  </si>
-  <si>
-    <t>TC_117</t>
-  </si>
-  <si>
-    <t>probateFormsRWxx.feature</t>
-  </si>
-  <si>
-    <t>TC_118</t>
-  </si>
-  <si>
-    <t>Verify that the county, estate name, and "Also Known As" (AKA) values are auto-populated from the selected estate.</t>
-  </si>
-  <si>
-    <t>TC_119</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered in all the text areas.</t>
-  </si>
-  <si>
-    <t>TC_120</t>
-  </si>
-  <si>
-    <t>Verify, the name entered in 1st text area is reflected in the signature.</t>
-  </si>
-  <si>
-    <t>TC_121</t>
-  </si>
-  <si>
-    <t>Verify that changes in the witness name field are reflected under the signature line and vice-versa.</t>
-  </si>
-  <si>
-    <t>TC_122</t>
-  </si>
-  <si>
-    <t>Reset the RWxx form</t>
-  </si>
-  <si>
-    <t>TC_123</t>
-  </si>
-  <si>
-    <t>probateFormsRW07.feature</t>
-  </si>
-  <si>
-    <t>TC_124</t>
-  </si>
-  <si>
-    <t>Verify, county, estate and file number aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_125</t>
-  </si>
-  <si>
-    <t>TC_126</t>
-  </si>
-  <si>
-    <t>Verify, on checking use 4 digit checkbox, changes in file number</t>
-  </si>
-  <si>
-    <t>TC_127</t>
-  </si>
-  <si>
-    <t>Verify, on clicking bene address field, multiple beneficiaries can be selected.</t>
-  </si>
-  <si>
-    <t>TC_128</t>
-  </si>
-  <si>
-    <t>Verify, beneficiary name and address should be displayed in the form.</t>
-  </si>
-  <si>
-    <t>TC_129</t>
-  </si>
-  <si>
-    <t>Verify, decedent died and county is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_130</t>
-  </si>
-  <si>
-    <t>Verify, on clicking name fiduciary contact list is displayed and multiple users can be selected.</t>
-  </si>
-  <si>
-    <t>TC_131</t>
-  </si>
-  <si>
-    <t>Verify, these contacts are common for all the forms.</t>
-  </si>
-  <si>
-    <t>TC_132</t>
-  </si>
-  <si>
-    <t>Verify, date can be entered.</t>
-  </si>
-  <si>
-    <t>TC_133</t>
-  </si>
-  <si>
-    <t>Verify, registrars address is auto fetched and is editable.</t>
-  </si>
-  <si>
-    <t>TC_134</t>
-  </si>
-  <si>
-    <t>Verify, corporate fiduciary type of contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_135</t>
-  </si>
-  <si>
-    <t>Verify, based on capacity contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_136</t>
-  </si>
-  <si>
-    <t>Verify, selection is cleared on clicking clear selection button.</t>
-  </si>
-  <si>
-    <t>TC_137</t>
-  </si>
-  <si>
-    <t>Reset the RW07 form</t>
-  </si>
-  <si>
-    <t>TC_138</t>
-  </si>
-  <si>
-    <t>probateFormsRW08.feature</t>
-  </si>
-  <si>
     <t>TC_139</t>
   </si>
   <si>
@@ -891,6 +891,9 @@
   </si>
   <si>
     <t>TC_151</t>
+  </si>
+  <si>
+    <t>TC_152</t>
   </si>
   <si>
     <t>Reset the RW08 form</t>
@@ -2117,10 +2120,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F152"/>
+  <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="F148" sqref="F148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2875,7 +2878,7 @@
         <v>58</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>8</v>
@@ -2883,16 +2886,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -2900,16 +2903,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -2917,16 +2920,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -2934,16 +2937,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -2951,16 +2954,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -2968,16 +2971,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -2985,16 +2988,16 @@
     </row>
     <row r="51" ht="28" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -3002,16 +3005,16 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -3019,16 +3022,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -3036,16 +3039,16 @@
     </row>
     <row r="54" ht="28" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -3053,16 +3056,16 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -3070,16 +3073,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -3087,16 +3090,16 @@
     </row>
     <row r="57" ht="28" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -3104,16 +3107,16 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -3121,16 +3124,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -3138,16 +3141,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -3155,16 +3158,16 @@
     </row>
     <row r="61" ht="28" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -3172,16 +3175,16 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3189,16 +3192,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3206,16 +3209,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3223,16 +3226,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3240,16 +3243,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3257,16 +3260,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3274,16 +3277,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3291,16 +3294,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3308,16 +3311,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3325,16 +3328,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3342,16 +3345,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3359,16 +3362,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3376,10 +3379,10 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" s="8" t="s">
         <v>154</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>155</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>58</v>
@@ -3393,13 +3396,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C75" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>157</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>8</v>
@@ -3410,13 +3413,13 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C76" s="9" t="s">
         <v>158</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>159</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>8</v>
@@ -3427,13 +3430,13 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C77" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>161</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>8</v>
@@ -3444,13 +3447,13 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C78" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>8</v>
@@ -3461,13 +3464,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>8</v>
@@ -3478,13 +3481,13 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C80" s="9" t="s">
         <v>166</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>167</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>8</v>
@@ -3495,13 +3498,13 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C81" s="9" t="s">
         <v>168</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>169</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>8</v>
@@ -3512,13 +3515,13 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C82" s="9" t="s">
         <v>170</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>171</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>8</v>
@@ -3529,13 +3532,13 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C83" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>173</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>8</v>
@@ -3546,13 +3549,13 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C84" s="9" t="s">
         <v>174</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>175</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>8</v>
@@ -3563,10 +3566,10 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>176</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>177</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>58</v>
@@ -3580,13 +3583,13 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86" s="8" t="s">
         <v>178</v>
-      </c>
-      <c r="B86" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>179</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>8</v>
@@ -3597,13 +3600,13 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C87" s="8" t="s">
         <v>180</v>
-      </c>
-      <c r="B87" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>181</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>8</v>
@@ -3614,13 +3617,13 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C88" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="B88" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>8</v>
@@ -3631,13 +3634,13 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C89" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>185</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>8</v>
@@ -3648,13 +3651,13 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>8</v>
@@ -3665,13 +3668,13 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>8</v>
@@ -3682,13 +3685,13 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>8</v>
@@ -3699,13 +3702,13 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>8</v>
@@ -3716,13 +3719,13 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>8</v>
@@ -3733,13 +3736,13 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C95" s="8" t="s">
         <v>191</v>
-      </c>
-      <c r="B95" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>192</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>8</v>
@@ -3750,10 +3753,10 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B96" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="B96" s="8" t="s">
-        <v>194</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>58</v>
@@ -3767,13 +3770,13 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>8</v>
@@ -3784,13 +3787,13 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>8</v>
@@ -3801,13 +3804,13 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>8</v>
@@ -3818,13 +3821,13 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>8</v>
@@ -3835,13 +3838,13 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>8</v>
@@ -3852,13 +3855,13 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>8</v>
@@ -3869,13 +3872,13 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>8</v>
@@ -3886,13 +3889,13 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C104" s="8" t="s">
         <v>202</v>
-      </c>
-      <c r="B104" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>203</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>8</v>
@@ -3903,13 +3906,13 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>8</v>
@@ -3920,13 +3923,13 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C106" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C106" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>8</v>
@@ -3937,10 +3940,10 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B107" s="8" t="s">
         <v>207</v>
-      </c>
-      <c r="B107" s="8" t="s">
-        <v>208</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>58</v>
@@ -3954,13 +3957,13 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>8</v>
@@ -3971,13 +3974,13 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>8</v>
@@ -3988,13 +3991,13 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C110" s="8" t="s">
         <v>211</v>
-      </c>
-      <c r="B110" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C110" s="8" t="s">
-        <v>212</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>8</v>
@@ -4005,13 +4008,13 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C111" s="8" t="s">
         <v>213</v>
-      </c>
-      <c r="B111" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C111" s="8" t="s">
-        <v>214</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>8</v>
@@ -4022,13 +4025,13 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C112" s="8" t="s">
         <v>215</v>
-      </c>
-      <c r="B112" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C112" s="8" t="s">
-        <v>216</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>8</v>
@@ -4039,13 +4042,13 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C113" s="8" t="s">
         <v>217</v>
-      </c>
-      <c r="B113" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C113" s="8" t="s">
-        <v>218</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>8</v>
@@ -4056,13 +4059,13 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>8</v>
@@ -4073,13 +4076,13 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C115" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="B115" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C115" s="8" t="s">
-        <v>221</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>8</v>
@@ -4090,13 +4093,13 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C116" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="B116" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C116" s="8" t="s">
-        <v>223</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>8</v>
@@ -4107,13 +4110,13 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C117" s="8" t="s">
         <v>224</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C117" s="8" t="s">
-        <v>225</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>8</v>
@@ -4124,10 +4127,10 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B118" s="8" t="s">
         <v>226</v>
-      </c>
-      <c r="B118" s="8" t="s">
-        <v>227</v>
       </c>
       <c r="C118" s="8" t="s">
         <v>58</v>
@@ -4141,13 +4144,13 @@
     </row>
     <row r="119" ht="28" spans="1:5">
       <c r="A119" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C119" s="10" t="s">
         <v>228</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="C119" s="10" t="s">
-        <v>229</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>8</v>
@@ -4158,13 +4161,13 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C120" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="B120" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="C120" s="8" t="s">
-        <v>231</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>8</v>
@@ -4175,13 +4178,13 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C121" s="8" t="s">
         <v>232</v>
-      </c>
-      <c r="B121" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="C121" s="8" t="s">
-        <v>233</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>8</v>
@@ -4192,13 +4195,13 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C122" s="8" t="s">
         <v>234</v>
-      </c>
-      <c r="B122" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="C122" s="8" t="s">
-        <v>235</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>8</v>
@@ -4209,13 +4212,13 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C123" s="8" t="s">
         <v>236</v>
-      </c>
-      <c r="B123" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="C123" s="8" t="s">
-        <v>237</v>
       </c>
       <c r="D123" s="5" t="s">
         <v>8</v>
@@ -4226,10 +4229,10 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B124" s="8" t="s">
         <v>238</v>
-      </c>
-      <c r="B124" s="8" t="s">
-        <v>239</v>
       </c>
       <c r="C124" s="8" t="s">
         <v>58</v>
@@ -4243,13 +4246,13 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C125" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="B125" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C125" s="8" t="s">
-        <v>241</v>
       </c>
       <c r="D125" s="5" t="s">
         <v>8</v>
@@ -4260,13 +4263,13 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D126" s="5" t="s">
         <v>8</v>
@@ -4277,13 +4280,13 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C127" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="B127" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C127" s="8" t="s">
-        <v>244</v>
       </c>
       <c r="D127" s="5" t="s">
         <v>8</v>
@@ -4294,13 +4297,13 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C128" s="8" t="s">
         <v>245</v>
-      </c>
-      <c r="B128" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C128" s="8" t="s">
-        <v>246</v>
       </c>
       <c r="D128" s="5" t="s">
         <v>8</v>
@@ -4311,13 +4314,13 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C129" s="8" t="s">
         <v>247</v>
-      </c>
-      <c r="B129" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C129" s="8" t="s">
-        <v>248</v>
       </c>
       <c r="D129" s="5" t="s">
         <v>8</v>
@@ -4328,13 +4331,13 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C130" s="8" t="s">
         <v>249</v>
-      </c>
-      <c r="B130" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C130" s="8" t="s">
-        <v>250</v>
       </c>
       <c r="D130" s="5" t="s">
         <v>8</v>
@@ -4345,13 +4348,13 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C131" s="8" t="s">
         <v>251</v>
-      </c>
-      <c r="B131" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C131" s="8" t="s">
-        <v>252</v>
       </c>
       <c r="D131" s="5" t="s">
         <v>8</v>
@@ -4362,13 +4365,13 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C132" s="8" t="s">
         <v>253</v>
-      </c>
-      <c r="B132" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C132" s="8" t="s">
-        <v>254</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>8</v>
@@ -4379,13 +4382,13 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C133" s="8" t="s">
         <v>255</v>
-      </c>
-      <c r="B133" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C133" s="8" t="s">
-        <v>256</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>8</v>
@@ -4396,13 +4399,13 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B134" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C134" s="8" t="s">
         <v>257</v>
-      </c>
-      <c r="B134" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C134" s="8" t="s">
-        <v>258</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>8</v>
@@ -4413,13 +4416,13 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C135" s="8" t="s">
         <v>259</v>
-      </c>
-      <c r="B135" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C135" s="8" t="s">
-        <v>260</v>
       </c>
       <c r="D135" s="5" t="s">
         <v>8</v>
@@ -4430,13 +4433,13 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C136" s="8" t="s">
         <v>261</v>
-      </c>
-      <c r="B136" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C136" s="8" t="s">
-        <v>262</v>
       </c>
       <c r="D136" s="5" t="s">
         <v>8</v>
@@ -4447,13 +4450,13 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C137" s="8" t="s">
         <v>263</v>
-      </c>
-      <c r="B137" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C137" s="8" t="s">
-        <v>264</v>
       </c>
       <c r="D137" s="5" t="s">
         <v>8</v>
@@ -4464,13 +4467,13 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C138" s="8" t="s">
         <v>265</v>
-      </c>
-      <c r="B138" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C138" s="8" t="s">
-        <v>266</v>
       </c>
       <c r="D138" s="5" t="s">
         <v>8</v>
@@ -4481,16 +4484,16 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B139" s="8" t="s">
         <v>267</v>
-      </c>
-      <c r="B139" s="8" t="s">
-        <v>268</v>
       </c>
       <c r="C139" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>8</v>
+        <v>268</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>8</v>
@@ -4501,13 +4504,13 @@
         <v>269</v>
       </c>
       <c r="B140" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C140" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="D140" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="C140" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="D140" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>8</v>
@@ -4518,13 +4521,13 @@
         <v>270</v>
       </c>
       <c r="B141" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C141" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D141" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="C141" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D141" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -4535,13 +4538,13 @@
         <v>271</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C142" s="8" t="s">
         <v>272</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>8</v>
+        <v>268</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -4552,13 +4555,13 @@
         <v>273</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C143" s="8" t="s">
         <v>274</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>8</v>
+        <v>268</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -4569,13 +4572,13 @@
         <v>275</v>
       </c>
       <c r="B144" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C144" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D144" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="C144" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D144" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>8</v>
@@ -4586,13 +4589,13 @@
         <v>276</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C145" s="8" t="s">
         <v>277</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>8</v>
+        <v>268</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>8</v>
@@ -4603,13 +4606,13 @@
         <v>278</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C146" s="8" t="s">
         <v>279</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>8</v>
+        <v>268</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>8</v>
@@ -4620,13 +4623,13 @@
         <v>280</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C147" s="10" t="s">
         <v>281</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>8</v>
+        <v>268</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>8</v>
@@ -4637,13 +4640,13 @@
         <v>282</v>
       </c>
       <c r="B148" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C148" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="D148" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="C148" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="D148" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>8</v>
@@ -4654,13 +4657,13 @@
         <v>283</v>
       </c>
       <c r="B149" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C149" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="D149" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="C149" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="D149" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>8</v>
@@ -4671,13 +4674,13 @@
         <v>284</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C150" s="10" t="s">
         <v>285</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>8</v>
+        <v>268</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>8</v>
@@ -4688,13 +4691,13 @@
         <v>286</v>
       </c>
       <c r="B151" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C151" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D151" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="C151" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="D151" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>8</v>
@@ -4705,15 +4708,32 @@
         <v>287</v>
       </c>
       <c r="B152" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C152" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D152" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="C152" s="8" t="s">
+      <c r="E152" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="D152" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E152" s="3" t="s">
+      <c r="B153" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C153" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="D153" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="E153" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4722,7 +4742,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E44 E138 E139 D1:D8 D44:D72 D138:D152 E2:E8 E45:E72 E140:E152 F2:F3 D123:E137 D9:E43 D73:E122">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D153:E153 D1:D8 D151:D152 E2:E8 E151:E152 F2:F3 D9:E42 D43:E73 D74:E138 D139:E150">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated code of RW03 as per review changes
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -206,412 +206,412 @@
     <t>Open Estate</t>
   </si>
   <si>
+    <t>TC_026</t>
+  </si>
+  <si>
+    <t>Verify, file no. is displayed at the top of the form.</t>
+  </si>
+  <si>
+    <t>TC_027</t>
+  </si>
+  <si>
+    <t>Verify, decedent information is displayed in section1 of the form.</t>
+  </si>
+  <si>
+    <t>TC_028</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 2 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_029</t>
+  </si>
+  <si>
+    <t>Verify, in section 2 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_030</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 3 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_031</t>
+  </si>
+  <si>
+    <t>Verify, in section 3 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_032</t>
+  </si>
+  <si>
+    <t>Verify, on clicking other checkbox, text area is enabled.</t>
+  </si>
+  <si>
+    <t>TC_033</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 4 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_034</t>
+  </si>
+  <si>
+    <t>Verify, on clicking last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_035</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_036</t>
+  </si>
+  <si>
+    <t>Verify, on selecting the contact its information is displayed in section 4.</t>
+  </si>
+  <si>
+    <t>TC_037</t>
+  </si>
+  <si>
+    <t>Verify, on clicking executor last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_038</t>
+  </si>
+  <si>
+    <t>Verify, 3 types of selection is available.</t>
+  </si>
+  <si>
+    <t>TC_039</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be dragged and dropped in a each of the type.</t>
+  </si>
+  <si>
+    <t>TC_040</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 5 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_041</t>
+  </si>
+  <si>
+    <t>Verify the selected contacts are displayed under executor, co executor and secondary co executor.</t>
+  </si>
+  <si>
+    <t>TC_042</t>
+  </si>
+  <si>
+    <t>Reset the RW01 form</t>
+  </si>
+  <si>
+    <t>TC_043</t>
+  </si>
+  <si>
+    <t>probateFormsRW02.feature</t>
+  </si>
+  <si>
+    <t>TC_044</t>
+  </si>
+  <si>
+    <t>Verify, correct county name is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_045</t>
+  </si>
+  <si>
+    <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
+  </si>
+  <si>
+    <t>TC_046</t>
+  </si>
+  <si>
+    <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
+  </si>
+  <si>
+    <t>TC_047</t>
+  </si>
+  <si>
+    <t>Verify, county, estate and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_048</t>
+  </si>
+  <si>
+    <t>Verify, the auto populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_049</t>
+  </si>
+  <si>
+    <t>Verify, names can be added in aka fields.</t>
+  </si>
+  <si>
+    <t>TC_050</t>
+  </si>
+  <si>
+    <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
+  </si>
+  <si>
+    <t>TC_051</t>
+  </si>
+  <si>
+    <t>Verify, amount can be entered in the input fields.</t>
+  </si>
+  <si>
+    <t>TC_052</t>
+  </si>
+  <si>
+    <t>Verify, total estimated value should display total of 1st and last field only.</t>
+  </si>
+  <si>
+    <t>TC_053</t>
+  </si>
+  <si>
+    <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_054</t>
+  </si>
+  <si>
+    <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_055</t>
+  </si>
+  <si>
+    <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
+  </si>
+  <si>
+    <t>TC_056</t>
+  </si>
+  <si>
+    <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
+  </si>
+  <si>
+    <t>TC_057</t>
+  </si>
+  <si>
+    <t>Verify that selecting option A keeps it selected without affecting option B.</t>
+  </si>
+  <si>
+    <t>TC_058</t>
+  </si>
+  <si>
+    <t>Verify, decedent died date is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_059</t>
+  </si>
+  <si>
+    <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
+  </si>
+  <si>
+    <t>TC_060</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
+  </si>
+  <si>
+    <t>TC_061</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B keeps it selected without affecting option A.</t>
+  </si>
+  <si>
+    <t>TC_062</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
+  </si>
+  <si>
+    <t>TC_063</t>
+  </si>
+  <si>
+    <t>Verify, multiple beneficiaries can be selected.</t>
+  </si>
+  <si>
+    <t>TC_064</t>
+  </si>
+  <si>
+    <t>Verify, bene contacts in the table.</t>
+  </si>
+  <si>
+    <t>TC_065</t>
+  </si>
+  <si>
+    <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
+  </si>
+  <si>
+    <t>TC_066</t>
+  </si>
+  <si>
+    <t>Verify, on checking "Display all heirs on attachment".</t>
+  </si>
+  <si>
+    <t>TC_067</t>
+  </si>
+  <si>
+    <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
+  </si>
+  <si>
+    <t>TC_068</t>
+  </si>
+  <si>
+    <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
+  </si>
+  <si>
+    <t>TC_069</t>
+  </si>
+  <si>
+    <t>Verify fees section.</t>
+  </si>
+  <si>
+    <t>TC_070</t>
+  </si>
+  <si>
+    <t>Verify, attorney can be selected.</t>
+  </si>
+  <si>
+    <t>TC_071</t>
+  </si>
+  <si>
+    <t>Verify, information in decree of the register.</t>
+  </si>
+  <si>
+    <t>TC_072</t>
+  </si>
+  <si>
+    <t>Reset the RW02 form</t>
+  </si>
+  <si>
+    <t>TC_073</t>
+  </si>
+  <si>
+    <t>probateFormsRW03.feature</t>
+  </si>
+  <si>
+    <t>TC_074</t>
+  </si>
+  <si>
+    <t>Verify county, estate and aka names are auto-populated on the form</t>
+  </si>
+  <si>
+    <t>TC_075</t>
+  </si>
+  <si>
+    <t>Verify, the auto-populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_076</t>
+  </si>
+  <si>
+    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
+  </si>
+  <si>
+    <t>TC_077</t>
+  </si>
+  <si>
+    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
+  </si>
+  <si>
+    <t>TC_078</t>
+  </si>
+  <si>
+    <t>Verify, names can be entered in witness fields.</t>
+  </si>
+  <si>
+    <t>TC_079</t>
+  </si>
+  <si>
+    <t>Verify, names updated from signature are reflected in witness names fields.</t>
+  </si>
+  <si>
+    <t>TC_080</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered in address, city, zip fields.</t>
+  </si>
+  <si>
+    <t>TC_081</t>
+  </si>
+  <si>
+    <t>Verify, form is auto saved.</t>
+  </si>
+  <si>
+    <t>TC_082</t>
+  </si>
+  <si>
+    <t>Verify form can be printed in pdf</t>
+  </si>
+  <si>
+    <t>TC_083</t>
+  </si>
+  <si>
+    <t>Reset the RW03 form</t>
+  </si>
+  <si>
+    <t>TC_084</t>
+  </si>
+  <si>
+    <t>probateFormsRW04.feature</t>
+  </si>
+  <si>
+    <t>TC_085</t>
+  </si>
+  <si>
+    <t>Verify, correct title is displayed on the form's header.</t>
+  </si>
+  <si>
+    <t>TC_086</t>
+  </si>
+  <si>
+    <t>Verify, county, and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_087</t>
+  </si>
+  <si>
+    <t>Verify, correct estate's name is displayed on the form.</t>
+  </si>
+  <si>
+    <t>TC_088</t>
+  </si>
+  <si>
+    <t>Verify, name of the decedent should be auto populated from the form.</t>
+  </si>
+  <si>
+    <t>TC_089</t>
+  </si>
+  <si>
+    <t>TC_090</t>
+  </si>
+  <si>
+    <t>TC_091</t>
+  </si>
+  <si>
+    <t>TC_092</t>
+  </si>
+  <si>
+    <t>TC_093</t>
+  </si>
+  <si>
+    <t>TC_094</t>
+  </si>
+  <si>
+    <t>Reset the RW04 form</t>
+  </si>
+  <si>
+    <t>TC_095</t>
+  </si>
+  <si>
+    <t>probateFormsRW05.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_026</t>
-  </si>
-  <si>
-    <t>Verify, file no. is displayed at the top of the form.</t>
-  </si>
-  <si>
-    <t>TC_027</t>
-  </si>
-  <si>
-    <t>Verify, decedent information is displayed in section1 of the form.</t>
-  </si>
-  <si>
-    <t>TC_028</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 2 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_029</t>
-  </si>
-  <si>
-    <t>Verify, in section 2 only 1 checkbox can be checked.</t>
-  </si>
-  <si>
-    <t>TC_030</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 3 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_031</t>
-  </si>
-  <si>
-    <t>Verify, in section 3 only 1 checkbox can be checked.</t>
-  </si>
-  <si>
-    <t>TC_032</t>
-  </si>
-  <si>
-    <t>Verify, on clicking other checkbox, text area is enabled.</t>
-  </si>
-  <si>
-    <t>TC_033</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 4 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_034</t>
-  </si>
-  <si>
-    <t>Verify, on clicking last name, a side bar is displayed.</t>
-  </si>
-  <si>
-    <t>TC_035</t>
-  </si>
-  <si>
-    <t>Verify, only 1 contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_036</t>
-  </si>
-  <si>
-    <t>Verify, on selecting the contact its information is displayed in section 4.</t>
-  </si>
-  <si>
-    <t>TC_037</t>
-  </si>
-  <si>
-    <t>Verify, on clicking executor last name, a side bar is displayed.</t>
-  </si>
-  <si>
-    <t>TC_038</t>
-  </si>
-  <si>
-    <t>Verify, 3 types of selection is available.</t>
-  </si>
-  <si>
-    <t>TC_039</t>
-  </si>
-  <si>
-    <t>Verify, only 1 contact can be dragged and dropped in a each of the type.</t>
-  </si>
-  <si>
-    <t>TC_040</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 5 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_041</t>
-  </si>
-  <si>
-    <t>Verify the selected contacts are displayed under executor, co executor and secondary co executor.</t>
-  </si>
-  <si>
-    <t>TC_042</t>
-  </si>
-  <si>
-    <t>Reset the RW01 form</t>
-  </si>
-  <si>
-    <t>TC_043</t>
-  </si>
-  <si>
-    <t>probateFormsRW02.feature</t>
-  </si>
-  <si>
-    <t>TC_044</t>
-  </si>
-  <si>
-    <t>Verify, correct county name is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_045</t>
-  </si>
-  <si>
-    <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
-  </si>
-  <si>
-    <t>TC_046</t>
-  </si>
-  <si>
-    <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
-  </si>
-  <si>
-    <t>TC_047</t>
-  </si>
-  <si>
-    <t>Verify, county, estate and aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_048</t>
-  </si>
-  <si>
-    <t>Verify, the auto populated fields are not editable.</t>
-  </si>
-  <si>
-    <t>TC_049</t>
-  </si>
-  <si>
-    <t>Verify, names can be added in aka fields.</t>
-  </si>
-  <si>
-    <t>TC_050</t>
-  </si>
-  <si>
-    <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
-  </si>
-  <si>
-    <t>TC_051</t>
-  </si>
-  <si>
-    <t>Verify, amount can be entered in the input fields.</t>
-  </si>
-  <si>
-    <t>TC_052</t>
-  </si>
-  <si>
-    <t>Verify, total estimated value should display total of 1st and last field only.</t>
-  </si>
-  <si>
-    <t>TC_053</t>
-  </si>
-  <si>
-    <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
-  </si>
-  <si>
-    <t>TC_054</t>
-  </si>
-  <si>
-    <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
-  </si>
-  <si>
-    <t>TC_055</t>
-  </si>
-  <si>
-    <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
-  </si>
-  <si>
-    <t>TC_056</t>
-  </si>
-  <si>
-    <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
-  </si>
-  <si>
-    <t>TC_057</t>
-  </si>
-  <si>
-    <t>Verify that selecting option A keeps it selected without affecting option B.</t>
-  </si>
-  <si>
-    <t>TC_058</t>
-  </si>
-  <si>
-    <t>Verify, decedent died date is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_059</t>
-  </si>
-  <si>
-    <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
-  </si>
-  <si>
-    <t>TC_060</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
-  </si>
-  <si>
-    <t>TC_061</t>
-  </si>
-  <si>
-    <t>Verify that selecting option B keeps it selected without affecting option A.</t>
-  </si>
-  <si>
-    <t>TC_062</t>
-  </si>
-  <si>
-    <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
-  </si>
-  <si>
-    <t>TC_063</t>
-  </si>
-  <si>
-    <t>Verify, multiple beneficiaries can be selected.</t>
-  </si>
-  <si>
-    <t>TC_064</t>
-  </si>
-  <si>
-    <t>Verify, bene contacts in the table.</t>
-  </si>
-  <si>
-    <t>TC_065</t>
-  </si>
-  <si>
-    <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
-  </si>
-  <si>
-    <t>TC_066</t>
-  </si>
-  <si>
-    <t>Verify, on checking "Display all heirs on attachment".</t>
-  </si>
-  <si>
-    <t>TC_067</t>
-  </si>
-  <si>
-    <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
-  </si>
-  <si>
-    <t>TC_068</t>
-  </si>
-  <si>
-    <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
-  </si>
-  <si>
-    <t>TC_069</t>
-  </si>
-  <si>
-    <t>Verify fees section.</t>
-  </si>
-  <si>
-    <t>TC_070</t>
-  </si>
-  <si>
-    <t>Verify, attorney can be selected.</t>
-  </si>
-  <si>
-    <t>TC_071</t>
-  </si>
-  <si>
-    <t>Verify, information in decree of the register.</t>
-  </si>
-  <si>
-    <t>TC_072</t>
-  </si>
-  <si>
-    <t>Reset the RW02 form</t>
-  </si>
-  <si>
-    <t>TC_073</t>
-  </si>
-  <si>
-    <t>probateFormsRW03.feature</t>
-  </si>
-  <si>
-    <t>TC_074</t>
-  </si>
-  <si>
-    <t>Verify county, estate and aka names are auto-populated on the form</t>
-  </si>
-  <si>
-    <t>TC_075</t>
-  </si>
-  <si>
-    <t>Verify, the auto-populated fields are not editable.</t>
-  </si>
-  <si>
-    <t>TC_076</t>
-  </si>
-  <si>
-    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
-  </si>
-  <si>
-    <t>TC_077</t>
-  </si>
-  <si>
-    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
-  </si>
-  <si>
-    <t>TC_078</t>
-  </si>
-  <si>
-    <t>Verify, names can be entered in witness fields.</t>
-  </si>
-  <si>
-    <t>TC_079</t>
-  </si>
-  <si>
-    <t>Verify, names updated from signature are reflected in witness names fields.</t>
-  </si>
-  <si>
-    <t>TC_080</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered in address, city, zip fields.</t>
-  </si>
-  <si>
-    <t>TC_081</t>
-  </si>
-  <si>
-    <t>Verify, form is auto saved.</t>
-  </si>
-  <si>
-    <t>TC_082</t>
-  </si>
-  <si>
-    <t>Verify form can be printed in pdf</t>
-  </si>
-  <si>
-    <t>TC_083</t>
-  </si>
-  <si>
-    <t>Reset the RW03 form</t>
-  </si>
-  <si>
-    <t>TC_084</t>
-  </si>
-  <si>
-    <t>probateFormsRW04.feature</t>
-  </si>
-  <si>
-    <t>TC_085</t>
-  </si>
-  <si>
-    <t>Verify, correct title is displayed on the form's header.</t>
-  </si>
-  <si>
-    <t>TC_086</t>
-  </si>
-  <si>
-    <t>Verify, county, and aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_087</t>
-  </si>
-  <si>
-    <t>Verify, correct estate's name is displayed on the form.</t>
-  </si>
-  <si>
-    <t>TC_088</t>
-  </si>
-  <si>
-    <t>Verify, name of the decedent should be auto populated from the form.</t>
-  </si>
-  <si>
-    <t>TC_089</t>
-  </si>
-  <si>
-    <t>TC_090</t>
-  </si>
-  <si>
-    <t>TC_091</t>
-  </si>
-  <si>
-    <t>TC_092</t>
-  </si>
-  <si>
-    <t>TC_093</t>
-  </si>
-  <si>
-    <t>TC_094</t>
-  </si>
-  <si>
-    <t>Reset the RW04 form</t>
-  </si>
-  <si>
-    <t>TC_095</t>
-  </si>
-  <si>
-    <t>probateFormsRW05.feature</t>
   </si>
   <si>
     <t>TC_096</t>
@@ -1686,7 +1686,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1709,10 +1709,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2237,8 +2233,8 @@
   <sheetPr/>
   <dimension ref="A1:F173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2687,7 +2683,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>8</v>
@@ -2695,16 +2691,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>8</v>
@@ -2712,16 +2708,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>8</v>
@@ -2729,16 +2725,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>8</v>
@@ -2746,16 +2742,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>8</v>
@@ -2763,16 +2759,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>8</v>
@@ -2780,16 +2776,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>8</v>
@@ -2797,16 +2793,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>8</v>
@@ -2814,16 +2810,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>8</v>
@@ -2831,16 +2827,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>8</v>
@@ -2848,16 +2844,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>8</v>
@@ -2865,16 +2861,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>8</v>
@@ -2882,16 +2878,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>8</v>
@@ -2899,16 +2895,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>8</v>
@@ -2916,16 +2912,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>8</v>
@@ -2933,16 +2929,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>8</v>
@@ -2950,16 +2946,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>8</v>
@@ -2967,16 +2963,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>8</v>
@@ -2984,10 +2980,10 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>58</v>
@@ -3001,13 +2997,13 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>97</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>8</v>
@@ -3018,13 +3014,13 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>99</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>8</v>
@@ -3035,13 +3031,13 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>101</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>8</v>
@@ -3052,13 +3048,13 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>103</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>8</v>
@@ -3069,13 +3065,13 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>8</v>
@@ -3086,13 +3082,13 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>8</v>
@@ -3103,13 +3099,13 @@
     </row>
     <row r="51" ht="28" spans="1:5">
       <c r="A51" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>108</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>109</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>8</v>
@@ -3120,13 +3116,13 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>8</v>
@@ -3137,13 +3133,13 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>113</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>8</v>
@@ -3154,13 +3150,13 @@
     </row>
     <row r="54" ht="28" spans="1:5">
       <c r="A54" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>8</v>
@@ -3171,13 +3167,13 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>8</v>
@@ -3188,13 +3184,13 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>119</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>8</v>
@@ -3205,13 +3201,13 @@
     </row>
     <row r="57" ht="28" spans="1:5">
       <c r="A57" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>121</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>8</v>
@@ -3222,13 +3218,13 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>123</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>8</v>
@@ -3239,13 +3235,13 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>8</v>
@@ -3256,13 +3252,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>8</v>
@@ -3273,13 +3269,13 @@
     </row>
     <row r="61" ht="28" spans="1:5">
       <c r="A61" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>129</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>8</v>
@@ -3290,13 +3286,13 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="9" t="s">
         <v>130</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>131</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>8</v>
@@ -3307,13 +3303,13 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C63" s="9" t="s">
         <v>132</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>133</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>8</v>
@@ -3324,13 +3320,13 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" s="9" t="s">
         <v>134</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>135</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>8</v>
@@ -3341,13 +3337,13 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C65" s="9" t="s">
         <v>136</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>137</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>8</v>
@@ -3358,13 +3354,13 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>138</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>139</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>8</v>
@@ -3375,13 +3371,13 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>140</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>141</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>8</v>
@@ -3392,13 +3388,13 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>142</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>143</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>8</v>
@@ -3409,13 +3405,13 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>144</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>145</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>8</v>
@@ -3426,13 +3422,13 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>146</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>147</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>8</v>
@@ -3443,13 +3439,13 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C71" s="9" t="s">
         <v>148</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>149</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>8</v>
@@ -3460,13 +3456,13 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>150</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>151</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>8</v>
@@ -3477,13 +3473,13 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C73" s="9" t="s">
         <v>152</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>153</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>8</v>
@@ -3494,15 +3490,15 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" s="8" t="s">
         <v>154</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>155</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E74" s="3" t="s">
@@ -3511,15 +3507,15 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C75" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B75" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E75" s="3" t="s">
@@ -3528,15 +3524,15 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C76" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B76" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E76" s="3" t="s">
@@ -3545,15 +3541,15 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C77" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B77" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E77" s="3" t="s">
@@ -3562,15 +3558,15 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C78" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B78" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E78" s="3" t="s">
@@ -3579,15 +3575,15 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="B79" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E79" s="3" t="s">
@@ -3596,15 +3592,15 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C80" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="B80" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="D80" s="5" t="s">
+      <c r="D80" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E80" s="3" t="s">
@@ -3613,15 +3609,15 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C81" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="B81" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E81" s="3" t="s">
@@ -3630,15 +3626,15 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C82" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="B82" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E82" s="3" t="s">
@@ -3647,15 +3643,15 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C83" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="B83" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="D83" s="5" t="s">
+      <c r="D83" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E83" s="3" t="s">
@@ -3664,15 +3660,15 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C84" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B84" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E84" s="3" t="s">
@@ -3681,15 +3677,15 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>176</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>177</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D85" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E85" s="3" t="s">
@@ -3698,15 +3694,15 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="B86" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="D86" s="5" t="s">
+      <c r="D86" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E86" s="3" t="s">
@@ -3715,15 +3711,15 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C87" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="B87" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="D87" s="5" t="s">
+      <c r="D87" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E87" s="3" t="s">
@@ -3732,15 +3728,15 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C88" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B88" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E88" s="3" t="s">
@@ -3749,15 +3745,15 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C89" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="B89" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="D89" s="5" t="s">
+      <c r="D89" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E89" s="3" t="s">
@@ -3766,15 +3762,15 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D90" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D90" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E90" s="3" t="s">
@@ -3783,15 +3779,15 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="D91" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D91" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E91" s="3" t="s">
@@ -3800,15 +3796,15 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="D92" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D92" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E92" s="3" t="s">
@@ -3817,15 +3813,15 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D93" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D93" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E93" s="3" t="s">
@@ -3834,15 +3830,15 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="D94" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D94" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E94" s="3" t="s">
@@ -3851,15 +3847,15 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C95" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="B95" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="D95" s="5" t="s">
+      <c r="D95" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E95" s="3" t="s">
@@ -3868,16 +3864,16 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B96" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="B96" s="8" t="s">
-        <v>194</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>8</v>
@@ -3888,13 +3884,13 @@
         <v>195</v>
       </c>
       <c r="B97" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D97" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -3905,13 +3901,13 @@
         <v>196</v>
       </c>
       <c r="B98" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D98" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="C98" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -3922,13 +3918,13 @@
         <v>197</v>
       </c>
       <c r="B99" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D99" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="C99" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="D99" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -3939,13 +3935,13 @@
         <v>198</v>
       </c>
       <c r="B100" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D100" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="C100" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D100" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -3956,13 +3952,13 @@
         <v>199</v>
       </c>
       <c r="B101" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D101" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="C101" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -3973,13 +3969,13 @@
         <v>200</v>
       </c>
       <c r="B102" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D102" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="C102" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="D102" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -3990,13 +3986,13 @@
         <v>201</v>
       </c>
       <c r="B103" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D103" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="C103" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -4007,13 +4003,13 @@
         <v>202</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>203</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -4024,13 +4020,13 @@
         <v>204</v>
       </c>
       <c r="B105" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D105" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="C105" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -4041,13 +4037,13 @@
         <v>205</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>206</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -4078,7 +4074,7 @@
         <v>208</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>8</v>
@@ -4095,7 +4091,7 @@
         <v>208</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>8</v>
@@ -4384,7 +4380,7 @@
         <v>239</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D126" s="5" t="s">
         <v>8</v>
@@ -4639,7 +4635,7 @@
         <v>268</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D141" s="5" t="s">
         <v>8</v>
@@ -4690,7 +4686,7 @@
         <v>268</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D144" s="5" t="s">
         <v>8</v>
@@ -4826,7 +4822,7 @@
         <v>268</v>
       </c>
       <c r="C152" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D152" s="5" t="s">
         <v>8</v>
@@ -4859,7 +4855,7 @@
       <c r="B154" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C154" s="11" t="s">
+      <c r="C154" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D154" s="5" t="s">
@@ -4876,7 +4872,7 @@
       <c r="B155" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C155" s="11" t="s">
+      <c r="C155" s="8" t="s">
         <v>293</v>
       </c>
       <c r="D155" s="5" t="s">
@@ -4893,7 +4889,7 @@
       <c r="B156" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C156" s="11" t="s">
+      <c r="C156" s="8" t="s">
         <v>295</v>
       </c>
       <c r="D156" s="5" t="s">
@@ -4910,7 +4906,7 @@
       <c r="B157" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C157" s="11" t="s">
+      <c r="C157" s="8" t="s">
         <v>297</v>
       </c>
       <c r="D157" s="5" t="s">
@@ -4927,7 +4923,7 @@
       <c r="B158" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C158" s="11" t="s">
+      <c r="C158" s="8" t="s">
         <v>299</v>
       </c>
       <c r="D158" s="5" t="s">
@@ -4944,7 +4940,7 @@
       <c r="B159" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C159" s="11" t="s">
+      <c r="C159" s="8" t="s">
         <v>301</v>
       </c>
       <c r="D159" s="5" t="s">
@@ -4961,7 +4957,7 @@
       <c r="B160" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C160" s="11" t="s">
+      <c r="C160" s="8" t="s">
         <v>303</v>
       </c>
       <c r="D160" s="5" t="s">
@@ -4978,7 +4974,7 @@
       <c r="B161" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C161" s="11" t="s">
+      <c r="C161" s="8" t="s">
         <v>305</v>
       </c>
       <c r="D161" s="5" t="s">
@@ -4995,7 +4991,7 @@
       <c r="B162" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C162" s="11" t="s">
+      <c r="C162" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D162" s="5" t="s">
@@ -5012,7 +5008,7 @@
       <c r="B163" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C163" s="11" t="s">
+      <c r="C163" s="8" t="s">
         <v>309</v>
       </c>
       <c r="D163" s="5" t="s">
@@ -5029,7 +5025,7 @@
       <c r="B164" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C164" s="11" t="s">
+      <c r="C164" s="8" t="s">
         <v>311</v>
       </c>
       <c r="D164" s="5" t="s">
@@ -5046,7 +5042,7 @@
       <c r="B165" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C165" s="11" t="s">
+      <c r="C165" s="8" t="s">
         <v>313</v>
       </c>
       <c r="D165" s="5" t="s">
@@ -5063,7 +5059,7 @@
       <c r="B166" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C166" s="11" t="s">
+      <c r="C166" s="8" t="s">
         <v>315</v>
       </c>
       <c r="D166" s="5" t="s">
@@ -5080,7 +5076,7 @@
       <c r="B167" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C167" s="11" t="s">
+      <c r="C167" s="8" t="s">
         <v>317</v>
       </c>
       <c r="D167" s="5" t="s">
@@ -5097,7 +5093,7 @@
       <c r="B168" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C168" s="11" t="s">
+      <c r="C168" s="8" t="s">
         <v>319</v>
       </c>
       <c r="D168" s="5" t="s">
@@ -5114,7 +5110,7 @@
       <c r="B169" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C169" s="11" t="s">
+      <c r="C169" s="8" t="s">
         <v>260</v>
       </c>
       <c r="D169" s="5" t="s">
@@ -5131,7 +5127,7 @@
       <c r="B170" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C170" s="11" t="s">
+      <c r="C170" s="8" t="s">
         <v>262</v>
       </c>
       <c r="D170" s="5" t="s">
@@ -5148,7 +5144,7 @@
       <c r="B171" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C171" s="12" t="s">
+      <c r="C171" s="10" t="s">
         <v>323</v>
       </c>
       <c r="D171" s="5" t="s">
@@ -5165,7 +5161,7 @@
       <c r="B172" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C172" s="11" t="s">
+      <c r="C172" s="8" t="s">
         <v>264</v>
       </c>
       <c r="D172" s="5" t="s">
@@ -5182,7 +5178,7 @@
       <c r="B173" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C173" s="11" t="s">
+      <c r="C173" s="8" t="s">
         <v>326</v>
       </c>
       <c r="D173" s="5" t="s">
@@ -5197,7 +5193,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E26 E138 E151 D1:D8 D26:D42 D138:D173 E2:E8 E27:E42 E139:E150 E152:E173 F2:F3 D9:E25 D43:E137">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E84 E95 D96:E96 E97 D1:D8 D84:D95 D97:D105 E2:E8 E85:E94 E98:E105 F2:F3 D43:E73 D74:E83 D9:E42 D106:E173">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated RW forms to save estate info using key-value pairs & modified RW06 to retrieve data from JSON
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -611,49 +611,49 @@
     <t>probateFormsRW05.feature</t>
   </si>
   <si>
+    <t>TC_096</t>
+  </si>
+  <si>
+    <t>TC_097</t>
+  </si>
+  <si>
+    <t>TC_098</t>
+  </si>
+  <si>
+    <t>TC_099</t>
+  </si>
+  <si>
+    <t>TC_100</t>
+  </si>
+  <si>
+    <t>TC_101</t>
+  </si>
+  <si>
+    <t>TC_102</t>
+  </si>
+  <si>
+    <t>TC_103</t>
+  </si>
+  <si>
+    <t>Verify, on checking notary checkbox, notary section displays.</t>
+  </si>
+  <si>
+    <t>TC_104</t>
+  </si>
+  <si>
+    <t>TC_105</t>
+  </si>
+  <si>
+    <t>Reset the RW05 form</t>
+  </si>
+  <si>
+    <t>TC_106</t>
+  </si>
+  <si>
+    <t>probateFormsRW06.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_096</t>
-  </si>
-  <si>
-    <t>TC_097</t>
-  </si>
-  <si>
-    <t>TC_098</t>
-  </si>
-  <si>
-    <t>TC_099</t>
-  </si>
-  <si>
-    <t>TC_100</t>
-  </si>
-  <si>
-    <t>TC_101</t>
-  </si>
-  <si>
-    <t>TC_102</t>
-  </si>
-  <si>
-    <t>TC_103</t>
-  </si>
-  <si>
-    <t>Verify, on checking notary checkbox, notary section displays.</t>
-  </si>
-  <si>
-    <t>TC_104</t>
-  </si>
-  <si>
-    <t>TC_105</t>
-  </si>
-  <si>
-    <t>Reset the RW05 form</t>
-  </si>
-  <si>
-    <t>TC_106</t>
-  </si>
-  <si>
-    <t>probateFormsRW06.feature</t>
   </si>
   <si>
     <t>TC_107</t>
@@ -2233,8 +2233,8 @@
   <sheetPr/>
   <dimension ref="A1:F173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E100" sqref="E100"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3872,8 +3872,8 @@
       <c r="C96" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D96" s="5" t="s">
-        <v>194</v>
+      <c r="D96" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>8</v>
@@ -3881,7 +3881,7 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>193</v>
@@ -3889,8 +3889,8 @@
       <c r="C97" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D97" s="5" t="s">
-        <v>194</v>
+      <c r="D97" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -3898,7 +3898,7 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>193</v>
@@ -3906,8 +3906,8 @@
       <c r="C98" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D98" s="5" t="s">
-        <v>194</v>
+      <c r="D98" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -3915,7 +3915,7 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>193</v>
@@ -3923,8 +3923,8 @@
       <c r="C99" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="D99" s="5" t="s">
-        <v>194</v>
+      <c r="D99" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -3932,7 +3932,7 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>193</v>
@@ -3940,8 +3940,8 @@
       <c r="C100" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="D100" s="5" t="s">
-        <v>194</v>
+      <c r="D100" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -3949,7 +3949,7 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>193</v>
@@ -3957,8 +3957,8 @@
       <c r="C101" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="D101" s="5" t="s">
-        <v>194</v>
+      <c r="D101" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -3966,7 +3966,7 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>193</v>
@@ -3974,8 +3974,8 @@
       <c r="C102" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="D102" s="5" t="s">
-        <v>194</v>
+      <c r="D102" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -3983,7 +3983,7 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>193</v>
@@ -3991,8 +3991,8 @@
       <c r="C103" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="D103" s="5" t="s">
-        <v>194</v>
+      <c r="D103" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -4000,16 +4000,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>193</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="D104" s="5" t="s">
-        <v>194</v>
+        <v>202</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -4017,7 +4017,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>193</v>
@@ -4025,8 +4025,8 @@
       <c r="C105" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D105" s="5" t="s">
-        <v>194</v>
+      <c r="D105" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -4034,16 +4034,16 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B106" s="8" t="s">
         <v>193</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="D106" s="5" t="s">
-        <v>194</v>
+        <v>205</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -4051,16 +4051,16 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B107" s="8" t="s">
         <v>207</v>
-      </c>
-      <c r="B107" s="8" t="s">
-        <v>208</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D107" s="5" t="s">
-        <v>8</v>
+      <c r="D107" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -4071,13 +4071,13 @@
         <v>209</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D108" s="5" t="s">
-        <v>8</v>
+      <c r="D108" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -4088,13 +4088,13 @@
         <v>210</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D109" s="5" t="s">
-        <v>8</v>
+      <c r="D109" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -4105,13 +4105,13 @@
         <v>211</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="D110" s="5" t="s">
-        <v>8</v>
+      <c r="D110" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -4122,13 +4122,13 @@
         <v>213</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C111" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="D111" s="5" t="s">
-        <v>8</v>
+      <c r="D111" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -4139,13 +4139,13 @@
         <v>215</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="D112" s="5" t="s">
-        <v>8</v>
+      <c r="D112" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -4156,13 +4156,13 @@
         <v>217</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C113" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="D113" s="5" t="s">
-        <v>8</v>
+      <c r="D113" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -4173,13 +4173,13 @@
         <v>219</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C114" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="D114" s="5" t="s">
-        <v>8</v>
+      <c r="D114" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -4190,13 +4190,13 @@
         <v>220</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C115" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="D115" s="5" t="s">
-        <v>8</v>
+      <c r="D115" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -4207,13 +4207,13 @@
         <v>222</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C116" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="D116" s="5" t="s">
-        <v>8</v>
+      <c r="D116" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -4224,13 +4224,13 @@
         <v>224</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C117" s="8" t="s">
         <v>225</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -5193,7 +5193,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E84 E95 D96:E96 E97 D1:D8 D84:D95 D97:D105 E2:E8 E85:E94 E98:E105 F2:F3 D43:E73 D74:E83 D9:E42 D106:E173">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E107 E153 D1:D8 D107:D116 D153:D173 E2:E8 E108:E116 E154:E173 F2:F3 D95:E106 D9:E94 D117:E152">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
works on all PDFs
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="327">
   <si>
     <t>ID</t>
   </si>
@@ -656,63 +656,63 @@
     <t>probateFormsRW06.feature</t>
   </si>
   <si>
+    <t>TC_108</t>
+  </si>
+  <si>
+    <t>TC_109</t>
+  </si>
+  <si>
+    <t>Verify, form is repeated based on the number of contacts selected.</t>
+  </si>
+  <si>
+    <t>TC_110</t>
+  </si>
+  <si>
+    <t>Verify, corporate fiduciary selected is reflected in the corporate name field.</t>
+  </si>
+  <si>
+    <t>TC_111</t>
+  </si>
+  <si>
+    <t>Verify, details of the selected contact's is displayed in the block under it.</t>
+  </si>
+  <si>
+    <t>TC_112</t>
+  </si>
+  <si>
+    <t>Verify, on clicking signature of person, beneficiary contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_113</t>
+  </si>
+  <si>
+    <t>TC_114</t>
+  </si>
+  <si>
+    <t>Verify, contact details are correctly displayed on each page.</t>
+  </si>
+  <si>
+    <t>TC_115</t>
+  </si>
+  <si>
+    <t>Verify, date and reason text box fields are not same for each field.</t>
+  </si>
+  <si>
+    <t>TC_116</t>
+  </si>
+  <si>
+    <t>Reset the RW06 form</t>
+  </si>
+  <si>
+    <t>TC_117</t>
+  </si>
+  <si>
+    <t>probateFormsRWxx.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>TC_108</t>
-  </si>
-  <si>
-    <t>TC_109</t>
-  </si>
-  <si>
-    <t>Verify, form is repeated based on the number of contacts selected.</t>
-  </si>
-  <si>
-    <t>TC_110</t>
-  </si>
-  <si>
-    <t>Verify, corporate fiduciary selected is reflected in the corporate name field.</t>
-  </si>
-  <si>
-    <t>TC_111</t>
-  </si>
-  <si>
-    <t>Verify, details of the selected contact's is displayed in the block under it.</t>
-  </si>
-  <si>
-    <t>TC_112</t>
-  </si>
-  <si>
-    <t>Verify, on clicking signature of person, beneficiary contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_113</t>
-  </si>
-  <si>
-    <t>TC_114</t>
-  </si>
-  <si>
-    <t>Verify, contact details are correctly displayed on each page.</t>
-  </si>
-  <si>
-    <t>TC_115</t>
-  </si>
-  <si>
-    <t>Verify, date and reason text box fields are not same for each field.</t>
-  </si>
-  <si>
-    <t>TC_116</t>
-  </si>
-  <si>
-    <t>Reset the RW06 form</t>
-  </si>
-  <si>
-    <t>TC_117</t>
-  </si>
-  <si>
-    <t>probateFormsRWxx.feature</t>
-  </si>
-  <si>
     <t>TC_118</t>
   </si>
   <si>
@@ -740,10 +740,10 @@
     <t>TC_122</t>
   </si>
   <si>
+    <t>TC_123</t>
+  </si>
+  <si>
     <t>Reset the RWxx form</t>
-  </si>
-  <si>
-    <t>TC_123</t>
   </si>
   <si>
     <t>probateFormsRW07.feature</t>
@@ -2231,10 +2231,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F175"/>
+  <dimension ref="A1:F176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -4077,7 +4077,7 @@
         <v>58</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -4085,7 +4085,7 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B109" s="8" t="s">
         <v>208</v>
@@ -4094,7 +4094,7 @@
         <v>156</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -4102,7 +4102,7 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B110" s="8" t="s">
         <v>208</v>
@@ -4111,7 +4111,7 @@
         <v>158</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -4119,16 +4119,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B111" s="8" t="s">
         <v>208</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -4136,16 +4136,16 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B112" s="8" t="s">
         <v>208</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -4153,16 +4153,16 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B113" s="8" t="s">
         <v>208</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -4170,16 +4170,16 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B114" s="8" t="s">
         <v>208</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -4187,16 +4187,16 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B115" s="8" t="s">
         <v>208</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -4204,16 +4204,16 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>208</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -4221,16 +4221,16 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B117" s="8" t="s">
         <v>208</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -4238,7 +4238,7 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>208</v>
@@ -4247,7 +4247,7 @@
         <v>172</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -4255,16 +4255,16 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B119" s="8" t="s">
         <v>208</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4272,16 +4272,16 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B120" s="8" t="s">
         <v>226</v>
-      </c>
-      <c r="B120" s="8" t="s">
-        <v>227</v>
       </c>
       <c r="C120" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D120" s="5" t="s">
-        <v>8</v>
+      <c r="D120" s="3" t="s">
+        <v>227</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4292,13 +4292,13 @@
         <v>228</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C121" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="D121" s="5" t="s">
-        <v>8</v>
+      <c r="D121" s="3" t="s">
+        <v>227</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4309,13 +4309,13 @@
         <v>230</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C122" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="D122" s="5" t="s">
-        <v>8</v>
+      <c r="D122" s="3" t="s">
+        <v>227</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4326,13 +4326,13 @@
         <v>232</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C123" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="D123" s="5" t="s">
-        <v>8</v>
+      <c r="D123" s="3" t="s">
+        <v>227</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>8</v>
@@ -4343,13 +4343,13 @@
         <v>234</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C124" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="D124" s="5" t="s">
-        <v>8</v>
+      <c r="D124" s="3" t="s">
+        <v>227</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>8</v>
@@ -4360,13 +4360,13 @@
         <v>236</v>
       </c>
       <c r="B125" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C125" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D125" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="C125" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="D125" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>8</v>
@@ -4374,16 +4374,16 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C126" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="B126" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C126" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D126" s="5" t="s">
-        <v>8</v>
+      <c r="D126" s="3" t="s">
+        <v>227</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>8</v>
@@ -4391,13 +4391,13 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B127" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>241</v>
+        <v>58</v>
       </c>
       <c r="D127" s="5" t="s">
         <v>8</v>
@@ -4408,13 +4408,13 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B128" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>104</v>
+        <v>241</v>
       </c>
       <c r="D128" s="5" t="s">
         <v>8</v>
@@ -4425,13 +4425,13 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B129" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>244</v>
+        <v>104</v>
       </c>
       <c r="D129" s="5" t="s">
         <v>8</v>
@@ -4442,13 +4442,13 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B130" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D130" s="5" t="s">
         <v>8</v>
@@ -4459,13 +4459,13 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B131" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D131" s="5" t="s">
         <v>8</v>
@@ -4476,13 +4476,13 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B132" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>8</v>
@@ -4493,13 +4493,13 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B133" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>8</v>
@@ -4510,13 +4510,13 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B134" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>8</v>
@@ -4527,13 +4527,13 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B135" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D135" s="5" t="s">
         <v>8</v>
@@ -4544,13 +4544,13 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B136" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D136" s="5" t="s">
         <v>8</v>
@@ -4561,13 +4561,13 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B137" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D137" s="5" t="s">
         <v>8</v>
@@ -4578,13 +4578,13 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B138" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D138" s="5" t="s">
         <v>8</v>
@@ -4595,13 +4595,13 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B139" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D139" s="5" t="s">
         <v>8</v>
@@ -4612,13 +4612,13 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B140" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D140" s="5" t="s">
         <v>8</v>
@@ -4629,13 +4629,13 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>268</v>
+        <v>239</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>58</v>
+        <v>266</v>
       </c>
       <c r="D141" s="5" t="s">
         <v>8</v>
@@ -4646,13 +4646,13 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B142" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>241</v>
+        <v>58</v>
       </c>
       <c r="D142" s="5" t="s">
         <v>8</v>
@@ -4663,13 +4663,13 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B143" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>104</v>
+        <v>241</v>
       </c>
       <c r="D143" s="5" t="s">
         <v>8</v>
@@ -4680,13 +4680,13 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B144" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>272</v>
+        <v>104</v>
       </c>
       <c r="D144" s="5" t="s">
         <v>8</v>
@@ -4697,13 +4697,13 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B145" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D145" s="5" t="s">
         <v>8</v>
@@ -4714,13 +4714,13 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B146" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>134</v>
+        <v>274</v>
       </c>
       <c r="D146" s="5" t="s">
         <v>8</v>
@@ -4731,13 +4731,13 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B147" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>277</v>
+        <v>134</v>
       </c>
       <c r="D147" s="5" t="s">
         <v>8</v>
@@ -4748,13 +4748,13 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B148" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D148" s="5" t="s">
         <v>8</v>
@@ -4763,15 +4763,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="149" ht="28" spans="1:5">
+    <row r="149" spans="1:5">
       <c r="A149" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B149" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="C149" s="10" t="s">
-        <v>281</v>
+      <c r="C149" s="8" t="s">
+        <v>279</v>
       </c>
       <c r="D149" s="5" t="s">
         <v>8</v>
@@ -4780,15 +4780,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" ht="28" spans="1:5">
       <c r="A150" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B150" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="C150" s="8" t="s">
-        <v>260</v>
+      <c r="C150" s="10" t="s">
+        <v>281</v>
       </c>
       <c r="D150" s="5" t="s">
         <v>8</v>
@@ -4799,13 +4799,13 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B151" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D151" s="5" t="s">
         <v>8</v>
@@ -4814,15 +4814,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" ht="28" spans="1:5">
+    <row r="152" spans="1:5">
       <c r="A152" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B152" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="C152" s="10" t="s">
-        <v>285</v>
+      <c r="C152" s="8" t="s">
+        <v>262</v>
       </c>
       <c r="D152" s="5" t="s">
         <v>8</v>
@@ -4831,15 +4831,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" ht="28" spans="1:5">
       <c r="A153" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B153" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="C153" s="8" t="s">
-        <v>264</v>
+      <c r="C153" s="10" t="s">
+        <v>285</v>
       </c>
       <c r="D153" s="5" t="s">
         <v>8</v>
@@ -4850,7 +4850,7 @@
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B154" s="8" t="s">
         <v>268</v>
@@ -4867,13 +4867,13 @@
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B155" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C155" s="8" t="s">
-        <v>289</v>
+        <v>264</v>
       </c>
       <c r="D155" s="5" t="s">
         <v>8</v>
@@ -4884,13 +4884,13 @@
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
       <c r="C156" s="8" t="s">
-        <v>58</v>
+        <v>289</v>
       </c>
       <c r="D156" s="5" t="s">
         <v>8</v>
@@ -4901,13 +4901,13 @@
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B157" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C157" s="8" t="s">
-        <v>293</v>
+        <v>58</v>
       </c>
       <c r="D157" s="5" t="s">
         <v>8</v>
@@ -4918,13 +4918,13 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B158" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D158" s="5" t="s">
         <v>8</v>
@@ -4935,13 +4935,13 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B159" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D159" s="5" t="s">
         <v>8</v>
@@ -4952,13 +4952,13 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B160" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D160" s="5" t="s">
         <v>8</v>
@@ -4969,13 +4969,13 @@
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B161" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C161" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D161" s="5" t="s">
         <v>8</v>
@@ -4986,13 +4986,13 @@
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B162" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D162" s="5" t="s">
         <v>8</v>
@@ -5003,13 +5003,13 @@
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B163" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D163" s="5" t="s">
         <v>8</v>
@@ -5020,13 +5020,13 @@
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B164" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C164" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D164" s="5" t="s">
         <v>8</v>
@@ -5037,13 +5037,13 @@
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B165" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C165" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D165" s="5" t="s">
         <v>8</v>
@@ -5054,13 +5054,13 @@
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B166" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D166" s="5" t="s">
         <v>8</v>
@@ -5071,13 +5071,13 @@
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B167" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D167" s="5" t="s">
         <v>8</v>
@@ -5088,13 +5088,13 @@
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B168" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D168" s="5" t="s">
         <v>8</v>
@@ -5105,13 +5105,13 @@
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B169" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D169" s="5" t="s">
         <v>8</v>
@@ -5122,13 +5122,13 @@
     </row>
     <row r="170" spans="1:5">
       <c r="A170" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B170" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D170" s="5" t="s">
         <v>8</v>
@@ -5139,13 +5139,13 @@
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B171" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C171" s="8" t="s">
-        <v>260</v>
+        <v>319</v>
       </c>
       <c r="D171" s="5" t="s">
         <v>8</v>
@@ -5156,13 +5156,13 @@
     </row>
     <row r="172" spans="1:5">
       <c r="A172" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B172" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C172" s="8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D172" s="5" t="s">
         <v>8</v>
@@ -5171,15 +5171,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="173" ht="28" spans="1:5">
+    <row r="173" spans="1:5">
       <c r="A173" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B173" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C173" s="10" t="s">
-        <v>323</v>
+      <c r="C173" s="8" t="s">
+        <v>262</v>
       </c>
       <c r="D173" s="5" t="s">
         <v>8</v>
@@ -5188,15 +5188,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" ht="28" spans="1:5">
       <c r="A174" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B174" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C174" s="8" t="s">
-        <v>264</v>
+      <c r="C174" s="10" t="s">
+        <v>323</v>
       </c>
       <c r="D174" s="5" t="s">
         <v>8</v>
@@ -5207,18 +5207,35 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B175" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C175" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D175" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C176" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="D175" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E175" s="3" t="s">
+      <c r="D176" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E176" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5227,7 +5244,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D93:D107 D108:D119 E2:E8 E93:E95 E96:E107 E108:E109 E110:E119 F2:F3 D9:E92 D120:E175">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D126:E126 D1:D8 D124:D125 E2:E8 E124:E125 F2:F3 D9:E119 D158:E176 D138:E157 D127:E137 D120:E123">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated code of all RW forms extraction of the values and their declaration
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="333">
   <si>
     <t>ID</t>
   </si>
@@ -305,291 +305,291 @@
     <t>TC_042</t>
   </si>
   <si>
+    <t>Verify form can be printed in pdf</t>
+  </si>
+  <si>
+    <t>TC_043</t>
+  </si>
+  <si>
     <t>Reset the RW01 form</t>
   </si>
   <si>
-    <t>TC_043</t>
+    <t>TC_044</t>
   </si>
   <si>
     <t>probateFormsRW02.feature</t>
   </si>
   <si>
-    <t>TC_044</t>
+    <t>TC_045</t>
   </si>
   <si>
     <t>Verify, correct county name is auto fetched.</t>
   </si>
   <si>
-    <t>TC_045</t>
+    <t>TC_046</t>
   </si>
   <si>
     <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
   </si>
   <si>
-    <t>TC_046</t>
+    <t>TC_047</t>
   </si>
   <si>
     <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
   </si>
   <si>
-    <t>TC_047</t>
+    <t>TC_048</t>
   </si>
   <si>
     <t>Verify, county, estate and aka names are auto populated on the form.</t>
   </si>
   <si>
-    <t>TC_048</t>
+    <t>TC_049</t>
   </si>
   <si>
     <t>Verify, the auto populated fields are not editable.</t>
   </si>
   <si>
-    <t>TC_049</t>
+    <t>TC_050</t>
   </si>
   <si>
     <t>Verify, names can be added in aka fields.</t>
   </si>
   <si>
-    <t>TC_050</t>
+    <t>TC_051</t>
   </si>
   <si>
     <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
   </si>
   <si>
-    <t>TC_051</t>
+    <t>TC_052</t>
   </si>
   <si>
     <t>Verify, amount can be entered in the input fields.</t>
   </si>
   <si>
-    <t>TC_052</t>
+    <t>TC_053</t>
   </si>
   <si>
     <t>Verify, total estimated value should display total of 1st and last field only.</t>
   </si>
   <si>
-    <t>TC_053</t>
+    <t>TC_054</t>
   </si>
   <si>
     <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
   </si>
   <si>
-    <t>TC_054</t>
+    <t>TC_055</t>
   </si>
   <si>
     <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
   </si>
   <si>
-    <t>TC_055</t>
+    <t>TC_056</t>
   </si>
   <si>
     <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
   </si>
   <si>
-    <t>TC_056</t>
+    <t>TC_057</t>
   </si>
   <si>
     <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
   </si>
   <si>
-    <t>TC_057</t>
+    <t>TC_058</t>
   </si>
   <si>
     <t>Verify that selecting option A keeps it selected without affecting option B.</t>
   </si>
   <si>
-    <t>TC_058</t>
+    <t>TC_059</t>
   </si>
   <si>
     <t>Verify, decedent died date is auto fetched.</t>
   </si>
   <si>
-    <t>TC_059</t>
+    <t>TC_060</t>
   </si>
   <si>
     <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
   </si>
   <si>
-    <t>TC_060</t>
+    <t>TC_061</t>
   </si>
   <si>
     <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
   </si>
   <si>
-    <t>TC_061</t>
+    <t>TC_062</t>
   </si>
   <si>
     <t>Verify that selecting option B keeps it selected without affecting option A.</t>
   </si>
   <si>
-    <t>TC_062</t>
+    <t>TC_063</t>
   </si>
   <si>
     <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
   </si>
   <si>
-    <t>TC_063</t>
+    <t>TC_064</t>
   </si>
   <si>
     <t>Verify, multiple beneficiaries can be selected.</t>
   </si>
   <si>
-    <t>TC_064</t>
+    <t>TC_065</t>
   </si>
   <si>
     <t>Verify, bene contacts in the table.</t>
   </si>
   <si>
-    <t>TC_065</t>
+    <t>TC_066</t>
   </si>
   <si>
     <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
   </si>
   <si>
-    <t>TC_066</t>
+    <t>TC_067</t>
   </si>
   <si>
     <t>Verify, on checking "Display all heirs on attachment".</t>
   </si>
   <si>
-    <t>TC_067</t>
+    <t>TC_068</t>
   </si>
   <si>
     <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
   </si>
   <si>
-    <t>TC_068</t>
+    <t>TC_069</t>
   </si>
   <si>
     <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
   </si>
   <si>
-    <t>TC_069</t>
+    <t>TC_070</t>
   </si>
   <si>
     <t>Verify fees section.</t>
   </si>
   <si>
-    <t>TC_070</t>
+    <t>TC_071</t>
   </si>
   <si>
     <t>Verify, attorney can be selected.</t>
   </si>
   <si>
-    <t>TC_071</t>
+    <t>TC_072</t>
   </si>
   <si>
     <t>Verify, information in decree of the register.</t>
   </si>
   <si>
-    <t>TC_072</t>
+    <t>TC_073</t>
+  </si>
+  <si>
+    <t>TC_074</t>
   </si>
   <si>
     <t>Reset the RW02 form</t>
   </si>
   <si>
-    <t>TC_073</t>
+    <t>TC_075</t>
   </si>
   <si>
     <t>probateFormsRW03.feature</t>
   </si>
   <si>
-    <t>TC_074</t>
+    <t>TC_076</t>
   </si>
   <si>
     <t>Verify county, estate and aka names are auto-populated on the form</t>
   </si>
   <si>
-    <t>TC_075</t>
+    <t>TC_077</t>
   </si>
   <si>
     <t>Verify, the auto-populated fields are not editable.</t>
   </si>
   <si>
-    <t>TC_076</t>
+    <t>TC_078</t>
   </si>
   <si>
     <t>Verify, witness's name is not auto populated and the fields are empty.</t>
   </si>
   <si>
-    <t>TC_077</t>
+    <t>TC_079</t>
   </si>
   <si>
     <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
   </si>
   <si>
-    <t>TC_078</t>
+    <t>TC_080</t>
   </si>
   <si>
     <t>Verify, names can be entered in witness fields.</t>
   </si>
   <si>
-    <t>TC_079</t>
+    <t>TC_081</t>
   </si>
   <si>
     <t>Verify, names updated from signature are reflected in witness names fields.</t>
   </si>
   <si>
-    <t>TC_080</t>
+    <t>TC_082</t>
   </si>
   <si>
     <t>Verify, text can be entered in address, city, zip fields.</t>
   </si>
   <si>
-    <t>TC_081</t>
+    <t>TC_083</t>
   </si>
   <si>
     <t>Verify, form is auto saved.</t>
   </si>
   <si>
-    <t>TC_082</t>
-  </si>
-  <si>
-    <t>Verify form can be printed in pdf</t>
-  </si>
-  <si>
-    <t>TC_083</t>
+    <t>TC_084</t>
+  </si>
+  <si>
+    <t>TC_085</t>
   </si>
   <si>
     <t>Reset the RW03 form</t>
   </si>
   <si>
-    <t>TC_084</t>
+    <t>TC_086</t>
   </si>
   <si>
     <t>probateFormsRW04.feature</t>
   </si>
   <si>
-    <t>TC_085</t>
+    <t>TC_087</t>
   </si>
   <si>
     <t>Verify, correct title is displayed on the form's header.</t>
   </si>
   <si>
-    <t>TC_086</t>
+    <t>TC_088</t>
   </si>
   <si>
     <t>Verify, county, and aka names are auto populated on the form.</t>
   </si>
   <si>
-    <t>TC_087</t>
+    <t>TC_089</t>
   </si>
   <si>
     <t>Verify, correct estate's name is displayed on the form.</t>
   </si>
   <si>
-    <t>TC_088</t>
+    <t>TC_090</t>
   </si>
   <si>
     <t>Verify, name of the decedent should be auto populated from the form.</t>
   </si>
   <si>
-    <t>TC_089</t>
-  </si>
-  <si>
-    <t>TC_090</t>
-  </si>
-  <si>
     <t>TC_091</t>
   </si>
   <si>
@@ -602,24 +602,24 @@
     <t>TC_094</t>
   </si>
   <si>
+    <t>TC_095</t>
+  </si>
+  <si>
+    <t>TC_096</t>
+  </si>
+  <si>
+    <t>TC_097</t>
+  </si>
+  <si>
     <t>Reset the RW04 form</t>
   </si>
   <si>
-    <t>TC_095</t>
+    <t>TC_098</t>
   </si>
   <si>
     <t>probateFormsRW05.feature</t>
   </si>
   <si>
-    <t>TC_096</t>
-  </si>
-  <si>
-    <t>TC_097</t>
-  </si>
-  <si>
-    <t>TC_098</t>
-  </si>
-  <si>
     <t>TC_099</t>
   </si>
   <si>
@@ -635,376 +635,394 @@
     <t>TC_103</t>
   </si>
   <si>
+    <t>TC_104</t>
+  </si>
+  <si>
+    <t>TC_105</t>
+  </si>
+  <si>
+    <t>TC_106</t>
+  </si>
+  <si>
     <t>Verify, on checking notary checkbox, notary section displays.</t>
   </si>
   <si>
-    <t>TC_104</t>
-  </si>
-  <si>
-    <t>TC_105</t>
-  </si>
-  <si>
-    <t>TC_106</t>
+    <t>TC_107</t>
+  </si>
+  <si>
+    <t>TC_108</t>
+  </si>
+  <si>
+    <t>TC_109</t>
   </si>
   <si>
     <t>Reset the RW05 form</t>
   </si>
   <si>
-    <t>TC_107</t>
+    <t>TC_110</t>
   </si>
   <si>
     <t>probateFormsRW06.feature</t>
   </si>
   <si>
-    <t>TC_108</t>
-  </si>
-  <si>
-    <t>TC_109</t>
+    <t>TC_111</t>
+  </si>
+  <si>
+    <t>TC_112</t>
+  </si>
+  <si>
+    <t>TC_113</t>
   </si>
   <si>
     <t>Verify, form is repeated based on the number of contacts selected.</t>
   </si>
   <si>
-    <t>TC_110</t>
+    <t>TC_114</t>
   </si>
   <si>
     <t>Verify, corporate fiduciary selected is reflected in the corporate name field.</t>
   </si>
   <si>
-    <t>TC_111</t>
+    <t>TC_115</t>
   </si>
   <si>
     <t>Verify, details of the selected contact's is displayed in the block under it.</t>
   </si>
   <si>
-    <t>TC_112</t>
+    <t>TC_116</t>
   </si>
   <si>
     <t>Verify, on clicking signature of person, beneficiary contact can be selected.</t>
   </si>
   <si>
-    <t>TC_113</t>
-  </si>
-  <si>
-    <t>TC_114</t>
+    <t>TC_117</t>
+  </si>
+  <si>
+    <t>TC_118</t>
   </si>
   <si>
     <t>Verify, contact details are correctly displayed on each page.</t>
   </si>
   <si>
-    <t>TC_115</t>
+    <t>TC_119</t>
   </si>
   <si>
     <t>Verify, date and reason text box fields are not same for each field.</t>
   </si>
   <si>
-    <t>TC_116</t>
+    <t>TC_120</t>
+  </si>
+  <si>
+    <t>TC_121</t>
   </si>
   <si>
     <t>Reset the RW06 form</t>
   </si>
   <si>
-    <t>TC_117</t>
+    <t>TC_122</t>
   </si>
   <si>
     <t>probateFormsRWxx.feature</t>
   </si>
   <si>
+    <t>TC_123</t>
+  </si>
+  <si>
+    <t>Verify that the county, estate name, and "Also Known As" (AKA) values are auto-populated from the selected estate.</t>
+  </si>
+  <si>
+    <t>TC_124</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered in all the text areas.</t>
+  </si>
+  <si>
+    <t>TC_125</t>
+  </si>
+  <si>
+    <t>Verify, the name entered in 1st text area is reflected in the signature.</t>
+  </si>
+  <si>
+    <t>TC_126</t>
+  </si>
+  <si>
+    <t>Verify that changes in the witness name field are reflected under the signature line and vice-versa.</t>
+  </si>
+  <si>
+    <t>TC_127</t>
+  </si>
+  <si>
+    <t>TC_128</t>
+  </si>
+  <si>
+    <t>Reset the RWxx form</t>
+  </si>
+  <si>
+    <t>TC_129</t>
+  </si>
+  <si>
+    <t>probateFormsRW07.feature</t>
+  </si>
+  <si>
+    <t>TC_130</t>
+  </si>
+  <si>
+    <t>Verify, county, estate and file number aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_131</t>
+  </si>
+  <si>
+    <t>TC_132</t>
+  </si>
+  <si>
+    <t>Verify, on checking use 4 digit checkbox, changes in file number</t>
+  </si>
+  <si>
+    <t>TC_133</t>
+  </si>
+  <si>
+    <t>Verify, on clicking bene address field, multiple beneficiaries can be selected.</t>
+  </si>
+  <si>
+    <t>TC_134</t>
+  </si>
+  <si>
+    <t>Verify, beneficiary name and address should be displayed in the form.</t>
+  </si>
+  <si>
+    <t>TC_135</t>
+  </si>
+  <si>
+    <t>Verify, decedent died and county is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_136</t>
+  </si>
+  <si>
+    <t>Verify, on clicking name fiduciary contact list is displayed and multiple users can be selected.</t>
+  </si>
+  <si>
+    <t>TC_137</t>
+  </si>
+  <si>
+    <t>Verify, these contacts are common for all the forms.</t>
+  </si>
+  <si>
+    <t>TC_138</t>
+  </si>
+  <si>
+    <t>Verify, date can be entered.</t>
+  </si>
+  <si>
+    <t>TC_139</t>
+  </si>
+  <si>
+    <t>Verify, registrars address is auto fetched and is editable.</t>
+  </si>
+  <si>
+    <t>TC_140</t>
+  </si>
+  <si>
+    <t>Verify, corporate fiduciary type of contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_141</t>
+  </si>
+  <si>
+    <t>Verify, based on capacity contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_142</t>
+  </si>
+  <si>
+    <t>Verify, selection is cleared on clicking clear selection button.</t>
+  </si>
+  <si>
+    <t>TC_143</t>
+  </si>
+  <si>
+    <t>Reset the RW07 form</t>
+  </si>
+  <si>
+    <t>TC_144</t>
+  </si>
+  <si>
+    <t>probateFormsRW08.feature</t>
+  </si>
+  <si>
+    <t>TC_145</t>
+  </si>
+  <si>
+    <t>TC_146</t>
+  </si>
+  <si>
+    <t>TC_147</t>
+  </si>
+  <si>
+    <t>Verify, Will number and other dates can be entered in correct format.</t>
+  </si>
+  <si>
+    <t>TC_148</t>
+  </si>
+  <si>
+    <t>Verify, checkboxes for file no field.</t>
+  </si>
+  <si>
+    <t>TC_149</t>
+  </si>
+  <si>
+    <t>TC_150</t>
+  </si>
+  <si>
+    <t>Verify, the beneficiaries selected beyond 6 are displayed on the attachment.</t>
+  </si>
+  <si>
+    <t>TC_151</t>
+  </si>
+  <si>
+    <t>Verify, count is correctly displayed.</t>
+  </si>
+  <si>
+    <t>TC_152</t>
+  </si>
+  <si>
+    <t>Verify, on clicking "Display ALL beneficiary on attachment" checkbox all the contacts are transferred on attachment.</t>
+  </si>
+  <si>
+    <t>TC_153</t>
+  </si>
+  <si>
+    <t>TC_154</t>
+  </si>
+  <si>
+    <t>TC_155</t>
+  </si>
+  <si>
+    <t>Verify, these 2 sections are common for RW07, RW08 and anything updated is reflected in all the forms.</t>
+  </si>
+  <si>
+    <t>TC_156</t>
+  </si>
+  <si>
+    <t>TC_157</t>
+  </si>
+  <si>
+    <t>TC_158</t>
+  </si>
+  <si>
+    <t>Reset the RW08 form</t>
+  </si>
+  <si>
+    <t>TC_159</t>
+  </si>
+  <si>
+    <t>probateFormsRW10.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>TC_118</t>
-  </si>
-  <si>
-    <t>Verify that the county, estate name, and "Also Known As" (AKA) values are auto-populated from the selected estate.</t>
-  </si>
-  <si>
-    <t>TC_119</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered in all the text areas.</t>
-  </si>
-  <si>
-    <t>TC_120</t>
-  </si>
-  <si>
-    <t>Verify, the name entered in 1st text area is reflected in the signature.</t>
-  </si>
-  <si>
-    <t>TC_121</t>
-  </si>
-  <si>
-    <t>Verify that changes in the witness name field are reflected under the signature line and vice-versa.</t>
-  </si>
-  <si>
-    <t>TC_122</t>
-  </si>
-  <si>
-    <t>TC_123</t>
-  </si>
-  <si>
-    <t>Reset the RWxx form</t>
-  </si>
-  <si>
-    <t>probateFormsRW07.feature</t>
-  </si>
-  <si>
-    <t>TC_124</t>
-  </si>
-  <si>
-    <t>Verify, county, estate and file number aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_125</t>
-  </si>
-  <si>
-    <t>TC_126</t>
-  </si>
-  <si>
-    <t>Verify, on checking use 4 digit checkbox, changes in file number</t>
-  </si>
-  <si>
-    <t>TC_127</t>
-  </si>
-  <si>
-    <t>Verify, on clicking bene address field, multiple beneficiaries can be selected.</t>
-  </si>
-  <si>
-    <t>TC_128</t>
-  </si>
-  <si>
-    <t>Verify, beneficiary name and address should be displayed in the form.</t>
-  </si>
-  <si>
-    <t>TC_129</t>
-  </si>
-  <si>
-    <t>Verify, decedent died and county is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_130</t>
-  </si>
-  <si>
-    <t>Verify, on clicking name fiduciary contact list is displayed and multiple users can be selected.</t>
-  </si>
-  <si>
-    <t>TC_131</t>
-  </si>
-  <si>
-    <t>Verify, these contacts are common for all the forms.</t>
-  </si>
-  <si>
-    <t>TC_132</t>
-  </si>
-  <si>
-    <t>Verify, date can be entered.</t>
-  </si>
-  <si>
-    <t>TC_133</t>
-  </si>
-  <si>
-    <t>Verify, registrars address is auto fetched and is editable.</t>
-  </si>
-  <si>
-    <t>TC_134</t>
-  </si>
-  <si>
-    <t>Verify, corporate fiduciary type of contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_135</t>
-  </si>
-  <si>
-    <t>Verify, based on capacity contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_136</t>
-  </si>
-  <si>
-    <t>Verify, selection is cleared on clicking clear selection button.</t>
-  </si>
-  <si>
-    <t>TC_137</t>
-  </si>
-  <si>
-    <t>Reset the RW07 form</t>
-  </si>
-  <si>
-    <t>TC_138</t>
-  </si>
-  <si>
-    <t>probateFormsRW08.feature</t>
-  </si>
-  <si>
-    <t>TC_139</t>
-  </si>
-  <si>
-    <t>TC_140</t>
-  </si>
-  <si>
-    <t>TC_141</t>
-  </si>
-  <si>
-    <t>Verify, Will number and other dates can be entered in correct format.</t>
-  </si>
-  <si>
-    <t>TC_142</t>
-  </si>
-  <si>
-    <t>Verify, checkboxes for file no field.</t>
-  </si>
-  <si>
-    <t>TC_143</t>
-  </si>
-  <si>
-    <t>TC_144</t>
-  </si>
-  <si>
-    <t>Verify, the beneficiaries selected beyond 6 are displayed on the attachment.</t>
-  </si>
-  <si>
-    <t>TC_145</t>
-  </si>
-  <si>
-    <t>Verify, count is correctly displayed.</t>
-  </si>
-  <si>
-    <t>TC_146</t>
-  </si>
-  <si>
-    <t>Verify, on clicking "Display ALL beneficiary on attachment" checkbox all the contacts are transferred on attachment.</t>
-  </si>
-  <si>
-    <t>TC_147</t>
-  </si>
-  <si>
-    <t>TC_148</t>
-  </si>
-  <si>
-    <t>TC_149</t>
-  </si>
-  <si>
-    <t>Verify, these 2 sections are common for RW07, RW08 and anything updated is reflected in all the forms.</t>
-  </si>
-  <si>
-    <t>TC_150</t>
-  </si>
-  <si>
-    <t>TC_151</t>
-  </si>
-  <si>
-    <t>TC_152</t>
-  </si>
-  <si>
-    <t>Reset the RW08 form</t>
-  </si>
-  <si>
-    <t>TC_153</t>
-  </si>
-  <si>
-    <t>probateFormsRW10.feature</t>
-  </si>
-  <si>
-    <t>TC_154</t>
+    <t>TC_160</t>
   </si>
   <si>
     <t>Verify, title of the form and if county is fetched from the decedent info.</t>
   </si>
   <si>
-    <t>TC_155</t>
+    <t>TC_161</t>
   </si>
   <si>
     <t>Verify, "Name of Decedent", "Date of Death", "File Number" is fetched from the decedent info.</t>
   </si>
   <si>
-    <t>TC_156</t>
+    <t>TC_162</t>
   </si>
   <si>
     <t>Verify, if above fetched details are editable.</t>
   </si>
   <si>
-    <t>TC_157</t>
+    <t>TC_163</t>
   </si>
   <si>
     <t>Verify, questionnaire is correctly displayed with yes or no options.</t>
   </si>
   <si>
-    <t>TC_158</t>
+    <t>TC_164</t>
   </si>
   <si>
     <t>Verify, either yes or no is clickable.</t>
   </si>
   <si>
-    <t>TC_159</t>
+    <t>TC_165</t>
   </si>
   <si>
     <t>Verify, if option "Yes" is selected in point 1, point 2 is enabled or not.</t>
   </si>
   <si>
-    <t>TC_160</t>
+    <t>TC_166</t>
   </si>
   <si>
     <t>Verify, if "No" is checked in point 1, then text box in point 2 is enabled.</t>
   </si>
   <si>
-    <t>TC_161</t>
+    <t>TC_167</t>
   </si>
   <si>
     <t>Verify, reason for to be mentioned, if no is ticked.</t>
   </si>
   <si>
-    <t>TC_162</t>
+    <t>TC_168</t>
   </si>
   <si>
     <t>Verify, if "Yes" is ticked, point 2 is disabled and text entered disappear.</t>
   </si>
   <si>
-    <t>TC_163</t>
+    <t>TC_169</t>
   </si>
   <si>
     <t>Verify, if "Yes" option is selected in point 1, then point 3 is enabled</t>
   </si>
   <si>
-    <t>TC_164</t>
+    <t>TC_170</t>
   </si>
   <si>
     <t>Verify, if "No" is checked in point 1, then point 3 is disabled.</t>
   </si>
   <si>
-    <t>TC_165</t>
+    <t>TC_171</t>
   </si>
   <si>
     <t>Verify, if "NO" is clicked text box in point 2 is enabled and empty.</t>
   </si>
   <si>
-    <t>TC_166</t>
+    <t>TC_172</t>
   </si>
   <si>
     <t>Verify, if No is checked, point 3 is disabled and text entered disappear.</t>
   </si>
   <si>
-    <t>TC_167</t>
+    <t>TC_173</t>
   </si>
   <si>
     <t>Verify, date field follows correct format.</t>
   </si>
   <si>
-    <t>TC_168</t>
-  </si>
-  <si>
-    <t>TC_169</t>
-  </si>
-  <si>
-    <t>TC_170</t>
+    <t>TC_174</t>
+  </si>
+  <si>
+    <t>TC_175</t>
+  </si>
+  <si>
+    <t>TC_176</t>
   </si>
   <si>
     <t>Verify, these 2 sections are common for RW07, RW08, RW10 and anything updated is reflected in all the forms.</t>
   </si>
   <si>
-    <t>TC_171</t>
-  </si>
-  <si>
-    <t>TC_172</t>
+    <t>TC_177</t>
+  </si>
+  <si>
+    <t>TC_178</t>
   </si>
   <si>
     <t>Reset the RW10 form</t>
@@ -1020,7 +1038,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1043,11 +1061,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF263238"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Arial"/>
       <charset val="1"/>
     </font>
@@ -1208,7 +1221,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1219,12 +1232,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF2A6099"/>
         <bgColor rgb="FF666699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -1551,18 +1558,21 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1571,37 +1581,37 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1616,77 +1626,74 @@
     <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1700,9 +1707,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -2231,10 +2235,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F176"/>
+  <dimension ref="A1:F179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="C125" sqref="C125"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2333,7 +2337,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -2418,7 +2422,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2676,10 +2680,10 @@
       <c r="A26" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D26" s="3" t="s">
@@ -2693,10 +2697,10 @@
       <c r="A27" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -2710,10 +2714,10 @@
       <c r="A28" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>62</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -2727,10 +2731,10 @@
       <c r="A29" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>64</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -2744,10 +2748,10 @@
       <c r="A30" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="8" t="s">
         <v>66</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -2761,10 +2765,10 @@
       <c r="A31" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="8" t="s">
         <v>68</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -2778,10 +2782,10 @@
       <c r="A32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="8" t="s">
         <v>70</v>
       </c>
       <c r="D32" s="3" t="s">
@@ -2795,10 +2799,10 @@
       <c r="A33" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="8" t="s">
         <v>72</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -2812,10 +2816,10 @@
       <c r="A34" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="8" t="s">
         <v>74</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -2829,10 +2833,10 @@
       <c r="A35" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -2846,10 +2850,10 @@
       <c r="A36" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="8" t="s">
         <v>78</v>
       </c>
       <c r="D36" s="3" t="s">
@@ -2863,10 +2867,10 @@
       <c r="A37" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="8" t="s">
         <v>80</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -2880,10 +2884,10 @@
       <c r="A38" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="8" t="s">
         <v>82</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -2897,10 +2901,10 @@
       <c r="A39" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="8" t="s">
         <v>84</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -2914,10 +2918,10 @@
       <c r="A40" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="8" t="s">
         <v>86</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -2931,10 +2935,10 @@
       <c r="A41" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="8" t="s">
         <v>88</v>
       </c>
       <c r="D41" s="3" t="s">
@@ -2948,10 +2952,10 @@
       <c r="A42" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="8" t="s">
         <v>90</v>
       </c>
       <c r="D42" s="3" t="s">
@@ -2965,10 +2969,10 @@
       <c r="A43" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="8" t="s">
         <v>92</v>
       </c>
       <c r="D43" s="3" t="s">
@@ -2982,11 +2986,11 @@
       <c r="A44" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>8</v>
@@ -2999,11 +3003,11 @@
       <c r="A45" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C45" s="9" t="s">
+      <c r="B45" s="7" t="s">
         <v>96</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>8</v>
@@ -3016,10 +3020,10 @@
       <c r="A46" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46" s="9" t="s">
+      <c r="B46" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>98</v>
       </c>
       <c r="D46" s="3" t="s">
@@ -3033,10 +3037,10 @@
       <c r="A47" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="9" t="s">
+      <c r="B47" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>100</v>
       </c>
       <c r="D47" s="3" t="s">
@@ -3050,10 +3054,10 @@
       <c r="A48" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C48" s="9" t="s">
+      <c r="B48" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>102</v>
       </c>
       <c r="D48" s="3" t="s">
@@ -3067,10 +3071,10 @@
       <c r="A49" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" s="9" t="s">
+      <c r="B49" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>104</v>
       </c>
       <c r="D49" s="3" t="s">
@@ -3084,10 +3088,10 @@
       <c r="A50" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B50" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C50" s="9" t="s">
+      <c r="B50" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>106</v>
       </c>
       <c r="D50" s="3" t="s">
@@ -3097,14 +3101,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" ht="28" spans="1:5">
+    <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B51" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C51" s="9" t="s">
+      <c r="B51" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>108</v>
       </c>
       <c r="D51" s="3" t="s">
@@ -3114,14 +3118,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" ht="28" spans="1:5">
       <c r="A52" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B52" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C52" s="9" t="s">
+      <c r="B52" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D52" s="3" t="s">
@@ -3135,10 +3139,10 @@
       <c r="A53" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C53" s="9" t="s">
+      <c r="B53" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>112</v>
       </c>
       <c r="D53" s="3" t="s">
@@ -3148,14 +3152,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" ht="28" spans="1:5">
+    <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" s="9" t="s">
+      <c r="B54" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>114</v>
       </c>
       <c r="D54" s="3" t="s">
@@ -3165,14 +3169,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" ht="28" spans="1:5">
       <c r="A55" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C55" s="9" t="s">
+      <c r="B55" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>116</v>
       </c>
       <c r="D55" s="3" t="s">
@@ -3186,10 +3190,10 @@
       <c r="A56" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B56" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C56" s="9" t="s">
+      <c r="B56" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="8" t="s">
         <v>118</v>
       </c>
       <c r="D56" s="3" t="s">
@@ -3199,14 +3203,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" ht="28" spans="1:5">
+    <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B57" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C57" s="9" t="s">
+      <c r="B57" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" s="8" t="s">
         <v>120</v>
       </c>
       <c r="D57" s="3" t="s">
@@ -3216,14 +3220,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" ht="28" spans="1:5">
       <c r="A58" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B58" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C58" s="9" t="s">
+      <c r="B58" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" s="8" t="s">
         <v>122</v>
       </c>
       <c r="D58" s="3" t="s">
@@ -3237,10 +3241,10 @@
       <c r="A59" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B59" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C59" s="9" t="s">
+      <c r="B59" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" s="8" t="s">
         <v>124</v>
       </c>
       <c r="D59" s="3" t="s">
@@ -3254,10 +3258,10 @@
       <c r="A60" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B60" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C60" s="9" t="s">
+      <c r="B60" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>126</v>
       </c>
       <c r="D60" s="3" t="s">
@@ -3267,14 +3271,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" ht="28" spans="1:5">
+    <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B61" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C61" s="9" t="s">
+      <c r="B61" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>128</v>
       </c>
       <c r="D61" s="3" t="s">
@@ -3284,14 +3288,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" ht="28" spans="1:5">
       <c r="A62" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B62" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C62" s="9" t="s">
+      <c r="B62" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>130</v>
       </c>
       <c r="D62" s="3" t="s">
@@ -3305,10 +3309,10 @@
       <c r="A63" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B63" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C63" s="9" t="s">
+      <c r="B63" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>132</v>
       </c>
       <c r="D63" s="3" t="s">
@@ -3322,10 +3326,10 @@
       <c r="A64" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B64" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C64" s="9" t="s">
+      <c r="B64" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C64" s="8" t="s">
         <v>134</v>
       </c>
       <c r="D64" s="3" t="s">
@@ -3339,10 +3343,10 @@
       <c r="A65" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B65" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C65" s="9" t="s">
+      <c r="B65" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>136</v>
       </c>
       <c r="D65" s="3" t="s">
@@ -3356,10 +3360,10 @@
       <c r="A66" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B66" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C66" s="9" t="s">
+      <c r="B66" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C66" s="8" t="s">
         <v>138</v>
       </c>
       <c r="D66" s="3" t="s">
@@ -3373,10 +3377,10 @@
       <c r="A67" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B67" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C67" s="9" t="s">
+      <c r="B67" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C67" s="8" t="s">
         <v>140</v>
       </c>
       <c r="D67" s="3" t="s">
@@ -3390,10 +3394,10 @@
       <c r="A68" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B68" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C68" s="9" t="s">
+      <c r="B68" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C68" s="8" t="s">
         <v>142</v>
       </c>
       <c r="D68" s="3" t="s">
@@ -3407,10 +3411,10 @@
       <c r="A69" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B69" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C69" s="9" t="s">
+      <c r="B69" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C69" s="8" t="s">
         <v>144</v>
       </c>
       <c r="D69" s="3" t="s">
@@ -3424,10 +3428,10 @@
       <c r="A70" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B70" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C70" s="9" t="s">
+      <c r="B70" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C70" s="8" t="s">
         <v>146</v>
       </c>
       <c r="D70" s="3" t="s">
@@ -3441,10 +3445,10 @@
       <c r="A71" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B71" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C71" s="9" t="s">
+      <c r="B71" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C71" s="8" t="s">
         <v>148</v>
       </c>
       <c r="D71" s="3" t="s">
@@ -3458,10 +3462,10 @@
       <c r="A72" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B72" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C72" s="9" t="s">
+      <c r="B72" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C72" s="8" t="s">
         <v>150</v>
       </c>
       <c r="D72" s="3" t="s">
@@ -3475,10 +3479,10 @@
       <c r="A73" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B73" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C73" s="9" t="s">
+      <c r="B73" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C73" s="8" t="s">
         <v>152</v>
       </c>
       <c r="D73" s="3" t="s">
@@ -3492,11 +3496,11 @@
       <c r="A74" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B74" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>58</v>
+      <c r="B74" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>8</v>
@@ -3507,13 +3511,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C75" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>156</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>8</v>
@@ -3524,13 +3528,13 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B76" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B76" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>158</v>
+      <c r="C76" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>8</v>
@@ -3541,13 +3545,13 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C77" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>160</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>8</v>
@@ -3558,13 +3562,13 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C78" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>162</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>8</v>
@@ -3575,13 +3579,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C79" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>164</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>8</v>
@@ -3592,13 +3596,13 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>8</v>
@@ -3609,13 +3613,13 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C81" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>168</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>8</v>
@@ -3626,13 +3630,13 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C82" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>8</v>
@@ -3643,13 +3647,13 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C83" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>172</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>8</v>
@@ -3660,13 +3664,13 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>174</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>8</v>
@@ -3677,13 +3681,13 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>157</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>8</v>
@@ -3694,13 +3698,13 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B86" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C86" s="8" t="s">
         <v>176</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>178</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>8</v>
@@ -3711,13 +3715,13 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B87" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>8</v>
@@ -3728,13 +3732,13 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B88" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>182</v>
+        <v>179</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>180</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>8</v>
@@ -3745,13 +3749,13 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>184</v>
+        <v>181</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>8</v>
@@ -3762,13 +3766,13 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>162</v>
+        <v>183</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>184</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>8</v>
@@ -3779,13 +3783,13 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C91" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="B91" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>164</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>8</v>
@@ -3798,11 +3802,11 @@
       <c r="A92" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B92" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>166</v>
+      <c r="B92" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>165</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>8</v>
@@ -3815,11 +3819,11 @@
       <c r="A93" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B93" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>168</v>
+      <c r="B93" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>8</v>
@@ -3832,11 +3836,11 @@
       <c r="A94" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B94" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>170</v>
+      <c r="B94" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>169</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>8</v>
@@ -3849,11 +3853,11 @@
       <c r="A95" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B95" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>191</v>
+      <c r="B95" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>171</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>8</v>
@@ -3864,13 +3868,13 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B96" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C96" s="8" t="s">
-        <v>58</v>
+        <v>191</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>8</v>
@@ -3881,13 +3885,13 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>102</v>
+        <v>192</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>8</v>
@@ -3898,13 +3902,13 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B98" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="C98" s="8" t="s">
-        <v>158</v>
+      <c r="B98" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>194</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>8</v>
@@ -3915,13 +3919,13 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B99" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B99" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C99" s="8" t="s">
-        <v>160</v>
+      <c r="C99" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>8</v>
@@ -3934,11 +3938,11 @@
       <c r="A100" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B100" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C100" s="8" t="s">
-        <v>162</v>
+      <c r="B100" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>8</v>
@@ -3951,11 +3955,11 @@
       <c r="A101" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="B101" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C101" s="8" t="s">
-        <v>164</v>
+      <c r="B101" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>8</v>
@@ -3968,11 +3972,11 @@
       <c r="A102" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="B102" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C102" s="8" t="s">
-        <v>166</v>
+      <c r="B102" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>163</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>8</v>
@@ -3985,11 +3989,11 @@
       <c r="A103" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B103" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C103" s="8" t="s">
-        <v>168</v>
+      <c r="B103" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>165</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>8</v>
@@ -4002,11 +4006,11 @@
       <c r="A104" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B104" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>202</v>
+      <c r="B104" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>8</v>
@@ -4017,13 +4021,13 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B105" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C105" s="8" t="s">
-        <v>170</v>
+        <v>202</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>169</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>8</v>
@@ -4034,13 +4038,13 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C106" s="9" t="s">
-        <v>172</v>
+        <v>203</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>171</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>8</v>
@@ -4051,13 +4055,13 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C107" s="7" t="s">
         <v>205</v>
-      </c>
-      <c r="B107" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C107" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>8</v>
@@ -4068,13 +4072,13 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="B108" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C108" s="8" t="s">
-        <v>58</v>
+        <v>206</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>8</v>
@@ -4085,13 +4089,13 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B109" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>196</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>8</v>
@@ -4102,13 +4106,13 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C110" s="7" t="s">
         <v>209</v>
-      </c>
-      <c r="B110" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C110" s="8" t="s">
-        <v>158</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>8</v>
@@ -4121,11 +4125,11 @@
       <c r="A111" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B111" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C111" s="8" t="s">
+      <c r="B111" s="7" t="s">
         <v>211</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>8</v>
@@ -4138,11 +4142,11 @@
       <c r="A112" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B112" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C112" s="8" t="s">
-        <v>213</v>
+      <c r="B112" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>8</v>
@@ -4153,13 +4157,13 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B113" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C113" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>8</v>
@@ -4170,13 +4174,13 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="B114" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C114" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>215</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>8</v>
@@ -4187,13 +4191,13 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="B115" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C115" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B115" s="7" t="s">
         <v>211</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>217</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>8</v>
@@ -4204,13 +4208,13 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C116" s="7" t="s">
         <v>219</v>
-      </c>
-      <c r="B116" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C116" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>8</v>
@@ -4221,13 +4225,13 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C117" s="7" t="s">
         <v>221</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C117" s="8" t="s">
-        <v>222</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>8</v>
@@ -4238,13 +4242,13 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B118" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C118" s="9" t="s">
-        <v>172</v>
+        <v>222</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>215</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>8</v>
@@ -4257,10 +4261,10 @@
       <c r="A119" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="B119" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C119" s="8" t="s">
+      <c r="B119" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C119" s="7" t="s">
         <v>224</v>
       </c>
       <c r="D119" s="3" t="s">
@@ -4274,31 +4278,31 @@
       <c r="A120" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="B120" s="8" t="s">
+      <c r="B120" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C120" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="C120" s="8" t="s">
-        <v>58</v>
-      </c>
       <c r="D120" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="E120" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="121" ht="28" spans="1:5">
-      <c r="A121" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B121" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C121" s="10" t="s">
-        <v>229</v>
+      <c r="B121" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>227</v>
+        <v>8</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4306,16 +4310,16 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="B122" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C122" s="8" t="s">
-        <v>231</v>
+        <v>228</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>229</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>227</v>
+        <v>8</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4323,33 +4327,33 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" ht="28" spans="1:5">
+      <c r="A124" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B123" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C123" s="8" t="s">
+      <c r="B124" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C124" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="D123" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="E123" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5">
-      <c r="A124" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="B124" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C124" s="8" t="s">
-        <v>235</v>
-      </c>
       <c r="D124" s="3" t="s">
-        <v>227</v>
+        <v>8</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>8</v>
@@ -4357,16 +4361,16 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B125" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C125" s="9" t="s">
-        <v>172</v>
+        <v>234</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>235</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>227</v>
+        <v>8</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>8</v>
@@ -4374,16 +4378,16 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C126" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="B126" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C126" s="8" t="s">
-        <v>238</v>
-      </c>
       <c r="D126" s="3" t="s">
-        <v>227</v>
+        <v>8</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>8</v>
@@ -4391,15 +4395,15 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="B127" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C127" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="C127" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D127" s="5" t="s">
+      <c r="D127" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E127" s="3" t="s">
@@ -4410,13 +4414,13 @@
       <c r="A128" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="B128" s="8" t="s">
-        <v>239</v>
+      <c r="B128" s="7" t="s">
+        <v>231</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="D128" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D128" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E128" s="3" t="s">
@@ -4425,15 +4429,15 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C129" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="B129" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C129" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D129" s="5" t="s">
+      <c r="D129" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E129" s="3" t="s">
@@ -4444,13 +4448,13 @@
       <c r="A130" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B130" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C130" s="8" t="s">
+      <c r="B130" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D130" s="5" t="s">
+      <c r="C130" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D130" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E130" s="3" t="s">
@@ -4461,13 +4465,13 @@
       <c r="A131" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="B131" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C131" s="8" t="s">
+      <c r="B131" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C131" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="D131" s="5" t="s">
+      <c r="D131" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E131" s="3" t="s">
@@ -4478,13 +4482,13 @@
       <c r="A132" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="B132" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C132" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="D132" s="5" t="s">
+      <c r="B132" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D132" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E132" s="3" t="s">
@@ -4493,15 +4497,15 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C133" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="B133" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C133" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="D133" s="5" t="s">
+      <c r="D133" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E133" s="3" t="s">
@@ -4510,15 +4514,15 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C134" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="B134" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C134" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="D134" s="5" t="s">
+      <c r="D134" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E134" s="3" t="s">
@@ -4527,15 +4531,15 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C135" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B135" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C135" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="D135" s="5" t="s">
+      <c r="D135" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E135" s="3" t="s">
@@ -4544,15 +4548,15 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C136" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="B136" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C136" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="D136" s="5" t="s">
+      <c r="D136" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E136" s="3" t="s">
@@ -4561,15 +4565,15 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C137" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="B137" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C137" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D137" s="5" t="s">
+      <c r="D137" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E137" s="3" t="s">
@@ -4578,15 +4582,15 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C138" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="B138" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C138" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="D138" s="5" t="s">
+      <c r="D138" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E138" s="3" t="s">
@@ -4595,15 +4599,15 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C139" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="B139" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C139" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="D139" s="5" t="s">
+      <c r="D139" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E139" s="3" t="s">
@@ -4612,15 +4616,15 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C140" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="B140" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C140" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="D140" s="5" t="s">
+      <c r="D140" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E140" s="3" t="s">
@@ -4629,15 +4633,15 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C141" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="B141" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C141" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="D141" s="5" t="s">
+      <c r="D141" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E141" s="3" t="s">
@@ -4646,15 +4650,15 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C142" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="B142" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C142" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D142" s="5" t="s">
+      <c r="D142" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E142" s="3" t="s">
@@ -4663,15 +4667,15 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C143" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="B143" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C143" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="D143" s="5" t="s">
+      <c r="D143" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E143" s="3" t="s">
@@ -4682,13 +4686,13 @@
       <c r="A144" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="B144" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C144" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D144" s="5" t="s">
+      <c r="B144" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C144" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="D144" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E144" s="3" t="s">
@@ -4697,15 +4701,15 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="B145" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C145" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="D145" s="5" t="s">
+      <c r="B145" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D145" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E145" s="3" t="s">
@@ -4714,15 +4718,15 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B146" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="B146" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C146" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="D146" s="5" t="s">
+      <c r="C146" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="D146" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E146" s="3" t="s">
@@ -4733,13 +4737,13 @@
       <c r="A147" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="B147" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C147" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D147" s="5" t="s">
+      <c r="B147" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D147" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E147" s="3" t="s">
@@ -4750,13 +4754,13 @@
       <c r="A148" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="B148" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C148" s="8" t="s">
+      <c r="B148" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C148" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="D148" s="5" t="s">
+      <c r="D148" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E148" s="3" t="s">
@@ -4767,10 +4771,10 @@
       <c r="A149" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="B149" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C149" s="8" t="s">
+      <c r="B149" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C149" s="7" t="s">
         <v>279</v>
       </c>
       <c r="D149" s="5" t="s">
@@ -4780,15 +4784,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" ht="28" spans="1:5">
+    <row r="150" spans="1:5">
       <c r="A150" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="B150" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C150" s="10" t="s">
-        <v>281</v>
+      <c r="B150" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C150" s="7" t="s">
+        <v>136</v>
       </c>
       <c r="D150" s="5" t="s">
         <v>8</v>
@@ -4799,13 +4803,13 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C151" s="7" t="s">
         <v>282</v>
-      </c>
-      <c r="B151" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C151" s="8" t="s">
-        <v>260</v>
       </c>
       <c r="D151" s="5" t="s">
         <v>8</v>
@@ -4818,11 +4822,11 @@
       <c r="A152" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="B152" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C152" s="8" t="s">
-        <v>262</v>
+      <c r="B152" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C152" s="7" t="s">
+        <v>284</v>
       </c>
       <c r="D152" s="5" t="s">
         <v>8</v>
@@ -4833,13 +4837,13 @@
     </row>
     <row r="153" ht="28" spans="1:5">
       <c r="A153" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="B153" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C153" s="10" t="s">
         <v>285</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>286</v>
       </c>
       <c r="D153" s="5" t="s">
         <v>8</v>
@@ -4850,13 +4854,13 @@
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="B154" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C154" s="8" t="s">
-        <v>172</v>
+        <v>287</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C154" s="7" t="s">
+        <v>265</v>
       </c>
       <c r="D154" s="5" t="s">
         <v>8</v>
@@ -4867,13 +4871,13 @@
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="B155" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C155" s="8" t="s">
-        <v>264</v>
+        <v>288</v>
+      </c>
+      <c r="B155" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C155" s="7" t="s">
+        <v>267</v>
       </c>
       <c r="D155" s="5" t="s">
         <v>8</v>
@@ -4882,15 +4886,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" ht="28" spans="1:5">
       <c r="A156" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="B156" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C156" s="8" t="s">
         <v>289</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C156" s="9" t="s">
+        <v>290</v>
       </c>
       <c r="D156" s="5" t="s">
         <v>8</v>
@@ -4901,13 +4905,13 @@
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="B157" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C157" s="8" t="s">
-        <v>58</v>
+      <c r="B157" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D157" s="5" t="s">
         <v>8</v>
@@ -4920,11 +4924,11 @@
       <c r="A158" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="B158" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C158" s="8" t="s">
-        <v>293</v>
+      <c r="B158" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C158" s="7" t="s">
+        <v>269</v>
       </c>
       <c r="D158" s="5" t="s">
         <v>8</v>
@@ -4935,13 +4939,13 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B159" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C159" s="7" t="s">
         <v>294</v>
-      </c>
-      <c r="B159" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C159" s="8" t="s">
-        <v>295</v>
       </c>
       <c r="D159" s="5" t="s">
         <v>8</v>
@@ -4952,16 +4956,16 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B160" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="B160" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C160" s="8" t="s">
+      <c r="C160" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D160" s="5" t="s">
         <v>297</v>
-      </c>
-      <c r="D160" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>8</v>
@@ -4971,14 +4975,14 @@
       <c r="A161" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="B161" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C161" s="8" t="s">
+      <c r="B161" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C161" s="7" t="s">
         <v>299</v>
       </c>
       <c r="D161" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>8</v>
@@ -4988,14 +4992,14 @@
       <c r="A162" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="B162" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C162" s="8" t="s">
+      <c r="B162" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C162" s="7" t="s">
         <v>301</v>
       </c>
       <c r="D162" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>8</v>
@@ -5005,14 +5009,14 @@
       <c r="A163" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="B163" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C163" s="8" t="s">
+      <c r="B163" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C163" s="7" t="s">
         <v>303</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>8</v>
@@ -5022,14 +5026,14 @@
       <c r="A164" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="B164" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C164" s="8" t="s">
+      <c r="B164" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C164" s="7" t="s">
         <v>305</v>
       </c>
       <c r="D164" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>8</v>
@@ -5039,14 +5043,14 @@
       <c r="A165" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="B165" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C165" s="8" t="s">
+      <c r="B165" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C165" s="7" t="s">
         <v>307</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>8</v>
@@ -5056,14 +5060,14 @@
       <c r="A166" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="B166" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C166" s="8" t="s">
+      <c r="B166" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C166" s="7" t="s">
         <v>309</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>8</v>
@@ -5073,14 +5077,14 @@
       <c r="A167" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="B167" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C167" s="8" t="s">
+      <c r="B167" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C167" s="7" t="s">
         <v>311</v>
       </c>
       <c r="D167" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>8</v>
@@ -5090,14 +5094,14 @@
       <c r="A168" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="B168" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C168" s="8" t="s">
+      <c r="B168" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C168" s="7" t="s">
         <v>313</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>8</v>
@@ -5107,14 +5111,14 @@
       <c r="A169" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="B169" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C169" s="8" t="s">
+      <c r="B169" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C169" s="7" t="s">
         <v>315</v>
       </c>
       <c r="D169" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>8</v>
@@ -5124,14 +5128,14 @@
       <c r="A170" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="B170" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C170" s="8" t="s">
+      <c r="B170" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C170" s="7" t="s">
         <v>317</v>
       </c>
       <c r="D170" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>8</v>
@@ -5141,14 +5145,14 @@
       <c r="A171" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="B171" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C171" s="8" t="s">
+      <c r="B171" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C171" s="7" t="s">
         <v>319</v>
       </c>
       <c r="D171" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>8</v>
@@ -5158,14 +5162,14 @@
       <c r="A172" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="B172" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C172" s="8" t="s">
-        <v>260</v>
+      <c r="B172" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C172" s="7" t="s">
+        <v>321</v>
       </c>
       <c r="D172" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>8</v>
@@ -5173,33 +5177,33 @@
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="B173" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C173" s="8" t="s">
-        <v>262</v>
+        <v>322</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C173" s="7" t="s">
+        <v>323</v>
       </c>
       <c r="D173" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="174" ht="28" spans="1:5">
+    <row r="174" spans="1:5">
       <c r="A174" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="B174" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C174" s="10" t="s">
-        <v>323</v>
+        <v>324</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C174" s="7" t="s">
+        <v>325</v>
       </c>
       <c r="D174" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>8</v>
@@ -5207,16 +5211,16 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="B175" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C175" s="8" t="s">
-        <v>264</v>
+        <v>326</v>
+      </c>
+      <c r="B175" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C175" s="7" t="s">
+        <v>265</v>
       </c>
       <c r="D175" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>8</v>
@@ -5224,18 +5228,69 @@
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="B176" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C176" s="8" t="s">
-        <v>326</v>
+        <v>327</v>
+      </c>
+      <c r="B176" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C176" s="7" t="s">
+        <v>267</v>
       </c>
       <c r="D176" s="5" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="E176" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" ht="28" spans="1:5">
+      <c r="A177" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B177" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C177" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="D177" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B178" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C178" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="D178" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B179" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C179" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="D179" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="E179" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5244,7 +5299,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D126:E126 D1:D8 D124:D125 E2:E8 E124:E125 F2:F3 D9:E119 D158:E176 D138:E157 D127:E137 D120:E123">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E128 E129 E160 D1:D8 D128:D148 D160:D179 E2:E8 E130:E143 E144:E148 E161:E179 F2:F3 D44:E81 D82:E127 D9:E43 D149:E159">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
works on all PDF
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="327">
   <si>
     <t>ID</t>
   </si>
@@ -305,12 +305,15 @@
     <t>TC_042</t>
   </si>
   <si>
+    <t>Verify form can be printed in pdf</t>
+  </si>
+  <si>
+    <t>TC_043</t>
+  </si>
+  <si>
     <t>Reset the RW01 form</t>
   </si>
   <si>
-    <t>TC_043</t>
-  </si>
-  <si>
     <t>probateFormsRW02.feature</t>
   </si>
   <si>
@@ -545,9 +548,6 @@
     <t>TC_082</t>
   </si>
   <si>
-    <t>Verify form can be printed in pdf</t>
-  </si>
-  <si>
     <t>TC_083</t>
   </si>
   <si>
@@ -602,16 +602,19 @@
     <t>TC_094</t>
   </si>
   <si>
+    <t>TC_095</t>
+  </si>
+  <si>
     <t>Reset the RW04 form</t>
   </si>
   <si>
-    <t>TC_095</t>
+    <t>TC_096</t>
   </si>
   <si>
     <t>probateFormsRW05.feature</t>
   </si>
   <si>
-    <t>TC_096</t>
+    <t>Yes</t>
   </si>
   <si>
     <t>TC_097</t>
@@ -708,9 +711,6 @@
   </si>
   <si>
     <t>probateFormsRWxx.feature</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>TC_118</t>
@@ -2231,10 +2231,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F176"/>
+  <dimension ref="A1:F178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="C125" sqref="C125"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119:D128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2983,10 +2983,10 @@
         <v>93</v>
       </c>
       <c r="B44" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>94</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>8</v>
@@ -2997,13 +2997,13 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>94</v>
-      </c>
       <c r="C45" s="9" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>8</v>
@@ -3014,13 +3014,13 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>97</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>98</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>8</v>
@@ -3031,13 +3031,13 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>100</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>8</v>
@@ -3048,13 +3048,13 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>102</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>8</v>
@@ -3065,13 +3065,13 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>103</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>104</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>8</v>
@@ -3082,47 +3082,47 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B50" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C50" s="9" t="s">
+      <c r="D50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" ht="28" spans="1:5">
-      <c r="A51" s="3" t="s">
+      <c r="B51" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B51" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C51" s="9" t="s">
+      <c r="D51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" ht="28" spans="1:5">
+      <c r="A52" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="3" t="s">
+      <c r="B52" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>110</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>8</v>
@@ -3133,47 +3133,47 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C53" s="9" t="s">
+      <c r="D53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" ht="28" spans="1:5">
-      <c r="A54" s="3" t="s">
+      <c r="B54" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" s="9" t="s">
+      <c r="D54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" ht="28" spans="1:5">
+      <c r="A55" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="3" t="s">
+      <c r="B55" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>115</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>116</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>8</v>
@@ -3184,47 +3184,47 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B56" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C56" s="9" t="s">
+      <c r="D56" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" ht="28" spans="1:5">
-      <c r="A57" s="3" t="s">
+      <c r="B57" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B57" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C57" s="9" t="s">
+      <c r="D57" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" ht="28" spans="1:5">
+      <c r="A58" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="3" t="s">
+      <c r="B58" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>8</v>
@@ -3235,13 +3235,13 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>8</v>
@@ -3252,47 +3252,47 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B60" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C60" s="9" t="s">
+      <c r="D60" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" ht="28" spans="1:5">
-      <c r="A61" s="3" t="s">
+      <c r="B61" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B61" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C61" s="9" t="s">
+      <c r="D61" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" ht="28" spans="1:5">
+      <c r="A62" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="3" t="s">
+      <c r="B62" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C62" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>8</v>
@@ -3303,13 +3303,13 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="9" t="s">
         <v>131</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>132</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>8</v>
@@ -3320,13 +3320,13 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C64" s="9" t="s">
         <v>133</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>134</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>8</v>
@@ -3337,13 +3337,13 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C65" s="9" t="s">
         <v>135</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>136</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>8</v>
@@ -3354,13 +3354,13 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>137</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>138</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>8</v>
@@ -3371,13 +3371,13 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>139</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>140</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>8</v>
@@ -3388,13 +3388,13 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>142</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>8</v>
@@ -3405,13 +3405,13 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>144</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>8</v>
@@ -3422,13 +3422,13 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>145</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>146</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>8</v>
@@ -3439,13 +3439,13 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C71" s="9" t="s">
         <v>147</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>148</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>8</v>
@@ -3456,13 +3456,13 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>150</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>8</v>
@@ -3473,13 +3473,13 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C73" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>152</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>8</v>
@@ -3490,13 +3490,13 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C74" s="9" t="s">
         <v>153</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>8</v>
@@ -3507,13 +3507,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B75" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="C75" s="9" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>8</v>
@@ -3524,13 +3524,13 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C76" s="9" t="s">
         <v>157</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>158</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>8</v>
@@ -3541,13 +3541,13 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C77" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>160</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>8</v>
@@ -3558,13 +3558,13 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" s="9" t="s">
         <v>161</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>162</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>8</v>
@@ -3575,13 +3575,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>163</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>164</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>8</v>
@@ -3592,13 +3592,13 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C80" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>8</v>
@@ -3609,13 +3609,13 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C81" s="9" t="s">
         <v>167</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>168</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>8</v>
@@ -3626,13 +3626,13 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C82" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>8</v>
@@ -3643,13 +3643,13 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C83" s="9" t="s">
         <v>171</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>172</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>8</v>
@@ -3660,13 +3660,13 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>8</v>
@@ -3677,13 +3677,13 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>58</v>
+        <v>155</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>174</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>8</v>
@@ -3694,13 +3694,13 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>178</v>
+        <v>58</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>8</v>
@@ -3711,13 +3711,13 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>8</v>
@@ -3728,13 +3728,13 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>8</v>
@@ -3745,13 +3745,13 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>8</v>
@@ -3762,13 +3762,13 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>8</v>
@@ -3779,13 +3779,13 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>8</v>
@@ -3796,13 +3796,13 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>8</v>
@@ -3813,13 +3813,13 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>8</v>
@@ -3830,13 +3830,13 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>8</v>
@@ -3847,13 +3847,13 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>8</v>
@@ -3864,13 +3864,13 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C96" s="8" t="s">
-        <v>58</v>
+        <v>176</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>8</v>
@@ -3881,13 +3881,13 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>102</v>
+        <v>192</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>8</v>
@@ -3898,16 +3898,16 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D98" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="B98" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C98" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -3918,13 +3918,13 @@
         <v>196</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -3932,16 +3932,16 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -3949,16 +3949,16 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -3966,16 +3966,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -3983,16 +3983,16 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -4000,16 +4000,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -4017,16 +4017,16 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -4034,16 +4034,16 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C106" s="9" t="s">
-        <v>172</v>
+        <v>194</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>203</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -4051,16 +4051,16 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -4068,16 +4068,16 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C108" s="8" t="s">
-        <v>58</v>
+        <v>194</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -4085,16 +4085,16 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>156</v>
+        <v>207</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -4102,13 +4102,13 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B110" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="B110" s="8" t="s">
-        <v>208</v>
-      </c>
       <c r="C110" s="8" t="s">
-        <v>158</v>
+        <v>58</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>8</v>
@@ -4122,10 +4122,10 @@
         <v>210</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>211</v>
+        <v>157</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>8</v>
@@ -4136,13 +4136,13 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>213</v>
+        <v>159</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>8</v>
@@ -4153,13 +4153,13 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>8</v>
@@ -4170,13 +4170,13 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>8</v>
@@ -4187,13 +4187,13 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>8</v>
@@ -4204,13 +4204,13 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>8</v>
@@ -4221,13 +4221,13 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>8</v>
@@ -4238,13 +4238,13 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C118" s="9" t="s">
-        <v>172</v>
+        <v>209</v>
+      </c>
+      <c r="C118" s="8" t="s">
+        <v>221</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>8</v>
@@ -4255,13 +4255,13 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C119" s="8" t="s">
         <v>223</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C119" s="8" t="s">
-        <v>224</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>8</v>
@@ -4272,33 +4272,33 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C120" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C121" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="B120" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C120" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="E120" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="121" ht="28" spans="1:5">
-      <c r="A121" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B121" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C121" s="10" t="s">
-        <v>229</v>
-      </c>
       <c r="D121" s="3" t="s">
-        <v>227</v>
+        <v>8</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4306,33 +4306,33 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>231</v>
+        <v>58</v>
       </c>
       <c r="D122" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" ht="28" spans="1:5">
+      <c r="A123" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B123" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="E122" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5">
-      <c r="A123" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B123" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C123" s="8" t="s">
-        <v>233</v>
+      <c r="C123" s="10" t="s">
+        <v>229</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>227</v>
+        <v>8</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>8</v>
@@ -4340,16 +4340,16 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>227</v>
+        <v>8</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>8</v>
@@ -4357,16 +4357,16 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C125" s="9" t="s">
-        <v>172</v>
+        <v>227</v>
+      </c>
+      <c r="C125" s="8" t="s">
+        <v>233</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>227</v>
+        <v>8</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>8</v>
@@ -4374,16 +4374,16 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>227</v>
+        <v>8</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>8</v>
@@ -4391,15 +4391,15 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C127" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D127" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C127" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D127" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E127" s="3" t="s">
@@ -4408,15 +4408,15 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="D128" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D128" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E128" s="3" t="s">
@@ -4425,15 +4425,15 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B129" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D129" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D129" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E129" s="3" t="s">
@@ -4442,15 +4442,15 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B130" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="D130" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D130" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E130" s="3" t="s">
@@ -4459,13 +4459,13 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B131" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>246</v>
+        <v>105</v>
       </c>
       <c r="D131" s="5" t="s">
         <v>8</v>
@@ -4476,13 +4476,13 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B132" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>8</v>
@@ -4493,13 +4493,13 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B133" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>8</v>
@@ -4510,13 +4510,13 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B134" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>8</v>
@@ -4527,13 +4527,13 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B135" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D135" s="5" t="s">
         <v>8</v>
@@ -4544,13 +4544,13 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B136" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D136" s="5" t="s">
         <v>8</v>
@@ -4561,13 +4561,13 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="3" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B137" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D137" s="5" t="s">
         <v>8</v>
@@ -4578,13 +4578,13 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B138" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D138" s="5" t="s">
         <v>8</v>
@@ -4595,13 +4595,13 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B139" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D139" s="5" t="s">
         <v>8</v>
@@ -4612,13 +4612,13 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B140" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D140" s="5" t="s">
         <v>8</v>
@@ -4629,13 +4629,13 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B141" s="8" t="s">
         <v>239</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D141" s="5" t="s">
         <v>8</v>
@@ -4646,13 +4646,13 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>268</v>
+        <v>239</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>58</v>
+        <v>264</v>
       </c>
       <c r="D142" s="5" t="s">
         <v>8</v>
@@ -4663,13 +4663,13 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>268</v>
+        <v>239</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="D143" s="5" t="s">
         <v>8</v>
@@ -4680,13 +4680,13 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B144" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="D144" s="5" t="s">
         <v>8</v>
@@ -4697,13 +4697,13 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B145" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>272</v>
+        <v>241</v>
       </c>
       <c r="D145" s="5" t="s">
         <v>8</v>
@@ -4714,13 +4714,13 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B146" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>274</v>
+        <v>105</v>
       </c>
       <c r="D146" s="5" t="s">
         <v>8</v>
@@ -4731,13 +4731,13 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B147" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>134</v>
+        <v>272</v>
       </c>
       <c r="D147" s="5" t="s">
         <v>8</v>
@@ -4748,13 +4748,13 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B148" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D148" s="5" t="s">
         <v>8</v>
@@ -4765,13 +4765,13 @@
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B149" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>279</v>
+        <v>135</v>
       </c>
       <c r="D149" s="5" t="s">
         <v>8</v>
@@ -4780,15 +4780,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" ht="28" spans="1:5">
+    <row r="150" spans="1:5">
       <c r="A150" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B150" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="C150" s="10" t="s">
-        <v>281</v>
+      <c r="C150" s="8" t="s">
+        <v>277</v>
       </c>
       <c r="D150" s="5" t="s">
         <v>8</v>
@@ -4799,13 +4799,13 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B151" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
       <c r="D151" s="5" t="s">
         <v>8</v>
@@ -4814,15 +4814,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" ht="28" spans="1:5">
       <c r="A152" s="3" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B152" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="C152" s="8" t="s">
-        <v>262</v>
+      <c r="C152" s="10" t="s">
+        <v>281</v>
       </c>
       <c r="D152" s="5" t="s">
         <v>8</v>
@@ -4831,15 +4831,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" ht="28" spans="1:5">
+    <row r="153" spans="1:5">
       <c r="A153" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B153" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="C153" s="10" t="s">
-        <v>285</v>
+      <c r="C153" s="8" t="s">
+        <v>260</v>
       </c>
       <c r="D153" s="5" t="s">
         <v>8</v>
@@ -4850,13 +4850,13 @@
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B154" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C154" s="8" t="s">
-        <v>172</v>
+        <v>262</v>
       </c>
       <c r="D154" s="5" t="s">
         <v>8</v>
@@ -4865,15 +4865,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" ht="28" spans="1:5">
       <c r="A155" s="3" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B155" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="C155" s="8" t="s">
-        <v>264</v>
+      <c r="C155" s="10" t="s">
+        <v>285</v>
       </c>
       <c r="D155" s="5" t="s">
         <v>8</v>
@@ -4884,13 +4884,13 @@
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B156" s="8" t="s">
         <v>268</v>
       </c>
       <c r="C156" s="8" t="s">
-        <v>289</v>
+        <v>92</v>
       </c>
       <c r="D156" s="5" t="s">
         <v>8</v>
@@ -4901,13 +4901,13 @@
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
       <c r="C157" s="8" t="s">
-        <v>58</v>
+        <v>264</v>
       </c>
       <c r="D157" s="5" t="s">
         <v>8</v>
@@ -4918,13 +4918,13 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D158" s="5" t="s">
         <v>8</v>
@@ -4935,13 +4935,13 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="3" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B159" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>295</v>
+        <v>58</v>
       </c>
       <c r="D159" s="5" t="s">
         <v>8</v>
@@ -4952,13 +4952,13 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B160" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D160" s="5" t="s">
         <v>8</v>
@@ -4969,13 +4969,13 @@
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="3" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B161" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C161" s="8" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D161" s="5" t="s">
         <v>8</v>
@@ -4986,13 +4986,13 @@
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="3" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B162" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D162" s="5" t="s">
         <v>8</v>
@@ -5003,13 +5003,13 @@
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="3" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B163" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D163" s="5" t="s">
         <v>8</v>
@@ -5020,13 +5020,13 @@
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B164" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C164" s="8" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D164" s="5" t="s">
         <v>8</v>
@@ -5037,13 +5037,13 @@
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B165" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C165" s="8" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D165" s="5" t="s">
         <v>8</v>
@@ -5054,13 +5054,13 @@
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B166" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D166" s="5" t="s">
         <v>8</v>
@@ -5071,13 +5071,13 @@
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B167" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D167" s="5" t="s">
         <v>8</v>
@@ -5088,13 +5088,13 @@
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B168" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D168" s="5" t="s">
         <v>8</v>
@@ -5105,13 +5105,13 @@
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B169" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D169" s="5" t="s">
         <v>8</v>
@@ -5122,13 +5122,13 @@
     </row>
     <row r="170" spans="1:5">
       <c r="A170" s="3" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B170" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D170" s="5" t="s">
         <v>8</v>
@@ -5139,13 +5139,13 @@
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="3" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B171" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C171" s="8" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D171" s="5" t="s">
         <v>8</v>
@@ -5156,13 +5156,13 @@
     </row>
     <row r="172" spans="1:5">
       <c r="A172" s="3" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B172" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C172" s="8" t="s">
-        <v>260</v>
+        <v>317</v>
       </c>
       <c r="D172" s="5" t="s">
         <v>8</v>
@@ -5173,13 +5173,13 @@
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="3" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B173" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C173" s="8" t="s">
-        <v>262</v>
+        <v>319</v>
       </c>
       <c r="D173" s="5" t="s">
         <v>8</v>
@@ -5188,15 +5188,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" ht="28" spans="1:5">
+    <row r="174" spans="1:5">
       <c r="A174" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B174" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C174" s="10" t="s">
-        <v>323</v>
+      <c r="C174" s="8" t="s">
+        <v>260</v>
       </c>
       <c r="D174" s="5" t="s">
         <v>8</v>
@@ -5207,13 +5207,13 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="3" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B175" s="8" t="s">
         <v>291</v>
       </c>
       <c r="C175" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D175" s="5" t="s">
         <v>8</v>
@@ -5222,20 +5222,54 @@
         <v>8</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
+    <row r="176" ht="28" spans="1:5">
       <c r="A176" s="3" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B176" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C176" s="8" t="s">
+      <c r="C176" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="D176" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C177" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D177" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C178" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="D176" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E176" s="3" t="s">
+      <c r="D178" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E178" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5244,7 +5278,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D126:E126 D1:D8 D124:D125 E2:E8 E124:E125 F2:F3 D9:E119 D158:E176 D138:E157 D127:E137 D120:E123">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E110 D1:D8 D98:D110 D119:D128 E2:E8 E98:E99 E100:E109 E119:E121 E122:E128 F2:F3 D129:E178 D111:E118 D9:E94 D95:E97">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
resolved issues of RW 2, 4, 6, 7, 8, 10 probate forms
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -665,6 +665,9 @@
     <t>probateFormsRW06.feature</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_111</t>
   </si>
   <si>
@@ -762,9 +765,6 @@
   </si>
   <si>
     <t>probateFormsRW07.feature</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>TC_130</t>
@@ -2237,8 +2237,8 @@
   <sheetPr/>
   <dimension ref="A1:F180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -4132,7 +4132,7 @@
         <v>58</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -4140,7 +4140,7 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B112" s="7" t="s">
         <v>211</v>
@@ -4149,7 +4149,7 @@
         <v>159</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -4157,7 +4157,7 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B113" s="7" t="s">
         <v>211</v>
@@ -4166,7 +4166,7 @@
         <v>161</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -4174,16 +4174,16 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B114" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -4191,16 +4191,16 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -4208,16 +4208,16 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B116" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -4225,16 +4225,16 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B117" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -4242,16 +4242,16 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B118" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -4259,16 +4259,16 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B119" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4276,16 +4276,16 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B120" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4293,7 +4293,7 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B121" s="7" t="s">
         <v>211</v>
@@ -4302,7 +4302,7 @@
         <v>92</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4310,16 +4310,16 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B122" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4327,10 +4327,10 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>58</v>
@@ -4344,13 +4344,13 @@
     </row>
     <row r="124" ht="28" spans="1:5">
       <c r="A124" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B124" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B124" s="7" t="s">
-        <v>231</v>
-      </c>
       <c r="C124" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>8</v>
@@ -4361,13 +4361,13 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>8</v>
@@ -4378,13 +4378,13 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>8</v>
@@ -4395,13 +4395,13 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>8</v>
@@ -4412,10 +4412,10 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C128" s="8" t="s">
         <v>92</v>
@@ -4429,13 +4429,13 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>8</v>
@@ -4446,16 +4446,16 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>8</v>
@@ -4466,13 +4466,13 @@
         <v>246</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>247</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -4483,13 +4483,13 @@
         <v>248</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C132" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>8</v>
@@ -4500,13 +4500,13 @@
         <v>249</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>250</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>8</v>
@@ -4517,13 +4517,13 @@
         <v>251</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C134" s="7" t="s">
         <v>252</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -4534,13 +4534,13 @@
         <v>253</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C135" s="7" t="s">
         <v>254</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -4551,13 +4551,13 @@
         <v>255</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C136" s="7" t="s">
         <v>256</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -4568,13 +4568,13 @@
         <v>257</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C137" s="7" t="s">
         <v>258</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -4585,13 +4585,13 @@
         <v>259</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C138" s="7" t="s">
         <v>260</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>8</v>
@@ -4602,13 +4602,13 @@
         <v>261</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C139" s="7" t="s">
         <v>262</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>8</v>
@@ -4619,13 +4619,13 @@
         <v>263</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C140" s="7" t="s">
         <v>264</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>8</v>
@@ -4636,13 +4636,13 @@
         <v>265</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C141" s="7" t="s">
         <v>266</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -4653,13 +4653,13 @@
         <v>267</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C142" s="7" t="s">
         <v>268</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -4670,13 +4670,13 @@
         <v>269</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C143" s="7" t="s">
         <v>270</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -4687,13 +4687,13 @@
         <v>271</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C144" s="7" t="s">
         <v>272</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>8</v>
@@ -5015,7 +5015,7 @@
       <c r="C163" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="D163" s="5" t="s">
+      <c r="D163" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E163" s="3" t="s">
@@ -5032,7 +5032,7 @@
       <c r="C164" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="D164" s="5" t="s">
+      <c r="D164" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E164" s="3" t="s">
@@ -5049,7 +5049,7 @@
       <c r="C165" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="D165" s="5" t="s">
+      <c r="D165" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E165" s="3" t="s">
@@ -5066,7 +5066,7 @@
       <c r="C166" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="D166" s="5" t="s">
+      <c r="D166" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E166" s="3" t="s">
@@ -5083,7 +5083,7 @@
       <c r="C167" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="D167" s="5" t="s">
+      <c r="D167" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E167" s="3" t="s">
@@ -5100,7 +5100,7 @@
       <c r="C168" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="D168" s="5" t="s">
+      <c r="D168" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E168" s="3" t="s">
@@ -5117,7 +5117,7 @@
       <c r="C169" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="D169" s="5" t="s">
+      <c r="D169" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E169" s="3" t="s">
@@ -5134,7 +5134,7 @@
       <c r="C170" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="D170" s="5" t="s">
+      <c r="D170" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E170" s="3" t="s">
@@ -5151,7 +5151,7 @@
       <c r="C171" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="D171" s="5" t="s">
+      <c r="D171" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E171" s="3" t="s">
@@ -5168,7 +5168,7 @@
       <c r="C172" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="D172" s="5" t="s">
+      <c r="D172" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E172" s="3" t="s">
@@ -5185,7 +5185,7 @@
       <c r="C173" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="D173" s="5" t="s">
+      <c r="D173" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E173" s="3" t="s">
@@ -5202,7 +5202,7 @@
       <c r="C174" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="D174" s="5" t="s">
+      <c r="D174" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E174" s="3" t="s">
@@ -5219,7 +5219,7 @@
       <c r="C175" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="D175" s="5" t="s">
+      <c r="D175" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E175" s="3" t="s">
@@ -5236,7 +5236,7 @@
       <c r="C176" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="D176" s="5" t="s">
+      <c r="D176" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E176" s="3" t="s">
@@ -5253,7 +5253,7 @@
       <c r="C177" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="D177" s="5" t="s">
+      <c r="D177" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E177" s="3" t="s">
@@ -5270,7 +5270,7 @@
       <c r="C178" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="D178" s="5" t="s">
+      <c r="D178" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E178" s="3" t="s">
@@ -5287,7 +5287,7 @@
       <c r="C179" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="D179" s="5" t="s">
+      <c r="D179" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E179" s="3" t="s">
@@ -5304,7 +5304,7 @@
       <c r="C180" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="D180" s="5" t="s">
+      <c r="D180" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E180" s="3" t="s">
@@ -5316,7 +5316,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E160 D1:D8 D130:D144 D145:D162 E2:E8 E130:E131 E132:E142 E143:E144 E145:E156 E157:E159 E161:E162 F2:F3 D105:E123 D9:E104 D163:E180 D124:E129">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E111 E129 D1:D8 D111:D121 D129:D145 E2:E8 E112:E121 E130:E145 F2:F3 D146:E164 D165:E180 D9:E110 D122:E128">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added 5 TCs of OC01 probate form and resolved issues of RW01 and RW02
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -320,6 +320,9 @@
     <t>probateFormsRW02.feature</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_045</t>
   </si>
   <si>
@@ -663,9 +666,6 @@
   </si>
   <si>
     <t>probateFormsRW06.feature</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>TC_111</t>
@@ -2237,8 +2237,8 @@
   <sheetPr/>
   <dimension ref="A1:F180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3010,7 +3010,7 @@
         <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -3018,16 +3018,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -3035,16 +3035,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -3052,16 +3052,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -3069,16 +3069,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -3086,16 +3086,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -3103,16 +3103,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -3120,16 +3120,16 @@
     </row>
     <row r="52" ht="28" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -3137,16 +3137,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -3154,16 +3154,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -3171,16 +3171,16 @@
     </row>
     <row r="55" ht="28" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -3188,16 +3188,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -3205,16 +3205,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -3222,16 +3222,16 @@
     </row>
     <row r="58" ht="28" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -3239,16 +3239,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -3256,16 +3256,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -3273,16 +3273,16 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -3290,16 +3290,16 @@
     </row>
     <row r="62" ht="28" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3307,16 +3307,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3324,16 +3324,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3341,16 +3341,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3358,16 +3358,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3375,16 +3375,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3392,16 +3392,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3409,16 +3409,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3426,16 +3426,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3443,16 +3443,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3460,16 +3460,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3477,16 +3477,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3494,7 +3494,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>96</v>
@@ -3503,7 +3503,7 @@
         <v>92</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>8</v>
@@ -3511,16 +3511,16 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>8</v>
@@ -3528,10 +3528,10 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>58</v>
@@ -3545,13 +3545,13 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B77" s="7" t="s">
-        <v>157</v>
-      </c>
       <c r="C77" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>8</v>
@@ -3562,13 +3562,13 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>8</v>
@@ -3579,13 +3579,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>8</v>
@@ -3596,13 +3596,13 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>8</v>
@@ -3613,13 +3613,13 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>8</v>
@@ -3630,13 +3630,13 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>8</v>
@@ -3647,13 +3647,13 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>8</v>
@@ -3664,13 +3664,13 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>8</v>
@@ -3681,10 +3681,10 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>92</v>
@@ -3698,13 +3698,13 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>8</v>
@@ -3715,10 +3715,10 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>58</v>
@@ -3732,13 +3732,13 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>178</v>
-      </c>
       <c r="C88" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>8</v>
@@ -3749,13 +3749,13 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>8</v>
@@ -3766,13 +3766,13 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>8</v>
@@ -3783,13 +3783,13 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>8</v>
@@ -3800,13 +3800,13 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>8</v>
@@ -3817,13 +3817,13 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>8</v>
@@ -3834,13 +3834,13 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>8</v>
@@ -3851,13 +3851,13 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>8</v>
@@ -3868,13 +3868,13 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>8</v>
@@ -3885,10 +3885,10 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>92</v>
@@ -3902,13 +3902,13 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>8</v>
@@ -3919,10 +3919,10 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>58</v>
@@ -3936,13 +3936,13 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B100" s="7" t="s">
-        <v>196</v>
-      </c>
       <c r="C100" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>8</v>
@@ -3953,13 +3953,13 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>8</v>
@@ -3970,13 +3970,13 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>8</v>
@@ -3987,13 +3987,13 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>8</v>
@@ -4004,13 +4004,13 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>8</v>
@@ -4021,13 +4021,13 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>8</v>
@@ -4038,13 +4038,13 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>8</v>
@@ -4055,13 +4055,13 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>8</v>
@@ -4072,13 +4072,13 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>8</v>
@@ -4089,10 +4089,10 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>92</v>
@@ -4106,13 +4106,13 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>8</v>
@@ -4123,16 +4123,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -4143,13 +4143,13 @@
         <v>213</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -4160,13 +4160,13 @@
         <v>214</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -4177,13 +4177,13 @@
         <v>215</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>216</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -4194,13 +4194,13 @@
         <v>217</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>218</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -4211,13 +4211,13 @@
         <v>219</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>220</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -4228,13 +4228,13 @@
         <v>221</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>222</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -4245,13 +4245,13 @@
         <v>223</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>216</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -4262,13 +4262,13 @@
         <v>224</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>225</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4279,13 +4279,13 @@
         <v>226</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>227</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4296,13 +4296,13 @@
         <v>228</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>92</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4313,13 +4313,13 @@
         <v>229</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>230</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4486,7 +4486,7 @@
         <v>245</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>8</v>
@@ -4741,7 +4741,7 @@
         <v>274</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>8</v>
@@ -4792,7 +4792,7 @@
         <v>274</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>8</v>
@@ -5316,7 +5316,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E111 E129 D1:D8 D111:D121 D129:D145 E2:E8 E112:E121 E130:E145 F2:F3 D146:E164 D165:E180 D9:E110 D122:E128">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E25 D1:D8 D25:D44 D45:D74 E2:E8 E26:E43 E44:E51 E52:E74 F2:F3 D9:E24 D110:E123 D124:E180 D75:E109">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
resolved issues of RW03
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -320,253 +320,253 @@
     <t>probateFormsRW02.feature</t>
   </si>
   <si>
+    <t>TC_045</t>
+  </si>
+  <si>
+    <t>Verify, correct county name is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_046</t>
+  </si>
+  <si>
+    <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
+  </si>
+  <si>
+    <t>TC_047</t>
+  </si>
+  <si>
+    <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
+  </si>
+  <si>
+    <t>TC_048</t>
+  </si>
+  <si>
+    <t>Verify, county, estate and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_049</t>
+  </si>
+  <si>
+    <t>Verify, the auto populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_050</t>
+  </si>
+  <si>
+    <t>Verify, names can be added in aka fields.</t>
+  </si>
+  <si>
+    <t>TC_051</t>
+  </si>
+  <si>
+    <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
+  </si>
+  <si>
+    <t>TC_052</t>
+  </si>
+  <si>
+    <t>Verify, amount can be entered in the input fields.</t>
+  </si>
+  <si>
+    <t>TC_053</t>
+  </si>
+  <si>
+    <t>Verify, total estimated value should display total of 1st and last field only.</t>
+  </si>
+  <si>
+    <t>TC_054</t>
+  </si>
+  <si>
+    <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_055</t>
+  </si>
+  <si>
+    <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_056</t>
+  </si>
+  <si>
+    <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
+  </si>
+  <si>
+    <t>TC_057</t>
+  </si>
+  <si>
+    <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
+  </si>
+  <si>
+    <t>TC_058</t>
+  </si>
+  <si>
+    <t>Verify that selecting option A keeps it selected without affecting option B.</t>
+  </si>
+  <si>
+    <t>TC_059</t>
+  </si>
+  <si>
+    <t>Verify, decedent died date is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_060</t>
+  </si>
+  <si>
+    <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
+  </si>
+  <si>
+    <t>TC_061</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
+  </si>
+  <si>
+    <t>TC_062</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B keeps it selected without affecting option A.</t>
+  </si>
+  <si>
+    <t>TC_063</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
+  </si>
+  <si>
+    <t>TC_064</t>
+  </si>
+  <si>
+    <t>Verify, multiple beneficiaries can be selected.</t>
+  </si>
+  <si>
+    <t>TC_065</t>
+  </si>
+  <si>
+    <t>Verify, bene contacts in the table.</t>
+  </si>
+  <si>
+    <t>TC_066</t>
+  </si>
+  <si>
+    <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
+  </si>
+  <si>
+    <t>TC_067</t>
+  </si>
+  <si>
+    <t>Verify, on checking "Display all heirs on attachment".</t>
+  </si>
+  <si>
+    <t>TC_068</t>
+  </si>
+  <si>
+    <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
+  </si>
+  <si>
+    <t>TC_069</t>
+  </si>
+  <si>
+    <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
+  </si>
+  <si>
+    <t>TC_070</t>
+  </si>
+  <si>
+    <t>Verify fees section.</t>
+  </si>
+  <si>
+    <t>TC_071</t>
+  </si>
+  <si>
+    <t>Verify, attorney can be selected.</t>
+  </si>
+  <si>
+    <t>TC_072</t>
+  </si>
+  <si>
+    <t>Verify, information in decree of the register.</t>
+  </si>
+  <si>
+    <t>TC_073</t>
+  </si>
+  <si>
+    <t>TC_074</t>
+  </si>
+  <si>
+    <t>Reset the RW02 form</t>
+  </si>
+  <si>
+    <t>TC_075</t>
+  </si>
+  <si>
+    <t>probateFormsRW03.feature</t>
+  </si>
+  <si>
+    <t>TC_076</t>
+  </si>
+  <si>
+    <t>Verify county, estate and aka names are auto-populated on the form</t>
+  </si>
+  <si>
+    <t>TC_077</t>
+  </si>
+  <si>
+    <t>Verify, the auto-populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_078</t>
+  </si>
+  <si>
+    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
+  </si>
+  <si>
+    <t>TC_079</t>
+  </si>
+  <si>
+    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
+  </si>
+  <si>
+    <t>TC_080</t>
+  </si>
+  <si>
+    <t>Verify, names can be entered in witness fields.</t>
+  </si>
+  <si>
+    <t>TC_081</t>
+  </si>
+  <si>
+    <t>Verify, names updated from signature are reflected in witness names fields.</t>
+  </si>
+  <si>
+    <t>TC_082</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered in address, city, zip fields.</t>
+  </si>
+  <si>
+    <t>TC_083</t>
+  </si>
+  <si>
+    <t>Verify, form is auto saved.</t>
+  </si>
+  <si>
+    <t>TC_084</t>
+  </si>
+  <si>
+    <t>TC_085</t>
+  </si>
+  <si>
+    <t>Reset the RW03 form</t>
+  </si>
+  <si>
+    <t>TC_086</t>
+  </si>
+  <si>
+    <t>probateFormsRW04.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_045</t>
-  </si>
-  <si>
-    <t>Verify, correct county name is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_046</t>
-  </si>
-  <si>
-    <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
-  </si>
-  <si>
-    <t>TC_047</t>
-  </si>
-  <si>
-    <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
-  </si>
-  <si>
-    <t>TC_048</t>
-  </si>
-  <si>
-    <t>Verify, county, estate and aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_049</t>
-  </si>
-  <si>
-    <t>Verify, the auto populated fields are not editable.</t>
-  </si>
-  <si>
-    <t>TC_050</t>
-  </si>
-  <si>
-    <t>Verify, names can be added in aka fields.</t>
-  </si>
-  <si>
-    <t>TC_051</t>
-  </si>
-  <si>
-    <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
-  </si>
-  <si>
-    <t>TC_052</t>
-  </si>
-  <si>
-    <t>Verify, amount can be entered in the input fields.</t>
-  </si>
-  <si>
-    <t>TC_053</t>
-  </si>
-  <si>
-    <t>Verify, total estimated value should display total of 1st and last field only.</t>
-  </si>
-  <si>
-    <t>TC_054</t>
-  </si>
-  <si>
-    <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
-  </si>
-  <si>
-    <t>TC_055</t>
-  </si>
-  <si>
-    <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
-  </si>
-  <si>
-    <t>TC_056</t>
-  </si>
-  <si>
-    <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
-  </si>
-  <si>
-    <t>TC_057</t>
-  </si>
-  <si>
-    <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
-  </si>
-  <si>
-    <t>TC_058</t>
-  </si>
-  <si>
-    <t>Verify that selecting option A keeps it selected without affecting option B.</t>
-  </si>
-  <si>
-    <t>TC_059</t>
-  </si>
-  <si>
-    <t>Verify, decedent died date is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_060</t>
-  </si>
-  <si>
-    <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
-  </si>
-  <si>
-    <t>TC_061</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
-  </si>
-  <si>
-    <t>TC_062</t>
-  </si>
-  <si>
-    <t>Verify that selecting option B keeps it selected without affecting option A.</t>
-  </si>
-  <si>
-    <t>TC_063</t>
-  </si>
-  <si>
-    <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
-  </si>
-  <si>
-    <t>TC_064</t>
-  </si>
-  <si>
-    <t>Verify, multiple beneficiaries can be selected.</t>
-  </si>
-  <si>
-    <t>TC_065</t>
-  </si>
-  <si>
-    <t>Verify, bene contacts in the table.</t>
-  </si>
-  <si>
-    <t>TC_066</t>
-  </si>
-  <si>
-    <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
-  </si>
-  <si>
-    <t>TC_067</t>
-  </si>
-  <si>
-    <t>Verify, on checking "Display all heirs on attachment".</t>
-  </si>
-  <si>
-    <t>TC_068</t>
-  </si>
-  <si>
-    <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
-  </si>
-  <si>
-    <t>TC_069</t>
-  </si>
-  <si>
-    <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
-  </si>
-  <si>
-    <t>TC_070</t>
-  </si>
-  <si>
-    <t>Verify fees section.</t>
-  </si>
-  <si>
-    <t>TC_071</t>
-  </si>
-  <si>
-    <t>Verify, attorney can be selected.</t>
-  </si>
-  <si>
-    <t>TC_072</t>
-  </si>
-  <si>
-    <t>Verify, information in decree of the register.</t>
-  </si>
-  <si>
-    <t>TC_073</t>
-  </si>
-  <si>
-    <t>TC_074</t>
-  </si>
-  <si>
-    <t>Reset the RW02 form</t>
-  </si>
-  <si>
-    <t>TC_075</t>
-  </si>
-  <si>
-    <t>probateFormsRW03.feature</t>
-  </si>
-  <si>
-    <t>TC_076</t>
-  </si>
-  <si>
-    <t>Verify county, estate and aka names are auto-populated on the form</t>
-  </si>
-  <si>
-    <t>TC_077</t>
-  </si>
-  <si>
-    <t>Verify, the auto-populated fields are not editable.</t>
-  </si>
-  <si>
-    <t>TC_078</t>
-  </si>
-  <si>
-    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
-  </si>
-  <si>
-    <t>TC_079</t>
-  </si>
-  <si>
-    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
-  </si>
-  <si>
-    <t>TC_080</t>
-  </si>
-  <si>
-    <t>Verify, names can be entered in witness fields.</t>
-  </si>
-  <si>
-    <t>TC_081</t>
-  </si>
-  <si>
-    <t>Verify, names updated from signature are reflected in witness names fields.</t>
-  </si>
-  <si>
-    <t>TC_082</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered in address, city, zip fields.</t>
-  </si>
-  <si>
-    <t>TC_083</t>
-  </si>
-  <si>
-    <t>Verify, form is auto saved.</t>
-  </si>
-  <si>
-    <t>TC_084</t>
-  </si>
-  <si>
-    <t>TC_085</t>
-  </si>
-  <si>
-    <t>Reset the RW03 form</t>
-  </si>
-  <si>
-    <t>TC_086</t>
-  </si>
-  <si>
-    <t>probateFormsRW04.feature</t>
   </si>
   <si>
     <t>TC_087</t>
@@ -2237,8 +2237,8 @@
   <sheetPr/>
   <dimension ref="A1:F180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3010,7 +3010,7 @@
         <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -3018,16 +3018,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -3035,16 +3035,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -3052,16 +3052,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -3069,16 +3069,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -3086,16 +3086,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -3103,16 +3103,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -3120,16 +3120,16 @@
     </row>
     <row r="52" ht="28" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -3137,16 +3137,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -3154,16 +3154,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -3171,16 +3171,16 @@
     </row>
     <row r="55" ht="28" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -3188,16 +3188,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -3205,16 +3205,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -3222,16 +3222,16 @@
     </row>
     <row r="58" ht="28" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -3239,16 +3239,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -3256,16 +3256,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -3273,16 +3273,16 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -3290,16 +3290,16 @@
     </row>
     <row r="62" ht="28" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3307,16 +3307,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3324,16 +3324,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3341,16 +3341,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3358,16 +3358,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3375,16 +3375,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3392,16 +3392,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3409,16 +3409,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3426,16 +3426,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3443,16 +3443,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3460,16 +3460,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3477,16 +3477,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3494,7 +3494,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>96</v>
@@ -3503,7 +3503,7 @@
         <v>92</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>8</v>
@@ -3511,16 +3511,16 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>8</v>
@@ -3528,10 +3528,10 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B76" s="7" t="s">
         <v>157</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>158</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>58</v>
@@ -3545,13 +3545,13 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C77" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>8</v>
@@ -3562,13 +3562,13 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C78" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>162</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>8</v>
@@ -3579,13 +3579,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C79" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>164</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>8</v>
@@ -3596,13 +3596,13 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>166</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>8</v>
@@ -3613,13 +3613,13 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C81" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>168</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>8</v>
@@ -3630,13 +3630,13 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C82" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>170</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>8</v>
@@ -3647,13 +3647,13 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C83" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>172</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>8</v>
@@ -3664,13 +3664,13 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>8</v>
@@ -3681,10 +3681,10 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>92</v>
@@ -3698,13 +3698,13 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C86" s="8" t="s">
         <v>176</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>177</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>8</v>
@@ -3715,16 +3715,16 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>8</v>
@@ -3735,13 +3735,13 @@
         <v>180</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>181</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>8</v>
@@ -3752,13 +3752,13 @@
         <v>182</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>183</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>8</v>
@@ -3769,13 +3769,13 @@
         <v>184</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>185</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>8</v>
@@ -3786,13 +3786,13 @@
         <v>186</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>187</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>8</v>
@@ -3803,13 +3803,13 @@
         <v>188</v>
       </c>
       <c r="B92" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D92" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>8</v>
@@ -3820,13 +3820,13 @@
         <v>189</v>
       </c>
       <c r="B93" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D93" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>8</v>
@@ -3837,13 +3837,13 @@
         <v>190</v>
       </c>
       <c r="B94" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D94" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>8</v>
@@ -3854,13 +3854,13 @@
         <v>191</v>
       </c>
       <c r="B95" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D95" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>8</v>
@@ -3871,13 +3871,13 @@
         <v>192</v>
       </c>
       <c r="B96" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D96" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>8</v>
@@ -3888,13 +3888,13 @@
         <v>193</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>92</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -3905,13 +3905,13 @@
         <v>194</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>195</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -3942,7 +3942,7 @@
         <v>197</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>8</v>
@@ -3959,7 +3959,7 @@
         <v>197</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>8</v>
@@ -3976,7 +3976,7 @@
         <v>197</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>8</v>
@@ -3993,7 +3993,7 @@
         <v>197</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>8</v>
@@ -4010,7 +4010,7 @@
         <v>197</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>8</v>
@@ -4027,7 +4027,7 @@
         <v>197</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>8</v>
@@ -4044,7 +4044,7 @@
         <v>197</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>8</v>
@@ -4078,7 +4078,7 @@
         <v>197</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>8</v>
@@ -4146,7 +4146,7 @@
         <v>212</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>8</v>
@@ -4163,7 +4163,7 @@
         <v>212</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>8</v>
@@ -4486,7 +4486,7 @@
         <v>245</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>8</v>
@@ -4741,7 +4741,7 @@
         <v>274</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>8</v>
@@ -4792,7 +4792,7 @@
         <v>274</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>8</v>
@@ -5316,7 +5316,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E25 D1:D8 D25:D44 D45:D74 E2:E8 E26:E43 E44:E51 E52:E74 F2:F3 D9:E24 D110:E123 D124:E180 D75:E109">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E74 E90 D1:D8 D74:D86 D87:D97 E2:E8 E75:E89 E91:E97 F2:F3 D43:E73 D9:E42 D98:E180">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
resolved issues of RW05 and RW06
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -620,52 +620,52 @@
     <t>probateFormsRW05.feature</t>
   </si>
   <si>
+    <t>TC_099</t>
+  </si>
+  <si>
+    <t>TC_100</t>
+  </si>
+  <si>
+    <t>TC_101</t>
+  </si>
+  <si>
+    <t>TC_102</t>
+  </si>
+  <si>
+    <t>TC_103</t>
+  </si>
+  <si>
+    <t>TC_104</t>
+  </si>
+  <si>
+    <t>TC_105</t>
+  </si>
+  <si>
+    <t>TC_106</t>
+  </si>
+  <si>
+    <t>Verify, on checking notary checkbox, notary section displays.</t>
+  </si>
+  <si>
+    <t>TC_107</t>
+  </si>
+  <si>
+    <t>TC_108</t>
+  </si>
+  <si>
+    <t>TC_109</t>
+  </si>
+  <si>
+    <t>Reset the RW05 form</t>
+  </si>
+  <si>
+    <t>TC_110</t>
+  </si>
+  <si>
+    <t>probateFormsRW06.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_099</t>
-  </si>
-  <si>
-    <t>TC_100</t>
-  </si>
-  <si>
-    <t>TC_101</t>
-  </si>
-  <si>
-    <t>TC_102</t>
-  </si>
-  <si>
-    <t>TC_103</t>
-  </si>
-  <si>
-    <t>TC_104</t>
-  </si>
-  <si>
-    <t>TC_105</t>
-  </si>
-  <si>
-    <t>TC_106</t>
-  </si>
-  <si>
-    <t>Verify, on checking notary checkbox, notary section displays.</t>
-  </si>
-  <si>
-    <t>TC_107</t>
-  </si>
-  <si>
-    <t>TC_108</t>
-  </si>
-  <si>
-    <t>TC_109</t>
-  </si>
-  <si>
-    <t>Reset the RW05 form</t>
-  </si>
-  <si>
-    <t>TC_110</t>
-  </si>
-  <si>
-    <t>probateFormsRW06.feature</t>
   </si>
   <si>
     <t>TC_111</t>
@@ -2237,8 +2237,8 @@
   <sheetPr/>
   <dimension ref="A1:F180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3928,7 +3928,7 @@
         <v>58</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>197</v>
+        <v>8</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -3936,7 +3936,7 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B100" s="7" t="s">
         <v>196</v>
@@ -3945,7 +3945,7 @@
         <v>104</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>197</v>
+        <v>8</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -3953,7 +3953,7 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B101" s="7" t="s">
         <v>196</v>
@@ -3962,7 +3962,7 @@
         <v>161</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>197</v>
+        <v>8</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -3970,7 +3970,7 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B102" s="7" t="s">
         <v>196</v>
@@ -3979,7 +3979,7 @@
         <v>163</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>197</v>
+        <v>8</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -3987,7 +3987,7 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B103" s="7" t="s">
         <v>196</v>
@@ -3996,7 +3996,7 @@
         <v>165</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>197</v>
+        <v>8</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -4004,7 +4004,7 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B104" s="7" t="s">
         <v>196</v>
@@ -4013,7 +4013,7 @@
         <v>167</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>197</v>
+        <v>8</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -4021,7 +4021,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B105" s="7" t="s">
         <v>196</v>
@@ -4030,7 +4030,7 @@
         <v>169</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>197</v>
+        <v>8</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -4038,7 +4038,7 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B106" s="7" t="s">
         <v>196</v>
@@ -4047,7 +4047,7 @@
         <v>171</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>197</v>
+        <v>8</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -4055,16 +4055,16 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B107" s="7" t="s">
         <v>196</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>197</v>
+        <v>8</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -4072,7 +4072,7 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B108" s="7" t="s">
         <v>196</v>
@@ -4081,7 +4081,7 @@
         <v>173</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>197</v>
+        <v>8</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -4089,7 +4089,7 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B109" s="7" t="s">
         <v>196</v>
@@ -4098,7 +4098,7 @@
         <v>92</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>197</v>
+        <v>8</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -4106,16 +4106,16 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B110" s="7" t="s">
         <v>196</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>197</v>
+        <v>8</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -4123,16 +4123,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B111" s="7" t="s">
         <v>211</v>
-      </c>
-      <c r="B111" s="7" t="s">
-        <v>212</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -4143,13 +4143,13 @@
         <v>213</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>159</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -4160,13 +4160,13 @@
         <v>214</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C113" s="7" t="s">
         <v>161</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -4177,13 +4177,13 @@
         <v>215</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>216</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -4194,13 +4194,13 @@
         <v>217</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>218</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -4211,13 +4211,13 @@
         <v>219</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>220</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -4228,13 +4228,13 @@
         <v>221</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>222</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -4245,13 +4245,13 @@
         <v>223</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>216</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -4262,13 +4262,13 @@
         <v>224</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>225</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4279,13 +4279,13 @@
         <v>226</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>227</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4296,13 +4296,13 @@
         <v>228</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>92</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4313,13 +4313,13 @@
         <v>229</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>230</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -5316,7 +5316,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E44 D1:D8 D40:D86 D99:D110 E2:E8 E40:E43 E45:E75 E76:E86 E99:E101 E102:E105 E106:E110 F2:F3 D9:E39 D87:E98 D124:E180 D111:E123">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E97 E98 D1:D8 D97:D110 D111:D121 E2:E8 E99:E110 E111:E113 E114:E121 F2:F3 D40:E86 D87:E96 D9:E39 D122:E180">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added the TC for the 08
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="334">
   <si>
     <t>ID</t>
   </si>
@@ -665,267 +665,267 @@
     <t>probateFormsRW06.feature</t>
   </si>
   <si>
+    <t>TC_111</t>
+  </si>
+  <si>
+    <t>TC_112</t>
+  </si>
+  <si>
+    <t>TC_113</t>
+  </si>
+  <si>
+    <t>Verify, form is repeated based on the number of contacts selected.</t>
+  </si>
+  <si>
+    <t>TC_114</t>
+  </si>
+  <si>
+    <t>Verify, corporate fiduciary selected is reflected in the corporate name field.</t>
+  </si>
+  <si>
+    <t>TC_115</t>
+  </si>
+  <si>
+    <t>Verify, details of the selected contact's is displayed in the block under it.</t>
+  </si>
+  <si>
+    <t>TC_116</t>
+  </si>
+  <si>
+    <t>Verify, on clicking signature of person, beneficiary contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_117</t>
+  </si>
+  <si>
+    <t>TC_118</t>
+  </si>
+  <si>
+    <t>Verify, contact details are correctly displayed on each page.</t>
+  </si>
+  <si>
+    <t>TC_119</t>
+  </si>
+  <si>
+    <t>Verify, date and reason text box fields are not same for each field.</t>
+  </si>
+  <si>
+    <t>TC_120</t>
+  </si>
+  <si>
+    <t>TC_121</t>
+  </si>
+  <si>
+    <t>Reset the RW06 form</t>
+  </si>
+  <si>
+    <t>TC_122</t>
+  </si>
+  <si>
+    <t>probateFormsRWxx.feature</t>
+  </si>
+  <si>
+    <t>TC_123</t>
+  </si>
+  <si>
+    <t>Verify that the county, estate name, and "Also Known As" (AKA) values are auto-populated from the selected estate.</t>
+  </si>
+  <si>
+    <t>TC_124</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered in all the text areas.</t>
+  </si>
+  <si>
+    <t>TC_125</t>
+  </si>
+  <si>
+    <t>Verify, the name entered in 1st text area is reflected in the signature.</t>
+  </si>
+  <si>
+    <t>TC_126</t>
+  </si>
+  <si>
+    <t>Verify that changes in the witness name field are reflected under the signature line and vice-versa.</t>
+  </si>
+  <si>
+    <t>TC_127</t>
+  </si>
+  <si>
+    <t>TC_128</t>
+  </si>
+  <si>
+    <t>Reset the RWxx form</t>
+  </si>
+  <si>
+    <t>TC_129</t>
+  </si>
+  <si>
+    <t>probateFormsRW07.feature</t>
+  </si>
+  <si>
+    <t>TC_130</t>
+  </si>
+  <si>
+    <t>Verify, county, estate and file number aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_131</t>
+  </si>
+  <si>
+    <t>TC_132</t>
+  </si>
+  <si>
+    <t>Verify, on checking use 4 digit checkbox, changes in file number</t>
+  </si>
+  <si>
+    <t>TC_133</t>
+  </si>
+  <si>
+    <t>Verify, on clicking bene address field, multiple beneficiaries can be selected.</t>
+  </si>
+  <si>
+    <t>TC_134</t>
+  </si>
+  <si>
+    <t>Verify, beneficiary name and address should be displayed in the form.</t>
+  </si>
+  <si>
+    <t>TC_135</t>
+  </si>
+  <si>
+    <t>Verify, decedent died and county is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_136</t>
+  </si>
+  <si>
+    <t>Verify, on clicking name fiduciary contact list is displayed and multiple users can be selected.</t>
+  </si>
+  <si>
+    <t>TC_137</t>
+  </si>
+  <si>
+    <t>Verify, these contacts are common for all the forms.</t>
+  </si>
+  <si>
+    <t>TC_138</t>
+  </si>
+  <si>
+    <t>Verify, date can be entered.</t>
+  </si>
+  <si>
+    <t>TC_139</t>
+  </si>
+  <si>
+    <t>Verify, registrars address is auto fetched and is editable.</t>
+  </si>
+  <si>
+    <t>TC_140</t>
+  </si>
+  <si>
+    <t>Verify, corporate fiduciary type of contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_141</t>
+  </si>
+  <si>
+    <t>Verify, based on capacity contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_142</t>
+  </si>
+  <si>
+    <t>Verify, selection is cleared on clicking clear selection button.</t>
+  </si>
+  <si>
+    <t>TC_143</t>
+  </si>
+  <si>
+    <t>Reset the RW07 form</t>
+  </si>
+  <si>
+    <t>TC_144</t>
+  </si>
+  <si>
+    <t>probateFormsRW08.feature</t>
+  </si>
+  <si>
+    <t>TC_145</t>
+  </si>
+  <si>
+    <t>TC_146</t>
+  </si>
+  <si>
+    <t>TC_147</t>
+  </si>
+  <si>
+    <t>Verify, Will number and other dates can be entered in correct format.</t>
+  </si>
+  <si>
+    <t>TC_148</t>
+  </si>
+  <si>
+    <t>Verify, checkboxes for file no field.</t>
+  </si>
+  <si>
+    <t>TC_149</t>
+  </si>
+  <si>
+    <t>TC_150</t>
+  </si>
+  <si>
+    <t>Verify, the beneficiaries selected beyond 6 are displayed on the attachment.</t>
+  </si>
+  <si>
+    <t>TC_151</t>
+  </si>
+  <si>
+    <t>Verify, count is correctly displayed.</t>
+  </si>
+  <si>
+    <t>TC_152</t>
+  </si>
+  <si>
+    <t>Verify, on clicking "Display ALL beneficiary on attachment" checkbox all the contacts are transferred on attachment.</t>
+  </si>
+  <si>
+    <t>TC_153</t>
+  </si>
+  <si>
+    <t>TC_154</t>
+  </si>
+  <si>
+    <t>TC_155</t>
+  </si>
+  <si>
+    <t>Verify, these 2 sections are common for RW07, RW08 and anything updated is reflected in all the forms.</t>
+  </si>
+  <si>
+    <t>TC_156</t>
+  </si>
+  <si>
+    <t>TC_157</t>
+  </si>
+  <si>
+    <t>TC_158</t>
+  </si>
+  <si>
+    <t>TC_159</t>
+  </si>
+  <si>
+    <t>Reset the RW08 form</t>
+  </si>
+  <si>
+    <t>TC_160</t>
+  </si>
+  <si>
+    <t>probateFormsRW10.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>TC_111</t>
-  </si>
-  <si>
-    <t>TC_112</t>
-  </si>
-  <si>
-    <t>TC_113</t>
-  </si>
-  <si>
-    <t>Verify, form is repeated based on the number of contacts selected.</t>
-  </si>
-  <si>
-    <t>TC_114</t>
-  </si>
-  <si>
-    <t>Verify, corporate fiduciary selected is reflected in the corporate name field.</t>
-  </si>
-  <si>
-    <t>TC_115</t>
-  </si>
-  <si>
-    <t>Verify, details of the selected contact's is displayed in the block under it.</t>
-  </si>
-  <si>
-    <t>TC_116</t>
-  </si>
-  <si>
-    <t>Verify, on clicking signature of person, beneficiary contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_117</t>
-  </si>
-  <si>
-    <t>TC_118</t>
-  </si>
-  <si>
-    <t>Verify, contact details are correctly displayed on each page.</t>
-  </si>
-  <si>
-    <t>TC_119</t>
-  </si>
-  <si>
-    <t>Verify, date and reason text box fields are not same for each field.</t>
-  </si>
-  <si>
-    <t>TC_120</t>
-  </si>
-  <si>
-    <t>TC_121</t>
-  </si>
-  <si>
-    <t>Reset the RW06 form</t>
-  </si>
-  <si>
-    <t>TC_122</t>
-  </si>
-  <si>
-    <t>probateFormsRWxx.feature</t>
-  </si>
-  <si>
-    <t>TC_123</t>
-  </si>
-  <si>
-    <t>Verify that the county, estate name, and "Also Known As" (AKA) values are auto-populated from the selected estate.</t>
-  </si>
-  <si>
-    <t>TC_124</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered in all the text areas.</t>
-  </si>
-  <si>
-    <t>TC_125</t>
-  </si>
-  <si>
-    <t>Verify, the name entered in 1st text area is reflected in the signature.</t>
-  </si>
-  <si>
-    <t>TC_126</t>
-  </si>
-  <si>
-    <t>Verify that changes in the witness name field are reflected under the signature line and vice-versa.</t>
-  </si>
-  <si>
-    <t>TC_127</t>
-  </si>
-  <si>
-    <t>TC_128</t>
-  </si>
-  <si>
-    <t>Reset the RWxx form</t>
-  </si>
-  <si>
-    <t>TC_129</t>
-  </si>
-  <si>
-    <t>probateFormsRW07.feature</t>
-  </si>
-  <si>
-    <t>TC_130</t>
-  </si>
-  <si>
-    <t>Verify, county, estate and file number aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_131</t>
-  </si>
-  <si>
-    <t>TC_132</t>
-  </si>
-  <si>
-    <t>Verify, on checking use 4 digit checkbox, changes in file number</t>
-  </si>
-  <si>
-    <t>TC_133</t>
-  </si>
-  <si>
-    <t>Verify, on clicking bene address field, multiple beneficiaries can be selected.</t>
-  </si>
-  <si>
-    <t>TC_134</t>
-  </si>
-  <si>
-    <t>Verify, beneficiary name and address should be displayed in the form.</t>
-  </si>
-  <si>
-    <t>TC_135</t>
-  </si>
-  <si>
-    <t>Verify, decedent died and county is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_136</t>
-  </si>
-  <si>
-    <t>Verify, on clicking name fiduciary contact list is displayed and multiple users can be selected.</t>
-  </si>
-  <si>
-    <t>TC_137</t>
-  </si>
-  <si>
-    <t>Verify, these contacts are common for all the forms.</t>
-  </si>
-  <si>
-    <t>TC_138</t>
-  </si>
-  <si>
-    <t>Verify, date can be entered.</t>
-  </si>
-  <si>
-    <t>TC_139</t>
-  </si>
-  <si>
-    <t>Verify, registrars address is auto fetched and is editable.</t>
-  </si>
-  <si>
-    <t>TC_140</t>
-  </si>
-  <si>
-    <t>Verify, corporate fiduciary type of contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_141</t>
-  </si>
-  <si>
-    <t>Verify, based on capacity contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_142</t>
-  </si>
-  <si>
-    <t>Verify, selection is cleared on clicking clear selection button.</t>
-  </si>
-  <si>
-    <t>TC_143</t>
-  </si>
-  <si>
-    <t>Reset the RW07 form</t>
-  </si>
-  <si>
-    <t>TC_144</t>
-  </si>
-  <si>
-    <t>probateFormsRW08.feature</t>
-  </si>
-  <si>
-    <t>TC_145</t>
-  </si>
-  <si>
-    <t>TC_146</t>
-  </si>
-  <si>
-    <t>TC_147</t>
-  </si>
-  <si>
-    <t>Verify, Will number and other dates can be entered in correct format.</t>
-  </si>
-  <si>
-    <t>TC_148</t>
-  </si>
-  <si>
-    <t>Verify, checkboxes for file no field.</t>
-  </si>
-  <si>
-    <t>TC_149</t>
-  </si>
-  <si>
-    <t>TC_150</t>
-  </si>
-  <si>
-    <t>Verify, the beneficiaries selected beyond 6 are displayed on the attachment.</t>
-  </si>
-  <si>
-    <t>TC_151</t>
-  </si>
-  <si>
-    <t>Verify, count is correctly displayed.</t>
-  </si>
-  <si>
-    <t>TC_152</t>
-  </si>
-  <si>
-    <t>Verify, on clicking "Display ALL beneficiary on attachment" checkbox all the contacts are transferred on attachment.</t>
-  </si>
-  <si>
-    <t>TC_153</t>
-  </si>
-  <si>
-    <t>TC_154</t>
-  </si>
-  <si>
-    <t>TC_155</t>
-  </si>
-  <si>
-    <t>Verify, these 2 sections are common for RW07, RW08 and anything updated is reflected in all the forms.</t>
-  </si>
-  <si>
-    <t>TC_156</t>
-  </si>
-  <si>
-    <t>TC_157</t>
-  </si>
-  <si>
-    <t>TC_158</t>
-  </si>
-  <si>
-    <t>TC_159</t>
-  </si>
-  <si>
-    <t>Reset the RW08 form</t>
-  </si>
-  <si>
-    <t>TC_160</t>
-  </si>
-  <si>
-    <t>probateFormsRW10.feature</t>
-  </si>
-  <si>
     <t>Verify, title of the form and if county is fetched from the decedent info.</t>
   </si>
   <si>
@@ -1023,6 +1023,9 @@
   </si>
   <si>
     <t>TC_178</t>
+  </si>
+  <si>
+    <t>TC_179</t>
   </si>
   <si>
     <t>Reset the RW10 form</t>
@@ -2235,10 +2238,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F180"/>
+  <dimension ref="A1:F181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161:D181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -4132,7 +4135,7 @@
         <v>58</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -4140,7 +4143,7 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B112" s="7" t="s">
         <v>211</v>
@@ -4149,7 +4152,7 @@
         <v>159</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -4157,7 +4160,7 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B113" s="7" t="s">
         <v>211</v>
@@ -4166,7 +4169,7 @@
         <v>161</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -4174,16 +4177,16 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B114" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -4191,16 +4194,16 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -4208,16 +4211,16 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B116" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -4225,16 +4228,16 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B117" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -4242,16 +4245,16 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B118" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -4259,16 +4262,16 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B119" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4276,16 +4279,16 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B120" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4293,7 +4296,7 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B121" s="7" t="s">
         <v>211</v>
@@ -4302,7 +4305,7 @@
         <v>92</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4310,16 +4313,16 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B122" s="7" t="s">
         <v>211</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4327,10 +4330,10 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B123" s="7" t="s">
         <v>231</v>
-      </c>
-      <c r="B123" s="7" t="s">
-        <v>232</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>58</v>
@@ -4344,13 +4347,13 @@
     </row>
     <row r="124" ht="28" spans="1:5">
       <c r="A124" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C124" s="9" t="s">
         <v>233</v>
-      </c>
-      <c r="B124" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C124" s="9" t="s">
-        <v>234</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>8</v>
@@ -4361,13 +4364,13 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C125" s="7" t="s">
         <v>235</v>
-      </c>
-      <c r="B125" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C125" s="7" t="s">
-        <v>236</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>8</v>
@@ -4378,13 +4381,13 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C126" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="B126" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C126" s="7" t="s">
-        <v>238</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>8</v>
@@ -4395,13 +4398,13 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C127" s="7" t="s">
         <v>239</v>
-      </c>
-      <c r="B127" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>240</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>8</v>
@@ -4412,10 +4415,10 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C128" s="8" t="s">
         <v>92</v>
@@ -4429,13 +4432,13 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C129" s="7" t="s">
         <v>242</v>
-      </c>
-      <c r="B129" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C129" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>8</v>
@@ -4446,10 +4449,10 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B130" s="7" t="s">
         <v>244</v>
-      </c>
-      <c r="B130" s="7" t="s">
-        <v>245</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>58</v>
@@ -4463,13 +4466,13 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C131" s="7" t="s">
         <v>246</v>
-      </c>
-      <c r="B131" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C131" s="7" t="s">
-        <v>247</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>8</v>
@@ -4480,10 +4483,10 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C132" s="7" t="s">
         <v>106</v>
@@ -4497,13 +4500,13 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C133" s="7" t="s">
         <v>249</v>
-      </c>
-      <c r="B133" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C133" s="7" t="s">
-        <v>250</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>8</v>
@@ -4514,13 +4517,13 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C134" s="7" t="s">
         <v>251</v>
-      </c>
-      <c r="B134" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C134" s="7" t="s">
-        <v>252</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>8</v>
@@ -4531,13 +4534,13 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C135" s="7" t="s">
         <v>253</v>
-      </c>
-      <c r="B135" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C135" s="7" t="s">
-        <v>254</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>8</v>
@@ -4548,13 +4551,13 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C136" s="7" t="s">
         <v>255</v>
-      </c>
-      <c r="B136" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C136" s="7" t="s">
-        <v>256</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>8</v>
@@ -4565,13 +4568,13 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C137" s="7" t="s">
         <v>257</v>
-      </c>
-      <c r="B137" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C137" s="7" t="s">
-        <v>258</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>8</v>
@@ -4582,13 +4585,13 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C138" s="7" t="s">
         <v>259</v>
-      </c>
-      <c r="B138" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C138" s="7" t="s">
-        <v>260</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>8</v>
@@ -4599,13 +4602,13 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C139" s="7" t="s">
         <v>261</v>
-      </c>
-      <c r="B139" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C139" s="7" t="s">
-        <v>262</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>8</v>
@@ -4616,13 +4619,13 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C140" s="7" t="s">
         <v>263</v>
-      </c>
-      <c r="B140" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C140" s="7" t="s">
-        <v>264</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>8</v>
@@ -4633,13 +4636,13 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C141" s="7" t="s">
         <v>265</v>
-      </c>
-      <c r="B141" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C141" s="7" t="s">
-        <v>266</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>8</v>
@@ -4650,13 +4653,13 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C142" s="7" t="s">
         <v>267</v>
-      </c>
-      <c r="B142" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C142" s="7" t="s">
-        <v>268</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>8</v>
@@ -4667,13 +4670,13 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C143" s="7" t="s">
         <v>269</v>
-      </c>
-      <c r="B143" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C143" s="7" t="s">
-        <v>270</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>8</v>
@@ -4684,13 +4687,13 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C144" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="B144" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C144" s="7" t="s">
-        <v>272</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>8</v>
@@ -4701,10 +4704,10 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B145" s="7" t="s">
         <v>273</v>
-      </c>
-      <c r="B145" s="7" t="s">
-        <v>274</v>
       </c>
       <c r="C145" s="7" t="s">
         <v>58</v>
@@ -4718,13 +4721,13 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C146" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>8</v>
@@ -4735,10 +4738,10 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C147" s="7" t="s">
         <v>106</v>
@@ -4752,13 +4755,13 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B148" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C148" s="7" t="s">
         <v>277</v>
-      </c>
-      <c r="B148" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C148" s="7" t="s">
-        <v>278</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>8</v>
@@ -4769,13 +4772,13 @@
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C149" s="7" t="s">
         <v>279</v>
-      </c>
-      <c r="B149" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C149" s="7" t="s">
-        <v>280</v>
       </c>
       <c r="D149" s="3" t="s">
         <v>8</v>
@@ -4786,10 +4789,10 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C150" s="7" t="s">
         <v>136</v>
@@ -4803,13 +4806,13 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C151" s="7" t="s">
         <v>282</v>
-      </c>
-      <c r="B151" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C151" s="7" t="s">
-        <v>283</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>8</v>
@@ -4820,13 +4823,13 @@
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C152" s="7" t="s">
         <v>284</v>
-      </c>
-      <c r="B152" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C152" s="7" t="s">
-        <v>285</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>8</v>
@@ -4837,13 +4840,13 @@
     </row>
     <row r="153" ht="28" spans="1:5">
       <c r="A153" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C153" s="9" t="s">
         <v>286</v>
-      </c>
-      <c r="B153" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C153" s="9" t="s">
-        <v>287</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>8</v>
@@ -4854,13 +4857,13 @@
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C154" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>8</v>
@@ -4871,13 +4874,13 @@
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>8</v>
@@ -4888,13 +4891,13 @@
     </row>
     <row r="156" ht="28" spans="1:5">
       <c r="A156" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C156" s="9" t="s">
         <v>290</v>
-      </c>
-      <c r="B156" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C156" s="9" t="s">
-        <v>291</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>8</v>
@@ -4905,10 +4908,10 @@
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C157" s="7" t="s">
         <v>92</v>
@@ -4922,13 +4925,13 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C158" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D158" s="3" t="s">
         <v>8</v>
@@ -4939,10 +4942,10 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C159" s="8" t="s">
         <v>92</v>
@@ -4956,13 +4959,13 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B160" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C160" s="7" t="s">
         <v>295</v>
-      </c>
-      <c r="B160" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C160" s="7" t="s">
-        <v>296</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>8</v>
@@ -4973,16 +4976,16 @@
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B161" s="7" t="s">
         <v>297</v>
-      </c>
-      <c r="B161" s="7" t="s">
-        <v>298</v>
       </c>
       <c r="C161" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>8</v>
@@ -4990,16 +4993,16 @@
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B162" s="7" t="s">
         <v>297</v>
-      </c>
-      <c r="B162" s="7" t="s">
-        <v>298</v>
       </c>
       <c r="C162" s="7" t="s">
         <v>299</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>8</v>
@@ -5010,13 +5013,13 @@
         <v>300</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C163" s="7" t="s">
         <v>301</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>8</v>
@@ -5027,13 +5030,13 @@
         <v>302</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C164" s="7" t="s">
         <v>303</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>8</v>
@@ -5044,13 +5047,13 @@
         <v>304</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C165" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="D165" s="5" t="s">
-        <v>8</v>
+      <c r="D165" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>8</v>
@@ -5061,13 +5064,13 @@
         <v>306</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C166" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="D166" s="5" t="s">
-        <v>8</v>
+      <c r="D166" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>8</v>
@@ -5078,13 +5081,13 @@
         <v>308</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C167" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="D167" s="5" t="s">
-        <v>8</v>
+      <c r="D167" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>8</v>
@@ -5095,13 +5098,13 @@
         <v>310</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C168" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="D168" s="5" t="s">
-        <v>8</v>
+      <c r="D168" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>8</v>
@@ -5112,13 +5115,13 @@
         <v>312</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C169" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="D169" s="5" t="s">
-        <v>8</v>
+      <c r="D169" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>8</v>
@@ -5129,13 +5132,13 @@
         <v>314</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C170" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="D170" s="5" t="s">
-        <v>8</v>
+      <c r="D170" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>8</v>
@@ -5146,13 +5149,13 @@
         <v>316</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C171" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="D171" s="5" t="s">
-        <v>8</v>
+      <c r="D171" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>8</v>
@@ -5163,13 +5166,13 @@
         <v>318</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C172" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="D172" s="5" t="s">
-        <v>8</v>
+      <c r="D172" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>8</v>
@@ -5180,13 +5183,13 @@
         <v>320</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C173" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="D173" s="5" t="s">
-        <v>8</v>
+      <c r="D173" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>8</v>
@@ -5197,13 +5200,13 @@
         <v>322</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C174" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="D174" s="5" t="s">
-        <v>8</v>
+      <c r="D174" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>8</v>
@@ -5214,13 +5217,13 @@
         <v>324</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C175" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="D175" s="5" t="s">
-        <v>8</v>
+      <c r="D175" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>8</v>
@@ -5231,13 +5234,13 @@
         <v>326</v>
       </c>
       <c r="B176" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C176" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="D176" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="C176" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="D176" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>8</v>
@@ -5248,13 +5251,13 @@
         <v>327</v>
       </c>
       <c r="B177" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C177" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D177" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="C177" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="D177" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>8</v>
@@ -5265,13 +5268,13 @@
         <v>328</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C178" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="D178" s="5" t="s">
-        <v>8</v>
+      <c r="D178" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>8</v>
@@ -5282,13 +5285,13 @@
         <v>330</v>
       </c>
       <c r="B179" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C179" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D179" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="C179" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="D179" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>8</v>
@@ -5299,15 +5302,32 @@
         <v>331</v>
       </c>
       <c r="B180" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C180" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="D180" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="C180" s="7" t="s">
+      <c r="E180" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="D180" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E180" s="3" t="s">
+      <c r="B181" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C181" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E181" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5316,7 +5336,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E97 E98 D1:D8 D97:D110 D111:D121 E2:E8 E99:E110 E111:E113 E114:E121 F2:F3 D40:E86 D87:E96 D9:E39 D122:E180">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D160:E160 D1:D8 D138:D159 D161:D181 E2:E8 E138:E141 E142:E159 E161:E162 E163:E177 E178:E179 E180:E181 F2:F3 D117:E137 D84:E116 D41:E83 D9:E40">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
code changes done for UAT copy
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -206,6 +206,9 @@
     <t>Open Estate</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_026</t>
   </si>
   <si>
@@ -663,9 +666,6 @@
   </si>
   <si>
     <t>probateFormsRW06.feature</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>TC_111</t>
@@ -2237,8 +2237,8 @@
   <sheetPr/>
   <dimension ref="A1:F180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:D180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2687,7 +2687,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>8</v>
@@ -2695,16 +2695,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>8</v>
@@ -2712,16 +2712,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>8</v>
@@ -2729,16 +2729,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>8</v>
@@ -2746,16 +2746,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>8</v>
@@ -2763,16 +2763,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>8</v>
@@ -2780,16 +2780,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>8</v>
@@ -2797,16 +2797,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>8</v>
@@ -2814,16 +2814,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>8</v>
@@ -2831,16 +2831,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>8</v>
@@ -2848,16 +2848,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>8</v>
@@ -2865,16 +2865,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>8</v>
@@ -2882,16 +2882,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>8</v>
@@ -2899,16 +2899,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>8</v>
@@ -2916,16 +2916,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>8</v>
@@ -2933,16 +2933,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>8</v>
@@ -2950,16 +2950,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>8</v>
@@ -2967,16 +2967,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>8</v>
@@ -2984,16 +2984,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>8</v>
@@ -3001,16 +3001,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -3018,16 +3018,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="C46" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -3035,16 +3035,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -3052,16 +3052,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -3069,16 +3069,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -3086,16 +3086,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -3103,16 +3103,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -3120,16 +3120,16 @@
     </row>
     <row r="52" ht="28" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -3137,16 +3137,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -3154,16 +3154,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -3171,16 +3171,16 @@
     </row>
     <row r="55" ht="28" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -3188,16 +3188,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -3205,16 +3205,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -3222,16 +3222,16 @@
     </row>
     <row r="58" ht="28" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -3239,16 +3239,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -3256,16 +3256,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -3273,16 +3273,16 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -3290,16 +3290,16 @@
     </row>
     <row r="62" ht="28" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3307,16 +3307,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3324,16 +3324,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3341,16 +3341,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3358,16 +3358,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3375,16 +3375,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3392,16 +3392,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3409,16 +3409,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3426,16 +3426,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3443,16 +3443,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3460,16 +3460,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3477,16 +3477,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3494,16 +3494,16 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>8</v>
@@ -3511,16 +3511,16 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>8</v>
@@ -3528,16 +3528,16 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>8</v>
@@ -3545,16 +3545,16 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B77" s="7" t="s">
-        <v>157</v>
-      </c>
       <c r="C77" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>8</v>
@@ -3562,16 +3562,16 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>8</v>
@@ -3579,16 +3579,16 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>8</v>
@@ -3596,16 +3596,16 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>8</v>
@@ -3613,16 +3613,16 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>8</v>
@@ -3630,16 +3630,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>8</v>
@@ -3647,16 +3647,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>8</v>
@@ -3664,16 +3664,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>8</v>
@@ -3681,16 +3681,16 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>8</v>
@@ -3698,16 +3698,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>8</v>
@@ -3715,16 +3715,16 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>8</v>
@@ -3732,16 +3732,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>178</v>
-      </c>
       <c r="C88" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>8</v>
@@ -3749,16 +3749,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>8</v>
@@ -3766,16 +3766,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>8</v>
@@ -3783,16 +3783,16 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>8</v>
@@ -3800,16 +3800,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>8</v>
@@ -3817,16 +3817,16 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>8</v>
@@ -3834,16 +3834,16 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>8</v>
@@ -3851,16 +3851,16 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>8</v>
@@ -3868,16 +3868,16 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>8</v>
@@ -3885,16 +3885,16 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -3902,16 +3902,16 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -3919,16 +3919,16 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -3936,16 +3936,16 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B100" s="7" t="s">
-        <v>196</v>
-      </c>
       <c r="C100" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -3953,16 +3953,16 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -3970,16 +3970,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -3987,16 +3987,16 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -4004,16 +4004,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -4021,16 +4021,16 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -4038,16 +4038,16 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -4055,16 +4055,16 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -4072,16 +4072,16 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -4089,16 +4089,16 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -4106,16 +4106,16 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -4123,16 +4123,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -4143,13 +4143,13 @@
         <v>213</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -4160,13 +4160,13 @@
         <v>214</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -4177,13 +4177,13 @@
         <v>215</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>216</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -4194,13 +4194,13 @@
         <v>217</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>218</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -4211,13 +4211,13 @@
         <v>219</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>220</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -4228,13 +4228,13 @@
         <v>221</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>222</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -4245,13 +4245,13 @@
         <v>223</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>216</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -4262,13 +4262,13 @@
         <v>224</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>225</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4279,13 +4279,13 @@
         <v>226</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>227</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4296,13 +4296,13 @@
         <v>228</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4313,13 +4313,13 @@
         <v>229</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>230</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4336,7 +4336,7 @@
         <v>58</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>8</v>
@@ -4353,7 +4353,7 @@
         <v>234</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>8</v>
@@ -4370,7 +4370,7 @@
         <v>236</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>8</v>
@@ -4387,7 +4387,7 @@
         <v>238</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>8</v>
@@ -4404,7 +4404,7 @@
         <v>240</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>8</v>
@@ -4418,10 +4418,10 @@
         <v>232</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>8</v>
@@ -4438,7 +4438,7 @@
         <v>243</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>8</v>
@@ -4455,7 +4455,7 @@
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>8</v>
@@ -4472,7 +4472,7 @@
         <v>247</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -4486,10 +4486,10 @@
         <v>245</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>8</v>
@@ -4506,7 +4506,7 @@
         <v>250</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>8</v>
@@ -4523,7 +4523,7 @@
         <v>252</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -4540,7 +4540,7 @@
         <v>254</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -4557,7 +4557,7 @@
         <v>256</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -4574,7 +4574,7 @@
         <v>258</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -4591,7 +4591,7 @@
         <v>260</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>8</v>
@@ -4608,7 +4608,7 @@
         <v>262</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>8</v>
@@ -4625,7 +4625,7 @@
         <v>264</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>8</v>
@@ -4642,7 +4642,7 @@
         <v>266</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -4659,7 +4659,7 @@
         <v>268</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -4676,7 +4676,7 @@
         <v>270</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -4693,7 +4693,7 @@
         <v>272</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>8</v>
@@ -4710,7 +4710,7 @@
         <v>58</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>8</v>
@@ -4727,7 +4727,7 @@
         <v>247</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>8</v>
@@ -4741,10 +4741,10 @@
         <v>274</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>8</v>
@@ -4761,7 +4761,7 @@
         <v>278</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>8</v>
@@ -4778,7 +4778,7 @@
         <v>280</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>8</v>
@@ -4792,10 +4792,10 @@
         <v>274</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>8</v>
@@ -4812,7 +4812,7 @@
         <v>283</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>8</v>
@@ -4829,7 +4829,7 @@
         <v>285</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>8</v>
@@ -4846,7 +4846,7 @@
         <v>287</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>8</v>
@@ -4863,7 +4863,7 @@
         <v>266</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>8</v>
@@ -4880,7 +4880,7 @@
         <v>268</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>8</v>
@@ -4897,7 +4897,7 @@
         <v>291</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>8</v>
@@ -4911,10 +4911,10 @@
         <v>274</v>
       </c>
       <c r="C157" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>8</v>
@@ -4931,7 +4931,7 @@
         <v>270</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>8</v>
@@ -4945,10 +4945,10 @@
         <v>274</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>8</v>
@@ -4965,7 +4965,7 @@
         <v>296</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>8</v>
@@ -4982,7 +4982,7 @@
         <v>58</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>8</v>
@@ -4999,7 +4999,7 @@
         <v>299</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>8</v>
@@ -5016,7 +5016,7 @@
         <v>301</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>8</v>
@@ -5033,7 +5033,7 @@
         <v>303</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>8</v>
@@ -5049,8 +5049,8 @@
       <c r="C165" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="D165" s="5" t="s">
-        <v>8</v>
+      <c r="D165" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>8</v>
@@ -5066,8 +5066,8 @@
       <c r="C166" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="D166" s="5" t="s">
-        <v>8</v>
+      <c r="D166" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>8</v>
@@ -5083,8 +5083,8 @@
       <c r="C167" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="D167" s="5" t="s">
-        <v>8</v>
+      <c r="D167" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>8</v>
@@ -5100,8 +5100,8 @@
       <c r="C168" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="D168" s="5" t="s">
-        <v>8</v>
+      <c r="D168" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>8</v>
@@ -5117,8 +5117,8 @@
       <c r="C169" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="D169" s="5" t="s">
-        <v>8</v>
+      <c r="D169" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>8</v>
@@ -5134,8 +5134,8 @@
       <c r="C170" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="D170" s="5" t="s">
-        <v>8</v>
+      <c r="D170" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>8</v>
@@ -5151,8 +5151,8 @@
       <c r="C171" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="D171" s="5" t="s">
-        <v>8</v>
+      <c r="D171" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>8</v>
@@ -5168,8 +5168,8 @@
       <c r="C172" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="D172" s="5" t="s">
-        <v>8</v>
+      <c r="D172" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>8</v>
@@ -5185,8 +5185,8 @@
       <c r="C173" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="D173" s="5" t="s">
-        <v>8</v>
+      <c r="D173" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>8</v>
@@ -5202,8 +5202,8 @@
       <c r="C174" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="D174" s="5" t="s">
-        <v>8</v>
+      <c r="D174" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>8</v>
@@ -5219,8 +5219,8 @@
       <c r="C175" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="D175" s="5" t="s">
-        <v>8</v>
+      <c r="D175" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>8</v>
@@ -5236,8 +5236,8 @@
       <c r="C176" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="D176" s="5" t="s">
-        <v>8</v>
+      <c r="D176" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>8</v>
@@ -5253,8 +5253,8 @@
       <c r="C177" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="D177" s="5" t="s">
-        <v>8</v>
+      <c r="D177" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>8</v>
@@ -5270,8 +5270,8 @@
       <c r="C178" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="D178" s="5" t="s">
-        <v>8</v>
+      <c r="D178" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>8</v>
@@ -5287,8 +5287,8 @@
       <c r="C179" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="D179" s="5" t="s">
-        <v>8</v>
+      <c r="D179" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>8</v>
@@ -5304,8 +5304,8 @@
       <c r="C180" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="D180" s="5" t="s">
-        <v>8</v>
+      <c r="D180" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>8</v>
@@ -5316,7 +5316,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E97 E98 D1:D8 D97:D110 D111:D121 E2:E8 E99:E110 E111:E113 E114:E121 F2:F3 D40:E86 D87:E96 D9:E39 D122:E180">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D26:D180 E2:E8 E26:E27 E28:E49 E50:E75 E76:E85 E86:E180 F2:F3 D9:E20 D21:E25">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
resolved issues on UAT copy
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -2237,8 +2237,8 @@
   <sheetPr/>
   <dimension ref="A1:F180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:D180"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="C185" sqref="C185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -5316,7 +5316,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D26:D180 E2:E8 E26:E27 E28:E49 E50:E75 E76:E85 E86:E180 F2:F3 D9:E20 D21:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E26 D1:D8 D26:D180 E2:E8 E27:E180 F2:F3 D9:E23 D24:E25">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added variables for RW02 and RW07
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -320,6 +320,9 @@
     <t>probateFormsRW02.feature</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_045</t>
   </si>
   <si>
@@ -762,9 +765,6 @@
   </si>
   <si>
     <t>probateFormsRW07.feature</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>TC_130</t>
@@ -2240,8 +2240,8 @@
   <sheetPr/>
   <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3013,7 +3013,7 @@
         <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -3021,16 +3021,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -3038,16 +3038,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -3055,16 +3055,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -3072,16 +3072,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -3089,16 +3089,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -3106,16 +3106,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -3123,16 +3123,16 @@
     </row>
     <row r="52" ht="28" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -3140,16 +3140,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -3157,16 +3157,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -3174,16 +3174,16 @@
     </row>
     <row r="55" ht="28" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -3191,16 +3191,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -3208,16 +3208,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -3225,16 +3225,16 @@
     </row>
     <row r="58" ht="28" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -3242,16 +3242,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -3259,16 +3259,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -3276,16 +3276,16 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -3293,16 +3293,16 @@
     </row>
     <row r="62" ht="28" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3310,16 +3310,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3327,16 +3327,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3344,16 +3344,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3361,16 +3361,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3378,16 +3378,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3395,16 +3395,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3412,16 +3412,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3429,16 +3429,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3446,16 +3446,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3463,16 +3463,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3480,16 +3480,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3497,7 +3497,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>96</v>
@@ -3506,7 +3506,7 @@
         <v>92</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>8</v>
@@ -3514,16 +3514,16 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>8</v>
@@ -3531,10 +3531,10 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>58</v>
@@ -3548,13 +3548,13 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B77" s="7" t="s">
-        <v>157</v>
-      </c>
       <c r="C77" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>8</v>
@@ -3565,13 +3565,13 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>8</v>
@@ -3582,13 +3582,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>8</v>
@@ -3599,13 +3599,13 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>8</v>
@@ -3616,13 +3616,13 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>8</v>
@@ -3633,13 +3633,13 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>8</v>
@@ -3650,13 +3650,13 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>8</v>
@@ -3667,13 +3667,13 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>8</v>
@@ -3684,10 +3684,10 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>92</v>
@@ -3701,13 +3701,13 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>8</v>
@@ -3718,10 +3718,10 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>58</v>
@@ -3735,13 +3735,13 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>178</v>
-      </c>
       <c r="C88" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>8</v>
@@ -3752,13 +3752,13 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>8</v>
@@ -3769,13 +3769,13 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>8</v>
@@ -3786,13 +3786,13 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>8</v>
@@ -3803,13 +3803,13 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>8</v>
@@ -3820,13 +3820,13 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>8</v>
@@ -3837,13 +3837,13 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>8</v>
@@ -3854,13 +3854,13 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>8</v>
@@ -3871,13 +3871,13 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>8</v>
@@ -3888,10 +3888,10 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>92</v>
@@ -3905,13 +3905,13 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>8</v>
@@ -3922,10 +3922,10 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>58</v>
@@ -3939,13 +3939,13 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B100" s="7" t="s">
-        <v>196</v>
-      </c>
       <c r="C100" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>8</v>
@@ -3956,13 +3956,13 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>8</v>
@@ -3973,13 +3973,13 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>8</v>
@@ -3990,13 +3990,13 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>8</v>
@@ -4007,13 +4007,13 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>8</v>
@@ -4024,13 +4024,13 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>8</v>
@@ -4041,13 +4041,13 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>8</v>
@@ -4058,13 +4058,13 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>8</v>
@@ -4075,13 +4075,13 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>8</v>
@@ -4092,10 +4092,10 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>92</v>
@@ -4109,13 +4109,13 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>8</v>
@@ -4126,10 +4126,10 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>58</v>
@@ -4143,13 +4143,13 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B112" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B112" s="7" t="s">
-        <v>211</v>
-      </c>
       <c r="C112" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>8</v>
@@ -4160,13 +4160,13 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>8</v>
@@ -4177,13 +4177,13 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>8</v>
@@ -4194,13 +4194,13 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>8</v>
@@ -4211,13 +4211,13 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>8</v>
@@ -4228,13 +4228,13 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>8</v>
@@ -4245,13 +4245,13 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>8</v>
@@ -4262,13 +4262,13 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>8</v>
@@ -4279,13 +4279,13 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>8</v>
@@ -4296,10 +4296,10 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>92</v>
@@ -4313,13 +4313,13 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>8</v>
@@ -4330,10 +4330,10 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>58</v>
@@ -4347,13 +4347,13 @@
     </row>
     <row r="124" ht="28" spans="1:5">
       <c r="A124" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B124" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B124" s="7" t="s">
-        <v>231</v>
-      </c>
       <c r="C124" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>8</v>
@@ -4364,13 +4364,13 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>8</v>
@@ -4381,13 +4381,13 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>8</v>
@@ -4398,13 +4398,13 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>8</v>
@@ -4415,10 +4415,10 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C128" s="8" t="s">
         <v>92</v>
@@ -4432,13 +4432,13 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>8</v>
@@ -4449,16 +4449,16 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>8</v>
@@ -4469,13 +4469,13 @@
         <v>246</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>247</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -4486,13 +4486,13 @@
         <v>248</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>8</v>
@@ -4503,13 +4503,13 @@
         <v>249</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>250</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>8</v>
@@ -4520,13 +4520,13 @@
         <v>251</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C134" s="7" t="s">
         <v>252</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -4537,13 +4537,13 @@
         <v>253</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C135" s="7" t="s">
         <v>254</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -4554,13 +4554,13 @@
         <v>255</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C136" s="7" t="s">
         <v>256</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -4571,13 +4571,13 @@
         <v>257</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C137" s="7" t="s">
         <v>258</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -4588,13 +4588,13 @@
         <v>259</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C138" s="7" t="s">
         <v>260</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>8</v>
@@ -4605,13 +4605,13 @@
         <v>261</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C139" s="7" t="s">
         <v>262</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>8</v>
@@ -4622,13 +4622,13 @@
         <v>263</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C140" s="7" t="s">
         <v>264</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>8</v>
@@ -4639,13 +4639,13 @@
         <v>265</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C141" s="7" t="s">
         <v>266</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -4656,13 +4656,13 @@
         <v>267</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C142" s="7" t="s">
         <v>268</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -4673,13 +4673,13 @@
         <v>269</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C143" s="7" t="s">
         <v>92</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -4690,13 +4690,13 @@
         <v>270</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C144" s="7" t="s">
         <v>271</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>8</v>
@@ -4707,13 +4707,13 @@
         <v>272</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C145" s="7" t="s">
         <v>273</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>8</v>
@@ -4761,7 +4761,7 @@
         <v>274</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>8</v>
@@ -4812,7 +4812,7 @@
         <v>274</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>8</v>
@@ -5353,7 +5353,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D145 E145 D1:D8 D41:D90 D130:D142 E2:E8 E41:E44 E45:E82 E83:E90 E130:E131 E132:E142 F2:F3 D146:E182 D91:E129 D9:E40 D143:E144">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E45 E129 D1:D8 D45:D74 D129:D145 E2:E8 E46:E74 E130:E142 E143:E145 F2:F3 D146:E182 D91:E128 D9:E40 D41:E44 D75:E90">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fixed issues of RW03 and RW07
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -503,6 +503,9 @@
     <t>probateFormsRW03.feature</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_076</t>
   </si>
   <si>
@@ -762,9 +765,6 @@
   </si>
   <si>
     <t>probateFormsRW07.feature</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>TC_130</t>
@@ -2240,8 +2240,8 @@
   <sheetPr/>
   <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3540,7 +3540,7 @@
         <v>58</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>8</v>
@@ -3548,16 +3548,16 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>8</v>
@@ -3565,16 +3565,16 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>8</v>
@@ -3582,16 +3582,16 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>8</v>
@@ -3599,16 +3599,16 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B80" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>8</v>
@@ -3616,16 +3616,16 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>8</v>
@@ -3633,16 +3633,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B82" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>8</v>
@@ -3650,16 +3650,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B83" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>8</v>
@@ -3667,16 +3667,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B84" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>8</v>
@@ -3684,7 +3684,7 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B85" s="7" t="s">
         <v>157</v>
@@ -3693,7 +3693,7 @@
         <v>92</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>8</v>
@@ -3701,16 +3701,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>8</v>
@@ -3718,10 +3718,10 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>58</v>
@@ -3735,13 +3735,13 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>178</v>
-      </c>
       <c r="C88" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>8</v>
@@ -3752,13 +3752,13 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>8</v>
@@ -3769,13 +3769,13 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>8</v>
@@ -3786,13 +3786,13 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>8</v>
@@ -3803,13 +3803,13 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>8</v>
@@ -3820,13 +3820,13 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>8</v>
@@ -3837,13 +3837,13 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>8</v>
@@ -3854,13 +3854,13 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>8</v>
@@ -3871,13 +3871,13 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>8</v>
@@ -3888,10 +3888,10 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>92</v>
@@ -3905,13 +3905,13 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>8</v>
@@ -3922,10 +3922,10 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>58</v>
@@ -3939,10 +3939,10 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="7" t="s">
         <v>197</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>196</v>
       </c>
       <c r="C100" s="7" t="s">
         <v>104</v>
@@ -3956,13 +3956,13 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>8</v>
@@ -3973,13 +3973,13 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>8</v>
@@ -3990,13 +3990,13 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>8</v>
@@ -4007,13 +4007,13 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>8</v>
@@ -4024,13 +4024,13 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>8</v>
@@ -4041,13 +4041,13 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>8</v>
@@ -4058,13 +4058,13 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>8</v>
@@ -4075,13 +4075,13 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>8</v>
@@ -4092,10 +4092,10 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>92</v>
@@ -4109,13 +4109,13 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>8</v>
@@ -4126,10 +4126,10 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>58</v>
@@ -4143,13 +4143,13 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B112" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B112" s="7" t="s">
-        <v>211</v>
-      </c>
       <c r="C112" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>8</v>
@@ -4160,13 +4160,13 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>8</v>
@@ -4177,13 +4177,13 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>8</v>
@@ -4194,13 +4194,13 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>8</v>
@@ -4211,13 +4211,13 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>8</v>
@@ -4228,13 +4228,13 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>8</v>
@@ -4245,13 +4245,13 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>8</v>
@@ -4262,13 +4262,13 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>8</v>
@@ -4279,13 +4279,13 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>8</v>
@@ -4296,10 +4296,10 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>92</v>
@@ -4313,13 +4313,13 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>8</v>
@@ -4330,10 +4330,10 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>58</v>
@@ -4347,13 +4347,13 @@
     </row>
     <row r="124" ht="28" spans="1:5">
       <c r="A124" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B124" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B124" s="7" t="s">
-        <v>231</v>
-      </c>
       <c r="C124" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>8</v>
@@ -4364,13 +4364,13 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>8</v>
@@ -4381,13 +4381,13 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>8</v>
@@ -4398,13 +4398,13 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>8</v>
@@ -4415,10 +4415,10 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C128" s="8" t="s">
         <v>92</v>
@@ -4432,13 +4432,13 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>8</v>
@@ -4449,16 +4449,16 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>8</v>
@@ -4469,13 +4469,13 @@
         <v>246</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>247</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -4486,13 +4486,13 @@
         <v>248</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C132" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>8</v>
@@ -4503,13 +4503,13 @@
         <v>249</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>250</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>8</v>
@@ -4520,13 +4520,13 @@
         <v>251</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C134" s="7" t="s">
         <v>252</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -4537,13 +4537,13 @@
         <v>253</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C135" s="7" t="s">
         <v>254</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -4554,13 +4554,13 @@
         <v>255</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C136" s="7" t="s">
         <v>256</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -4571,13 +4571,13 @@
         <v>257</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C137" s="7" t="s">
         <v>258</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -4588,13 +4588,13 @@
         <v>259</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C138" s="7" t="s">
         <v>260</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>8</v>
@@ -4605,13 +4605,13 @@
         <v>261</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C139" s="7" t="s">
         <v>262</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>8</v>
@@ -4622,13 +4622,13 @@
         <v>263</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C140" s="7" t="s">
         <v>264</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>8</v>
@@ -4639,13 +4639,13 @@
         <v>265</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C141" s="7" t="s">
         <v>266</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -4656,13 +4656,13 @@
         <v>267</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C142" s="7" t="s">
         <v>268</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -4673,13 +4673,13 @@
         <v>269</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C143" s="7" t="s">
         <v>92</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -4690,13 +4690,13 @@
         <v>270</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C144" s="7" t="s">
         <v>271</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>8</v>
@@ -4707,13 +4707,13 @@
         <v>272</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C145" s="7" t="s">
         <v>273</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>245</v>
+        <v>158</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>8</v>
@@ -5353,7 +5353,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E44 D129:E129 D1:D8 D42:D85 D130:D145 E2:E8 E42:E43 E45:E74 E75:E85 E130:E131 E132:E145 F2:F3 D9:E41 D86:E128 D146:E182">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E130 E144 D1:D8 D130:D144 E2:E8 E131:E143 F2:F3 D76:E85 D148:E182 D9:E75 D86:E126 D127:E129 D145:E147">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Make changes in PDF validation
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -764,166 +764,166 @@
     <t>probateFormsRW07.feature</t>
   </si>
   <si>
+    <t>TC_130</t>
+  </si>
+  <si>
+    <t>Verify, county, estate and file number aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_131</t>
+  </si>
+  <si>
+    <t>TC_132</t>
+  </si>
+  <si>
+    <t>Verify, on checking use 4 digit checkbox, changes in file number</t>
+  </si>
+  <si>
+    <t>TC_133</t>
+  </si>
+  <si>
+    <t>Verify, on clicking bene address field, multiple beneficiaries can be selected.</t>
+  </si>
+  <si>
+    <t>TC_134</t>
+  </si>
+  <si>
+    <t>Verify, beneficiary name and address should be displayed in the form.</t>
+  </si>
+  <si>
+    <t>TC_135</t>
+  </si>
+  <si>
+    <t>Verify, decedent died and county is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_136</t>
+  </si>
+  <si>
+    <t>Verify, on clicking name fiduciary contact list is displayed and multiple users can be selected.</t>
+  </si>
+  <si>
+    <t>TC_137</t>
+  </si>
+  <si>
+    <t>Verify, these contacts are common for all the forms.</t>
+  </si>
+  <si>
+    <t>TC_138</t>
+  </si>
+  <si>
+    <t>Verify, date can be entered.</t>
+  </si>
+  <si>
+    <t>TC_139</t>
+  </si>
+  <si>
+    <t>Verify, registrars address is auto fetched and is editable.</t>
+  </si>
+  <si>
+    <t>TC_140</t>
+  </si>
+  <si>
+    <t>Verify, corporate fiduciary type of contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_141</t>
+  </si>
+  <si>
+    <t>Verify, based on capacity contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_142</t>
+  </si>
+  <si>
+    <t>TC_143</t>
+  </si>
+  <si>
+    <t>Verify, selection is cleared on clicking clear selection button.</t>
+  </si>
+  <si>
+    <t>TC_144</t>
+  </si>
+  <si>
+    <t>Reset the RW07 form</t>
+  </si>
+  <si>
+    <t>probateFormsRW08.feature</t>
+  </si>
+  <si>
+    <t>TC_145</t>
+  </si>
+  <si>
+    <t>TC_146</t>
+  </si>
+  <si>
+    <t>TC_147</t>
+  </si>
+  <si>
+    <t>Verify, Will number and other dates can be entered in correct format.</t>
+  </si>
+  <si>
+    <t>TC_148</t>
+  </si>
+  <si>
+    <t>Verify, checkboxes for file no field.</t>
+  </si>
+  <si>
+    <t>TC_149</t>
+  </si>
+  <si>
+    <t>TC_150</t>
+  </si>
+  <si>
+    <t>Verify, the beneficiaries selected beyond 6 are displayed on the attachment.</t>
+  </si>
+  <si>
+    <t>TC_151</t>
+  </si>
+  <si>
+    <t>Verify, count is correctly displayed.</t>
+  </si>
+  <si>
+    <t>TC_152</t>
+  </si>
+  <si>
+    <t>Verify, on clicking "Display ALL beneficiary on attachment" checkbox all the contacts are transferred on attachment.</t>
+  </si>
+  <si>
+    <t>TC_153</t>
+  </si>
+  <si>
+    <t>TC_154</t>
+  </si>
+  <si>
+    <t>TC_155</t>
+  </si>
+  <si>
+    <t>Verify, these 2 sections are common for RW07, RW08 and anything updated is reflected in all the forms.</t>
+  </si>
+  <si>
+    <t>TC_156</t>
+  </si>
+  <si>
+    <t>TC_157</t>
+  </si>
+  <si>
+    <t>TC_158</t>
+  </si>
+  <si>
+    <t>TC_159</t>
+  </si>
+  <si>
+    <t>Reset the RW08 form</t>
+  </si>
+  <si>
+    <t>TC_160</t>
+  </si>
+  <si>
+    <t>probateFormsRW10.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_130</t>
-  </si>
-  <si>
-    <t>Verify, county, estate and file number aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_131</t>
-  </si>
-  <si>
-    <t>TC_132</t>
-  </si>
-  <si>
-    <t>Verify, on checking use 4 digit checkbox, changes in file number</t>
-  </si>
-  <si>
-    <t>TC_133</t>
-  </si>
-  <si>
-    <t>Verify, on clicking bene address field, multiple beneficiaries can be selected.</t>
-  </si>
-  <si>
-    <t>TC_134</t>
-  </si>
-  <si>
-    <t>Verify, beneficiary name and address should be displayed in the form.</t>
-  </si>
-  <si>
-    <t>TC_135</t>
-  </si>
-  <si>
-    <t>Verify, decedent died and county is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_136</t>
-  </si>
-  <si>
-    <t>Verify, on clicking name fiduciary contact list is displayed and multiple users can be selected.</t>
-  </si>
-  <si>
-    <t>TC_137</t>
-  </si>
-  <si>
-    <t>Verify, these contacts are common for all the forms.</t>
-  </si>
-  <si>
-    <t>TC_138</t>
-  </si>
-  <si>
-    <t>Verify, date can be entered.</t>
-  </si>
-  <si>
-    <t>TC_139</t>
-  </si>
-  <si>
-    <t>Verify, registrars address is auto fetched and is editable.</t>
-  </si>
-  <si>
-    <t>TC_140</t>
-  </si>
-  <si>
-    <t>Verify, corporate fiduciary type of contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_141</t>
-  </si>
-  <si>
-    <t>Verify, based on capacity contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_142</t>
-  </si>
-  <si>
-    <t>TC_143</t>
-  </si>
-  <si>
-    <t>Verify, selection is cleared on clicking clear selection button.</t>
-  </si>
-  <si>
-    <t>TC_144</t>
-  </si>
-  <si>
-    <t>Reset the RW07 form</t>
-  </si>
-  <si>
-    <t>probateFormsRW08.feature</t>
-  </si>
-  <si>
-    <t>TC_145</t>
-  </si>
-  <si>
-    <t>TC_146</t>
-  </si>
-  <si>
-    <t>TC_147</t>
-  </si>
-  <si>
-    <t>Verify, Will number and other dates can be entered in correct format.</t>
-  </si>
-  <si>
-    <t>TC_148</t>
-  </si>
-  <si>
-    <t>Verify, checkboxes for file no field.</t>
-  </si>
-  <si>
-    <t>TC_149</t>
-  </si>
-  <si>
-    <t>TC_150</t>
-  </si>
-  <si>
-    <t>Verify, the beneficiaries selected beyond 6 are displayed on the attachment.</t>
-  </si>
-  <si>
-    <t>TC_151</t>
-  </si>
-  <si>
-    <t>Verify, count is correctly displayed.</t>
-  </si>
-  <si>
-    <t>TC_152</t>
-  </si>
-  <si>
-    <t>Verify, on clicking "Display ALL beneficiary on attachment" checkbox all the contacts are transferred on attachment.</t>
-  </si>
-  <si>
-    <t>TC_153</t>
-  </si>
-  <si>
-    <t>TC_154</t>
-  </si>
-  <si>
-    <t>TC_155</t>
-  </si>
-  <si>
-    <t>Verify, these 2 sections are common for RW07, RW08 and anything updated is reflected in all the forms.</t>
-  </si>
-  <si>
-    <t>TC_156</t>
-  </si>
-  <si>
-    <t>TC_157</t>
-  </si>
-  <si>
-    <t>TC_158</t>
-  </si>
-  <si>
-    <t>TC_159</t>
-  </si>
-  <si>
-    <t>Reset the RW08 form</t>
-  </si>
-  <si>
-    <t>TC_160</t>
-  </si>
-  <si>
-    <t>probateFormsRW10.feature</t>
   </si>
   <si>
     <t>Verify, title of the form and if county is fetched from the decedent info.</t>
@@ -2240,8 +2240,8 @@
   <sheetPr/>
   <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="D141" sqref="D141:D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -4458,7 +4458,7 @@
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>8</v>
@@ -4466,16 +4466,16 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B131" s="7" t="s">
         <v>244</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -4483,7 +4483,7 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B132" s="7" t="s">
         <v>244</v>
@@ -4492,7 +4492,7 @@
         <v>106</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>8</v>
@@ -4500,16 +4500,16 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B133" s="7" t="s">
         <v>244</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>8</v>
@@ -4517,16 +4517,16 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B134" s="7" t="s">
         <v>244</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -4534,16 +4534,16 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B135" s="7" t="s">
         <v>244</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -4551,16 +4551,16 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B136" s="7" t="s">
         <v>244</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -4568,16 +4568,16 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B137" s="7" t="s">
         <v>244</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -4585,16 +4585,16 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B138" s="7" t="s">
         <v>244</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>8</v>
@@ -4602,16 +4602,16 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B139" s="7" t="s">
         <v>244</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>8</v>
@@ -4619,16 +4619,16 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B140" s="7" t="s">
         <v>244</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>8</v>
@@ -4636,16 +4636,16 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B141" s="7" t="s">
         <v>244</v>
       </c>
       <c r="C141" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -4653,16 +4653,16 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B142" s="7" t="s">
         <v>244</v>
       </c>
       <c r="C142" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -4670,7 +4670,7 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B143" s="7" t="s">
         <v>244</v>
@@ -4679,7 +4679,7 @@
         <v>92</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -4687,16 +4687,16 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B144" s="7" t="s">
         <v>244</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>8</v>
@@ -4704,16 +4704,16 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B145" s="7" t="s">
         <v>244</v>
       </c>
       <c r="C145" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>245</v>
+        <v>8</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>8</v>
@@ -4721,10 +4721,10 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>58</v>
@@ -4738,13 +4738,13 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>8</v>
@@ -4755,10 +4755,10 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C148" s="7" t="s">
         <v>106</v>
@@ -4772,13 +4772,13 @@
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C149" s="7" t="s">
         <v>277</v>
-      </c>
-      <c r="B149" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C149" s="7" t="s">
-        <v>278</v>
       </c>
       <c r="D149" s="3" t="s">
         <v>8</v>
@@ -4789,13 +4789,13 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C150" s="7" t="s">
         <v>279</v>
-      </c>
-      <c r="B150" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C150" s="7" t="s">
-        <v>280</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>8</v>
@@ -4806,10 +4806,10 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C151" s="7" t="s">
         <v>136</v>
@@ -4823,13 +4823,13 @@
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C152" s="7" t="s">
         <v>282</v>
-      </c>
-      <c r="B152" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C152" s="7" t="s">
-        <v>283</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>8</v>
@@ -4840,13 +4840,13 @@
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C153" s="7" t="s">
         <v>284</v>
-      </c>
-      <c r="B153" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C153" s="7" t="s">
-        <v>285</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>8</v>
@@ -4857,13 +4857,13 @@
     </row>
     <row r="154" ht="28" spans="1:5">
       <c r="A154" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C154" s="9" t="s">
         <v>286</v>
-      </c>
-      <c r="B154" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C154" s="9" t="s">
-        <v>287</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>8</v>
@@ -4874,13 +4874,13 @@
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>8</v>
@@ -4891,13 +4891,13 @@
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C156" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>8</v>
@@ -4908,13 +4908,13 @@
     </row>
     <row r="157" ht="28" spans="1:5">
       <c r="A157" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B157" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C157" s="9" t="s">
         <v>290</v>
-      </c>
-      <c r="B157" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C157" s="9" t="s">
-        <v>291</v>
       </c>
       <c r="D157" s="3" t="s">
         <v>8</v>
@@ -4925,10 +4925,10 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C158" s="7" t="s">
         <v>92</v>
@@ -4942,13 +4942,13 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C159" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D159" s="3" t="s">
         <v>8</v>
@@ -4959,10 +4959,10 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C160" s="8" t="s">
         <v>92</v>
@@ -4976,13 +4976,13 @@
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B161" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C161" s="7" t="s">
         <v>295</v>
-      </c>
-      <c r="B161" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C161" s="7" t="s">
-        <v>296</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>8</v>
@@ -4993,16 +4993,16 @@
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B162" s="7" t="s">
         <v>297</v>
-      </c>
-      <c r="B162" s="7" t="s">
-        <v>298</v>
       </c>
       <c r="C162" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>8</v>
@@ -5010,16 +5010,16 @@
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B163" s="7" t="s">
         <v>297</v>
-      </c>
-      <c r="B163" s="7" t="s">
-        <v>298</v>
       </c>
       <c r="C163" s="7" t="s">
         <v>299</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>8</v>
@@ -5030,13 +5030,13 @@
         <v>300</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C164" s="7" t="s">
         <v>301</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>8</v>
@@ -5047,13 +5047,13 @@
         <v>302</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C165" s="7" t="s">
         <v>303</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>8</v>
@@ -5064,13 +5064,13 @@
         <v>304</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C166" s="7" t="s">
         <v>305</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>8</v>
@@ -5081,13 +5081,13 @@
         <v>306</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C167" s="7" t="s">
         <v>307</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>8</v>
@@ -5098,13 +5098,13 @@
         <v>308</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C168" s="7" t="s">
         <v>309</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>8</v>
@@ -5115,13 +5115,13 @@
         <v>310</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C169" s="7" t="s">
         <v>311</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>8</v>
@@ -5132,13 +5132,13 @@
         <v>312</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C170" s="7" t="s">
         <v>313</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>8</v>
@@ -5149,13 +5149,13 @@
         <v>314</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C171" s="7" t="s">
         <v>315</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>8</v>
@@ -5166,13 +5166,13 @@
         <v>316</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C172" s="7" t="s">
         <v>317</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>8</v>
@@ -5183,13 +5183,13 @@
         <v>318</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C173" s="7" t="s">
         <v>319</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>8</v>
@@ -5200,13 +5200,13 @@
         <v>320</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C174" s="7" t="s">
         <v>321</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>8</v>
@@ -5217,13 +5217,13 @@
         <v>322</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C175" s="7" t="s">
         <v>323</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>8</v>
@@ -5234,13 +5234,13 @@
         <v>324</v>
       </c>
       <c r="B176" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C176" s="7" t="s">
         <v>325</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>8</v>
@@ -5251,13 +5251,13 @@
         <v>326</v>
       </c>
       <c r="B177" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C177" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="D177" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="C177" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="D177" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>8</v>
@@ -5268,13 +5268,13 @@
         <v>327</v>
       </c>
       <c r="B178" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C178" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D178" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="C178" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="D178" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>8</v>
@@ -5285,13 +5285,13 @@
         <v>328</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C179" s="9" t="s">
         <v>329</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>8</v>
@@ -5302,13 +5302,13 @@
         <v>330</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C180" s="8" t="s">
         <v>92</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>8</v>
@@ -5319,13 +5319,13 @@
         <v>331</v>
       </c>
       <c r="B181" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C181" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="D181" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="C181" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="D181" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>8</v>
@@ -5336,13 +5336,13 @@
         <v>332</v>
       </c>
       <c r="B182" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C182" s="7" t="s">
         <v>333</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>8</v>
+        <v>298</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>8</v>
@@ -5353,7 +5353,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E44 D129:E129 D1:D8 D42:D85 D130:D145 E2:E8 E42:E43 E45:E74 E75:E85 E130:E131 E132:E145 F2:F3 D9:E41 D86:E128 D146:E182">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E145 D1:D8 D141:D161 E2:E8 E141:E144 E146:E161 F2:F3 D108:E129 D130:E140 D9:E107 D162:E182">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fixed issues of RW06
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -503,169 +503,169 @@
     <t>probateFormsRW03.feature</t>
   </si>
   <si>
+    <t>TC_076</t>
+  </si>
+  <si>
+    <t>Verify county, estate and aka names are auto-populated on the form</t>
+  </si>
+  <si>
+    <t>TC_077</t>
+  </si>
+  <si>
+    <t>Verify, the auto-populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_078</t>
+  </si>
+  <si>
+    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
+  </si>
+  <si>
+    <t>TC_079</t>
+  </si>
+  <si>
+    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
+  </si>
+  <si>
+    <t>TC_080</t>
+  </si>
+  <si>
+    <t>Verify, names can be entered in witness fields.</t>
+  </si>
+  <si>
+    <t>TC_081</t>
+  </si>
+  <si>
+    <t>Verify, names updated from signature are reflected in witness names fields.</t>
+  </si>
+  <si>
+    <t>TC_082</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered in address, city, zip fields.</t>
+  </si>
+  <si>
+    <t>TC_083</t>
+  </si>
+  <si>
+    <t>Verify, form is auto saved.</t>
+  </si>
+  <si>
+    <t>TC_084</t>
+  </si>
+  <si>
+    <t>TC_085</t>
+  </si>
+  <si>
+    <t>Reset the RW03 form</t>
+  </si>
+  <si>
+    <t>TC_086</t>
+  </si>
+  <si>
+    <t>probateFormsRW04.feature</t>
+  </si>
+  <si>
+    <t>TC_087</t>
+  </si>
+  <si>
+    <t>Verify, correct title is displayed on the form's header.</t>
+  </si>
+  <si>
+    <t>TC_088</t>
+  </si>
+  <si>
+    <t>Verify, county, and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_089</t>
+  </si>
+  <si>
+    <t>Verify, correct estate's name is displayed on the form.</t>
+  </si>
+  <si>
+    <t>TC_090</t>
+  </si>
+  <si>
+    <t>Verify, name of the decedent should be auto populated from the form.</t>
+  </si>
+  <si>
+    <t>TC_091</t>
+  </si>
+  <si>
+    <t>TC_092</t>
+  </si>
+  <si>
+    <t>TC_093</t>
+  </si>
+  <si>
+    <t>TC_094</t>
+  </si>
+  <si>
+    <t>TC_095</t>
+  </si>
+  <si>
+    <t>TC_096</t>
+  </si>
+  <si>
+    <t>TC_097</t>
+  </si>
+  <si>
+    <t>Reset the RW04 form</t>
+  </si>
+  <si>
+    <t>TC_098</t>
+  </si>
+  <si>
+    <t>probateFormsRW05.feature</t>
+  </si>
+  <si>
+    <t>TC_099</t>
+  </si>
+  <si>
+    <t>TC_100</t>
+  </si>
+  <si>
+    <t>TC_101</t>
+  </si>
+  <si>
+    <t>TC_102</t>
+  </si>
+  <si>
+    <t>TC_103</t>
+  </si>
+  <si>
+    <t>TC_104</t>
+  </si>
+  <si>
+    <t>TC_105</t>
+  </si>
+  <si>
+    <t>TC_106</t>
+  </si>
+  <si>
+    <t>Verify, on checking notary checkbox, notary section displays.</t>
+  </si>
+  <si>
+    <t>TC_107</t>
+  </si>
+  <si>
+    <t>TC_108</t>
+  </si>
+  <si>
+    <t>TC_109</t>
+  </si>
+  <si>
+    <t>Reset the RW05 form</t>
+  </si>
+  <si>
+    <t>TC_110</t>
+  </si>
+  <si>
+    <t>probateFormsRW06.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_076</t>
-  </si>
-  <si>
-    <t>Verify county, estate and aka names are auto-populated on the form</t>
-  </si>
-  <si>
-    <t>TC_077</t>
-  </si>
-  <si>
-    <t>Verify, the auto-populated fields are not editable.</t>
-  </si>
-  <si>
-    <t>TC_078</t>
-  </si>
-  <si>
-    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
-  </si>
-  <si>
-    <t>TC_079</t>
-  </si>
-  <si>
-    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
-  </si>
-  <si>
-    <t>TC_080</t>
-  </si>
-  <si>
-    <t>Verify, names can be entered in witness fields.</t>
-  </si>
-  <si>
-    <t>TC_081</t>
-  </si>
-  <si>
-    <t>Verify, names updated from signature are reflected in witness names fields.</t>
-  </si>
-  <si>
-    <t>TC_082</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered in address, city, zip fields.</t>
-  </si>
-  <si>
-    <t>TC_083</t>
-  </si>
-  <si>
-    <t>Verify, form is auto saved.</t>
-  </si>
-  <si>
-    <t>TC_084</t>
-  </si>
-  <si>
-    <t>TC_085</t>
-  </si>
-  <si>
-    <t>Reset the RW03 form</t>
-  </si>
-  <si>
-    <t>TC_086</t>
-  </si>
-  <si>
-    <t>probateFormsRW04.feature</t>
-  </si>
-  <si>
-    <t>TC_087</t>
-  </si>
-  <si>
-    <t>Verify, correct title is displayed on the form's header.</t>
-  </si>
-  <si>
-    <t>TC_088</t>
-  </si>
-  <si>
-    <t>Verify, county, and aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_089</t>
-  </si>
-  <si>
-    <t>Verify, correct estate's name is displayed on the form.</t>
-  </si>
-  <si>
-    <t>TC_090</t>
-  </si>
-  <si>
-    <t>Verify, name of the decedent should be auto populated from the form.</t>
-  </si>
-  <si>
-    <t>TC_091</t>
-  </si>
-  <si>
-    <t>TC_092</t>
-  </si>
-  <si>
-    <t>TC_093</t>
-  </si>
-  <si>
-    <t>TC_094</t>
-  </si>
-  <si>
-    <t>TC_095</t>
-  </si>
-  <si>
-    <t>TC_096</t>
-  </si>
-  <si>
-    <t>TC_097</t>
-  </si>
-  <si>
-    <t>Reset the RW04 form</t>
-  </si>
-  <si>
-    <t>TC_098</t>
-  </si>
-  <si>
-    <t>probateFormsRW05.feature</t>
-  </si>
-  <si>
-    <t>TC_099</t>
-  </si>
-  <si>
-    <t>TC_100</t>
-  </si>
-  <si>
-    <t>TC_101</t>
-  </si>
-  <si>
-    <t>TC_102</t>
-  </si>
-  <si>
-    <t>TC_103</t>
-  </si>
-  <si>
-    <t>TC_104</t>
-  </si>
-  <si>
-    <t>TC_105</t>
-  </si>
-  <si>
-    <t>TC_106</t>
-  </si>
-  <si>
-    <t>Verify, on checking notary checkbox, notary section displays.</t>
-  </si>
-  <si>
-    <t>TC_107</t>
-  </si>
-  <si>
-    <t>TC_108</t>
-  </si>
-  <si>
-    <t>TC_109</t>
-  </si>
-  <si>
-    <t>Reset the RW05 form</t>
-  </si>
-  <si>
-    <t>TC_110</t>
-  </si>
-  <si>
-    <t>probateFormsRW06.feature</t>
   </si>
   <si>
     <t>TC_111</t>
@@ -2240,8 +2240,8 @@
   <sheetPr/>
   <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3540,7 +3540,7 @@
         <v>58</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>8</v>
@@ -3548,16 +3548,16 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>8</v>
@@ -3565,16 +3565,16 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>8</v>
@@ -3582,16 +3582,16 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>8</v>
@@ -3599,16 +3599,16 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B80" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>8</v>
@@ -3616,16 +3616,16 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>8</v>
@@ -3633,16 +3633,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B82" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>8</v>
@@ -3650,16 +3650,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B83" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>8</v>
@@ -3667,16 +3667,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B84" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>8</v>
@@ -3684,7 +3684,7 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B85" s="7" t="s">
         <v>157</v>
@@ -3693,7 +3693,7 @@
         <v>92</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>8</v>
@@ -3701,16 +3701,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>8</v>
@@ -3718,10 +3718,10 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>58</v>
@@ -3735,13 +3735,13 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C88" s="7" t="s">
         <v>180</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>181</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>8</v>
@@ -3752,13 +3752,13 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C89" s="7" t="s">
         <v>182</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>183</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>8</v>
@@ -3769,13 +3769,13 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C90" s="7" t="s">
         <v>184</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>185</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>8</v>
@@ -3786,13 +3786,13 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C91" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>187</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>8</v>
@@ -3803,13 +3803,13 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>8</v>
@@ -3820,13 +3820,13 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>8</v>
@@ -3837,13 +3837,13 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>8</v>
@@ -3854,13 +3854,13 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>8</v>
@@ -3871,13 +3871,13 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>8</v>
@@ -3888,10 +3888,10 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>92</v>
@@ -3905,13 +3905,13 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C98" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="B98" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>8</v>
@@ -3922,10 +3922,10 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B99" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>197</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>58</v>
@@ -3939,10 +3939,10 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C100" s="7" t="s">
         <v>104</v>
@@ -3956,13 +3956,13 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>8</v>
@@ -3973,13 +3973,13 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>8</v>
@@ -3990,13 +3990,13 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>8</v>
@@ -4007,13 +4007,13 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>8</v>
@@ -4024,13 +4024,13 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>8</v>
@@ -4041,13 +4041,13 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>8</v>
@@ -4058,13 +4058,13 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C107" s="7" t="s">
         <v>205</v>
-      </c>
-      <c r="B107" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="C107" s="7" t="s">
-        <v>206</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>8</v>
@@ -4075,13 +4075,13 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>8</v>
@@ -4092,10 +4092,10 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>92</v>
@@ -4109,13 +4109,13 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C110" s="7" t="s">
         <v>209</v>
-      </c>
-      <c r="B110" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="C110" s="7" t="s">
-        <v>210</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>8</v>
@@ -4126,16 +4126,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B111" s="7" t="s">
         <v>211</v>
-      </c>
-      <c r="B111" s="7" t="s">
-        <v>212</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -4146,13 +4146,13 @@
         <v>213</v>
       </c>
       <c r="B112" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D112" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="C112" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -4163,13 +4163,13 @@
         <v>214</v>
       </c>
       <c r="B113" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D113" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="C113" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -4180,13 +4180,13 @@
         <v>215</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>216</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -4197,13 +4197,13 @@
         <v>217</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>218</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -4214,13 +4214,13 @@
         <v>219</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>220</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -4231,13 +4231,13 @@
         <v>221</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>222</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -4248,13 +4248,13 @@
         <v>223</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>216</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -4265,13 +4265,13 @@
         <v>224</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>225</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4282,13 +4282,13 @@
         <v>226</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>227</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4299,13 +4299,13 @@
         <v>228</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>92</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4316,13 +4316,13 @@
         <v>229</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>230</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>8</v>
+        <v>212</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4458,7 +4458,7 @@
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>8</v>
@@ -4475,7 +4475,7 @@
         <v>247</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -4492,7 +4492,7 @@
         <v>106</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>8</v>
@@ -4509,7 +4509,7 @@
         <v>250</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>8</v>
@@ -4526,7 +4526,7 @@
         <v>252</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -4543,7 +4543,7 @@
         <v>254</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -4560,7 +4560,7 @@
         <v>256</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -4577,7 +4577,7 @@
         <v>258</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -4594,7 +4594,7 @@
         <v>260</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>8</v>
@@ -4611,7 +4611,7 @@
         <v>262</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>8</v>
@@ -4628,7 +4628,7 @@
         <v>264</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>8</v>
@@ -4645,7 +4645,7 @@
         <v>266</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -4662,7 +4662,7 @@
         <v>268</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -4679,7 +4679,7 @@
         <v>92</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -4696,7 +4696,7 @@
         <v>271</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>8</v>
@@ -4713,7 +4713,7 @@
         <v>273</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>8</v>
@@ -5353,7 +5353,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E130 E144 D1:D8 D130:D144 E2:E8 E131:E143 F2:F3 D76:E85 D148:E182 D9:E75 D86:E126 D127:E129 D145:E147">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E86 D1:D8 D86:D109 E2:E8 E87:E109 F2:F3 D122:E182 D9:E20 D21:E85 D110:E121">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fixed RW02 and updated OC01 on UAT
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -212,115 +212,115 @@
     <t>Verify, file no. is displayed at the top of the form.</t>
   </si>
   <si>
+    <t>TC_027</t>
+  </si>
+  <si>
+    <t>Verify, decedent information is displayed in section1 of the form.</t>
+  </si>
+  <si>
+    <t>TC_028</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 2 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_029</t>
+  </si>
+  <si>
+    <t>Verify, in section 2 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_030</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 3 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_031</t>
+  </si>
+  <si>
+    <t>Verify, in section 3 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_032</t>
+  </si>
+  <si>
+    <t>Verify, on clicking other checkbox, text area is enabled.</t>
+  </si>
+  <si>
+    <t>TC_033</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 4 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_034</t>
+  </si>
+  <si>
+    <t>Verify, on clicking last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_035</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_036</t>
+  </si>
+  <si>
+    <t>Verify, on selecting the contact its information is displayed in section 4.</t>
+  </si>
+  <si>
+    <t>TC_037</t>
+  </si>
+  <si>
+    <t>Verify, on clicking executor last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_038</t>
+  </si>
+  <si>
+    <t>Verify, 3 types of selection is available.</t>
+  </si>
+  <si>
+    <t>TC_039</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be dragged and dropped in a each of the type.</t>
+  </si>
+  <si>
+    <t>TC_040</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 5 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_041</t>
+  </si>
+  <si>
+    <t>Verify the selected contacts are displayed under executor, co executor and secondary co executor.</t>
+  </si>
+  <si>
+    <t>TC_042</t>
+  </si>
+  <si>
+    <t>Verify form can be printed in pdf</t>
+  </si>
+  <si>
+    <t>TC_043</t>
+  </si>
+  <si>
+    <t>Reset the RW01 form</t>
+  </si>
+  <si>
+    <t>TC_044</t>
+  </si>
+  <si>
+    <t>probateFormsRW02.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_027</t>
-  </si>
-  <si>
-    <t>Verify, decedent information is displayed in section1 of the form.</t>
-  </si>
-  <si>
-    <t>TC_028</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 2 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_029</t>
-  </si>
-  <si>
-    <t>Verify, in section 2 only 1 checkbox can be checked.</t>
-  </si>
-  <si>
-    <t>TC_030</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 3 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_031</t>
-  </si>
-  <si>
-    <t>Verify, in section 3 only 1 checkbox can be checked.</t>
-  </si>
-  <si>
-    <t>TC_032</t>
-  </si>
-  <si>
-    <t>Verify, on clicking other checkbox, text area is enabled.</t>
-  </si>
-  <si>
-    <t>TC_033</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 4 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_034</t>
-  </si>
-  <si>
-    <t>Verify, on clicking last name, a side bar is displayed.</t>
-  </si>
-  <si>
-    <t>TC_035</t>
-  </si>
-  <si>
-    <t>Verify, only 1 contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_036</t>
-  </si>
-  <si>
-    <t>Verify, on selecting the contact its information is displayed in section 4.</t>
-  </si>
-  <si>
-    <t>TC_037</t>
-  </si>
-  <si>
-    <t>Verify, on clicking executor last name, a side bar is displayed.</t>
-  </si>
-  <si>
-    <t>TC_038</t>
-  </si>
-  <si>
-    <t>Verify, 3 types of selection is available.</t>
-  </si>
-  <si>
-    <t>TC_039</t>
-  </si>
-  <si>
-    <t>Verify, only 1 contact can be dragged and dropped in a each of the type.</t>
-  </si>
-  <si>
-    <t>TC_040</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 5 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_041</t>
-  </si>
-  <si>
-    <t>Verify the selected contacts are displayed under executor, co executor and secondary co executor.</t>
-  </si>
-  <si>
-    <t>TC_042</t>
-  </si>
-  <si>
-    <t>Verify form can be printed in pdf</t>
-  </si>
-  <si>
-    <t>TC_043</t>
-  </si>
-  <si>
-    <t>Reset the RW01 form</t>
-  </si>
-  <si>
-    <t>TC_044</t>
-  </si>
-  <si>
-    <t>probateFormsRW02.feature</t>
   </si>
   <si>
     <t>TC_045</t>
@@ -2246,8 +2246,8 @@
   <sheetPr/>
   <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="C188" sqref="C188"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2713,7 +2713,7 @@
         <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>8</v>
@@ -2721,16 +2721,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>8</v>
@@ -2738,16 +2738,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>8</v>
@@ -2755,16 +2755,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>8</v>
@@ -2772,16 +2772,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>8</v>
@@ -2789,16 +2789,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>8</v>
@@ -2806,16 +2806,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>8</v>
@@ -2823,16 +2823,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>8</v>
@@ -2840,16 +2840,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>8</v>
@@ -2857,16 +2857,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>8</v>
@@ -2874,16 +2874,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>8</v>
@@ -2891,16 +2891,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>8</v>
@@ -2908,16 +2908,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>8</v>
@@ -2925,16 +2925,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>8</v>
@@ -2942,16 +2942,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>8</v>
@@ -2959,16 +2959,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>8</v>
@@ -2976,16 +2976,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>8</v>
@@ -2993,16 +2993,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>8</v>
@@ -3010,16 +3010,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -3030,13 +3030,13 @@
         <v>98</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>99</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -3047,13 +3047,13 @@
         <v>100</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>101</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -3064,13 +3064,13 @@
         <v>102</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>103</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -3081,13 +3081,13 @@
         <v>104</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>105</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -3098,13 +3098,13 @@
         <v>106</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>107</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -3115,13 +3115,13 @@
         <v>108</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>109</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -3132,13 +3132,13 @@
         <v>110</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>111</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -3149,13 +3149,13 @@
         <v>112</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -3166,13 +3166,13 @@
         <v>114</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>115</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -3183,13 +3183,13 @@
         <v>116</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>117</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -3200,13 +3200,13 @@
         <v>118</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>119</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -3217,13 +3217,13 @@
         <v>120</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>121</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -3234,13 +3234,13 @@
         <v>122</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>123</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -3251,13 +3251,13 @@
         <v>124</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>125</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -3268,13 +3268,13 @@
         <v>126</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>127</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -3285,13 +3285,13 @@
         <v>128</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>129</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -3302,13 +3302,13 @@
         <v>130</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>131</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3319,13 +3319,13 @@
         <v>132</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>133</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3336,13 +3336,13 @@
         <v>134</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>135</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3353,13 +3353,13 @@
         <v>136</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>137</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3370,13 +3370,13 @@
         <v>138</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>139</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3387,13 +3387,13 @@
         <v>140</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>141</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3404,13 +3404,13 @@
         <v>142</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>143</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3421,13 +3421,13 @@
         <v>144</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>145</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3438,13 +3438,13 @@
         <v>146</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>147</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3455,13 +3455,13 @@
         <v>148</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>149</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3472,13 +3472,13 @@
         <v>150</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>151</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3489,13 +3489,13 @@
         <v>152</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>153</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3506,13 +3506,13 @@
         <v>154</v>
       </c>
       <c r="B74" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>8</v>
@@ -3523,13 +3523,13 @@
         <v>155</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>156</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>8</v>
@@ -3546,7 +3546,7 @@
         <v>58</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>8</v>
@@ -3563,7 +3563,7 @@
         <v>160</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>8</v>
@@ -3580,7 +3580,7 @@
         <v>162</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>8</v>
@@ -3597,7 +3597,7 @@
         <v>164</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>8</v>
@@ -3614,7 +3614,7 @@
         <v>166</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>8</v>
@@ -3631,7 +3631,7 @@
         <v>168</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>8</v>
@@ -3648,7 +3648,7 @@
         <v>170</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>8</v>
@@ -3665,7 +3665,7 @@
         <v>172</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>8</v>
@@ -3682,7 +3682,7 @@
         <v>174</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>8</v>
@@ -3696,10 +3696,10 @@
         <v>158</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>8</v>
@@ -3716,7 +3716,7 @@
         <v>177</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>8</v>
@@ -3733,7 +3733,7 @@
         <v>58</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>8</v>
@@ -3750,7 +3750,7 @@
         <v>181</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>8</v>
@@ -3767,7 +3767,7 @@
         <v>183</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>8</v>
@@ -3784,7 +3784,7 @@
         <v>185</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>8</v>
@@ -3801,7 +3801,7 @@
         <v>187</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>8</v>
@@ -3818,7 +3818,7 @@
         <v>166</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>8</v>
@@ -3835,7 +3835,7 @@
         <v>168</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>8</v>
@@ -3852,7 +3852,7 @@
         <v>170</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>8</v>
@@ -3869,7 +3869,7 @@
         <v>172</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>8</v>
@@ -3886,7 +3886,7 @@
         <v>174</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>8</v>
@@ -3900,10 +3900,10 @@
         <v>179</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -3920,7 +3920,7 @@
         <v>195</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -3937,7 +3937,7 @@
         <v>58</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -3954,7 +3954,7 @@
         <v>105</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -3971,7 +3971,7 @@
         <v>162</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -3988,7 +3988,7 @@
         <v>164</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -4005,7 +4005,7 @@
         <v>166</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -4022,7 +4022,7 @@
         <v>168</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -4039,7 +4039,7 @@
         <v>170</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -4056,7 +4056,7 @@
         <v>172</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -4073,7 +4073,7 @@
         <v>206</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -4090,7 +4090,7 @@
         <v>174</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -4104,10 +4104,10 @@
         <v>197</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -4124,7 +4124,7 @@
         <v>210</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -4141,7 +4141,7 @@
         <v>58</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -4158,7 +4158,7 @@
         <v>160</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -4175,7 +4175,7 @@
         <v>162</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -4192,7 +4192,7 @@
         <v>216</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -4209,7 +4209,7 @@
         <v>218</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -4226,7 +4226,7 @@
         <v>220</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -4243,7 +4243,7 @@
         <v>222</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -4260,7 +4260,7 @@
         <v>216</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -4277,7 +4277,7 @@
         <v>225</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4294,7 +4294,7 @@
         <v>227</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4308,10 +4308,10 @@
         <v>212</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4328,7 +4328,7 @@
         <v>230</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4345,7 +4345,7 @@
         <v>58</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>8</v>
@@ -4362,7 +4362,7 @@
         <v>234</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>8</v>
@@ -4379,7 +4379,7 @@
         <v>236</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>8</v>
@@ -4396,7 +4396,7 @@
         <v>238</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>8</v>
@@ -4413,7 +4413,7 @@
         <v>240</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>8</v>
@@ -4427,10 +4427,10 @@
         <v>232</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>8</v>
@@ -4447,7 +4447,7 @@
         <v>243</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>8</v>
@@ -4464,7 +4464,7 @@
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>8</v>
@@ -4481,7 +4481,7 @@
         <v>247</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -4498,7 +4498,7 @@
         <v>107</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>8</v>
@@ -4515,7 +4515,7 @@
         <v>250</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>8</v>
@@ -4532,7 +4532,7 @@
         <v>252</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -4549,7 +4549,7 @@
         <v>254</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -4566,7 +4566,7 @@
         <v>256</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -4583,7 +4583,7 @@
         <v>258</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -4600,7 +4600,7 @@
         <v>260</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>8</v>
@@ -4617,7 +4617,7 @@
         <v>262</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>8</v>
@@ -4634,7 +4634,7 @@
         <v>264</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>8</v>
@@ -4651,7 +4651,7 @@
         <v>266</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -4668,7 +4668,7 @@
         <v>268</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -4682,10 +4682,10 @@
         <v>245</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -4702,7 +4702,7 @@
         <v>271</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>8</v>
@@ -4719,7 +4719,7 @@
         <v>273</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>8</v>
@@ -4736,7 +4736,7 @@
         <v>58</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>8</v>
@@ -4753,7 +4753,7 @@
         <v>247</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>8</v>
@@ -4770,7 +4770,7 @@
         <v>107</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>8</v>
@@ -4787,7 +4787,7 @@
         <v>279</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>8</v>
@@ -4804,7 +4804,7 @@
         <v>281</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>8</v>
@@ -4821,7 +4821,7 @@
         <v>137</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>8</v>
@@ -4838,7 +4838,7 @@
         <v>284</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>8</v>
@@ -4855,7 +4855,7 @@
         <v>286</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>8</v>
@@ -4872,7 +4872,7 @@
         <v>288</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>8</v>
@@ -4889,7 +4889,7 @@
         <v>266</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>8</v>
@@ -4906,7 +4906,7 @@
         <v>268</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>8</v>
@@ -4923,7 +4923,7 @@
         <v>292</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>8</v>
@@ -4937,10 +4937,10 @@
         <v>275</v>
       </c>
       <c r="C158" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>8</v>
@@ -4957,7 +4957,7 @@
         <v>271</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>8</v>
@@ -4971,10 +4971,10 @@
         <v>275</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>8</v>
@@ -4991,7 +4991,7 @@
         <v>297</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>8</v>
@@ -5008,7 +5008,7 @@
         <v>58</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>8</v>
@@ -5025,7 +5025,7 @@
         <v>301</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>8</v>
@@ -5042,7 +5042,7 @@
         <v>303</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>8</v>
@@ -5059,7 +5059,7 @@
         <v>305</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>8</v>
@@ -5076,7 +5076,7 @@
         <v>307</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>8</v>
@@ -5093,7 +5093,7 @@
         <v>309</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>8</v>
@@ -5110,7 +5110,7 @@
         <v>311</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>8</v>
@@ -5127,7 +5127,7 @@
         <v>313</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>8</v>
@@ -5144,7 +5144,7 @@
         <v>315</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>8</v>
@@ -5161,7 +5161,7 @@
         <v>317</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>8</v>
@@ -5178,7 +5178,7 @@
         <v>319</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>8</v>
@@ -5195,7 +5195,7 @@
         <v>321</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>8</v>
@@ -5212,7 +5212,7 @@
         <v>323</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>8</v>
@@ -5229,7 +5229,7 @@
         <v>325</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>8</v>
@@ -5246,7 +5246,7 @@
         <v>327</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>8</v>
@@ -5263,7 +5263,7 @@
         <v>266</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>8</v>
@@ -5280,7 +5280,7 @@
         <v>268</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>8</v>
@@ -5297,7 +5297,7 @@
         <v>331</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>8</v>
@@ -5311,10 +5311,10 @@
         <v>299</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>8</v>
@@ -5331,7 +5331,7 @@
         <v>271</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>8</v>
@@ -5348,7 +5348,7 @@
         <v>335</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>8</v>
@@ -5359,7 +5359,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D27:D182 E2:E8 E27:E28 E29:E182 F2:F3 D9:E26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E24 D1:D8 D24:D44 D45:D74 E2:E8 E25:E44 E45:E53 E54:E74 F2:F3 D9:E23 D75:E182">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fixed RW02, RW07, RW08, RW10 issues
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -2246,8 +2246,8 @@
   <sheetPr/>
   <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -5359,7 +5359,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E24 D1:D8 D24:D44 D45:D74 E2:E8 E25:E44 E45:E53 E54:E74 F2:F3 D9:E23 D75:E182">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E45 E109 E110 D1:D8 D45:D74 D109:D123 E2:E8 E46:E74 E111:E121 E122:E123 F2:F3 D124:E158 D159:E182 D9:E44 D75:E108">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update code as per enhancements
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="336">
   <si>
     <t>ID</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>Open Estate</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
   <si>
     <t>TC_026</t>
@@ -2243,8 +2246,8 @@
   <sheetPr/>
   <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68:D104"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2693,7 +2696,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>8</v>
@@ -2701,16 +2704,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>8</v>
@@ -2718,16 +2721,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>8</v>
@@ -2735,16 +2738,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>8</v>
@@ -2752,16 +2755,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>8</v>
@@ -2769,16 +2772,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>8</v>
@@ -2786,16 +2789,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>8</v>
@@ -2803,16 +2806,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>8</v>
@@ -2820,16 +2823,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>8</v>
@@ -2837,16 +2840,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>8</v>
@@ -2854,16 +2857,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>8</v>
@@ -2871,16 +2874,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>8</v>
@@ -2888,16 +2891,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>8</v>
@@ -2905,16 +2908,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>8</v>
@@ -2922,16 +2925,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>8</v>
@@ -2939,16 +2942,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>8</v>
@@ -2956,16 +2959,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>8</v>
@@ -2973,16 +2976,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>8</v>
@@ -2990,16 +2993,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>8</v>
@@ -3007,16 +3010,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -3024,16 +3027,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="C46" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -3041,16 +3044,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -3058,16 +3061,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -3075,16 +3078,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -3092,16 +3095,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -3109,16 +3112,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -3126,16 +3129,16 @@
     </row>
     <row r="52" ht="28" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -3143,16 +3146,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -3160,16 +3163,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -3177,16 +3180,16 @@
     </row>
     <row r="55" ht="28" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -3194,16 +3197,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -3211,16 +3214,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -3228,16 +3231,16 @@
     </row>
     <row r="58" ht="28" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -3245,16 +3248,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -3262,16 +3265,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -3279,16 +3282,16 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -3296,16 +3299,16 @@
     </row>
     <row r="62" ht="28" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3313,16 +3316,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3330,16 +3333,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3347,16 +3350,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3364,16 +3367,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3381,16 +3384,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3398,16 +3401,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3415,16 +3418,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3432,16 +3435,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3449,16 +3452,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3466,16 +3469,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3483,16 +3486,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3500,13 +3503,13 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>8</v>
@@ -3517,16 +3520,16 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>8</v>
@@ -3534,16 +3537,16 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>8</v>
@@ -3551,16 +3554,16 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B77" s="7" t="s">
-        <v>157</v>
-      </c>
       <c r="C77" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>8</v>
@@ -3568,16 +3571,16 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>8</v>
@@ -3585,16 +3588,16 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>8</v>
@@ -3602,16 +3605,16 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>8</v>
@@ -3619,16 +3622,16 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>8</v>
@@ -3636,16 +3639,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>8</v>
@@ -3653,16 +3656,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>8</v>
@@ -3670,16 +3673,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>8</v>
@@ -3687,16 +3690,16 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>8</v>
@@ -3704,16 +3707,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>8</v>
@@ -3721,16 +3724,16 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>8</v>
@@ -3738,16 +3741,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>178</v>
-      </c>
       <c r="C88" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>8</v>
@@ -3755,16 +3758,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>8</v>
@@ -3772,16 +3775,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>8</v>
@@ -3789,16 +3792,16 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>8</v>
@@ -3806,16 +3809,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>8</v>
@@ -3823,16 +3826,16 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>8</v>
@@ -3840,16 +3843,16 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>8</v>
@@ -3857,16 +3860,16 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>8</v>
@@ -3874,16 +3877,16 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>8</v>
@@ -3891,16 +3894,16 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -3908,16 +3911,16 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -3925,16 +3928,16 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -3942,16 +3945,16 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B100" s="7" t="s">
-        <v>196</v>
-      </c>
       <c r="C100" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -3959,16 +3962,16 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -3976,16 +3979,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -3993,16 +3996,16 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -4010,16 +4013,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -4027,16 +4030,16 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -4044,16 +4047,16 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -4061,16 +4064,16 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -4078,16 +4081,16 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -4095,16 +4098,16 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -4112,16 +4115,16 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -4129,16 +4132,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -4146,16 +4149,16 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B112" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B112" s="7" t="s">
-        <v>211</v>
-      </c>
       <c r="C112" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -4163,16 +4166,16 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -4180,16 +4183,16 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -4197,16 +4200,16 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -4214,16 +4217,16 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -4231,16 +4234,16 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -4248,16 +4251,16 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -4265,16 +4268,16 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4282,16 +4285,16 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4299,16 +4302,16 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4316,16 +4319,16 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4333,16 +4336,16 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>8</v>
@@ -4350,16 +4353,16 @@
     </row>
     <row r="124" ht="28" spans="1:5">
       <c r="A124" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B124" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B124" s="7" t="s">
-        <v>231</v>
-      </c>
       <c r="C124" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>8</v>
@@ -4367,16 +4370,16 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>8</v>
@@ -4384,16 +4387,16 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>8</v>
@@ -4401,16 +4404,16 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>8</v>
@@ -4418,16 +4421,16 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>8</v>
@@ -4435,16 +4438,16 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>8</v>
@@ -4452,16 +4455,16 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>8</v>
@@ -4469,16 +4472,16 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B131" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="B131" s="7" t="s">
-        <v>244</v>
-      </c>
       <c r="C131" s="7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -4486,16 +4489,16 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>8</v>
@@ -4503,16 +4506,16 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>8</v>
@@ -4520,16 +4523,16 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -4537,16 +4540,16 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -4554,16 +4557,16 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -4571,16 +4574,16 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -4588,16 +4591,16 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>8</v>
@@ -4605,16 +4608,16 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>8</v>
@@ -4622,16 +4625,16 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>8</v>
@@ -4639,16 +4642,16 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C141" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -4656,16 +4659,16 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C142" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -4673,16 +4676,16 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -4690,16 +4693,16 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>8</v>
@@ -4707,16 +4710,16 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C145" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>8</v>
@@ -4724,16 +4727,16 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>8</v>
@@ -4741,16 +4744,16 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B147" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="B147" s="7" t="s">
-        <v>274</v>
-      </c>
       <c r="C147" s="7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>8</v>
@@ -4758,16 +4761,16 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>8</v>
@@ -4775,16 +4778,16 @@
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C149" s="7" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>8</v>
@@ -4792,16 +4795,16 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>8</v>
@@ -4809,16 +4812,16 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>8</v>
@@ -4826,16 +4829,16 @@
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C152" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>8</v>
@@ -4843,16 +4846,16 @@
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C153" s="7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>8</v>
@@ -4860,16 +4863,16 @@
     </row>
     <row r="154" ht="28" spans="1:5">
       <c r="A154" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>8</v>
@@ -4877,16 +4880,16 @@
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>8</v>
@@ -4894,16 +4897,16 @@
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C156" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>8</v>
@@ -4911,16 +4914,16 @@
     </row>
     <row r="157" ht="28" spans="1:5">
       <c r="A157" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>8</v>
@@ -4928,16 +4931,16 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C158" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>8</v>
@@ -4945,16 +4948,16 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C159" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>8</v>
@@ -4962,16 +4965,16 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="3" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>8</v>
@@ -4979,16 +4982,16 @@
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C161" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>8</v>
@@ -4996,16 +4999,16 @@
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="3" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C162" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>8</v>
@@ -5013,16 +5016,16 @@
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B163" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="B163" s="7" t="s">
-        <v>298</v>
-      </c>
       <c r="C163" s="7" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>8</v>
@@ -5030,16 +5033,16 @@
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C164" s="7" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>8</v>
@@ -5047,16 +5050,16 @@
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C165" s="7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>8</v>
@@ -5064,16 +5067,16 @@
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C166" s="7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>8</v>
@@ -5081,16 +5084,16 @@
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C167" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>8</v>
@@ -5098,16 +5101,16 @@
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C168" s="7" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>8</v>
@@ -5115,16 +5118,16 @@
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C169" s="7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>8</v>
@@ -5132,16 +5135,16 @@
     </row>
     <row r="170" spans="1:5">
       <c r="A170" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C170" s="7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>8</v>
@@ -5149,16 +5152,16 @@
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C171" s="7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>8</v>
@@ -5166,16 +5169,16 @@
     </row>
     <row r="172" spans="1:5">
       <c r="A172" s="3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C172" s="7" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>8</v>
@@ -5183,16 +5186,16 @@
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C173" s="7" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>8</v>
@@ -5200,16 +5203,16 @@
     </row>
     <row r="174" spans="1:5">
       <c r="A174" s="3" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C174" s="7" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>8</v>
@@ -5217,16 +5220,16 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C175" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>8</v>
@@ -5234,16 +5237,16 @@
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B176" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C176" s="7" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>8</v>
@@ -5251,16 +5254,16 @@
     </row>
     <row r="177" spans="1:5">
       <c r="A177" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C177" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>8</v>
@@ -5268,16 +5271,16 @@
     </row>
     <row r="178" spans="1:5">
       <c r="A178" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C178" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>8</v>
@@ -5285,16 +5288,16 @@
     </row>
     <row r="179" ht="28" spans="1:5">
       <c r="A179" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>8</v>
@@ -5302,16 +5305,16 @@
     </row>
     <row r="180" spans="1:5">
       <c r="A180" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>8</v>
@@ -5319,16 +5322,16 @@
     </row>
     <row r="181" spans="1:5">
       <c r="A181" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C181" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>8</v>
@@ -5336,16 +5339,16 @@
     </row>
     <row r="182" spans="1:5">
       <c r="A182" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B182" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C182" s="7" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>8</v>
@@ -5356,7 +5359,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D68:D104 E2:E8 E68:E74 E75:E86 E87:E104 F2:F3 D37:E67 D9:E36 D105:E182">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E28 D1:D8 D26:D182 E2:E8 E26:E27 E29:E35 E36:E44 E45:E75 E76:E182 F2:F3 D9:E25">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added 3 TCs of OC01 form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -2246,8 +2246,8 @@
   <sheetPr/>
   <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:D182"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -5359,7 +5359,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D26:D182 E2:E8 E26:E27 E28:E44 E45:E75 E76:E182 F2:F3 D9:E22 D23:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 E2:E8 F2:F3 D26:E182 D9:E25">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
resolved issues of RW01, RW02 and RW06 and added TCs of OC02 form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6350" tabRatio="500"/>
+    <workbookView windowWidth="19200" windowHeight="6800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioMapping" sheetId="1" r:id="rId1"/>
@@ -206,655 +206,655 @@
     <t>Open Estate</t>
   </si>
   <si>
+    <t>TC_026</t>
+  </si>
+  <si>
+    <t>Verify, file no. is displayed at the top of the form.</t>
+  </si>
+  <si>
+    <t>TC_027</t>
+  </si>
+  <si>
+    <t>Verify, decedent information is displayed in section1 of the form.</t>
+  </si>
+  <si>
+    <t>TC_028</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 2 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_029</t>
+  </si>
+  <si>
+    <t>Verify, in section 2 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_030</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 3 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_031</t>
+  </si>
+  <si>
+    <t>Verify, in section 3 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_032</t>
+  </si>
+  <si>
+    <t>Verify, on clicking other checkbox, text area is enabled.</t>
+  </si>
+  <si>
+    <t>TC_033</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 4 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_034</t>
+  </si>
+  <si>
+    <t>Verify, on clicking last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_035</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_036</t>
+  </si>
+  <si>
+    <t>Verify, on selecting the contact its information is displayed in section 4.</t>
+  </si>
+  <si>
+    <t>TC_037</t>
+  </si>
+  <si>
+    <t>Verify, on clicking executor last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_038</t>
+  </si>
+  <si>
+    <t>Verify, 3 types of selection is available.</t>
+  </si>
+  <si>
+    <t>TC_039</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be dragged and dropped in a each of the type.</t>
+  </si>
+  <si>
+    <t>TC_040</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 5 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_041</t>
+  </si>
+  <si>
+    <t>Verify the selected contacts are displayed under executor, co executor and secondary co executor.</t>
+  </si>
+  <si>
+    <t>TC_042</t>
+  </si>
+  <si>
+    <t>Verify form can be printed in pdf</t>
+  </si>
+  <si>
+    <t>TC_043</t>
+  </si>
+  <si>
+    <t>Reset the RW01 form</t>
+  </si>
+  <si>
+    <t>TC_044</t>
+  </si>
+  <si>
+    <t>probateFormsRW02.feature</t>
+  </si>
+  <si>
+    <t>TC_045</t>
+  </si>
+  <si>
+    <t>Verify, correct county name is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_046</t>
+  </si>
+  <si>
+    <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
+  </si>
+  <si>
+    <t>TC_047</t>
+  </si>
+  <si>
+    <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
+  </si>
+  <si>
+    <t>TC_048</t>
+  </si>
+  <si>
+    <t>Verify, county, estate and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_049</t>
+  </si>
+  <si>
+    <t>Verify, the auto populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_050</t>
+  </si>
+  <si>
+    <t>Verify, names can be added in aka fields.</t>
+  </si>
+  <si>
+    <t>TC_051</t>
+  </si>
+  <si>
+    <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
+  </si>
+  <si>
+    <t>TC_052</t>
+  </si>
+  <si>
+    <t>Verify, amount can be entered in the input fields.</t>
+  </si>
+  <si>
+    <t>TC_053</t>
+  </si>
+  <si>
+    <t>Verify, total estimated value should display total of 1st and last field only.</t>
+  </si>
+  <si>
+    <t>TC_054</t>
+  </si>
+  <si>
+    <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_055</t>
+  </si>
+  <si>
+    <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
+  </si>
+  <si>
+    <t>TC_056</t>
+  </si>
+  <si>
+    <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
+  </si>
+  <si>
+    <t>TC_057</t>
+  </si>
+  <si>
+    <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
+  </si>
+  <si>
+    <t>TC_058</t>
+  </si>
+  <si>
+    <t>Verify that selecting option A keeps it selected without affecting option B.</t>
+  </si>
+  <si>
+    <t>TC_059</t>
+  </si>
+  <si>
+    <t>Verify, decedent died date is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_060</t>
+  </si>
+  <si>
+    <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
+  </si>
+  <si>
+    <t>TC_061</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
+  </si>
+  <si>
+    <t>TC_062</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B keeps it selected without affecting option A.</t>
+  </si>
+  <si>
+    <t>TC_063</t>
+  </si>
+  <si>
+    <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
+  </si>
+  <si>
+    <t>TC_064</t>
+  </si>
+  <si>
+    <t>Verify, multiple beneficiaries can be selected.</t>
+  </si>
+  <si>
+    <t>TC_065</t>
+  </si>
+  <si>
+    <t>Verify, bene contacts in the table.</t>
+  </si>
+  <si>
+    <t>TC_066</t>
+  </si>
+  <si>
+    <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
+  </si>
+  <si>
+    <t>TC_067</t>
+  </si>
+  <si>
+    <t>Verify, on checking "Display all heirs on attachment".</t>
+  </si>
+  <si>
+    <t>TC_068</t>
+  </si>
+  <si>
+    <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
+  </si>
+  <si>
+    <t>TC_069</t>
+  </si>
+  <si>
+    <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
+  </si>
+  <si>
+    <t>TC_070</t>
+  </si>
+  <si>
+    <t>Verify fees section.</t>
+  </si>
+  <si>
+    <t>TC_071</t>
+  </si>
+  <si>
+    <t>Verify, attorney can be selected.</t>
+  </si>
+  <si>
+    <t>TC_072</t>
+  </si>
+  <si>
+    <t>Verify, information in decree of the register.</t>
+  </si>
+  <si>
+    <t>TC_073</t>
+  </si>
+  <si>
+    <t>TC_074</t>
+  </si>
+  <si>
+    <t>Reset the RW02 form</t>
+  </si>
+  <si>
+    <t>TC_075</t>
+  </si>
+  <si>
+    <t>probateFormsRW03.feature</t>
+  </si>
+  <si>
+    <t>TC_076</t>
+  </si>
+  <si>
+    <t>Verify county, estate and aka names are auto-populated on the form</t>
+  </si>
+  <si>
+    <t>TC_077</t>
+  </si>
+  <si>
+    <t>Verify, the auto-populated fields are not editable.</t>
+  </si>
+  <si>
+    <t>TC_078</t>
+  </si>
+  <si>
+    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
+  </si>
+  <si>
+    <t>TC_079</t>
+  </si>
+  <si>
+    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
+  </si>
+  <si>
+    <t>TC_080</t>
+  </si>
+  <si>
+    <t>Verify, names can be entered in witness fields.</t>
+  </si>
+  <si>
+    <t>TC_081</t>
+  </si>
+  <si>
+    <t>Verify, names updated from signature are reflected in witness names fields.</t>
+  </si>
+  <si>
+    <t>TC_082</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered in address, city, zip fields.</t>
+  </si>
+  <si>
+    <t>TC_083</t>
+  </si>
+  <si>
+    <t>Verify, form is auto saved.</t>
+  </si>
+  <si>
+    <t>TC_084</t>
+  </si>
+  <si>
+    <t>TC_085</t>
+  </si>
+  <si>
+    <t>Reset the RW03 form</t>
+  </si>
+  <si>
+    <t>TC_086</t>
+  </si>
+  <si>
+    <t>probateFormsRW04.feature</t>
+  </si>
+  <si>
+    <t>TC_087</t>
+  </si>
+  <si>
+    <t>Verify, correct title is displayed on the form's header.</t>
+  </si>
+  <si>
+    <t>TC_088</t>
+  </si>
+  <si>
+    <t>Verify, county, and aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_089</t>
+  </si>
+  <si>
+    <t>Verify, correct estate's name is displayed on the form.</t>
+  </si>
+  <si>
+    <t>TC_090</t>
+  </si>
+  <si>
+    <t>Verify, name of the decedent should be auto populated from the form.</t>
+  </si>
+  <si>
+    <t>TC_091</t>
+  </si>
+  <si>
+    <t>TC_092</t>
+  </si>
+  <si>
+    <t>TC_093</t>
+  </si>
+  <si>
+    <t>TC_094</t>
+  </si>
+  <si>
+    <t>TC_095</t>
+  </si>
+  <si>
+    <t>TC_096</t>
+  </si>
+  <si>
+    <t>TC_097</t>
+  </si>
+  <si>
+    <t>Reset the RW04 form</t>
+  </si>
+  <si>
+    <t>TC_098</t>
+  </si>
+  <si>
+    <t>probateFormsRW05.feature</t>
+  </si>
+  <si>
+    <t>TC_099</t>
+  </si>
+  <si>
+    <t>TC_100</t>
+  </si>
+  <si>
+    <t>TC_101</t>
+  </si>
+  <si>
+    <t>TC_102</t>
+  </si>
+  <si>
+    <t>TC_103</t>
+  </si>
+  <si>
+    <t>TC_104</t>
+  </si>
+  <si>
+    <t>TC_105</t>
+  </si>
+  <si>
+    <t>TC_106</t>
+  </si>
+  <si>
+    <t>Verify, on checking notary checkbox, notary section displays.</t>
+  </si>
+  <si>
+    <t>TC_107</t>
+  </si>
+  <si>
+    <t>TC_108</t>
+  </si>
+  <si>
+    <t>TC_109</t>
+  </si>
+  <si>
+    <t>Reset the RW05 form</t>
+  </si>
+  <si>
+    <t>TC_110</t>
+  </si>
+  <si>
+    <t>probateFormsRW06.feature</t>
+  </si>
+  <si>
+    <t>TC_111</t>
+  </si>
+  <si>
+    <t>TC_112</t>
+  </si>
+  <si>
+    <t>TC_113</t>
+  </si>
+  <si>
+    <t>Verify, form is repeated based on the number of contacts selected.</t>
+  </si>
+  <si>
+    <t>TC_114</t>
+  </si>
+  <si>
+    <t>Verify, corporate fiduciary selected is reflected in the corporate name field.</t>
+  </si>
+  <si>
+    <t>TC_115</t>
+  </si>
+  <si>
+    <t>Verify, details of the selected contact's is displayed in the block under it.</t>
+  </si>
+  <si>
+    <t>TC_116</t>
+  </si>
+  <si>
+    <t>Verify, on clicking signature of person, beneficiary contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_117</t>
+  </si>
+  <si>
+    <t>TC_118</t>
+  </si>
+  <si>
+    <t>Verify, contact details are correctly displayed on each page.</t>
+  </si>
+  <si>
+    <t>TC_119</t>
+  </si>
+  <si>
+    <t>Verify, date and reason text box fields are not same for each field.</t>
+  </si>
+  <si>
+    <t>TC_120</t>
+  </si>
+  <si>
+    <t>TC_121</t>
+  </si>
+  <si>
+    <t>Reset the RW06 form</t>
+  </si>
+  <si>
+    <t>TC_122</t>
+  </si>
+  <si>
+    <t>probateFormsRWxx.feature</t>
+  </si>
+  <si>
+    <t>TC_123</t>
+  </si>
+  <si>
+    <t>Verify that the county, estate name, and "Also Known As" (AKA) values are auto-populated from the selected estate.</t>
+  </si>
+  <si>
+    <t>TC_124</t>
+  </si>
+  <si>
+    <t>Verify, text can be entered in all the text areas.</t>
+  </si>
+  <si>
+    <t>TC_125</t>
+  </si>
+  <si>
+    <t>Verify, the name entered in 1st text area is reflected in the signature.</t>
+  </si>
+  <si>
+    <t>TC_126</t>
+  </si>
+  <si>
+    <t>Verify that changes in the witness name field are reflected under the signature line and vice-versa.</t>
+  </si>
+  <si>
+    <t>TC_127</t>
+  </si>
+  <si>
+    <t>TC_128</t>
+  </si>
+  <si>
+    <t>Reset the RWxx form</t>
+  </si>
+  <si>
+    <t>TC_129</t>
+  </si>
+  <si>
+    <t>probateFormsRW07.feature</t>
+  </si>
+  <si>
+    <t>TC_130</t>
+  </si>
+  <si>
+    <t>Verify, county, estate and file number aka names are auto populated on the form.</t>
+  </si>
+  <si>
+    <t>TC_131</t>
+  </si>
+  <si>
+    <t>TC_132</t>
+  </si>
+  <si>
+    <t>Verify, on checking use 4 digit checkbox, changes in file number</t>
+  </si>
+  <si>
+    <t>TC_133</t>
+  </si>
+  <si>
+    <t>Verify, on clicking bene address field, multiple beneficiaries can be selected.</t>
+  </si>
+  <si>
+    <t>TC_134</t>
+  </si>
+  <si>
+    <t>Verify, beneficiary name and address should be displayed in the form.</t>
+  </si>
+  <si>
+    <t>TC_135</t>
+  </si>
+  <si>
+    <t>Verify, decedent died and county is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_136</t>
+  </si>
+  <si>
+    <t>Verify, on clicking name fiduciary contact list is displayed and multiple users can be selected.</t>
+  </si>
+  <si>
+    <t>TC_137</t>
+  </si>
+  <si>
+    <t>Verify, these contacts are common for all the forms.</t>
+  </si>
+  <si>
+    <t>TC_138</t>
+  </si>
+  <si>
+    <t>Verify, date can be entered.</t>
+  </si>
+  <si>
+    <t>TC_139</t>
+  </si>
+  <si>
+    <t>Verify, registrars address is auto fetched and is editable.</t>
+  </si>
+  <si>
+    <t>TC_140</t>
+  </si>
+  <si>
+    <t>Verify, corporate fiduciary type of contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_141</t>
+  </si>
+  <si>
+    <t>Verify, based on capacity contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_142</t>
+  </si>
+  <si>
+    <t>TC_143</t>
+  </si>
+  <si>
+    <t>Verify, selection is cleared on clicking clear selection button.</t>
+  </si>
+  <si>
+    <t>TC_144</t>
+  </si>
+  <si>
+    <t>Reset the RW07 form</t>
+  </si>
+  <si>
+    <t>TC_145</t>
+  </si>
+  <si>
+    <t>probateFormsRW08.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_026</t>
-  </si>
-  <si>
-    <t>Verify, file no. is displayed at the top of the form.</t>
-  </si>
-  <si>
-    <t>TC_027</t>
-  </si>
-  <si>
-    <t>Verify, decedent information is displayed in section1 of the form.</t>
-  </si>
-  <si>
-    <t>TC_028</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 2 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_029</t>
-  </si>
-  <si>
-    <t>Verify, in section 2 only 1 checkbox can be checked.</t>
-  </si>
-  <si>
-    <t>TC_030</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 3 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_031</t>
-  </si>
-  <si>
-    <t>Verify, in section 3 only 1 checkbox can be checked.</t>
-  </si>
-  <si>
-    <t>TC_032</t>
-  </si>
-  <si>
-    <t>Verify, on clicking other checkbox, text area is enabled.</t>
-  </si>
-  <si>
-    <t>TC_033</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 4 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_034</t>
-  </si>
-  <si>
-    <t>Verify, on clicking last name, a side bar is displayed.</t>
-  </si>
-  <si>
-    <t>TC_035</t>
-  </si>
-  <si>
-    <t>Verify, only 1 contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_036</t>
-  </si>
-  <si>
-    <t>Verify, on selecting the contact its information is displayed in section 4.</t>
-  </si>
-  <si>
-    <t>TC_037</t>
-  </si>
-  <si>
-    <t>Verify, on clicking executor last name, a side bar is displayed.</t>
-  </si>
-  <si>
-    <t>TC_038</t>
-  </si>
-  <si>
-    <t>Verify, 3 types of selection is available.</t>
-  </si>
-  <si>
-    <t>TC_039</t>
-  </si>
-  <si>
-    <t>Verify, only 1 contact can be dragged and dropped in a each of the type.</t>
-  </si>
-  <si>
-    <t>TC_040</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 5 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_041</t>
-  </si>
-  <si>
-    <t>Verify the selected contacts are displayed under executor, co executor and secondary co executor.</t>
-  </si>
-  <si>
-    <t>TC_042</t>
-  </si>
-  <si>
-    <t>Verify form can be printed in pdf</t>
-  </si>
-  <si>
-    <t>TC_043</t>
-  </si>
-  <si>
-    <t>Reset the RW01 form</t>
-  </si>
-  <si>
-    <t>TC_044</t>
-  </si>
-  <si>
-    <t>probateFormsRW02.feature</t>
-  </si>
-  <si>
-    <t>TC_045</t>
-  </si>
-  <si>
-    <t>Verify, correct county name is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_046</t>
-  </si>
-  <si>
-    <t>Verify, names of fiduciary type of contact is displayed at the top.</t>
-  </si>
-  <si>
-    <t>TC_047</t>
-  </si>
-  <si>
-    <t>Verify, if the names exceed the line, contacts are displayed in the attachment.</t>
-  </si>
-  <si>
-    <t>TC_048</t>
-  </si>
-  <si>
-    <t>Verify, county, estate and aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_049</t>
-  </si>
-  <si>
-    <t>Verify, the auto populated fields are not editable.</t>
-  </si>
-  <si>
-    <t>TC_050</t>
-  </si>
-  <si>
-    <t>Verify, names can be added in aka fields.</t>
-  </si>
-  <si>
-    <t>TC_051</t>
-  </si>
-  <si>
-    <t>Verify, values can be selected from the dropdown of "Estimate of value of decedents property at death"</t>
-  </si>
-  <si>
-    <t>TC_052</t>
-  </si>
-  <si>
-    <t>Verify, amount can be entered in the input fields.</t>
-  </si>
-  <si>
-    <t>TC_053</t>
-  </si>
-  <si>
-    <t>Verify, total estimated value should display total of 1st and last field only.</t>
-  </si>
-  <si>
-    <t>TC_054</t>
-  </si>
-  <si>
-    <t>Verify that checking the "Use Principal Residence" checkbox copies the address details from the "principal residence at" field to the "Real estate in Pennsylvania situated at" field.</t>
-  </si>
-  <si>
-    <t>TC_055</t>
-  </si>
-  <si>
-    <t>Verify that unchecking the checkbox does not clear the "Real estate in Pennsylvania situated at" field.</t>
-  </si>
-  <si>
-    <t>TC_056</t>
-  </si>
-  <si>
-    <t>Verify that the form auto-saves after the address is copied via the checkbox.</t>
-  </si>
-  <si>
-    <t>TC_057</t>
-  </si>
-  <si>
-    <t>Verify that the "Real estate in Pennsylvania situated at" field remains editable after copying the address.</t>
-  </si>
-  <si>
-    <t>TC_058</t>
-  </si>
-  <si>
-    <t>Verify that selecting option A keeps it selected without affecting option B.</t>
-  </si>
-  <si>
-    <t>TC_059</t>
-  </si>
-  <si>
-    <t>Verify, decedent died date is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_060</t>
-  </si>
-  <si>
-    <t>Verify, codicil dates are auto fetched and on updating it, updates the values in decedent tab.</t>
-  </si>
-  <si>
-    <t>TC_061</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered state relevant circumstances and exception on checking exceptions checkbox.</t>
-  </si>
-  <si>
-    <t>TC_062</t>
-  </si>
-  <si>
-    <t>Verify that selecting option B keeps it selected without affecting option A.</t>
-  </si>
-  <si>
-    <t>TC_063</t>
-  </si>
-  <si>
-    <t>Verify that selecting option B enables the beneficiaries' selection at the bottom of page 1.</t>
-  </si>
-  <si>
-    <t>TC_064</t>
-  </si>
-  <si>
-    <t>Verify, multiple beneficiaries can be selected.</t>
-  </si>
-  <si>
-    <t>TC_065</t>
-  </si>
-  <si>
-    <t>Verify, bene contacts in the table.</t>
-  </si>
-  <si>
-    <t>TC_066</t>
-  </si>
-  <si>
-    <t>Verify, if the selected contacts are exceed count of 4 then, it should be transferred to attachment.</t>
-  </si>
-  <si>
-    <t>TC_067</t>
-  </si>
-  <si>
-    <t>Verify, on checking "Display all heirs on attachment".</t>
-  </si>
-  <si>
-    <t>TC_068</t>
-  </si>
-  <si>
-    <t>Verify that deselecting option B disables the beneficiaries' selection.</t>
-  </si>
-  <si>
-    <t>TC_069</t>
-  </si>
-  <si>
-    <t>Verify, on page 2 petitioner's name are by default printed on the table.</t>
-  </si>
-  <si>
-    <t>TC_070</t>
-  </si>
-  <si>
-    <t>Verify fees section.</t>
-  </si>
-  <si>
-    <t>TC_071</t>
-  </si>
-  <si>
-    <t>Verify, attorney can be selected.</t>
-  </si>
-  <si>
-    <t>TC_072</t>
-  </si>
-  <si>
-    <t>Verify, information in decree of the register.</t>
-  </si>
-  <si>
-    <t>TC_073</t>
-  </si>
-  <si>
-    <t>TC_074</t>
-  </si>
-  <si>
-    <t>Reset the RW02 form</t>
-  </si>
-  <si>
-    <t>TC_075</t>
-  </si>
-  <si>
-    <t>probateFormsRW03.feature</t>
-  </si>
-  <si>
-    <t>TC_076</t>
-  </si>
-  <si>
-    <t>Verify county, estate and aka names are auto-populated on the form</t>
-  </si>
-  <si>
-    <t>TC_077</t>
-  </si>
-  <si>
-    <t>Verify, the auto-populated fields are not editable.</t>
-  </si>
-  <si>
-    <t>TC_078</t>
-  </si>
-  <si>
-    <t>Verify, witness's name is not auto populated and the fields are empty.</t>
-  </si>
-  <si>
-    <t>TC_079</t>
-  </si>
-  <si>
-    <t>Verify, witnesses  name, address and signature should be editable and in yellow background.</t>
-  </si>
-  <si>
-    <t>TC_080</t>
-  </si>
-  <si>
-    <t>Verify, names can be entered in witness fields.</t>
-  </si>
-  <si>
-    <t>TC_081</t>
-  </si>
-  <si>
-    <t>Verify, names updated from signature are reflected in witness names fields.</t>
-  </si>
-  <si>
-    <t>TC_082</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered in address, city, zip fields.</t>
-  </si>
-  <si>
-    <t>TC_083</t>
-  </si>
-  <si>
-    <t>Verify, form is auto saved.</t>
-  </si>
-  <si>
-    <t>TC_084</t>
-  </si>
-  <si>
-    <t>TC_085</t>
-  </si>
-  <si>
-    <t>Reset the RW03 form</t>
-  </si>
-  <si>
-    <t>TC_086</t>
-  </si>
-  <si>
-    <t>probateFormsRW04.feature</t>
-  </si>
-  <si>
-    <t>TC_087</t>
-  </si>
-  <si>
-    <t>Verify, correct title is displayed on the form's header.</t>
-  </si>
-  <si>
-    <t>TC_088</t>
-  </si>
-  <si>
-    <t>Verify, county, and aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_089</t>
-  </si>
-  <si>
-    <t>Verify, correct estate's name is displayed on the form.</t>
-  </si>
-  <si>
-    <t>TC_090</t>
-  </si>
-  <si>
-    <t>Verify, name of the decedent should be auto populated from the form.</t>
-  </si>
-  <si>
-    <t>TC_091</t>
-  </si>
-  <si>
-    <t>TC_092</t>
-  </si>
-  <si>
-    <t>TC_093</t>
-  </si>
-  <si>
-    <t>TC_094</t>
-  </si>
-  <si>
-    <t>TC_095</t>
-  </si>
-  <si>
-    <t>TC_096</t>
-  </si>
-  <si>
-    <t>TC_097</t>
-  </si>
-  <si>
-    <t>Reset the RW04 form</t>
-  </si>
-  <si>
-    <t>TC_098</t>
-  </si>
-  <si>
-    <t>probateFormsRW05.feature</t>
-  </si>
-  <si>
-    <t>TC_099</t>
-  </si>
-  <si>
-    <t>TC_100</t>
-  </si>
-  <si>
-    <t>TC_101</t>
-  </si>
-  <si>
-    <t>TC_102</t>
-  </si>
-  <si>
-    <t>TC_103</t>
-  </si>
-  <si>
-    <t>TC_104</t>
-  </si>
-  <si>
-    <t>TC_105</t>
-  </si>
-  <si>
-    <t>TC_106</t>
-  </si>
-  <si>
-    <t>Verify, on checking notary checkbox, notary section displays.</t>
-  </si>
-  <si>
-    <t>TC_107</t>
-  </si>
-  <si>
-    <t>TC_108</t>
-  </si>
-  <si>
-    <t>TC_109</t>
-  </si>
-  <si>
-    <t>Reset the RW05 form</t>
-  </si>
-  <si>
-    <t>TC_110</t>
-  </si>
-  <si>
-    <t>probateFormsRW06.feature</t>
-  </si>
-  <si>
-    <t>TC_111</t>
-  </si>
-  <si>
-    <t>TC_112</t>
-  </si>
-  <si>
-    <t>TC_113</t>
-  </si>
-  <si>
-    <t>Verify, form is repeated based on the number of contacts selected.</t>
-  </si>
-  <si>
-    <t>TC_114</t>
-  </si>
-  <si>
-    <t>Verify, corporate fiduciary selected is reflected in the corporate name field.</t>
-  </si>
-  <si>
-    <t>TC_115</t>
-  </si>
-  <si>
-    <t>Verify, details of the selected contact's is displayed in the block under it.</t>
-  </si>
-  <si>
-    <t>TC_116</t>
-  </si>
-  <si>
-    <t>Verify, on clicking signature of person, beneficiary contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_117</t>
-  </si>
-  <si>
-    <t>TC_118</t>
-  </si>
-  <si>
-    <t>Verify, contact details are correctly displayed on each page.</t>
-  </si>
-  <si>
-    <t>TC_119</t>
-  </si>
-  <si>
-    <t>Verify, date and reason text box fields are not same for each field.</t>
-  </si>
-  <si>
-    <t>TC_120</t>
-  </si>
-  <si>
-    <t>TC_121</t>
-  </si>
-  <si>
-    <t>Reset the RW06 form</t>
-  </si>
-  <si>
-    <t>TC_122</t>
-  </si>
-  <si>
-    <t>probateFormsRWxx.feature</t>
-  </si>
-  <si>
-    <t>TC_123</t>
-  </si>
-  <si>
-    <t>Verify that the county, estate name, and "Also Known As" (AKA) values are auto-populated from the selected estate.</t>
-  </si>
-  <si>
-    <t>TC_124</t>
-  </si>
-  <si>
-    <t>Verify, text can be entered in all the text areas.</t>
-  </si>
-  <si>
-    <t>TC_125</t>
-  </si>
-  <si>
-    <t>Verify, the name entered in 1st text area is reflected in the signature.</t>
-  </si>
-  <si>
-    <t>TC_126</t>
-  </si>
-  <si>
-    <t>Verify that changes in the witness name field are reflected under the signature line and vice-versa.</t>
-  </si>
-  <si>
-    <t>TC_127</t>
-  </si>
-  <si>
-    <t>TC_128</t>
-  </si>
-  <si>
-    <t>Reset the RWxx form</t>
-  </si>
-  <si>
-    <t>TC_129</t>
-  </si>
-  <si>
-    <t>probateFormsRW07.feature</t>
-  </si>
-  <si>
-    <t>TC_130</t>
-  </si>
-  <si>
-    <t>Verify, county, estate and file number aka names are auto populated on the form.</t>
-  </si>
-  <si>
-    <t>TC_131</t>
-  </si>
-  <si>
-    <t>TC_132</t>
-  </si>
-  <si>
-    <t>Verify, on checking use 4 digit checkbox, changes in file number</t>
-  </si>
-  <si>
-    <t>TC_133</t>
-  </si>
-  <si>
-    <t>Verify, on clicking bene address field, multiple beneficiaries can be selected.</t>
-  </si>
-  <si>
-    <t>TC_134</t>
-  </si>
-  <si>
-    <t>Verify, beneficiary name and address should be displayed in the form.</t>
-  </si>
-  <si>
-    <t>TC_135</t>
-  </si>
-  <si>
-    <t>Verify, decedent died and county is auto fetched.</t>
-  </si>
-  <si>
-    <t>TC_136</t>
-  </si>
-  <si>
-    <t>Verify, on clicking name fiduciary contact list is displayed and multiple users can be selected.</t>
-  </si>
-  <si>
-    <t>TC_137</t>
-  </si>
-  <si>
-    <t>Verify, these contacts are common for all the forms.</t>
-  </si>
-  <si>
-    <t>TC_138</t>
-  </si>
-  <si>
-    <t>Verify, date can be entered.</t>
-  </si>
-  <si>
-    <t>TC_139</t>
-  </si>
-  <si>
-    <t>Verify, registrars address is auto fetched and is editable.</t>
-  </si>
-  <si>
-    <t>TC_140</t>
-  </si>
-  <si>
-    <t>Verify, corporate fiduciary type of contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_141</t>
-  </si>
-  <si>
-    <t>Verify, based on capacity contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_142</t>
-  </si>
-  <si>
-    <t>TC_143</t>
-  </si>
-  <si>
-    <t>Verify, selection is cleared on clicking clear selection button.</t>
-  </si>
-  <si>
-    <t>TC_144</t>
-  </si>
-  <si>
-    <t>Reset the RW07 form</t>
-  </si>
-  <si>
-    <t>TC_145</t>
-  </si>
-  <si>
-    <t>probateFormsRW08.feature</t>
   </si>
   <si>
     <t>TC_146</t>
@@ -2246,8 +2246,8 @@
   <sheetPr/>
   <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="C161" sqref="C161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2696,7 +2696,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>8</v>
@@ -2704,16 +2704,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>8</v>
@@ -2721,16 +2721,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>8</v>
@@ -2738,16 +2738,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>8</v>
@@ -2755,16 +2755,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>8</v>
@@ -2772,16 +2772,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>8</v>
@@ -2789,16 +2789,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>8</v>
@@ -2806,16 +2806,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>8</v>
@@ -2823,16 +2823,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>8</v>
@@ -2840,16 +2840,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>8</v>
@@ -2857,16 +2857,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>8</v>
@@ -2874,16 +2874,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>8</v>
@@ -2891,16 +2891,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>8</v>
@@ -2908,16 +2908,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>8</v>
@@ -2925,16 +2925,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>8</v>
@@ -2942,16 +2942,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>8</v>
@@ -2959,16 +2959,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>8</v>
@@ -2976,16 +2976,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>8</v>
@@ -2993,16 +2993,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>8</v>
@@ -3010,16 +3010,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -3027,16 +3027,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>99</v>
-      </c>
       <c r="D46" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -3044,16 +3044,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>101</v>
-      </c>
       <c r="D47" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -3061,16 +3061,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B48" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>103</v>
-      </c>
       <c r="D48" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -3078,16 +3078,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B49" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>105</v>
-      </c>
       <c r="D49" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -3095,16 +3095,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>107</v>
-      </c>
       <c r="D50" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -3112,16 +3112,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B51" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>109</v>
-      </c>
       <c r="D51" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -3129,16 +3129,16 @@
     </row>
     <row r="52" ht="28" spans="1:5">
       <c r="A52" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B52" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>111</v>
-      </c>
       <c r="D52" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -3146,16 +3146,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B53" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="D53" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -3163,16 +3163,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B54" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>115</v>
-      </c>
       <c r="D54" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -3180,16 +3180,16 @@
     </row>
     <row r="55" ht="28" spans="1:5">
       <c r="A55" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B55" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>117</v>
-      </c>
       <c r="D55" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -3197,16 +3197,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>119</v>
-      </c>
       <c r="D56" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -3214,16 +3214,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B57" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="D57" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -3231,16 +3231,16 @@
     </row>
     <row r="58" ht="28" spans="1:5">
       <c r="A58" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B58" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>123</v>
-      </c>
       <c r="D58" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -3248,16 +3248,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>125</v>
-      </c>
       <c r="D59" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -3265,16 +3265,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>127</v>
-      </c>
       <c r="D60" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -3282,16 +3282,16 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B61" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>129</v>
-      </c>
       <c r="D61" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -3299,16 +3299,16 @@
     </row>
     <row r="62" ht="28" spans="1:5">
       <c r="A62" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B62" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>131</v>
-      </c>
       <c r="D62" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3316,16 +3316,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B63" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>133</v>
-      </c>
       <c r="D63" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3333,16 +3333,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C64" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B64" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>135</v>
-      </c>
       <c r="D64" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3350,16 +3350,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B65" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>137</v>
-      </c>
       <c r="D65" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3367,16 +3367,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C66" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B66" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="D66" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3384,16 +3384,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C67" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>141</v>
-      </c>
       <c r="D67" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3401,16 +3401,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C68" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B68" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>143</v>
-      </c>
       <c r="D68" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3418,16 +3418,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C69" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="B69" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>145</v>
-      </c>
       <c r="D69" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3435,16 +3435,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C70" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B70" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>147</v>
-      </c>
       <c r="D70" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3452,16 +3452,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C71" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B71" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>149</v>
-      </c>
       <c r="D71" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3469,16 +3469,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C72" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B72" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>151</v>
-      </c>
       <c r="D72" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3486,16 +3486,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C73" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B73" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>153</v>
-      </c>
       <c r="D73" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3503,16 +3503,16 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>8</v>
@@ -3520,16 +3520,16 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C75" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B75" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>156</v>
-      </c>
       <c r="D75" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>8</v>
@@ -3537,16 +3537,16 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B76" s="7" t="s">
         <v>157</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>158</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>8</v>
@@ -3554,16 +3554,16 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C77" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B77" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>160</v>
-      </c>
       <c r="D77" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>8</v>
@@ -3571,16 +3571,16 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C78" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B78" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>162</v>
-      </c>
       <c r="D78" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>8</v>
@@ -3588,16 +3588,16 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C79" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="B79" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>164</v>
-      </c>
       <c r="D79" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>8</v>
@@ -3605,16 +3605,16 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="B80" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>166</v>
-      </c>
       <c r="D80" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>8</v>
@@ -3622,16 +3622,16 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C81" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="B81" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>168</v>
-      </c>
       <c r="D81" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>8</v>
@@ -3639,16 +3639,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C82" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="B82" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>170</v>
-      </c>
       <c r="D82" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>8</v>
@@ -3656,16 +3656,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C83" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="B83" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>172</v>
-      </c>
       <c r="D83" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>8</v>
@@ -3673,16 +3673,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="B84" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>174</v>
-      </c>
       <c r="D84" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>8</v>
@@ -3690,16 +3690,16 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>8</v>
@@ -3707,16 +3707,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C86" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B86" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>177</v>
-      </c>
       <c r="D86" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>8</v>
@@ -3724,16 +3724,16 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>8</v>
@@ -3741,16 +3741,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C88" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>181</v>
-      </c>
       <c r="D88" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>8</v>
@@ -3758,16 +3758,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C89" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="B89" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>183</v>
-      </c>
       <c r="D89" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>8</v>
@@ -3775,16 +3775,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C90" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B90" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>185</v>
-      </c>
       <c r="D90" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>8</v>
@@ -3792,16 +3792,16 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C91" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B91" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>187</v>
-      </c>
       <c r="D91" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>8</v>
@@ -3809,16 +3809,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>8</v>
@@ -3826,16 +3826,16 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>8</v>
@@ -3843,16 +3843,16 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>8</v>
@@ -3860,16 +3860,16 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>8</v>
@@ -3877,16 +3877,16 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>8</v>
@@ -3894,16 +3894,16 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -3911,16 +3911,16 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C98" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B98" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>195</v>
-      </c>
       <c r="D98" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -3928,16 +3928,16 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B99" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>197</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -3945,16 +3945,16 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -3962,16 +3962,16 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -3979,16 +3979,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -3996,16 +3996,16 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -4013,16 +4013,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -4030,16 +4030,16 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -4047,16 +4047,16 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -4064,16 +4064,16 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C107" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B107" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="C107" s="7" t="s">
-        <v>206</v>
-      </c>
       <c r="D107" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -4081,16 +4081,16 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -4098,16 +4098,16 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -4115,16 +4115,16 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C110" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="B110" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="C110" s="7" t="s">
-        <v>210</v>
-      </c>
       <c r="D110" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -4132,16 +4132,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B111" s="7" t="s">
         <v>211</v>
-      </c>
-      <c r="B111" s="7" t="s">
-        <v>212</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -4149,16 +4149,16 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -4166,16 +4166,16 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -4183,16 +4183,16 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C114" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="B114" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C114" s="7" t="s">
-        <v>216</v>
-      </c>
       <c r="D114" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -4200,16 +4200,16 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C115" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="B115" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C115" s="7" t="s">
-        <v>218</v>
-      </c>
       <c r="D115" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -4217,16 +4217,16 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C116" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="B116" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C116" s="7" t="s">
-        <v>220</v>
-      </c>
       <c r="D116" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -4234,16 +4234,16 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C117" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="B117" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C117" s="7" t="s">
-        <v>222</v>
-      </c>
       <c r="D117" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -4251,16 +4251,16 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -4268,16 +4268,16 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C119" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="B119" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>225</v>
-      </c>
       <c r="D119" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4285,16 +4285,16 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C120" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="B120" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C120" s="7" t="s">
-        <v>227</v>
-      </c>
       <c r="D120" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4302,16 +4302,16 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4319,16 +4319,16 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C122" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="B122" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C122" s="7" t="s">
-        <v>230</v>
-      </c>
       <c r="D122" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4336,16 +4336,16 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B123" s="7" t="s">
         <v>231</v>
-      </c>
-      <c r="B123" s="7" t="s">
-        <v>232</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>8</v>
@@ -4353,16 +4353,16 @@
     </row>
     <row r="124" ht="28" spans="1:5">
       <c r="A124" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C124" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="B124" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C124" s="9" t="s">
-        <v>234</v>
-      </c>
       <c r="D124" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>8</v>
@@ -4370,16 +4370,16 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C125" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="B125" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C125" s="7" t="s">
-        <v>236</v>
-      </c>
       <c r="D125" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>8</v>
@@ -4387,16 +4387,16 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C126" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="B126" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C126" s="7" t="s">
-        <v>238</v>
-      </c>
       <c r="D126" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>8</v>
@@ -4404,16 +4404,16 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C127" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="B127" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>240</v>
-      </c>
       <c r="D127" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>8</v>
@@ -4421,16 +4421,16 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>8</v>
@@ -4438,16 +4438,16 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C129" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="B129" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C129" s="7" t="s">
-        <v>243</v>
-      </c>
       <c r="D129" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>8</v>
@@ -4455,16 +4455,16 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B130" s="7" t="s">
         <v>244</v>
-      </c>
-      <c r="B130" s="7" t="s">
-        <v>245</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>8</v>
@@ -4472,16 +4472,16 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C131" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="B131" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C131" s="7" t="s">
-        <v>247</v>
-      </c>
       <c r="D131" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -4489,16 +4489,16 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>8</v>
@@ -4506,16 +4506,16 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C133" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="B133" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C133" s="7" t="s">
-        <v>250</v>
-      </c>
       <c r="D133" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>8</v>
@@ -4523,16 +4523,16 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C134" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="B134" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C134" s="7" t="s">
-        <v>252</v>
-      </c>
       <c r="D134" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -4540,16 +4540,16 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C135" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B135" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C135" s="7" t="s">
-        <v>254</v>
-      </c>
       <c r="D135" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -4557,16 +4557,16 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C136" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="B136" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C136" s="7" t="s">
-        <v>256</v>
-      </c>
       <c r="D136" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -4574,16 +4574,16 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C137" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="B137" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C137" s="7" t="s">
-        <v>258</v>
-      </c>
       <c r="D137" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -4591,16 +4591,16 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C138" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="B138" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C138" s="7" t="s">
-        <v>260</v>
-      </c>
       <c r="D138" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>8</v>
@@ -4608,16 +4608,16 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C139" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="B139" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C139" s="7" t="s">
-        <v>262</v>
-      </c>
       <c r="D139" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>8</v>
@@ -4625,16 +4625,16 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C140" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="B140" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C140" s="7" t="s">
-        <v>264</v>
-      </c>
       <c r="D140" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>8</v>
@@ -4642,16 +4642,16 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C141" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="B141" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C141" s="7" t="s">
-        <v>266</v>
-      </c>
       <c r="D141" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -4659,16 +4659,16 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C142" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="B142" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C142" s="7" t="s">
-        <v>268</v>
-      </c>
       <c r="D142" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -4676,16 +4676,16 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -4693,16 +4693,16 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C144" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="B144" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C144" s="7" t="s">
-        <v>271</v>
-      </c>
       <c r="D144" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>8</v>
@@ -4710,16 +4710,16 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C145" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="B145" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C145" s="7" t="s">
-        <v>273</v>
-      </c>
       <c r="D145" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>8</v>
@@ -4727,16 +4727,16 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B146" s="7" t="s">
         <v>274</v>
-      </c>
-      <c r="B146" s="7" t="s">
-        <v>275</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>59</v>
+        <v>275</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>8</v>
@@ -4747,13 +4747,13 @@
         <v>276</v>
       </c>
       <c r="B147" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="D147" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="C147" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="D147" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>8</v>
@@ -4764,13 +4764,13 @@
         <v>277</v>
       </c>
       <c r="B148" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C148" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D148" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="C148" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D148" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>8</v>
@@ -4781,13 +4781,13 @@
         <v>278</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C149" s="7" t="s">
         <v>279</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>59</v>
+        <v>275</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>8</v>
@@ -4798,13 +4798,13 @@
         <v>280</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C150" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>59</v>
+        <v>275</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>8</v>
@@ -4815,13 +4815,13 @@
         <v>282</v>
       </c>
       <c r="B151" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D151" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="C151" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D151" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>8</v>
@@ -4832,13 +4832,13 @@
         <v>283</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C152" s="7" t="s">
         <v>284</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>59</v>
+        <v>275</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>8</v>
@@ -4849,13 +4849,13 @@
         <v>285</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>286</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>59</v>
+        <v>275</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>8</v>
@@ -4866,13 +4866,13 @@
         <v>287</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C154" s="9" t="s">
         <v>288</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>59</v>
+        <v>275</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>8</v>
@@ -4883,13 +4883,13 @@
         <v>289</v>
       </c>
       <c r="B155" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C155" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="D155" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="C155" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="D155" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>8</v>
@@ -4900,13 +4900,13 @@
         <v>290</v>
       </c>
       <c r="B156" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C156" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D156" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="C156" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="D156" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>8</v>
@@ -4917,13 +4917,13 @@
         <v>291</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C157" s="9" t="s">
         <v>292</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>59</v>
+        <v>275</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>8</v>
@@ -4934,13 +4934,13 @@
         <v>293</v>
       </c>
       <c r="B158" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C158" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D158" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="C158" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D158" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>8</v>
@@ -4951,13 +4951,13 @@
         <v>294</v>
       </c>
       <c r="B159" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C159" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="D159" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="C159" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="D159" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>8</v>
@@ -4968,13 +4968,13 @@
         <v>295</v>
       </c>
       <c r="B160" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C160" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D160" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="C160" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D160" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>8</v>
@@ -4985,13 +4985,13 @@
         <v>296</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C161" s="7" t="s">
         <v>297</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>59</v>
+        <v>275</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>8</v>
@@ -5008,7 +5008,7 @@
         <v>58</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>8</v>
@@ -5025,7 +5025,7 @@
         <v>301</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>8</v>
@@ -5042,7 +5042,7 @@
         <v>303</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>8</v>
@@ -5059,7 +5059,7 @@
         <v>305</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>8</v>
@@ -5076,7 +5076,7 @@
         <v>307</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>8</v>
@@ -5093,7 +5093,7 @@
         <v>309</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>8</v>
@@ -5110,7 +5110,7 @@
         <v>311</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>8</v>
@@ -5127,7 +5127,7 @@
         <v>313</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>8</v>
@@ -5144,7 +5144,7 @@
         <v>315</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>8</v>
@@ -5161,7 +5161,7 @@
         <v>317</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>8</v>
@@ -5178,7 +5178,7 @@
         <v>319</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>8</v>
@@ -5195,7 +5195,7 @@
         <v>321</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>8</v>
@@ -5212,7 +5212,7 @@
         <v>323</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>8</v>
@@ -5229,7 +5229,7 @@
         <v>325</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>8</v>
@@ -5246,7 +5246,7 @@
         <v>327</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>8</v>
@@ -5260,10 +5260,10 @@
         <v>299</v>
       </c>
       <c r="C177" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>8</v>
@@ -5277,10 +5277,10 @@
         <v>299</v>
       </c>
       <c r="C178" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>8</v>
@@ -5297,7 +5297,7 @@
         <v>331</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>8</v>
@@ -5311,10 +5311,10 @@
         <v>299</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>8</v>
@@ -5328,10 +5328,10 @@
         <v>299</v>
       </c>
       <c r="C181" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>8</v>
@@ -5348,7 +5348,7 @@
         <v>335</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>8</v>
@@ -5359,7 +5359,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 E2:E8 F2:F3 D9:E182">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E127 D1:D8 D127:D145 D146:D160 E2:E8 E128:E129 E130:E144 E145:E151 E152:E160 F2:F3 D107:E126 D9:E106 D161:E182">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update the OC01 TC change
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -206,6 +206,9 @@
     <t>Open Estate</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_026</t>
   </si>
   <si>
@@ -852,9 +855,6 @@
   </si>
   <si>
     <t>probateFormsRW08.feature</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>TC_146</t>
@@ -2246,8 +2246,8 @@
   <sheetPr/>
   <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2696,7 +2696,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>8</v>
@@ -2704,16 +2704,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>8</v>
@@ -2721,16 +2721,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>8</v>
@@ -2738,16 +2738,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>8</v>
@@ -2755,16 +2755,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>8</v>
@@ -2772,16 +2772,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>8</v>
@@ -2789,16 +2789,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>8</v>
@@ -2806,16 +2806,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>8</v>
@@ -2823,16 +2823,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>8</v>
@@ -2840,16 +2840,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>8</v>
@@ -2857,16 +2857,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>8</v>
@@ -2874,16 +2874,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>8</v>
@@ -2891,16 +2891,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>8</v>
@@ -2908,16 +2908,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>8</v>
@@ -2925,16 +2925,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>8</v>
@@ -2942,16 +2942,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>8</v>
@@ -2959,16 +2959,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>8</v>
@@ -2976,16 +2976,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>8</v>
@@ -2993,16 +2993,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>8</v>
@@ -3010,16 +3010,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -3027,16 +3027,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="C46" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -3044,16 +3044,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -3061,16 +3061,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -3078,16 +3078,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -3095,16 +3095,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -3112,16 +3112,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -3129,16 +3129,16 @@
     </row>
     <row r="52" ht="28" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -3146,16 +3146,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -3163,16 +3163,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -3180,16 +3180,16 @@
     </row>
     <row r="55" ht="28" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -3197,16 +3197,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -3214,16 +3214,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -3231,16 +3231,16 @@
     </row>
     <row r="58" ht="28" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -3248,16 +3248,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -3265,16 +3265,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -3282,16 +3282,16 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -3299,16 +3299,16 @@
     </row>
     <row r="62" ht="28" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3316,16 +3316,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3333,16 +3333,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3350,16 +3350,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3367,16 +3367,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3384,16 +3384,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3401,16 +3401,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3418,16 +3418,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3435,16 +3435,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3452,16 +3452,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3469,16 +3469,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3486,16 +3486,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3503,16 +3503,16 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>8</v>
@@ -3520,16 +3520,16 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>8</v>
@@ -3537,16 +3537,16 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>8</v>
@@ -3554,16 +3554,16 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B77" s="7" t="s">
-        <v>157</v>
-      </c>
       <c r="C77" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>8</v>
@@ -3571,16 +3571,16 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>8</v>
@@ -3588,16 +3588,16 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>8</v>
@@ -3605,16 +3605,16 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>8</v>
@@ -3622,16 +3622,16 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>8</v>
@@ -3639,16 +3639,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>8</v>
@@ -3656,16 +3656,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>8</v>
@@ -3673,16 +3673,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>8</v>
@@ -3690,16 +3690,16 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>8</v>
@@ -3707,16 +3707,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>8</v>
@@ -3724,16 +3724,16 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>8</v>
@@ -3741,16 +3741,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>178</v>
-      </c>
       <c r="C88" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>8</v>
@@ -3758,16 +3758,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>8</v>
@@ -3775,16 +3775,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>8</v>
@@ -3792,16 +3792,16 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>8</v>
@@ -3809,16 +3809,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>8</v>
@@ -3826,16 +3826,16 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>8</v>
@@ -3843,16 +3843,16 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>8</v>
@@ -3860,16 +3860,16 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>8</v>
@@ -3877,16 +3877,16 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>8</v>
@@ -3894,16 +3894,16 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -3911,16 +3911,16 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -3928,16 +3928,16 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -3945,16 +3945,16 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B100" s="7" t="s">
-        <v>196</v>
-      </c>
       <c r="C100" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -3962,16 +3962,16 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -3979,16 +3979,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -3996,16 +3996,16 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -4013,16 +4013,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -4030,16 +4030,16 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -4047,16 +4047,16 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -4064,16 +4064,16 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -4081,16 +4081,16 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -4098,16 +4098,16 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -4115,16 +4115,16 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -4132,16 +4132,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -4149,16 +4149,16 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B112" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B112" s="7" t="s">
-        <v>211</v>
-      </c>
       <c r="C112" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -4166,16 +4166,16 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -4183,16 +4183,16 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -4200,16 +4200,16 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -4217,16 +4217,16 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -4234,16 +4234,16 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -4251,16 +4251,16 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -4268,16 +4268,16 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4285,16 +4285,16 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4302,16 +4302,16 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4319,16 +4319,16 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4336,16 +4336,16 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>8</v>
@@ -4353,16 +4353,16 @@
     </row>
     <row r="124" ht="28" spans="1:5">
       <c r="A124" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B124" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B124" s="7" t="s">
-        <v>231</v>
-      </c>
       <c r="C124" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>8</v>
@@ -4370,16 +4370,16 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>8</v>
@@ -4387,16 +4387,16 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>8</v>
@@ -4404,16 +4404,16 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>8</v>
@@ -4421,16 +4421,16 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>8</v>
@@ -4438,16 +4438,16 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>8</v>
@@ -4455,16 +4455,16 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>8</v>
@@ -4472,16 +4472,16 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B131" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="B131" s="7" t="s">
-        <v>244</v>
-      </c>
       <c r="C131" s="7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -4489,16 +4489,16 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>8</v>
@@ -4506,16 +4506,16 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>8</v>
@@ -4523,16 +4523,16 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -4540,16 +4540,16 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -4557,16 +4557,16 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -4574,16 +4574,16 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -4591,16 +4591,16 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>8</v>
@@ -4608,16 +4608,16 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>8</v>
@@ -4625,16 +4625,16 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>8</v>
@@ -4642,16 +4642,16 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C141" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -4659,16 +4659,16 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C142" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -4676,16 +4676,16 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -4693,16 +4693,16 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>8</v>
@@ -4710,16 +4710,16 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C145" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>8</v>
@@ -4727,16 +4727,16 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>8</v>
@@ -4747,13 +4747,13 @@
         <v>276</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>8</v>
@@ -4764,13 +4764,13 @@
         <v>277</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>8</v>
@@ -4781,13 +4781,13 @@
         <v>278</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C149" s="7" t="s">
         <v>279</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>8</v>
@@ -4798,13 +4798,13 @@
         <v>280</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C150" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>8</v>
@@ -4815,13 +4815,13 @@
         <v>282</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>8</v>
@@ -4832,13 +4832,13 @@
         <v>283</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C152" s="7" t="s">
         <v>284</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>8</v>
@@ -4849,13 +4849,13 @@
         <v>285</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>286</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>8</v>
@@ -4866,13 +4866,13 @@
         <v>287</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C154" s="9" t="s">
         <v>288</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>8</v>
@@ -4883,13 +4883,13 @@
         <v>289</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>8</v>
@@ -4900,13 +4900,13 @@
         <v>290</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C156" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>8</v>
@@ -4917,13 +4917,13 @@
         <v>291</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C157" s="9" t="s">
         <v>292</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>8</v>
@@ -4934,13 +4934,13 @@
         <v>293</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C158" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>8</v>
@@ -4951,13 +4951,13 @@
         <v>294</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C159" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>8</v>
@@ -4968,13 +4968,13 @@
         <v>295</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>8</v>
@@ -4985,13 +4985,13 @@
         <v>296</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C161" s="7" t="s">
         <v>297</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>275</v>
+        <v>59</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>8</v>
@@ -5008,7 +5008,7 @@
         <v>58</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>8</v>
@@ -5025,7 +5025,7 @@
         <v>301</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>8</v>
@@ -5042,7 +5042,7 @@
         <v>303</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>8</v>
@@ -5059,7 +5059,7 @@
         <v>305</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>8</v>
@@ -5076,7 +5076,7 @@
         <v>307</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>8</v>
@@ -5093,7 +5093,7 @@
         <v>309</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>8</v>
@@ -5110,7 +5110,7 @@
         <v>311</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>8</v>
@@ -5127,7 +5127,7 @@
         <v>313</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>8</v>
@@ -5144,7 +5144,7 @@
         <v>315</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>8</v>
@@ -5161,7 +5161,7 @@
         <v>317</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>8</v>
@@ -5178,7 +5178,7 @@
         <v>319</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>8</v>
@@ -5195,7 +5195,7 @@
         <v>321</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>8</v>
@@ -5212,7 +5212,7 @@
         <v>323</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>8</v>
@@ -5229,7 +5229,7 @@
         <v>325</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>8</v>
@@ -5246,7 +5246,7 @@
         <v>327</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>8</v>
@@ -5260,10 +5260,10 @@
         <v>299</v>
       </c>
       <c r="C177" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>8</v>
@@ -5277,10 +5277,10 @@
         <v>299</v>
       </c>
       <c r="C178" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>8</v>
@@ -5297,7 +5297,7 @@
         <v>331</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>8</v>
@@ -5311,10 +5311,10 @@
         <v>299</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>8</v>
@@ -5328,10 +5328,10 @@
         <v>299</v>
       </c>
       <c r="C181" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>8</v>
@@ -5348,7 +5348,7 @@
         <v>335</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>8</v>
@@ -5359,7 +5359,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E127 D1:D8 D127:D145 D146:D160 E2:E8 E128:E129 E130:E144 E145:E151 E152:E160 F2:F3 D107:E126 D9:E106 D161:E182">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D182:E182 D1:D8 E2:E8 F2:F3 D26:E181 D9:E25">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update the RW02 TC according to UI change
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -206,121 +206,121 @@
     <t>Open Estate</t>
   </si>
   <si>
+    <t>TC_026</t>
+  </si>
+  <si>
+    <t>Verify, file no. is displayed at the top of the form.</t>
+  </si>
+  <si>
+    <t>TC_027</t>
+  </si>
+  <si>
+    <t>Verify, decedent information is displayed in section1 of the form.</t>
+  </si>
+  <si>
+    <t>TC_028</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 2 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_029</t>
+  </si>
+  <si>
+    <t>Verify, in section 2 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_030</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 3 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_031</t>
+  </si>
+  <si>
+    <t>Verify, in section 3 only 1 checkbox can be checked.</t>
+  </si>
+  <si>
+    <t>TC_032</t>
+  </si>
+  <si>
+    <t>Verify, on clicking other checkbox, text area is enabled.</t>
+  </si>
+  <si>
+    <t>TC_033</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 4 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_034</t>
+  </si>
+  <si>
+    <t>Verify, on clicking last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_035</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be selected.</t>
+  </si>
+  <si>
+    <t>TC_036</t>
+  </si>
+  <si>
+    <t>Verify, on selecting the contact its information is displayed in section 4.</t>
+  </si>
+  <si>
+    <t>TC_037</t>
+  </si>
+  <si>
+    <t>Verify, on clicking executor last name, a side bar is displayed.</t>
+  </si>
+  <si>
+    <t>TC_038</t>
+  </si>
+  <si>
+    <t>Verify, 3 types of selection is available.</t>
+  </si>
+  <si>
+    <t>TC_039</t>
+  </si>
+  <si>
+    <t>Verify, only 1 contact can be dragged and dropped in a each of the type.</t>
+  </si>
+  <si>
+    <t>TC_040</t>
+  </si>
+  <si>
+    <t>Verify, on clicking section 5 an informative text box appears.</t>
+  </si>
+  <si>
+    <t>TC_041</t>
+  </si>
+  <si>
+    <t>Verify the selected contacts are displayed under executor, co executor and secondary co executor.</t>
+  </si>
+  <si>
+    <t>TC_042</t>
+  </si>
+  <si>
+    <t>Verify form can be printed in pdf</t>
+  </si>
+  <si>
+    <t>TC_043</t>
+  </si>
+  <si>
+    <t>Reset the RW01 form</t>
+  </si>
+  <si>
+    <t>TC_044</t>
+  </si>
+  <si>
+    <t>probateFormsRW02.feature</t>
+  </si>
+  <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_026</t>
-  </si>
-  <si>
-    <t>Verify, file no. is displayed at the top of the form.</t>
-  </si>
-  <si>
-    <t>TC_027</t>
-  </si>
-  <si>
-    <t>Verify, decedent information is displayed in section1 of the form.</t>
-  </si>
-  <si>
-    <t>TC_028</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 2 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_029</t>
-  </si>
-  <si>
-    <t>Verify, in section 2 only 1 checkbox can be checked.</t>
-  </si>
-  <si>
-    <t>TC_030</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 3 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_031</t>
-  </si>
-  <si>
-    <t>Verify, in section 3 only 1 checkbox can be checked.</t>
-  </si>
-  <si>
-    <t>TC_032</t>
-  </si>
-  <si>
-    <t>Verify, on clicking other checkbox, text area is enabled.</t>
-  </si>
-  <si>
-    <t>TC_033</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 4 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_034</t>
-  </si>
-  <si>
-    <t>Verify, on clicking last name, a side bar is displayed.</t>
-  </si>
-  <si>
-    <t>TC_035</t>
-  </si>
-  <si>
-    <t>Verify, only 1 contact can be selected.</t>
-  </si>
-  <si>
-    <t>TC_036</t>
-  </si>
-  <si>
-    <t>Verify, on selecting the contact its information is displayed in section 4.</t>
-  </si>
-  <si>
-    <t>TC_037</t>
-  </si>
-  <si>
-    <t>Verify, on clicking executor last name, a side bar is displayed.</t>
-  </si>
-  <si>
-    <t>TC_038</t>
-  </si>
-  <si>
-    <t>Verify, 3 types of selection is available.</t>
-  </si>
-  <si>
-    <t>TC_039</t>
-  </si>
-  <si>
-    <t>Verify, only 1 contact can be dragged and dropped in a each of the type.</t>
-  </si>
-  <si>
-    <t>TC_040</t>
-  </si>
-  <si>
-    <t>Verify, on clicking section 5 an informative text box appears.</t>
-  </si>
-  <si>
-    <t>TC_041</t>
-  </si>
-  <si>
-    <t>Verify the selected contacts are displayed under executor, co executor and secondary co executor.</t>
-  </si>
-  <si>
-    <t>TC_042</t>
-  </si>
-  <si>
-    <t>Verify form can be printed in pdf</t>
-  </si>
-  <si>
-    <t>TC_043</t>
-  </si>
-  <si>
-    <t>Reset the RW01 form</t>
-  </si>
-  <si>
-    <t>TC_044</t>
-  </si>
-  <si>
-    <t>probateFormsRW02.feature</t>
   </si>
   <si>
     <t>TC_045</t>
@@ -2246,8 +2246,8 @@
   <sheetPr/>
   <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D182" sqref="D182"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45:D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2696,7 +2696,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>8</v>
@@ -2704,16 +2704,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>8</v>
@@ -2721,16 +2721,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>8</v>
@@ -2738,16 +2738,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>8</v>
@@ -2755,16 +2755,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>8</v>
@@ -2772,16 +2772,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>8</v>
@@ -2789,16 +2789,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>8</v>
@@ -2806,16 +2806,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>8</v>
@@ -2823,16 +2823,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>8</v>
@@ -2840,16 +2840,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>8</v>
@@ -2857,16 +2857,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>8</v>
@@ -2874,16 +2874,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>8</v>
@@ -2891,16 +2891,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>8</v>
@@ -2908,16 +2908,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>8</v>
@@ -2925,16 +2925,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>8</v>
@@ -2942,16 +2942,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>8</v>
@@ -2959,16 +2959,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>8</v>
@@ -2976,16 +2976,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>8</v>
@@ -2993,16 +2993,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>8</v>
@@ -3010,16 +3010,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -3030,13 +3030,13 @@
         <v>98</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>99</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -3047,13 +3047,13 @@
         <v>100</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>101</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -3064,13 +3064,13 @@
         <v>102</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>103</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -3081,13 +3081,13 @@
         <v>104</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>105</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -3098,13 +3098,13 @@
         <v>106</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>107</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -3115,13 +3115,13 @@
         <v>108</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>109</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -3132,13 +3132,13 @@
         <v>110</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>111</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -3149,13 +3149,13 @@
         <v>112</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -3166,13 +3166,13 @@
         <v>114</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>115</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -3183,13 +3183,13 @@
         <v>116</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>117</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -3200,13 +3200,13 @@
         <v>118</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>119</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -3217,13 +3217,13 @@
         <v>120</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>121</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -3234,13 +3234,13 @@
         <v>122</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>123</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -3251,13 +3251,13 @@
         <v>124</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>125</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -3268,13 +3268,13 @@
         <v>126</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>127</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -3285,13 +3285,13 @@
         <v>128</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>129</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -3302,13 +3302,13 @@
         <v>130</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>131</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3319,13 +3319,13 @@
         <v>132</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>133</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3336,13 +3336,13 @@
         <v>134</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>135</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3353,13 +3353,13 @@
         <v>136</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>137</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3370,13 +3370,13 @@
         <v>138</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>139</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3387,13 +3387,13 @@
         <v>140</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>141</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3404,13 +3404,13 @@
         <v>142</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>143</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3421,13 +3421,13 @@
         <v>144</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>145</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3438,13 +3438,13 @@
         <v>146</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>147</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3455,13 +3455,13 @@
         <v>148</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>149</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3472,13 +3472,13 @@
         <v>150</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>151</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3489,13 +3489,13 @@
         <v>152</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>153</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3506,13 +3506,13 @@
         <v>154</v>
       </c>
       <c r="B74" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>8</v>
@@ -3523,13 +3523,13 @@
         <v>155</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>156</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>8</v>
@@ -3546,7 +3546,7 @@
         <v>58</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>8</v>
@@ -3563,7 +3563,7 @@
         <v>160</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>8</v>
@@ -3580,7 +3580,7 @@
         <v>162</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>8</v>
@@ -3597,7 +3597,7 @@
         <v>164</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>8</v>
@@ -3614,7 +3614,7 @@
         <v>166</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>8</v>
@@ -3631,7 +3631,7 @@
         <v>168</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>8</v>
@@ -3648,7 +3648,7 @@
         <v>170</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>8</v>
@@ -3665,7 +3665,7 @@
         <v>172</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>8</v>
@@ -3682,7 +3682,7 @@
         <v>174</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>8</v>
@@ -3696,10 +3696,10 @@
         <v>158</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>8</v>
@@ -3716,7 +3716,7 @@
         <v>177</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>8</v>
@@ -3733,7 +3733,7 @@
         <v>58</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>8</v>
@@ -3750,7 +3750,7 @@
         <v>181</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>8</v>
@@ -3767,7 +3767,7 @@
         <v>183</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>8</v>
@@ -3784,7 +3784,7 @@
         <v>185</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>8</v>
@@ -3801,7 +3801,7 @@
         <v>187</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>8</v>
@@ -3818,7 +3818,7 @@
         <v>166</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>8</v>
@@ -3835,7 +3835,7 @@
         <v>168</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>8</v>
@@ -3852,7 +3852,7 @@
         <v>170</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>8</v>
@@ -3869,7 +3869,7 @@
         <v>172</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>8</v>
@@ -3886,7 +3886,7 @@
         <v>174</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>8</v>
@@ -3900,10 +3900,10 @@
         <v>179</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -3920,7 +3920,7 @@
         <v>195</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -3937,7 +3937,7 @@
         <v>58</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -3954,7 +3954,7 @@
         <v>105</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -3971,7 +3971,7 @@
         <v>162</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -3988,7 +3988,7 @@
         <v>164</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -4005,7 +4005,7 @@
         <v>166</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -4022,7 +4022,7 @@
         <v>168</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -4039,7 +4039,7 @@
         <v>170</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -4056,7 +4056,7 @@
         <v>172</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -4073,7 +4073,7 @@
         <v>206</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -4090,7 +4090,7 @@
         <v>174</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -4104,10 +4104,10 @@
         <v>197</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -4124,7 +4124,7 @@
         <v>210</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -4141,7 +4141,7 @@
         <v>58</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -4158,7 +4158,7 @@
         <v>160</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -4175,7 +4175,7 @@
         <v>162</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -4192,7 +4192,7 @@
         <v>216</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -4209,7 +4209,7 @@
         <v>218</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -4226,7 +4226,7 @@
         <v>220</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -4243,7 +4243,7 @@
         <v>222</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -4260,7 +4260,7 @@
         <v>216</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -4277,7 +4277,7 @@
         <v>225</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4294,7 +4294,7 @@
         <v>227</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4308,10 +4308,10 @@
         <v>212</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4328,7 +4328,7 @@
         <v>230</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4345,7 +4345,7 @@
         <v>58</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>8</v>
@@ -4362,7 +4362,7 @@
         <v>234</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>8</v>
@@ -4379,7 +4379,7 @@
         <v>236</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>8</v>
@@ -4396,7 +4396,7 @@
         <v>238</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>8</v>
@@ -4413,7 +4413,7 @@
         <v>240</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>8</v>
@@ -4427,10 +4427,10 @@
         <v>232</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>8</v>
@@ -4447,7 +4447,7 @@
         <v>243</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>8</v>
@@ -4464,7 +4464,7 @@
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>8</v>
@@ -4481,7 +4481,7 @@
         <v>247</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -4498,7 +4498,7 @@
         <v>107</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>8</v>
@@ -4515,7 +4515,7 @@
         <v>250</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>8</v>
@@ -4532,7 +4532,7 @@
         <v>252</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -4549,7 +4549,7 @@
         <v>254</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -4566,7 +4566,7 @@
         <v>256</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -4583,7 +4583,7 @@
         <v>258</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -4600,7 +4600,7 @@
         <v>260</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>8</v>
@@ -4617,7 +4617,7 @@
         <v>262</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>8</v>
@@ -4634,7 +4634,7 @@
         <v>264</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>8</v>
@@ -4651,7 +4651,7 @@
         <v>266</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -4668,7 +4668,7 @@
         <v>268</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -4682,10 +4682,10 @@
         <v>245</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -4702,7 +4702,7 @@
         <v>271</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>8</v>
@@ -4719,7 +4719,7 @@
         <v>273</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>8</v>
@@ -4736,7 +4736,7 @@
         <v>58</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>8</v>
@@ -4753,7 +4753,7 @@
         <v>247</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>8</v>
@@ -4770,7 +4770,7 @@
         <v>107</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>8</v>
@@ -4787,7 +4787,7 @@
         <v>279</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>8</v>
@@ -4804,7 +4804,7 @@
         <v>281</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>8</v>
@@ -4821,7 +4821,7 @@
         <v>137</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>8</v>
@@ -4838,7 +4838,7 @@
         <v>284</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>8</v>
@@ -4855,7 +4855,7 @@
         <v>286</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>8</v>
@@ -4872,7 +4872,7 @@
         <v>288</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>8</v>
@@ -4889,7 +4889,7 @@
         <v>266</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>8</v>
@@ -4906,7 +4906,7 @@
         <v>268</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>8</v>
@@ -4923,7 +4923,7 @@
         <v>292</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>8</v>
@@ -4937,10 +4937,10 @@
         <v>275</v>
       </c>
       <c r="C158" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>8</v>
@@ -4957,7 +4957,7 @@
         <v>271</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>8</v>
@@ -4971,10 +4971,10 @@
         <v>275</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>8</v>
@@ -4991,7 +4991,7 @@
         <v>297</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>8</v>
@@ -5008,7 +5008,7 @@
         <v>58</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>8</v>
@@ -5025,7 +5025,7 @@
         <v>301</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>8</v>
@@ -5042,7 +5042,7 @@
         <v>303</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>8</v>
@@ -5059,7 +5059,7 @@
         <v>305</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>8</v>
@@ -5076,7 +5076,7 @@
         <v>307</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>8</v>
@@ -5093,7 +5093,7 @@
         <v>309</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>8</v>
@@ -5110,7 +5110,7 @@
         <v>311</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>8</v>
@@ -5127,7 +5127,7 @@
         <v>313</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>8</v>
@@ -5144,7 +5144,7 @@
         <v>315</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>8</v>
@@ -5161,7 +5161,7 @@
         <v>317</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>8</v>
@@ -5178,7 +5178,7 @@
         <v>319</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>8</v>
@@ -5195,7 +5195,7 @@
         <v>321</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>8</v>
@@ -5212,7 +5212,7 @@
         <v>323</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>8</v>
@@ -5229,7 +5229,7 @@
         <v>325</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>8</v>
@@ -5246,7 +5246,7 @@
         <v>327</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>8</v>
@@ -5263,7 +5263,7 @@
         <v>266</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>8</v>
@@ -5280,7 +5280,7 @@
         <v>268</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>8</v>
@@ -5297,7 +5297,7 @@
         <v>331</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>8</v>
@@ -5311,10 +5311,10 @@
         <v>299</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>8</v>
@@ -5331,7 +5331,7 @@
         <v>271</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>8</v>
@@ -5348,7 +5348,7 @@
         <v>335</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>8</v>
@@ -5359,7 +5359,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D182:E182 D1:D8 E2:E8 F2:F3 D26:E181 D9:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D45:D75 D76:D78 D107:D122 E2:E8 E45:E46 E47:E72 E73:E74 E75:E78 E107:E110 E111:E122 F2:F3 D9:E21 D123:E182 D79:E106 D22:E44">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
resolved issues of RW02, RW08 and RW10 form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="441">
   <si>
     <t>ID</t>
   </si>
@@ -320,6 +320,9 @@
     <t>probateFormsRW02.feature</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_045</t>
   </si>
   <si>
@@ -854,9 +857,6 @@
     <t>probateFormsRW08.feature</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>TC_146</t>
   </si>
   <si>
@@ -1035,6 +1035,321 @@
   </si>
   <si>
     <t>Reset the RW10 form</t>
+  </si>
+  <si>
+    <t>TC_182</t>
+  </si>
+  <si>
+    <t>probateFormsOC01.feature</t>
+  </si>
+  <si>
+    <t>TC_183</t>
+  </si>
+  <si>
+    <t>Verify that the Estate Name and County fields, file no are preloaded and displayed correctly as read-only fields.</t>
+  </si>
+  <si>
+    <t>TC_184</t>
+  </si>
+  <si>
+    <t>Verify, file no can be edited.</t>
+  </si>
+  <si>
+    <t>TC_185</t>
+  </si>
+  <si>
+    <t>Verify that the sidebar appears and allows attorney selection.</t>
+  </si>
+  <si>
+    <t>TC_186</t>
+  </si>
+  <si>
+    <t>Verify, correct attorney details are fetched in the subsequent fields.</t>
+  </si>
+  <si>
+    <t>TC_187</t>
+  </si>
+  <si>
+    <t>Verify that selecting an attorney updates the attorney details in related forms.</t>
+  </si>
+  <si>
+    <t>TC_188</t>
+  </si>
+  <si>
+    <t>Verify that Estate Name, and Date of Death fields are preloaded and non-editable.</t>
+  </si>
+  <si>
+    <t>TC_189</t>
+  </si>
+  <si>
+    <t>Verify that clicking on the Petitioner field opens the sidebar and allows fiduciary selection.</t>
+  </si>
+  <si>
+    <t>TC_190</t>
+  </si>
+  <si>
+    <t>Verify, only 2 petitioners are visible on the form and rest are attached.</t>
+  </si>
+  <si>
+    <t>TC_191</t>
+  </si>
+  <si>
+    <t>Verify, selected petitioner can be swapped and deleted.</t>
+  </si>
+  <si>
+    <t>TC_192</t>
+  </si>
+  <si>
+    <t>Verify that changes to the "Date of Will" and "Date of Codicil" fields update the estate record automatically.</t>
+  </si>
+  <si>
+    <t>TC_193</t>
+  </si>
+  <si>
+    <t>Verify that the decedent's name is preloaded from the estate record and displayed as non-editable.</t>
+  </si>
+  <si>
+    <t>TC_194</t>
+  </si>
+  <si>
+    <t>Verify, can add multiple children and DoB.</t>
+  </si>
+  <si>
+    <t>TC_195</t>
+  </si>
+  <si>
+    <t>Verify, "Name of Estate" from page 2 is auto fetched at the top of this and next page.</t>
+  </si>
+  <si>
+    <t>TC_196</t>
+  </si>
+  <si>
+    <t>Verify, rest of the selected beneficiaries are displayed as a part of attachment.</t>
+  </si>
+  <si>
+    <t>TC_197</t>
+  </si>
+  <si>
+    <t>Verify, attachment is displayed on both the pages.</t>
+  </si>
+  <si>
+    <t>TC_198</t>
+  </si>
+  <si>
+    <t>Verify, if the initials are added then name address disappears, if initials are removed then name and address appears.</t>
+  </si>
+  <si>
+    <t>TC_199</t>
+  </si>
+  <si>
+    <t>Verify, comments can be added for that particular beneficiary.</t>
+  </si>
+  <si>
+    <t>TC_200</t>
+  </si>
+  <si>
+    <t>Verify, relationship of the beneficiary with the given estate/trust is displayed under relationship section.</t>
+  </si>
+  <si>
+    <t>TC_201</t>
+  </si>
+  <si>
+    <t>Verify, interest value for each beneficiary.</t>
+  </si>
+  <si>
+    <t>TC_202</t>
+  </si>
+  <si>
+    <t>Verify, if the display as attachment checkbox is checked then all the beneficiaries are displayed in attachment.</t>
+  </si>
+  <si>
+    <t>TC_203</t>
+  </si>
+  <si>
+    <t>Verify correct count of main and attachment is displayed.</t>
+  </si>
+  <si>
+    <t>TC_204</t>
+  </si>
+  <si>
+    <t>Verify that the decedent's name is preloaded and displayed as read-only.</t>
+  </si>
+  <si>
+    <t>TC_205</t>
+  </si>
+  <si>
+    <t>Verify that while adding new claimant if initials is empty then Name and Address fields should be required and vice versa for initials.</t>
+  </si>
+  <si>
+    <t>TC_206</t>
+  </si>
+  <si>
+    <t>Verify that while adding claimant if Name and Address is there then initials is not required.</t>
+  </si>
+  <si>
+    <t>TC_207</t>
+  </si>
+  <si>
+    <t>Verify that a user can add a new claimant successfully.</t>
+  </si>
+  <si>
+    <t>TC_208</t>
+  </si>
+  <si>
+    <t>Verify that claimants exceeding four are moved to the attachment.</t>
+  </si>
+  <si>
+    <t>TC_209</t>
+  </si>
+  <si>
+    <t>Verify that totals for "Above" and "Attachment" update dynamically.</t>
+  </si>
+  <si>
+    <t>TC_210</t>
+  </si>
+  <si>
+    <t>Verify the decedent's name is preloaded as read-only.</t>
+  </si>
+  <si>
+    <t>TC_211</t>
+  </si>
+  <si>
+    <t>Verify, if both the checkboxes in point 11 is checked then only spouse field is enabled.</t>
+  </si>
+  <si>
+    <t>TC_212</t>
+  </si>
+  <si>
+    <t>Verify, date, payment and interest can be added.</t>
+  </si>
+  <si>
+    <t>TC_213</t>
+  </si>
+  <si>
+    <t>Verify that fiduciary fields appear when "Yes" is selected.</t>
+  </si>
+  <si>
+    <t>TC_214</t>
+  </si>
+  <si>
+    <t>Verify that the decedent's name is preloaded as a read-only field from the estate details.</t>
+  </si>
+  <si>
+    <t>TC_215</t>
+  </si>
+  <si>
+    <t>Verify that litigation-related fields are enabled only when litigation status is set to "Yes."</t>
+  </si>
+  <si>
+    <t>TC_216</t>
+  </si>
+  <si>
+    <t>Verify that the decedent's name is preloaded as a read-only field.</t>
+  </si>
+  <si>
+    <t>TC_217</t>
+  </si>
+  <si>
+    <t>Verify date, description and amount can be added in multiline</t>
+  </si>
+  <si>
+    <t>TC_218</t>
+  </si>
+  <si>
+    <t>Verify, reserve request amount can be added.</t>
+  </si>
+  <si>
+    <t>TC_219</t>
+  </si>
+  <si>
+    <t>Verify, trust's name is auto fetched.</t>
+  </si>
+  <si>
+    <t>TC_220</t>
+  </si>
+  <si>
+    <t>Verify, if displayed on checkbox is checked, then the contacts are displayed on the form.</t>
+  </si>
+  <si>
+    <t>TC_221</t>
+  </si>
+  <si>
+    <t>Verify, all the contacts are moved to attachment if the display all bene in attachment checkbox is checked.</t>
+  </si>
+  <si>
+    <t>TC_222</t>
+  </si>
+  <si>
+    <t>Verify, only 1 fiduciary contact can be selected and all its details are displayed.</t>
+  </si>
+  <si>
+    <t>TC_223</t>
+  </si>
+  <si>
+    <t>Verify, warning is displayed for selecting capacity.</t>
+  </si>
+  <si>
+    <t>TC_224</t>
+  </si>
+  <si>
+    <t>Verify, on the basis of capacity selected, contact can be selected and displayed on the form.</t>
+  </si>
+  <si>
+    <t>TC_225</t>
+  </si>
+  <si>
+    <t>Verify, trust's name is auto fetched and correctly displayed.</t>
+  </si>
+  <si>
+    <t>TC_226</t>
+  </si>
+  <si>
+    <t>Verify, first individual petitioner selected in page 2 is displayed here under individual petitioner.</t>
+  </si>
+  <si>
+    <t>TC_227</t>
+  </si>
+  <si>
+    <t>Verify, rest of the individual petitioners are displayed as a part of attachment.</t>
+  </si>
+  <si>
+    <t>TC_228</t>
+  </si>
+  <si>
+    <t>TC_229</t>
+  </si>
+  <si>
+    <t>Verify, if the notification if the selected contact is removed from the estate.</t>
+  </si>
+  <si>
+    <t>TC_230</t>
+  </si>
+  <si>
+    <t>Verify, if the contact is removed, it is removed from the form as well.</t>
+  </si>
+  <si>
+    <t>TC_231</t>
+  </si>
+  <si>
+    <t>Verify, if for a user role of beny is removed.</t>
+  </si>
+  <si>
+    <t>TC_232</t>
+  </si>
+  <si>
+    <t>Verify, if for a user role of beny, fiduciary, attorney is removed.</t>
+  </si>
+  <si>
+    <t>TC_233</t>
+  </si>
+  <si>
+    <t>Reset Roles of Removed Contacts</t>
+  </si>
+  <si>
+    <t>TC_234</t>
+  </si>
+  <si>
+    <t>Reset the OC01 form</t>
   </si>
 </sst>
 </file>
@@ -2244,10 +2559,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F182"/>
+  <dimension ref="A1:F235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3019,7 +3334,7 @@
         <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -3027,16 +3342,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -3044,16 +3359,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -3061,16 +3376,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -3078,16 +3393,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -3095,16 +3410,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -3112,16 +3427,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -3129,16 +3444,16 @@
     </row>
     <row r="52" ht="28" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -3146,16 +3461,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -3163,16 +3478,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -3180,16 +3495,16 @@
     </row>
     <row r="55" ht="28" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -3197,16 +3512,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -3214,16 +3529,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -3231,16 +3546,16 @@
     </row>
     <row r="58" ht="28" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -3248,16 +3563,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -3265,16 +3580,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -3282,16 +3597,16 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -3299,16 +3614,16 @@
     </row>
     <row r="62" ht="28" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3316,16 +3631,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3333,16 +3648,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3350,16 +3665,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3367,16 +3682,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3384,16 +3699,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3401,16 +3716,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3418,16 +3733,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3435,16 +3750,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3452,16 +3767,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3469,16 +3784,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3486,16 +3801,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3503,7 +3818,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>96</v>
@@ -3512,7 +3827,7 @@
         <v>92</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>8</v>
@@ -3520,16 +3835,16 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>8</v>
@@ -3537,10 +3852,10 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>58</v>
@@ -3554,13 +3869,13 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B77" s="7" t="s">
-        <v>157</v>
-      </c>
       <c r="C77" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>8</v>
@@ -3571,13 +3886,13 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>8</v>
@@ -3588,13 +3903,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>8</v>
@@ -3605,13 +3920,13 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>8</v>
@@ -3622,13 +3937,13 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>8</v>
@@ -3639,13 +3954,13 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>8</v>
@@ -3656,13 +3971,13 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>8</v>
@@ -3673,13 +3988,13 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>8</v>
@@ -3690,10 +4005,10 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>92</v>
@@ -3707,13 +4022,13 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>8</v>
@@ -3724,10 +4039,10 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>58</v>
@@ -3741,13 +4056,13 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>178</v>
-      </c>
       <c r="C88" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>8</v>
@@ -3758,13 +4073,13 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>8</v>
@@ -3775,13 +4090,13 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>8</v>
@@ -3792,13 +4107,13 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>8</v>
@@ -3809,13 +4124,13 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>8</v>
@@ -3826,13 +4141,13 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>8</v>
@@ -3843,13 +4158,13 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>8</v>
@@ -3860,13 +4175,13 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>8</v>
@@ -3877,13 +4192,13 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>8</v>
@@ -3894,10 +4209,10 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>92</v>
@@ -3911,13 +4226,13 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>8</v>
@@ -3928,10 +4243,10 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>58</v>
@@ -3945,13 +4260,13 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B100" s="7" t="s">
-        <v>196</v>
-      </c>
       <c r="C100" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>8</v>
@@ -3962,13 +4277,13 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>8</v>
@@ -3979,13 +4294,13 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>8</v>
@@ -3996,13 +4311,13 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>8</v>
@@ -4013,13 +4328,13 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>8</v>
@@ -4030,13 +4345,13 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>8</v>
@@ -4047,13 +4362,13 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>8</v>
@@ -4064,13 +4379,13 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>8</v>
@@ -4081,13 +4396,13 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>8</v>
@@ -4098,10 +4413,10 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>92</v>
@@ -4115,13 +4430,13 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>8</v>
@@ -4132,10 +4447,10 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>58</v>
@@ -4149,13 +4464,13 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B112" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B112" s="7" t="s">
-        <v>211</v>
-      </c>
       <c r="C112" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>8</v>
@@ -4166,13 +4481,13 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>8</v>
@@ -4183,13 +4498,13 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>8</v>
@@ -4200,13 +4515,13 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>8</v>
@@ -4217,13 +4532,13 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>8</v>
@@ -4234,13 +4549,13 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>8</v>
@@ -4251,13 +4566,13 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>8</v>
@@ -4268,13 +4583,13 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>8</v>
@@ -4285,13 +4600,13 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>8</v>
@@ -4302,10 +4617,10 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>92</v>
@@ -4319,13 +4634,13 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>8</v>
@@ -4336,10 +4651,10 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>58</v>
@@ -4353,13 +4668,13 @@
     </row>
     <row r="124" ht="28" spans="1:5">
       <c r="A124" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B124" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B124" s="7" t="s">
-        <v>231</v>
-      </c>
       <c r="C124" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>8</v>
@@ -4370,13 +4685,13 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>8</v>
@@ -4387,13 +4702,13 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>8</v>
@@ -4404,13 +4719,13 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>8</v>
@@ -4421,10 +4736,10 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C128" s="8" t="s">
         <v>92</v>
@@ -4438,13 +4753,13 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>8</v>
@@ -4455,10 +4770,10 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>58</v>
@@ -4472,13 +4787,13 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B131" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="B131" s="7" t="s">
-        <v>244</v>
-      </c>
       <c r="C131" s="7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>8</v>
@@ -4489,13 +4804,13 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>8</v>
@@ -4506,13 +4821,13 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>8</v>
@@ -4523,13 +4838,13 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>8</v>
@@ -4540,13 +4855,13 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>8</v>
@@ -4557,13 +4872,13 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>8</v>
@@ -4574,13 +4889,13 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>8</v>
@@ -4591,13 +4906,13 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>8</v>
@@ -4608,13 +4923,13 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>8</v>
@@ -4625,13 +4940,13 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>8</v>
@@ -4642,13 +4957,13 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C141" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>8</v>
@@ -4659,13 +4974,13 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C142" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>8</v>
@@ -4676,10 +4991,10 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C143" s="7" t="s">
         <v>92</v>
@@ -4693,13 +5008,13 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>8</v>
@@ -4710,13 +5025,13 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C145" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>8</v>
@@ -4727,16 +5042,16 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>8</v>
@@ -4747,13 +5062,13 @@
         <v>276</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>8</v>
@@ -4764,13 +5079,13 @@
         <v>277</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>8</v>
@@ -4781,13 +5096,13 @@
         <v>278</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C149" s="7" t="s">
         <v>279</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>8</v>
@@ -4798,13 +5113,13 @@
         <v>280</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C150" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>8</v>
@@ -4815,13 +5130,13 @@
         <v>282</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>8</v>
@@ -4832,13 +5147,13 @@
         <v>283</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C152" s="7" t="s">
         <v>284</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>8</v>
@@ -4849,13 +5164,13 @@
         <v>285</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>286</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>8</v>
@@ -4866,13 +5181,13 @@
         <v>287</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C154" s="9" t="s">
         <v>288</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>8</v>
@@ -4883,13 +5198,13 @@
         <v>289</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>8</v>
@@ -4900,13 +5215,13 @@
         <v>290</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C156" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>8</v>
@@ -4917,13 +5232,13 @@
         <v>291</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C157" s="9" t="s">
         <v>292</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>8</v>
@@ -4934,13 +5249,13 @@
         <v>293</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C158" s="7" t="s">
         <v>92</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>8</v>
@@ -4951,13 +5266,13 @@
         <v>294</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C159" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>8</v>
@@ -4968,13 +5283,13 @@
         <v>295</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C160" s="8" t="s">
         <v>92</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>8</v>
@@ -4985,13 +5300,13 @@
         <v>296</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C161" s="7" t="s">
         <v>297</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>8</v>
@@ -5260,7 +5575,7 @@
         <v>299</v>
       </c>
       <c r="C177" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D177" s="3" t="s">
         <v>8</v>
@@ -5277,7 +5592,7 @@
         <v>299</v>
       </c>
       <c r="C178" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D178" s="3" t="s">
         <v>8</v>
@@ -5328,7 +5643,7 @@
         <v>299</v>
       </c>
       <c r="C181" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D181" s="3" t="s">
         <v>8</v>
@@ -5351,6 +5666,907 @@
         <v>8</v>
       </c>
       <c r="E182" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B183" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C183" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="184" ht="28" spans="1:5">
+      <c r="A184" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B184" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C184" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="B185" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C185" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B186" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C186" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="B187" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C187" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B188" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C188" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B189" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C189" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B190" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C190" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B191" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C191" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="B192" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C192" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="193" ht="28" spans="1:5">
+      <c r="A193" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B193" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C193" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B194" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C194" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="B195" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C195" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E195" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B196" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C196" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B197" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C197" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B198" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C198" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="D198" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E198" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="199" ht="28" spans="1:5">
+      <c r="A199" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B199" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C199" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E199" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="A200" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="B200" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C200" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="201" ht="28" spans="1:5">
+      <c r="A201" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="B201" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C201" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
+      <c r="A202" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B202" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C202" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="203" ht="28" spans="1:5">
+      <c r="A203" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B203" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C203" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B204" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C204" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B205" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C205" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="D205" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E205" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="206" ht="28" spans="1:5">
+      <c r="A206" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B206" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C206" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="A207" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B207" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C207" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="B208" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C208" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="D208" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E208" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B209" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C209" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
+      <c r="A210" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B210" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C210" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="D210" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="B211" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C211" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="D211" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="B212" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C212" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="D212" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
+      <c r="A213" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="B213" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C213" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E213" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
+      <c r="A214" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B214" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C214" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E214" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
+      <c r="A215" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="B215" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C215" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="D215" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E215" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
+      <c r="A216" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B216" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C216" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="D216" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E216" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
+      <c r="A217" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="B217" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C217" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="D217" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E217" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5">
+      <c r="A218" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B218" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C218" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="D218" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E218" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5">
+      <c r="A219" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B219" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C219" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="D219" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E219" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
+      <c r="A220" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B220" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C220" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E220" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5">
+      <c r="A221" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B221" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C221" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="D221" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E221" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="222" ht="28" spans="1:5">
+      <c r="A222" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="B222" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C222" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E222" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5">
+      <c r="A223" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B223" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C223" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D223" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E223" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5">
+      <c r="A224" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B224" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C224" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E224" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5">
+      <c r="A225" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="B225" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C225" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E225" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5">
+      <c r="A226" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="B226" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C226" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="D226" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E226" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5">
+      <c r="A227" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="B227" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C227" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="D227" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E227" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5">
+      <c r="A228" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="B228" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C228" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="D228" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E228" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5">
+      <c r="A229" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B229" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C229" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5">
+      <c r="A230" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="B230" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C230" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="D230" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E230" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5">
+      <c r="A231" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="B231" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C231" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="D231" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E231" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5">
+      <c r="A232" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="B232" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C232" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E232" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5">
+      <c r="A233" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="B233" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C233" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E233" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5">
+      <c r="A234" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="B234" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C234" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="D234" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E234" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5">
+      <c r="A235" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="B235" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C235" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E235" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5359,7 +6575,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E127 D1:D8 D127:D145 D146:D160 E2:E8 E128:E129 E130:E144 E145:E151 E152:E160 F2:F3 D107:E126 D9:E106 D161:E182">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 D1:D8 D11:D44 D45:D74 D75:D232 E2:E8 E12:E25 E26:E44 E45:E75 E76:E129 E130:E145 E146:E232 F2:F3 D9:E10 D233:E235">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update the RW forms PDF validation
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -206,6 +206,9 @@
     <t>Open Estate</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>TC_026</t>
   </si>
   <si>
@@ -663,9 +666,6 @@
   </si>
   <si>
     <t>probateFormsRW06.feature</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>TC_111</t>
@@ -2561,8 +2561,8 @@
   <sheetPr/>
   <dimension ref="A1:F235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
+      <selection activeCell="D240" sqref="D240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3011,7 +3011,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>8</v>
@@ -3019,16 +3019,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>8</v>
@@ -3036,16 +3036,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>8</v>
@@ -3053,16 +3053,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>8</v>
@@ -3070,16 +3070,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>8</v>
@@ -3087,16 +3087,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>8</v>
@@ -3104,16 +3104,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>8</v>
@@ -3121,16 +3121,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>8</v>
@@ -3138,16 +3138,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>8</v>
@@ -3155,16 +3155,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>8</v>
@@ -3172,16 +3172,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>8</v>
@@ -3189,16 +3189,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>8</v>
@@ -3206,16 +3206,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>8</v>
@@ -3223,16 +3223,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>8</v>
@@ -3240,16 +3240,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>8</v>
@@ -3257,16 +3257,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>8</v>
@@ -3274,16 +3274,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>8</v>
@@ -3291,16 +3291,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>8</v>
@@ -3308,16 +3308,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>8</v>
@@ -3325,16 +3325,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -3342,16 +3342,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="C46" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -3359,16 +3359,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -3376,16 +3376,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -3393,16 +3393,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -3410,16 +3410,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -3427,16 +3427,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -3444,16 +3444,16 @@
     </row>
     <row r="52" ht="28" spans="1:5">
       <c r="A52" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -3461,16 +3461,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -3478,16 +3478,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -3495,16 +3495,16 @@
     </row>
     <row r="55" ht="28" spans="1:5">
       <c r="A55" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -3512,16 +3512,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -3529,16 +3529,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -3546,16 +3546,16 @@
     </row>
     <row r="58" ht="28" spans="1:5">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -3563,16 +3563,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -3580,16 +3580,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -3597,16 +3597,16 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -3614,16 +3614,16 @@
     </row>
     <row r="62" ht="28" spans="1:5">
       <c r="A62" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3631,16 +3631,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3648,16 +3648,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3665,16 +3665,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3682,16 +3682,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3699,16 +3699,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3716,16 +3716,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3733,16 +3733,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3750,16 +3750,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3767,16 +3767,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3784,16 +3784,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3801,16 +3801,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3818,16 +3818,16 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>8</v>
@@ -3835,16 +3835,16 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>8</v>
@@ -3852,16 +3852,16 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>8</v>
@@ -3869,16 +3869,16 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B77" s="7" t="s">
-        <v>157</v>
-      </c>
       <c r="C77" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>8</v>
@@ -3886,16 +3886,16 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>8</v>
@@ -3903,16 +3903,16 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>8</v>
@@ -3920,16 +3920,16 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>8</v>
@@ -3937,16 +3937,16 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>8</v>
@@ -3954,16 +3954,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>8</v>
@@ -3971,16 +3971,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>8</v>
@@ -3988,16 +3988,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>8</v>
@@ -4005,16 +4005,16 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>8</v>
@@ -4022,16 +4022,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>8</v>
@@ -4039,16 +4039,16 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>8</v>
@@ -4056,16 +4056,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>178</v>
-      </c>
       <c r="C88" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>8</v>
@@ -4073,16 +4073,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>8</v>
@@ -4090,16 +4090,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>8</v>
@@ -4107,16 +4107,16 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>8</v>
@@ -4124,16 +4124,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>8</v>
@@ -4141,16 +4141,16 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>8</v>
@@ -4158,16 +4158,16 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>8</v>
@@ -4175,16 +4175,16 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>8</v>
@@ -4192,16 +4192,16 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>8</v>
@@ -4209,16 +4209,16 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -4226,16 +4226,16 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -4243,16 +4243,16 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -4260,16 +4260,16 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B100" s="7" t="s">
-        <v>196</v>
-      </c>
       <c r="C100" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -4277,16 +4277,16 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -4294,16 +4294,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -4311,16 +4311,16 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -4328,16 +4328,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -4345,16 +4345,16 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -4362,16 +4362,16 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -4379,16 +4379,16 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -4396,16 +4396,16 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -4413,16 +4413,16 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -4430,16 +4430,16 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -4447,16 +4447,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -4467,13 +4467,13 @@
         <v>213</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -4484,13 +4484,13 @@
         <v>214</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -4501,13 +4501,13 @@
         <v>215</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>216</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -4518,13 +4518,13 @@
         <v>217</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>218</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -4535,13 +4535,13 @@
         <v>219</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>220</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -4552,13 +4552,13 @@
         <v>221</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>222</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -4569,13 +4569,13 @@
         <v>223</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>216</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -4586,13 +4586,13 @@
         <v>224</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>225</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4603,13 +4603,13 @@
         <v>226</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>227</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4620,13 +4620,13 @@
         <v>228</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4637,13 +4637,13 @@
         <v>229</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>230</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>212</v>
+        <v>59</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4660,7 +4660,7 @@
         <v>58</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>8</v>
@@ -4677,7 +4677,7 @@
         <v>234</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>8</v>
@@ -4694,7 +4694,7 @@
         <v>236</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>8</v>
@@ -4711,7 +4711,7 @@
         <v>238</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>8</v>
@@ -4728,7 +4728,7 @@
         <v>240</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>8</v>
@@ -4742,10 +4742,10 @@
         <v>232</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>8</v>
@@ -4762,7 +4762,7 @@
         <v>243</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>8</v>
@@ -4779,7 +4779,7 @@
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>8</v>
@@ -4796,7 +4796,7 @@
         <v>247</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -4810,10 +4810,10 @@
         <v>245</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>8</v>
@@ -4830,7 +4830,7 @@
         <v>250</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>8</v>
@@ -4847,7 +4847,7 @@
         <v>252</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -4864,7 +4864,7 @@
         <v>254</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -4881,7 +4881,7 @@
         <v>256</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -4898,7 +4898,7 @@
         <v>258</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -4915,7 +4915,7 @@
         <v>260</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>8</v>
@@ -4932,7 +4932,7 @@
         <v>262</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>8</v>
@@ -4949,7 +4949,7 @@
         <v>264</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>8</v>
@@ -4966,7 +4966,7 @@
         <v>266</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -4983,7 +4983,7 @@
         <v>268</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -4997,10 +4997,10 @@
         <v>245</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -5017,7 +5017,7 @@
         <v>271</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>8</v>
@@ -5034,7 +5034,7 @@
         <v>273</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>8</v>
@@ -5051,7 +5051,7 @@
         <v>58</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>8</v>
@@ -5068,7 +5068,7 @@
         <v>247</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>8</v>
@@ -5082,10 +5082,10 @@
         <v>275</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>8</v>
@@ -5102,7 +5102,7 @@
         <v>279</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>8</v>
@@ -5119,7 +5119,7 @@
         <v>281</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>8</v>
@@ -5133,10 +5133,10 @@
         <v>275</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>8</v>
@@ -5153,7 +5153,7 @@
         <v>284</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>8</v>
@@ -5170,7 +5170,7 @@
         <v>286</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>8</v>
@@ -5187,7 +5187,7 @@
         <v>288</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>8</v>
@@ -5204,7 +5204,7 @@
         <v>266</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>8</v>
@@ -5221,7 +5221,7 @@
         <v>268</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>8</v>
@@ -5238,7 +5238,7 @@
         <v>292</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>8</v>
@@ -5252,10 +5252,10 @@
         <v>275</v>
       </c>
       <c r="C158" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>8</v>
@@ -5272,7 +5272,7 @@
         <v>271</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>8</v>
@@ -5286,10 +5286,10 @@
         <v>275</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>8</v>
@@ -5306,7 +5306,7 @@
         <v>297</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>8</v>
@@ -5323,7 +5323,7 @@
         <v>58</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>8</v>
@@ -5340,7 +5340,7 @@
         <v>301</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>8</v>
@@ -5357,7 +5357,7 @@
         <v>303</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>8</v>
@@ -5374,7 +5374,7 @@
         <v>305</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>8</v>
@@ -5391,7 +5391,7 @@
         <v>307</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>8</v>
@@ -5408,7 +5408,7 @@
         <v>309</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>8</v>
@@ -5425,7 +5425,7 @@
         <v>311</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>8</v>
@@ -5442,7 +5442,7 @@
         <v>313</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>8</v>
@@ -5459,7 +5459,7 @@
         <v>315</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>8</v>
@@ -5476,7 +5476,7 @@
         <v>317</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>8</v>
@@ -5493,7 +5493,7 @@
         <v>319</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>8</v>
@@ -5510,7 +5510,7 @@
         <v>321</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>8</v>
@@ -5527,7 +5527,7 @@
         <v>323</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>8</v>
@@ -5544,7 +5544,7 @@
         <v>325</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>8</v>
@@ -5561,7 +5561,7 @@
         <v>327</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>8</v>
@@ -5578,7 +5578,7 @@
         <v>266</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>8</v>
@@ -5595,7 +5595,7 @@
         <v>268</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>8</v>
@@ -5612,7 +5612,7 @@
         <v>331</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>8</v>
@@ -5626,10 +5626,10 @@
         <v>299</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>8</v>
@@ -5646,7 +5646,7 @@
         <v>271</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>8</v>
@@ -5663,7 +5663,7 @@
         <v>335</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>8</v>
@@ -5680,7 +5680,7 @@
         <v>58</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E183" s="3" t="s">
         <v>8</v>
@@ -5697,7 +5697,7 @@
         <v>339</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E184" s="3" t="s">
         <v>8</v>
@@ -5714,7 +5714,7 @@
         <v>341</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E185" s="3" t="s">
         <v>8</v>
@@ -5731,7 +5731,7 @@
         <v>343</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E186" s="3" t="s">
         <v>8</v>
@@ -5748,7 +5748,7 @@
         <v>345</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E187" s="3" t="s">
         <v>8</v>
@@ -5765,7 +5765,7 @@
         <v>347</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>8</v>
@@ -5782,7 +5782,7 @@
         <v>349</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>8</v>
@@ -5799,7 +5799,7 @@
         <v>351</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E190" s="3" t="s">
         <v>8</v>
@@ -5816,7 +5816,7 @@
         <v>353</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E191" s="3" t="s">
         <v>8</v>
@@ -5833,7 +5833,7 @@
         <v>355</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E192" s="3" t="s">
         <v>8</v>
@@ -5850,7 +5850,7 @@
         <v>357</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E193" s="3" t="s">
         <v>8</v>
@@ -5867,7 +5867,7 @@
         <v>359</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E194" s="3" t="s">
         <v>8</v>
@@ -5884,7 +5884,7 @@
         <v>361</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E195" s="3" t="s">
         <v>8</v>
@@ -5901,7 +5901,7 @@
         <v>363</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E196" s="3" t="s">
         <v>8</v>
@@ -5918,7 +5918,7 @@
         <v>365</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E197" s="3" t="s">
         <v>8</v>
@@ -5935,7 +5935,7 @@
         <v>367</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E198" s="3" t="s">
         <v>8</v>
@@ -5952,7 +5952,7 @@
         <v>369</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E199" s="3" t="s">
         <v>8</v>
@@ -5969,7 +5969,7 @@
         <v>371</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E200" s="3" t="s">
         <v>8</v>
@@ -5986,7 +5986,7 @@
         <v>373</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>8</v>
@@ -6003,7 +6003,7 @@
         <v>375</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E202" s="3" t="s">
         <v>8</v>
@@ -6020,7 +6020,7 @@
         <v>377</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>8</v>
@@ -6037,7 +6037,7 @@
         <v>379</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E204" s="3" t="s">
         <v>8</v>
@@ -6054,7 +6054,7 @@
         <v>381</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E205" s="3" t="s">
         <v>8</v>
@@ -6071,7 +6071,7 @@
         <v>383</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E206" s="3" t="s">
         <v>8</v>
@@ -6088,7 +6088,7 @@
         <v>385</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E207" s="3" t="s">
         <v>8</v>
@@ -6105,7 +6105,7 @@
         <v>387</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E208" s="3" t="s">
         <v>8</v>
@@ -6122,7 +6122,7 @@
         <v>389</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E209" s="3" t="s">
         <v>8</v>
@@ -6139,7 +6139,7 @@
         <v>391</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E210" s="3" t="s">
         <v>8</v>
@@ -6156,7 +6156,7 @@
         <v>393</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E211" s="3" t="s">
         <v>8</v>
@@ -6173,7 +6173,7 @@
         <v>395</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E212" s="3" t="s">
         <v>8</v>
@@ -6190,7 +6190,7 @@
         <v>397</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E213" s="3" t="s">
         <v>8</v>
@@ -6207,7 +6207,7 @@
         <v>399</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E214" s="3" t="s">
         <v>8</v>
@@ -6224,7 +6224,7 @@
         <v>401</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E215" s="3" t="s">
         <v>8</v>
@@ -6241,7 +6241,7 @@
         <v>403</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E216" s="3" t="s">
         <v>8</v>
@@ -6258,7 +6258,7 @@
         <v>405</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E217" s="3" t="s">
         <v>8</v>
@@ -6275,7 +6275,7 @@
         <v>407</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E218" s="3" t="s">
         <v>8</v>
@@ -6292,7 +6292,7 @@
         <v>409</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E219" s="3" t="s">
         <v>8</v>
@@ -6309,7 +6309,7 @@
         <v>411</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E220" s="3" t="s">
         <v>8</v>
@@ -6326,7 +6326,7 @@
         <v>413</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E221" s="3" t="s">
         <v>8</v>
@@ -6343,7 +6343,7 @@
         <v>415</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E222" s="3" t="s">
         <v>8</v>
@@ -6360,7 +6360,7 @@
         <v>417</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E223" s="3" t="s">
         <v>8</v>
@@ -6377,7 +6377,7 @@
         <v>419</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E224" s="3" t="s">
         <v>8</v>
@@ -6394,7 +6394,7 @@
         <v>421</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E225" s="3" t="s">
         <v>8</v>
@@ -6411,7 +6411,7 @@
         <v>423</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E226" s="3" t="s">
         <v>8</v>
@@ -6428,7 +6428,7 @@
         <v>425</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E227" s="3" t="s">
         <v>8</v>
@@ -6445,7 +6445,7 @@
         <v>427</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E228" s="3" t="s">
         <v>8</v>
@@ -6459,10 +6459,10 @@
         <v>337</v>
       </c>
       <c r="C229" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E229" s="3" t="s">
         <v>8</v>
@@ -6479,7 +6479,7 @@
         <v>430</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E230" s="3" t="s">
         <v>8</v>
@@ -6496,7 +6496,7 @@
         <v>432</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E231" s="3" t="s">
         <v>8</v>
@@ -6513,7 +6513,7 @@
         <v>434</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E232" s="3" t="s">
         <v>8</v>
@@ -6530,7 +6530,7 @@
         <v>436</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E233" s="3" t="s">
         <v>8</v>
@@ -6547,7 +6547,7 @@
         <v>438</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E234" s="3" t="s">
         <v>8</v>
@@ -6564,7 +6564,7 @@
         <v>440</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E235" s="3" t="s">
         <v>8</v>
@@ -6575,7 +6575,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D18:D110 D111:D122 D123:D201 E2:E8 E18:E22 E23:E42 E43:E47 E48:E201 F2:F3 D9:E17 D202:E235">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D26:D235 E2:E8 E26:E27 E28:E145 E146:E161 E162:E235 F2:F3 D9:E25">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update the RW Forms
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -2561,8 +2561,8 @@
   <sheetPr/>
   <dimension ref="A1:F235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="D240" sqref="D240"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -6575,7 +6575,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D26:D235 E2:E8 E26:E27 E28:E145 E146:E161 E162:E235 F2:F3 D9:E25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D26:D235 E2:E8 E26:E27 E28:E40 E41:E42 E43:E107 E108:E129 E130:E145 E146:E235 F2:F3 D22:E25 D9:E21">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update the RW Form
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -2561,8 +2561,8 @@
   <sheetPr/>
   <dimension ref="A1:F235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="C181" sqref="C181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -5680,7 +5680,7 @@
         <v>58</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E183" s="3" t="s">
         <v>8</v>
@@ -5697,7 +5697,7 @@
         <v>339</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E184" s="3" t="s">
         <v>8</v>
@@ -5714,7 +5714,7 @@
         <v>341</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E185" s="3" t="s">
         <v>8</v>
@@ -5731,7 +5731,7 @@
         <v>343</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E186" s="3" t="s">
         <v>8</v>
@@ -5748,7 +5748,7 @@
         <v>345</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E187" s="3" t="s">
         <v>8</v>
@@ -5765,7 +5765,7 @@
         <v>347</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>8</v>
@@ -5782,7 +5782,7 @@
         <v>349</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>8</v>
@@ -5799,7 +5799,7 @@
         <v>351</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E190" s="3" t="s">
         <v>8</v>
@@ -5816,7 +5816,7 @@
         <v>353</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E191" s="3" t="s">
         <v>8</v>
@@ -5833,7 +5833,7 @@
         <v>355</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E192" s="3" t="s">
         <v>8</v>
@@ -5850,7 +5850,7 @@
         <v>357</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E193" s="3" t="s">
         <v>8</v>
@@ -5867,7 +5867,7 @@
         <v>359</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E194" s="3" t="s">
         <v>8</v>
@@ -5884,7 +5884,7 @@
         <v>361</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E195" s="3" t="s">
         <v>8</v>
@@ -5901,7 +5901,7 @@
         <v>363</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E196" s="3" t="s">
         <v>8</v>
@@ -5918,7 +5918,7 @@
         <v>365</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E197" s="3" t="s">
         <v>8</v>
@@ -5935,7 +5935,7 @@
         <v>367</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E198" s="3" t="s">
         <v>8</v>
@@ -5952,7 +5952,7 @@
         <v>369</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E199" s="3" t="s">
         <v>8</v>
@@ -5969,7 +5969,7 @@
         <v>371</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E200" s="3" t="s">
         <v>8</v>
@@ -5986,7 +5986,7 @@
         <v>373</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>8</v>
@@ -6003,7 +6003,7 @@
         <v>375</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E202" s="3" t="s">
         <v>8</v>
@@ -6020,7 +6020,7 @@
         <v>377</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>8</v>
@@ -6037,7 +6037,7 @@
         <v>379</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E204" s="3" t="s">
         <v>8</v>
@@ -6054,7 +6054,7 @@
         <v>381</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E205" s="3" t="s">
         <v>8</v>
@@ -6071,7 +6071,7 @@
         <v>383</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E206" s="3" t="s">
         <v>8</v>
@@ -6088,7 +6088,7 @@
         <v>385</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E207" s="3" t="s">
         <v>8</v>
@@ -6105,7 +6105,7 @@
         <v>387</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E208" s="3" t="s">
         <v>8</v>
@@ -6122,7 +6122,7 @@
         <v>389</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E209" s="3" t="s">
         <v>8</v>
@@ -6139,7 +6139,7 @@
         <v>391</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E210" s="3" t="s">
         <v>8</v>
@@ -6156,7 +6156,7 @@
         <v>393</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E211" s="3" t="s">
         <v>8</v>
@@ -6173,7 +6173,7 @@
         <v>395</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E212" s="3" t="s">
         <v>8</v>
@@ -6190,7 +6190,7 @@
         <v>397</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E213" s="3" t="s">
         <v>8</v>
@@ -6207,7 +6207,7 @@
         <v>399</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E214" s="3" t="s">
         <v>8</v>
@@ -6224,7 +6224,7 @@
         <v>401</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E215" s="3" t="s">
         <v>8</v>
@@ -6241,7 +6241,7 @@
         <v>403</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E216" s="3" t="s">
         <v>8</v>
@@ -6258,7 +6258,7 @@
         <v>405</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E217" s="3" t="s">
         <v>8</v>
@@ -6275,7 +6275,7 @@
         <v>407</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E218" s="3" t="s">
         <v>8</v>
@@ -6292,7 +6292,7 @@
         <v>409</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E219" s="3" t="s">
         <v>8</v>
@@ -6309,7 +6309,7 @@
         <v>411</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E220" s="3" t="s">
         <v>8</v>
@@ -6326,7 +6326,7 @@
         <v>413</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E221" s="3" t="s">
         <v>8</v>
@@ -6343,7 +6343,7 @@
         <v>415</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E222" s="3" t="s">
         <v>8</v>
@@ -6360,7 +6360,7 @@
         <v>417</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E223" s="3" t="s">
         <v>8</v>
@@ -6377,7 +6377,7 @@
         <v>419</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E224" s="3" t="s">
         <v>8</v>
@@ -6394,7 +6394,7 @@
         <v>421</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E225" s="3" t="s">
         <v>8</v>
@@ -6411,7 +6411,7 @@
         <v>423</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E226" s="3" t="s">
         <v>8</v>
@@ -6428,7 +6428,7 @@
         <v>425</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E227" s="3" t="s">
         <v>8</v>
@@ -6445,7 +6445,7 @@
         <v>427</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E228" s="3" t="s">
         <v>8</v>
@@ -6462,7 +6462,7 @@
         <v>93</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E229" s="3" t="s">
         <v>8</v>
@@ -6479,7 +6479,7 @@
         <v>430</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E230" s="3" t="s">
         <v>8</v>
@@ -6496,7 +6496,7 @@
         <v>432</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E231" s="3" t="s">
         <v>8</v>
@@ -6513,7 +6513,7 @@
         <v>434</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E232" s="3" t="s">
         <v>8</v>
@@ -6530,7 +6530,7 @@
         <v>436</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E233" s="3" t="s">
         <v>8</v>
@@ -6547,7 +6547,7 @@
         <v>438</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E234" s="3" t="s">
         <v>8</v>
@@ -6564,7 +6564,7 @@
         <v>440</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E235" s="3" t="s">
         <v>8</v>
@@ -6575,7 +6575,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D8 D26:D235 E2:E8 E26:E27 E28:E40 E41:E42 E43:E107 E108:E129 E130:E145 E146:E235 F2:F3 D22:E25 D9:E21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E183 D1:D8 D183:D235 E2:E8 E184:E192 E193:E235 F2:F3 D9:E25 D26:E182">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
resolved issues of RW08
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="440">
   <si>
     <t>ID</t>
   </si>
@@ -204,9 +204,6 @@
   </si>
   <si>
     <t>Open Estate</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>TC_026</t>
@@ -2561,8 +2558,8 @@
   <sheetPr/>
   <dimension ref="A1:F235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="C181" sqref="C181"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="C191" sqref="C191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3011,7 +3008,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>8</v>
@@ -3019,16 +3016,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>8</v>
@@ -3036,16 +3033,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>8</v>
@@ -3053,16 +3050,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>8</v>
@@ -3070,16 +3067,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>8</v>
@@ -3087,16 +3084,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>8</v>
@@ -3104,16 +3101,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>8</v>
@@ -3121,16 +3118,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>8</v>
@@ -3138,16 +3135,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>8</v>
@@ -3155,16 +3152,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>8</v>
@@ -3172,16 +3169,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>8</v>
@@ -3189,16 +3186,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>8</v>
@@ -3206,16 +3203,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>8</v>
@@ -3223,16 +3220,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>8</v>
@@ -3240,16 +3237,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>8</v>
@@ -3257,16 +3254,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>8</v>
@@ -3274,16 +3271,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>8</v>
@@ -3291,16 +3288,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>8</v>
@@ -3308,16 +3305,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>8</v>
@@ -3325,16 +3322,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -3342,16 +3339,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>99</v>
-      </c>
       <c r="D46" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -3359,16 +3356,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>101</v>
-      </c>
       <c r="D47" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -3376,16 +3373,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B48" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>103</v>
-      </c>
       <c r="D48" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -3393,16 +3390,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B49" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>105</v>
-      </c>
       <c r="D49" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -3410,16 +3407,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>107</v>
-      </c>
       <c r="D50" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -3427,16 +3424,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B51" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>109</v>
-      </c>
       <c r="D51" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -3444,16 +3441,16 @@
     </row>
     <row r="52" ht="28" spans="1:5">
       <c r="A52" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B52" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>111</v>
-      </c>
       <c r="D52" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -3461,16 +3458,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B53" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="D53" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -3478,16 +3475,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B54" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>115</v>
-      </c>
       <c r="D54" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -3495,16 +3492,16 @@
     </row>
     <row r="55" ht="28" spans="1:5">
       <c r="A55" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B55" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>117</v>
-      </c>
       <c r="D55" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -3512,16 +3509,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>119</v>
-      </c>
       <c r="D56" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -3529,16 +3526,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B57" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="D57" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -3546,16 +3543,16 @@
     </row>
     <row r="58" ht="28" spans="1:5">
       <c r="A58" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B58" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>123</v>
-      </c>
       <c r="D58" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -3563,16 +3560,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>125</v>
-      </c>
       <c r="D59" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -3580,16 +3577,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>127</v>
-      </c>
       <c r="D60" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -3597,16 +3594,16 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B61" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>129</v>
-      </c>
       <c r="D61" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -3614,16 +3611,16 @@
     </row>
     <row r="62" ht="28" spans="1:5">
       <c r="A62" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B62" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>131</v>
-      </c>
       <c r="D62" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3631,16 +3628,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B63" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>133</v>
-      </c>
       <c r="D63" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3648,16 +3645,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C64" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B64" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>135</v>
-      </c>
       <c r="D64" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3665,16 +3662,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B65" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>137</v>
-      </c>
       <c r="D65" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3682,16 +3679,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C66" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B66" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="D66" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3699,16 +3696,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C67" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>141</v>
-      </c>
       <c r="D67" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3716,16 +3713,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C68" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B68" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>143</v>
-      </c>
       <c r="D68" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3733,16 +3730,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C69" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="B69" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>145</v>
-      </c>
       <c r="D69" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3750,16 +3747,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C70" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B70" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>147</v>
-      </c>
       <c r="D70" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3767,16 +3764,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C71" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B71" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>149</v>
-      </c>
       <c r="D71" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3784,16 +3781,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C72" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B72" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>151</v>
-      </c>
       <c r="D72" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3801,16 +3798,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C73" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B73" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>153</v>
-      </c>
       <c r="D73" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3818,16 +3815,16 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>8</v>
@@ -3835,16 +3832,16 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C75" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B75" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>156</v>
-      </c>
       <c r="D75" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>8</v>
@@ -3852,16 +3849,16 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B76" s="7" t="s">
         <v>157</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>158</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>8</v>
@@ -3869,16 +3866,16 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C77" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B77" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>160</v>
-      </c>
       <c r="D77" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>8</v>
@@ -3886,16 +3883,16 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C78" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B78" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>162</v>
-      </c>
       <c r="D78" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>8</v>
@@ -3903,16 +3900,16 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C79" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="B79" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>164</v>
-      </c>
       <c r="D79" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>8</v>
@@ -3920,16 +3917,16 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="B80" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>166</v>
-      </c>
       <c r="D80" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>8</v>
@@ -3937,16 +3934,16 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C81" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="B81" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>168</v>
-      </c>
       <c r="D81" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>8</v>
@@ -3954,16 +3951,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C82" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="B82" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>170</v>
-      </c>
       <c r="D82" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>8</v>
@@ -3971,16 +3968,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C83" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="B83" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>172</v>
-      </c>
       <c r="D83" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>8</v>
@@ -3988,16 +3985,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="B84" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>174</v>
-      </c>
       <c r="D84" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>8</v>
@@ -4005,16 +4002,16 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>8</v>
@@ -4022,16 +4019,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C86" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B86" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>177</v>
-      </c>
       <c r="D86" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>8</v>
@@ -4039,16 +4036,16 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>8</v>
@@ -4056,16 +4053,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C88" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>181</v>
-      </c>
       <c r="D88" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>8</v>
@@ -4073,16 +4070,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C89" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="B89" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>183</v>
-      </c>
       <c r="D89" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>8</v>
@@ -4090,16 +4087,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C90" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B90" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>185</v>
-      </c>
       <c r="D90" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>8</v>
@@ -4107,16 +4104,16 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C91" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B91" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>187</v>
-      </c>
       <c r="D91" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>8</v>
@@ -4124,16 +4121,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>8</v>
@@ -4141,16 +4138,16 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>8</v>
@@ -4158,16 +4155,16 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>8</v>
@@ -4175,16 +4172,16 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>8</v>
@@ -4192,16 +4189,16 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>8</v>
@@ -4209,16 +4206,16 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>8</v>
@@ -4226,16 +4223,16 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C98" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B98" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>195</v>
-      </c>
       <c r="D98" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>8</v>
@@ -4243,16 +4240,16 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B99" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>197</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>8</v>
@@ -4260,16 +4257,16 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>8</v>
@@ -4277,16 +4274,16 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>8</v>
@@ -4294,16 +4291,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>8</v>
@@ -4311,16 +4308,16 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>8</v>
@@ -4328,16 +4325,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>8</v>
@@ -4345,16 +4342,16 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>8</v>
@@ -4362,16 +4359,16 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>8</v>
@@ -4379,16 +4376,16 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C107" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B107" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="C107" s="7" t="s">
-        <v>206</v>
-      </c>
       <c r="D107" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>8</v>
@@ -4396,16 +4393,16 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>8</v>
@@ -4413,16 +4410,16 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>8</v>
@@ -4430,16 +4427,16 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C110" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="B110" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="C110" s="7" t="s">
-        <v>210</v>
-      </c>
       <c r="D110" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>8</v>
@@ -4447,16 +4444,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B111" s="7" t="s">
         <v>211</v>
-      </c>
-      <c r="B111" s="7" t="s">
-        <v>212</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>8</v>
@@ -4464,16 +4461,16 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>8</v>
@@ -4481,16 +4478,16 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>8</v>
@@ -4498,16 +4495,16 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C114" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="B114" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C114" s="7" t="s">
-        <v>216</v>
-      </c>
       <c r="D114" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>8</v>
@@ -4515,16 +4512,16 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C115" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="B115" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C115" s="7" t="s">
-        <v>218</v>
-      </c>
       <c r="D115" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>8</v>
@@ -4532,16 +4529,16 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C116" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="B116" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C116" s="7" t="s">
-        <v>220</v>
-      </c>
       <c r="D116" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>8</v>
@@ -4549,16 +4546,16 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C117" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="B117" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C117" s="7" t="s">
-        <v>222</v>
-      </c>
       <c r="D117" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>8</v>
@@ -4566,16 +4563,16 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>8</v>
@@ -4583,16 +4580,16 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C119" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="B119" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>225</v>
-      </c>
       <c r="D119" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>8</v>
@@ -4600,16 +4597,16 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C120" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="B120" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C120" s="7" t="s">
-        <v>227</v>
-      </c>
       <c r="D120" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>8</v>
@@ -4617,16 +4614,16 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>8</v>
@@ -4634,16 +4631,16 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C122" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="B122" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C122" s="7" t="s">
-        <v>230</v>
-      </c>
       <c r="D122" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>8</v>
@@ -4651,16 +4648,16 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B123" s="7" t="s">
         <v>231</v>
-      </c>
-      <c r="B123" s="7" t="s">
-        <v>232</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>8</v>
@@ -4668,16 +4665,16 @@
     </row>
     <row r="124" ht="28" spans="1:5">
       <c r="A124" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C124" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="B124" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C124" s="9" t="s">
-        <v>234</v>
-      </c>
       <c r="D124" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>8</v>
@@ -4685,16 +4682,16 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C125" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="B125" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C125" s="7" t="s">
-        <v>236</v>
-      </c>
       <c r="D125" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>8</v>
@@ -4702,16 +4699,16 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C126" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="B126" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C126" s="7" t="s">
-        <v>238</v>
-      </c>
       <c r="D126" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E126" s="3" t="s">
         <v>8</v>
@@ -4719,16 +4716,16 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C127" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="B127" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>240</v>
-      </c>
       <c r="D127" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>8</v>
@@ -4736,16 +4733,16 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>8</v>
@@ -4753,16 +4750,16 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C129" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="B129" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C129" s="7" t="s">
-        <v>243</v>
-      </c>
       <c r="D129" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>8</v>
@@ -4770,16 +4767,16 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B130" s="7" t="s">
         <v>244</v>
-      </c>
-      <c r="B130" s="7" t="s">
-        <v>245</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>8</v>
@@ -4787,16 +4784,16 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C131" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="B131" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C131" s="7" t="s">
-        <v>247</v>
-      </c>
       <c r="D131" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>8</v>
@@ -4804,16 +4801,16 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>8</v>
@@ -4821,16 +4818,16 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C133" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="B133" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C133" s="7" t="s">
-        <v>250</v>
-      </c>
       <c r="D133" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>8</v>
@@ -4838,16 +4835,16 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C134" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="B134" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C134" s="7" t="s">
-        <v>252</v>
-      </c>
       <c r="D134" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>8</v>
@@ -4855,16 +4852,16 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C135" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B135" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C135" s="7" t="s">
-        <v>254</v>
-      </c>
       <c r="D135" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>8</v>
@@ -4872,16 +4869,16 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C136" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="B136" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C136" s="7" t="s">
-        <v>256</v>
-      </c>
       <c r="D136" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>8</v>
@@ -4889,16 +4886,16 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C137" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="B137" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C137" s="7" t="s">
-        <v>258</v>
-      </c>
       <c r="D137" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>8</v>
@@ -4906,16 +4903,16 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C138" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="B138" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C138" s="7" t="s">
-        <v>260</v>
-      </c>
       <c r="D138" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>8</v>
@@ -4923,16 +4920,16 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C139" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="B139" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C139" s="7" t="s">
-        <v>262</v>
-      </c>
       <c r="D139" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>8</v>
@@ -4940,16 +4937,16 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C140" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="B140" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C140" s="7" t="s">
-        <v>264</v>
-      </c>
       <c r="D140" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>8</v>
@@ -4957,16 +4954,16 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C141" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="B141" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C141" s="7" t="s">
-        <v>266</v>
-      </c>
       <c r="D141" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>8</v>
@@ -4974,16 +4971,16 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C142" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="B142" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C142" s="7" t="s">
-        <v>268</v>
-      </c>
       <c r="D142" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>8</v>
@@ -4991,16 +4988,16 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
@@ -5008,16 +5005,16 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C144" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="B144" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C144" s="7" t="s">
-        <v>271</v>
-      </c>
       <c r="D144" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>8</v>
@@ -5025,16 +5022,16 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C145" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="B145" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C145" s="7" t="s">
-        <v>273</v>
-      </c>
       <c r="D145" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>8</v>
@@ -5042,16 +5039,16 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B146" s="7" t="s">
         <v>274</v>
-      </c>
-      <c r="B146" s="7" t="s">
-        <v>275</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>8</v>
@@ -5059,16 +5056,16 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>8</v>
@@ -5076,16 +5073,16 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>8</v>
@@ -5093,16 +5090,16 @@
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C149" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="B149" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="C149" s="7" t="s">
-        <v>279</v>
-      </c>
       <c r="D149" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>8</v>
@@ -5110,16 +5107,16 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C150" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="B150" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="C150" s="7" t="s">
-        <v>281</v>
-      </c>
       <c r="D150" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>8</v>
@@ -5127,16 +5124,16 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>8</v>
@@ -5144,16 +5141,16 @@
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C152" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="B152" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="C152" s="7" t="s">
-        <v>284</v>
-      </c>
       <c r="D152" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>8</v>
@@ -5161,16 +5158,16 @@
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C153" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="B153" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="C153" s="7" t="s">
-        <v>286</v>
-      </c>
       <c r="D153" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>8</v>
@@ -5178,16 +5175,16 @@
     </row>
     <row r="154" ht="28" spans="1:5">
       <c r="A154" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C154" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B154" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="C154" s="9" t="s">
-        <v>288</v>
-      </c>
       <c r="D154" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>8</v>
@@ -5195,16 +5192,16 @@
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>8</v>
@@ -5212,16 +5209,16 @@
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C156" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>8</v>
@@ -5229,16 +5226,16 @@
     </row>
     <row r="157" ht="28" spans="1:5">
       <c r="A157" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B157" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C157" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="B157" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="C157" s="9" t="s">
-        <v>292</v>
-      </c>
       <c r="D157" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>8</v>
@@ -5246,16 +5243,16 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C158" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>8</v>
@@ -5263,16 +5260,16 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C159" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>8</v>
@@ -5280,16 +5277,16 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>8</v>
@@ -5297,16 +5294,16 @@
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B161" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C161" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="B161" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="C161" s="7" t="s">
-        <v>297</v>
-      </c>
       <c r="D161" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>8</v>
@@ -5314,16 +5311,16 @@
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B162" s="7" t="s">
         <v>298</v>
-      </c>
-      <c r="B162" s="7" t="s">
-        <v>299</v>
       </c>
       <c r="C162" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>8</v>
@@ -5331,16 +5328,16 @@
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B163" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C163" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="B163" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C163" s="7" t="s">
-        <v>301</v>
-      </c>
       <c r="D163" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>8</v>
@@ -5348,16 +5345,16 @@
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B164" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C164" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="B164" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C164" s="7" t="s">
-        <v>303</v>
-      </c>
       <c r="D164" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>8</v>
@@ -5365,16 +5362,16 @@
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B165" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C165" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="B165" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C165" s="7" t="s">
-        <v>305</v>
-      </c>
       <c r="D165" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>8</v>
@@ -5382,16 +5379,16 @@
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B166" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C166" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="B166" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C166" s="7" t="s">
-        <v>307</v>
-      </c>
       <c r="D166" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>8</v>
@@ -5399,16 +5396,16 @@
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B167" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C167" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="B167" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C167" s="7" t="s">
-        <v>309</v>
-      </c>
       <c r="D167" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>8</v>
@@ -5416,16 +5413,16 @@
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B168" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C168" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="B168" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C168" s="7" t="s">
-        <v>311</v>
-      </c>
       <c r="D168" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>8</v>
@@ -5433,16 +5430,16 @@
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B169" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C169" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="B169" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C169" s="7" t="s">
-        <v>313</v>
-      </c>
       <c r="D169" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>8</v>
@@ -5450,16 +5447,16 @@
     </row>
     <row r="170" spans="1:5">
       <c r="A170" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B170" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C170" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="B170" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C170" s="7" t="s">
-        <v>315</v>
-      </c>
       <c r="D170" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>8</v>
@@ -5467,16 +5464,16 @@
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B171" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C171" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="B171" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C171" s="7" t="s">
-        <v>317</v>
-      </c>
       <c r="D171" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>8</v>
@@ -5484,16 +5481,16 @@
     </row>
     <row r="172" spans="1:5">
       <c r="A172" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B172" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C172" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="B172" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C172" s="7" t="s">
-        <v>319</v>
-      </c>
       <c r="D172" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>8</v>
@@ -5501,16 +5498,16 @@
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C173" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="B173" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C173" s="7" t="s">
-        <v>321</v>
-      </c>
       <c r="D173" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>8</v>
@@ -5518,16 +5515,16 @@
     </row>
     <row r="174" spans="1:5">
       <c r="A174" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C174" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="B174" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C174" s="7" t="s">
-        <v>323</v>
-      </c>
       <c r="D174" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>8</v>
@@ -5535,16 +5532,16 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B175" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C175" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="B175" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C175" s="7" t="s">
-        <v>325</v>
-      </c>
       <c r="D175" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>8</v>
@@ -5552,16 +5549,16 @@
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B176" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C176" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="B176" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C176" s="7" t="s">
-        <v>327</v>
-      </c>
       <c r="D176" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>8</v>
@@ -5569,16 +5566,16 @@
     </row>
     <row r="177" spans="1:5">
       <c r="A177" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C177" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E177" s="3" t="s">
         <v>8</v>
@@ -5586,16 +5583,16 @@
     </row>
     <row r="178" spans="1:5">
       <c r="A178" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C178" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>8</v>
@@ -5603,16 +5600,16 @@
     </row>
     <row r="179" ht="28" spans="1:5">
       <c r="A179" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B179" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C179" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="B179" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C179" s="9" t="s">
-        <v>331</v>
-      </c>
       <c r="D179" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>8</v>
@@ -5620,16 +5617,16 @@
     </row>
     <row r="180" spans="1:5">
       <c r="A180" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E180" s="3" t="s">
         <v>8</v>
@@ -5637,16 +5634,16 @@
     </row>
     <row r="181" spans="1:5">
       <c r="A181" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C181" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>8</v>
@@ -5654,16 +5651,16 @@
     </row>
     <row r="182" spans="1:5">
       <c r="A182" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B182" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C182" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="B182" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C182" s="7" t="s">
-        <v>335</v>
-      </c>
       <c r="D182" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>8</v>
@@ -5671,10 +5668,10 @@
     </row>
     <row r="183" spans="1:5">
       <c r="A183" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B183" s="7" t="s">
         <v>336</v>
-      </c>
-      <c r="B183" s="7" t="s">
-        <v>337</v>
       </c>
       <c r="C183" s="7" t="s">
         <v>58</v>
@@ -5688,13 +5685,13 @@
     </row>
     <row r="184" ht="28" spans="1:5">
       <c r="A184" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B184" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C184" s="9" t="s">
         <v>338</v>
-      </c>
-      <c r="B184" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C184" s="9" t="s">
-        <v>339</v>
       </c>
       <c r="D184" s="3" t="s">
         <v>8</v>
@@ -5705,13 +5702,13 @@
     </row>
     <row r="185" spans="1:5">
       <c r="A185" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B185" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C185" s="7" t="s">
         <v>340</v>
-      </c>
-      <c r="B185" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C185" s="7" t="s">
-        <v>341</v>
       </c>
       <c r="D185" s="3" t="s">
         <v>8</v>
@@ -5722,13 +5719,13 @@
     </row>
     <row r="186" spans="1:5">
       <c r="A186" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B186" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C186" s="7" t="s">
         <v>342</v>
-      </c>
-      <c r="B186" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C186" s="7" t="s">
-        <v>343</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>8</v>
@@ -5739,13 +5736,13 @@
     </row>
     <row r="187" spans="1:5">
       <c r="A187" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B187" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C187" s="7" t="s">
         <v>344</v>
-      </c>
-      <c r="B187" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C187" s="7" t="s">
-        <v>345</v>
       </c>
       <c r="D187" s="3" t="s">
         <v>8</v>
@@ -5756,13 +5753,13 @@
     </row>
     <row r="188" spans="1:5">
       <c r="A188" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="B188" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C188" s="7" t="s">
         <v>346</v>
-      </c>
-      <c r="B188" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C188" s="7" t="s">
-        <v>347</v>
       </c>
       <c r="D188" s="3" t="s">
         <v>8</v>
@@ -5773,13 +5770,13 @@
     </row>
     <row r="189" spans="1:5">
       <c r="A189" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B189" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C189" s="7" t="s">
         <v>348</v>
-      </c>
-      <c r="B189" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C189" s="7" t="s">
-        <v>349</v>
       </c>
       <c r="D189" s="3" t="s">
         <v>8</v>
@@ -5790,13 +5787,13 @@
     </row>
     <row r="190" spans="1:5">
       <c r="A190" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B190" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C190" s="7" t="s">
         <v>350</v>
-      </c>
-      <c r="B190" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C190" s="7" t="s">
-        <v>351</v>
       </c>
       <c r="D190" s="3" t="s">
         <v>8</v>
@@ -5807,13 +5804,13 @@
     </row>
     <row r="191" spans="1:5">
       <c r="A191" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="B191" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C191" s="7" t="s">
         <v>352</v>
-      </c>
-      <c r="B191" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C191" s="7" t="s">
-        <v>353</v>
       </c>
       <c r="D191" s="3" t="s">
         <v>8</v>
@@ -5824,13 +5821,13 @@
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="B192" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C192" s="7" t="s">
         <v>354</v>
-      </c>
-      <c r="B192" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C192" s="7" t="s">
-        <v>355</v>
       </c>
       <c r="D192" s="3" t="s">
         <v>8</v>
@@ -5841,13 +5838,13 @@
     </row>
     <row r="193" ht="28" spans="1:5">
       <c r="A193" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B193" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C193" s="9" t="s">
         <v>356</v>
-      </c>
-      <c r="B193" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C193" s="9" t="s">
-        <v>357</v>
       </c>
       <c r="D193" s="3" t="s">
         <v>8</v>
@@ -5858,13 +5855,13 @@
     </row>
     <row r="194" spans="1:5">
       <c r="A194" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B194" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C194" s="9" t="s">
         <v>358</v>
-      </c>
-      <c r="B194" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C194" s="9" t="s">
-        <v>359</v>
       </c>
       <c r="D194" s="3" t="s">
         <v>8</v>
@@ -5875,13 +5872,13 @@
     </row>
     <row r="195" spans="1:5">
       <c r="A195" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="B195" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C195" s="7" t="s">
         <v>360</v>
-      </c>
-      <c r="B195" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C195" s="7" t="s">
-        <v>361</v>
       </c>
       <c r="D195" s="3" t="s">
         <v>8</v>
@@ -5892,13 +5889,13 @@
     </row>
     <row r="196" spans="1:5">
       <c r="A196" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B196" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C196" s="7" t="s">
         <v>362</v>
-      </c>
-      <c r="B196" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C196" s="7" t="s">
-        <v>363</v>
       </c>
       <c r="D196" s="3" t="s">
         <v>8</v>
@@ -5909,13 +5906,13 @@
     </row>
     <row r="197" spans="1:5">
       <c r="A197" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="B197" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C197" s="7" t="s">
         <v>364</v>
-      </c>
-      <c r="B197" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C197" s="7" t="s">
-        <v>365</v>
       </c>
       <c r="D197" s="3" t="s">
         <v>8</v>
@@ -5926,13 +5923,13 @@
     </row>
     <row r="198" spans="1:5">
       <c r="A198" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="B198" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C198" s="7" t="s">
         <v>366</v>
-      </c>
-      <c r="B198" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C198" s="7" t="s">
-        <v>367</v>
       </c>
       <c r="D198" s="3" t="s">
         <v>8</v>
@@ -5943,13 +5940,13 @@
     </row>
     <row r="199" ht="28" spans="1:5">
       <c r="A199" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B199" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C199" s="9" t="s">
         <v>368</v>
-      </c>
-      <c r="B199" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C199" s="9" t="s">
-        <v>369</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>8</v>
@@ -5960,13 +5957,13 @@
     </row>
     <row r="200" spans="1:5">
       <c r="A200" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="B200" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C200" s="7" t="s">
         <v>370</v>
-      </c>
-      <c r="B200" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C200" s="7" t="s">
-        <v>371</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>8</v>
@@ -5977,13 +5974,13 @@
     </row>
     <row r="201" ht="28" spans="1:5">
       <c r="A201" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B201" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C201" s="9" t="s">
         <v>372</v>
-      </c>
-      <c r="B201" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C201" s="9" t="s">
-        <v>373</v>
       </c>
       <c r="D201" s="3" t="s">
         <v>8</v>
@@ -5994,13 +5991,13 @@
     </row>
     <row r="202" spans="1:5">
       <c r="A202" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B202" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C202" s="7" t="s">
         <v>374</v>
-      </c>
-      <c r="B202" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C202" s="7" t="s">
-        <v>375</v>
       </c>
       <c r="D202" s="3" t="s">
         <v>8</v>
@@ -6011,13 +6008,13 @@
     </row>
     <row r="203" ht="28" spans="1:5">
       <c r="A203" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B203" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C203" s="9" t="s">
         <v>376</v>
-      </c>
-      <c r="B203" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C203" s="9" t="s">
-        <v>377</v>
       </c>
       <c r="D203" s="3" t="s">
         <v>8</v>
@@ -6028,13 +6025,13 @@
     </row>
     <row r="204" spans="1:5">
       <c r="A204" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="B204" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C204" s="7" t="s">
         <v>378</v>
-      </c>
-      <c r="B204" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C204" s="7" t="s">
-        <v>379</v>
       </c>
       <c r="D204" s="3" t="s">
         <v>8</v>
@@ -6045,13 +6042,13 @@
     </row>
     <row r="205" spans="1:5">
       <c r="A205" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B205" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C205" s="7" t="s">
         <v>380</v>
-      </c>
-      <c r="B205" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C205" s="7" t="s">
-        <v>381</v>
       </c>
       <c r="D205" s="3" t="s">
         <v>8</v>
@@ -6062,13 +6059,13 @@
     </row>
     <row r="206" ht="28" spans="1:5">
       <c r="A206" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="B206" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C206" s="9" t="s">
         <v>382</v>
-      </c>
-      <c r="B206" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C206" s="9" t="s">
-        <v>383</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>8</v>
@@ -6079,13 +6076,13 @@
     </row>
     <row r="207" spans="1:5">
       <c r="A207" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="B207" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C207" s="7" t="s">
         <v>384</v>
-      </c>
-      <c r="B207" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C207" s="7" t="s">
-        <v>385</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>8</v>
@@ -6096,13 +6093,13 @@
     </row>
     <row r="208" spans="1:5">
       <c r="A208" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="B208" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C208" s="7" t="s">
         <v>386</v>
-      </c>
-      <c r="B208" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C208" s="7" t="s">
-        <v>387</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>8</v>
@@ -6113,13 +6110,13 @@
     </row>
     <row r="209" spans="1:5">
       <c r="A209" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="B209" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C209" s="7" t="s">
         <v>388</v>
-      </c>
-      <c r="B209" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C209" s="7" t="s">
-        <v>389</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>8</v>
@@ -6130,13 +6127,13 @@
     </row>
     <row r="210" spans="1:5">
       <c r="A210" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="B210" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C210" s="7" t="s">
         <v>390</v>
-      </c>
-      <c r="B210" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C210" s="7" t="s">
-        <v>391</v>
       </c>
       <c r="D210" s="3" t="s">
         <v>8</v>
@@ -6147,13 +6144,13 @@
     </row>
     <row r="211" spans="1:5">
       <c r="A211" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="B211" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C211" s="7" t="s">
         <v>392</v>
-      </c>
-      <c r="B211" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C211" s="7" t="s">
-        <v>393</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>8</v>
@@ -6164,13 +6161,13 @@
     </row>
     <row r="212" spans="1:5">
       <c r="A212" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B212" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C212" s="7" t="s">
         <v>394</v>
-      </c>
-      <c r="B212" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C212" s="7" t="s">
-        <v>395</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>8</v>
@@ -6181,13 +6178,13 @@
     </row>
     <row r="213" spans="1:5">
       <c r="A213" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B213" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C213" s="7" t="s">
         <v>396</v>
-      </c>
-      <c r="B213" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C213" s="7" t="s">
-        <v>397</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>8</v>
@@ -6198,13 +6195,13 @@
     </row>
     <row r="214" spans="1:5">
       <c r="A214" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B214" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C214" s="7" t="s">
         <v>398</v>
-      </c>
-      <c r="B214" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C214" s="7" t="s">
-        <v>399</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>8</v>
@@ -6215,13 +6212,13 @@
     </row>
     <row r="215" spans="1:5">
       <c r="A215" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B215" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C215" s="7" t="s">
         <v>400</v>
-      </c>
-      <c r="B215" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C215" s="7" t="s">
-        <v>401</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>8</v>
@@ -6232,13 +6229,13 @@
     </row>
     <row r="216" spans="1:5">
       <c r="A216" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B216" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C216" s="7" t="s">
         <v>402</v>
-      </c>
-      <c r="B216" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C216" s="7" t="s">
-        <v>403</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>8</v>
@@ -6249,13 +6246,13 @@
     </row>
     <row r="217" spans="1:5">
       <c r="A217" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="B217" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C217" s="7" t="s">
         <v>404</v>
-      </c>
-      <c r="B217" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C217" s="7" t="s">
-        <v>405</v>
       </c>
       <c r="D217" s="3" t="s">
         <v>8</v>
@@ -6266,13 +6263,13 @@
     </row>
     <row r="218" spans="1:5">
       <c r="A218" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="B218" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C218" s="7" t="s">
         <v>406</v>
-      </c>
-      <c r="B218" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C218" s="7" t="s">
-        <v>407</v>
       </c>
       <c r="D218" s="3" t="s">
         <v>8</v>
@@ -6283,13 +6280,13 @@
     </row>
     <row r="219" spans="1:5">
       <c r="A219" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B219" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C219" s="7" t="s">
         <v>408</v>
-      </c>
-      <c r="B219" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C219" s="7" t="s">
-        <v>409</v>
       </c>
       <c r="D219" s="3" t="s">
         <v>8</v>
@@ -6300,13 +6297,13 @@
     </row>
     <row r="220" spans="1:5">
       <c r="A220" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B220" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C220" s="7" t="s">
         <v>410</v>
-      </c>
-      <c r="B220" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C220" s="7" t="s">
-        <v>411</v>
       </c>
       <c r="D220" s="3" t="s">
         <v>8</v>
@@ -6317,13 +6314,13 @@
     </row>
     <row r="221" spans="1:5">
       <c r="A221" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B221" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C221" s="7" t="s">
         <v>412</v>
-      </c>
-      <c r="B221" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C221" s="7" t="s">
-        <v>413</v>
       </c>
       <c r="D221" s="3" t="s">
         <v>8</v>
@@ -6334,13 +6331,13 @@
     </row>
     <row r="222" ht="28" spans="1:5">
       <c r="A222" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B222" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C222" s="9" t="s">
         <v>414</v>
-      </c>
-      <c r="B222" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C222" s="9" t="s">
-        <v>415</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>8</v>
@@ -6351,13 +6348,13 @@
     </row>
     <row r="223" spans="1:5">
       <c r="A223" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B223" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C223" s="7" t="s">
         <v>416</v>
-      </c>
-      <c r="B223" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C223" s="7" t="s">
-        <v>417</v>
       </c>
       <c r="D223" s="3" t="s">
         <v>8</v>
@@ -6368,13 +6365,13 @@
     </row>
     <row r="224" spans="1:5">
       <c r="A224" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="B224" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C224" s="7" t="s">
         <v>418</v>
-      </c>
-      <c r="B224" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C224" s="7" t="s">
-        <v>419</v>
       </c>
       <c r="D224" s="3" t="s">
         <v>8</v>
@@ -6385,13 +6382,13 @@
     </row>
     <row r="225" spans="1:5">
       <c r="A225" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B225" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C225" s="7" t="s">
         <v>420</v>
-      </c>
-      <c r="B225" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C225" s="7" t="s">
-        <v>421</v>
       </c>
       <c r="D225" s="3" t="s">
         <v>8</v>
@@ -6402,13 +6399,13 @@
     </row>
     <row r="226" spans="1:5">
       <c r="A226" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="B226" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C226" s="7" t="s">
         <v>422</v>
-      </c>
-      <c r="B226" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C226" s="7" t="s">
-        <v>423</v>
       </c>
       <c r="D226" s="3" t="s">
         <v>8</v>
@@ -6419,13 +6416,13 @@
     </row>
     <row r="227" spans="1:5">
       <c r="A227" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B227" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C227" s="7" t="s">
         <v>424</v>
-      </c>
-      <c r="B227" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C227" s="7" t="s">
-        <v>425</v>
       </c>
       <c r="D227" s="3" t="s">
         <v>8</v>
@@ -6436,13 +6433,13 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="B228" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C228" s="7" t="s">
         <v>426</v>
-      </c>
-      <c r="B228" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C228" s="7" t="s">
-        <v>427</v>
       </c>
       <c r="D228" s="3" t="s">
         <v>8</v>
@@ -6453,13 +6450,13 @@
     </row>
     <row r="229" spans="1:5">
       <c r="A229" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B229" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C229" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D229" s="3" t="s">
         <v>8</v>
@@ -6470,13 +6467,13 @@
     </row>
     <row r="230" spans="1:5">
       <c r="A230" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B230" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C230" s="7" t="s">
         <v>429</v>
-      </c>
-      <c r="B230" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C230" s="7" t="s">
-        <v>430</v>
       </c>
       <c r="D230" s="3" t="s">
         <v>8</v>
@@ -6487,13 +6484,13 @@
     </row>
     <row r="231" spans="1:5">
       <c r="A231" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B231" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C231" s="7" t="s">
         <v>431</v>
-      </c>
-      <c r="B231" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C231" s="7" t="s">
-        <v>432</v>
       </c>
       <c r="D231" s="3" t="s">
         <v>8</v>
@@ -6504,13 +6501,13 @@
     </row>
     <row r="232" spans="1:5">
       <c r="A232" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="B232" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C232" s="7" t="s">
         <v>433</v>
-      </c>
-      <c r="B232" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C232" s="7" t="s">
-        <v>434</v>
       </c>
       <c r="D232" s="3" t="s">
         <v>8</v>
@@ -6521,13 +6518,13 @@
     </row>
     <row r="233" spans="1:5">
       <c r="A233" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="B233" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C233" s="7" t="s">
         <v>435</v>
-      </c>
-      <c r="B233" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C233" s="7" t="s">
-        <v>436</v>
       </c>
       <c r="D233" s="3" t="s">
         <v>8</v>
@@ -6538,13 +6535,13 @@
     </row>
     <row r="234" spans="1:5">
       <c r="A234" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B234" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C234" s="7" t="s">
         <v>437</v>
-      </c>
-      <c r="B234" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C234" s="7" t="s">
-        <v>438</v>
       </c>
       <c r="D234" s="3" t="s">
         <v>8</v>
@@ -6555,13 +6552,13 @@
     </row>
     <row r="235" spans="1:5">
       <c r="A235" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B235" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C235" s="7" t="s">
         <v>439</v>
-      </c>
-      <c r="B235" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C235" s="7" t="s">
-        <v>440</v>
       </c>
       <c r="D235" s="3" t="s">
         <v>8</v>
@@ -6575,7 +6572,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E183 D1:D8 D183:D235 E2:E8 E184:E192 E193:E235 F2:F3 D9:E25 D26:E182">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E23 D235:E235 D1:D8 D23:D234 E2:E8 E24:E182 E183:E234 F2:F3 D9:E22">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
works on OC02 TCs
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="440">
   <si>
     <t>ID</t>
   </si>
@@ -912,9 +912,6 @@
   </si>
   <si>
     <t>TC_158</t>
-  </si>
-  <si>
-    <t>TC_159</t>
   </si>
   <si>
     <t>TC_160</t>
@@ -2559,10 +2556,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F235"/>
+  <dimension ref="A1:F234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="C181" sqref="C181"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="C212" sqref="C212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3334,7 +3331,7 @@
         <v>58</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>8</v>
@@ -3351,7 +3348,7 @@
         <v>99</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>8</v>
@@ -3368,7 +3365,7 @@
         <v>101</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>8</v>
@@ -3385,7 +3382,7 @@
         <v>103</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>8</v>
@@ -3402,7 +3399,7 @@
         <v>105</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>8</v>
@@ -3419,7 +3416,7 @@
         <v>107</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>8</v>
@@ -3436,7 +3433,7 @@
         <v>109</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>8</v>
@@ -3453,7 +3450,7 @@
         <v>111</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>8</v>
@@ -3470,7 +3467,7 @@
         <v>113</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>8</v>
@@ -3487,7 +3484,7 @@
         <v>115</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>8</v>
@@ -3504,7 +3501,7 @@
         <v>117</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>8</v>
@@ -3521,7 +3518,7 @@
         <v>119</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>8</v>
@@ -3538,7 +3535,7 @@
         <v>121</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>8</v>
@@ -3555,7 +3552,7 @@
         <v>123</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>8</v>
@@ -3572,7 +3569,7 @@
         <v>125</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>8</v>
@@ -3589,7 +3586,7 @@
         <v>127</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>8</v>
@@ -3606,7 +3603,7 @@
         <v>129</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>8</v>
@@ -3623,7 +3620,7 @@
         <v>131</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>8</v>
@@ -3640,7 +3637,7 @@
         <v>133</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>8</v>
@@ -3657,7 +3654,7 @@
         <v>135</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>8</v>
@@ -3674,7 +3671,7 @@
         <v>137</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>8</v>
@@ -3691,7 +3688,7 @@
         <v>139</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>8</v>
@@ -3708,7 +3705,7 @@
         <v>141</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>8</v>
@@ -3725,7 +3722,7 @@
         <v>143</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
@@ -3742,7 +3739,7 @@
         <v>145</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>8</v>
@@ -3759,7 +3756,7 @@
         <v>147</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>8</v>
@@ -3776,7 +3773,7 @@
         <v>149</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>8</v>
@@ -3793,7 +3790,7 @@
         <v>151</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>8</v>
@@ -3810,7 +3807,7 @@
         <v>153</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>8</v>
@@ -3827,7 +3824,7 @@
         <v>93</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>8</v>
@@ -3844,7 +3841,7 @@
         <v>156</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>8</v>
@@ -5255,7 +5252,7 @@
         <v>93</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>8</v>
@@ -5285,8 +5282,8 @@
       <c r="B160" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="C160" s="8" t="s">
-        <v>93</v>
+      <c r="C160" s="7" t="s">
+        <v>296</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>59</v>
@@ -5297,13 +5294,13 @@
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>275</v>
+        <v>298</v>
       </c>
       <c r="C161" s="7" t="s">
-        <v>297</v>
+        <v>58</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>59</v>
@@ -5314,13 +5311,13 @@
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B162" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="B162" s="7" t="s">
-        <v>299</v>
-      </c>
       <c r="C162" s="7" t="s">
-        <v>58</v>
+        <v>300</v>
       </c>
       <c r="D162" s="3" t="s">
         <v>59</v>
@@ -5331,13 +5328,13 @@
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C163" s="7" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>59</v>
@@ -5348,13 +5345,13 @@
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C164" s="7" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D164" s="3" t="s">
         <v>59</v>
@@ -5365,13 +5362,13 @@
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C165" s="7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D165" s="3" t="s">
         <v>59</v>
@@ -5382,13 +5379,13 @@
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C166" s="7" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D166" s="3" t="s">
         <v>59</v>
@@ -5399,13 +5396,13 @@
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C167" s="7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D167" s="3" t="s">
         <v>59</v>
@@ -5416,13 +5413,13 @@
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C168" s="7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D168" s="3" t="s">
         <v>59</v>
@@ -5433,13 +5430,13 @@
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C169" s="7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D169" s="3" t="s">
         <v>59</v>
@@ -5450,13 +5447,13 @@
     </row>
     <row r="170" spans="1:5">
       <c r="A170" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C170" s="7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D170" s="3" t="s">
         <v>59</v>
@@ -5467,13 +5464,13 @@
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C171" s="7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D171" s="3" t="s">
         <v>59</v>
@@ -5484,13 +5481,13 @@
     </row>
     <row r="172" spans="1:5">
       <c r="A172" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C172" s="7" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D172" s="3" t="s">
         <v>59</v>
@@ -5501,13 +5498,13 @@
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C173" s="7" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D173" s="3" t="s">
         <v>59</v>
@@ -5518,13 +5515,13 @@
     </row>
     <row r="174" spans="1:5">
       <c r="A174" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C174" s="7" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D174" s="3" t="s">
         <v>59</v>
@@ -5535,13 +5532,13 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C175" s="7" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D175" s="3" t="s">
         <v>59</v>
@@ -5552,13 +5549,13 @@
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B176" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C176" s="7" t="s">
-        <v>327</v>
+        <v>266</v>
       </c>
       <c r="D176" s="3" t="s">
         <v>59</v>
@@ -5572,10 +5569,10 @@
         <v>328</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C177" s="7" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D177" s="3" t="s">
         <v>59</v>
@@ -5584,15 +5581,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
+    <row r="178" ht="28" spans="1:5">
       <c r="A178" s="3" t="s">
         <v>329</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C178" s="7" t="s">
-        <v>268</v>
+        <v>298</v>
+      </c>
+      <c r="C178" s="9" t="s">
+        <v>330</v>
       </c>
       <c r="D178" s="3" t="s">
         <v>59</v>
@@ -5601,15 +5598,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="179" ht="28" spans="1:5">
+    <row r="179" spans="1:5">
       <c r="A179" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C179" s="9" t="s">
-        <v>331</v>
+        <v>298</v>
+      </c>
+      <c r="C179" s="8" t="s">
+        <v>93</v>
       </c>
       <c r="D179" s="3" t="s">
         <v>59</v>
@@ -5623,10 +5620,10 @@
         <v>332</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C180" s="8" t="s">
-        <v>93</v>
+        <v>298</v>
+      </c>
+      <c r="C180" s="7" t="s">
+        <v>271</v>
       </c>
       <c r="D180" s="3" t="s">
         <v>59</v>
@@ -5640,10 +5637,10 @@
         <v>333</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C181" s="7" t="s">
-        <v>271</v>
+        <v>334</v>
       </c>
       <c r="D181" s="3" t="s">
         <v>59</v>
@@ -5654,30 +5651,30 @@
     </row>
     <row r="182" spans="1:5">
       <c r="A182" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B182" s="7" t="s">
-        <v>299</v>
+        <v>336</v>
       </c>
       <c r="C182" s="7" t="s">
-        <v>335</v>
+        <v>58</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
+    <row r="183" ht="28" spans="1:5">
       <c r="A183" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B183" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="B183" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C183" s="7" t="s">
-        <v>58</v>
+      <c r="C183" s="9" t="s">
+        <v>338</v>
       </c>
       <c r="D183" s="3" t="s">
         <v>8</v>
@@ -5686,15 +5683,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="184" ht="28" spans="1:5">
+    <row r="184" spans="1:5">
       <c r="A184" s="3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B184" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C184" s="9" t="s">
-        <v>339</v>
+        <v>336</v>
+      </c>
+      <c r="C184" s="7" t="s">
+        <v>340</v>
       </c>
       <c r="D184" s="3" t="s">
         <v>8</v>
@@ -5705,13 +5702,13 @@
     </row>
     <row r="185" spans="1:5">
       <c r="A185" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C185" s="7" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D185" s="3" t="s">
         <v>8</v>
@@ -5722,13 +5719,13 @@
     </row>
     <row r="186" spans="1:5">
       <c r="A186" s="3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B186" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C186" s="7" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>8</v>
@@ -5739,13 +5736,13 @@
     </row>
     <row r="187" spans="1:5">
       <c r="A187" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C187" s="7" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D187" s="3" t="s">
         <v>8</v>
@@ -5756,13 +5753,13 @@
     </row>
     <row r="188" spans="1:5">
       <c r="A188" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C188" s="7" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D188" s="3" t="s">
         <v>8</v>
@@ -5773,13 +5770,13 @@
     </row>
     <row r="189" spans="1:5">
       <c r="A189" s="3" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C189" s="7" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D189" s="3" t="s">
         <v>8</v>
@@ -5790,13 +5787,13 @@
     </row>
     <row r="190" spans="1:5">
       <c r="A190" s="3" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B190" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C190" s="7" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D190" s="3" t="s">
         <v>8</v>
@@ -5807,13 +5804,13 @@
     </row>
     <row r="191" spans="1:5">
       <c r="A191" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B191" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C191" s="7" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D191" s="3" t="s">
         <v>8</v>
@@ -5822,15 +5819,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="192" spans="1:5">
+    <row r="192" ht="28" spans="1:5">
       <c r="A192" s="3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B192" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C192" s="7" t="s">
-        <v>355</v>
+        <v>336</v>
+      </c>
+      <c r="C192" s="9" t="s">
+        <v>356</v>
       </c>
       <c r="D192" s="3" t="s">
         <v>8</v>
@@ -5839,15 +5836,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="193" ht="28" spans="1:5">
+    <row r="193" spans="1:5">
       <c r="A193" s="3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B193" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D193" s="3" t="s">
         <v>8</v>
@@ -5858,13 +5855,13 @@
     </row>
     <row r="194" spans="1:5">
       <c r="A194" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B194" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C194" s="9" t="s">
-        <v>359</v>
+        <v>336</v>
+      </c>
+      <c r="C194" s="7" t="s">
+        <v>360</v>
       </c>
       <c r="D194" s="3" t="s">
         <v>8</v>
@@ -5875,13 +5872,13 @@
     </row>
     <row r="195" spans="1:5">
       <c r="A195" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B195" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C195" s="7" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D195" s="3" t="s">
         <v>8</v>
@@ -5892,13 +5889,13 @@
     </row>
     <row r="196" spans="1:5">
       <c r="A196" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C196" s="7" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D196" s="3" t="s">
         <v>8</v>
@@ -5909,13 +5906,13 @@
     </row>
     <row r="197" spans="1:5">
       <c r="A197" s="3" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B197" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C197" s="7" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D197" s="3" t="s">
         <v>8</v>
@@ -5924,15 +5921,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
+    <row r="198" ht="28" spans="1:5">
       <c r="A198" s="3" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B198" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C198" s="7" t="s">
-        <v>367</v>
+        <v>336</v>
+      </c>
+      <c r="C198" s="9" t="s">
+        <v>368</v>
       </c>
       <c r="D198" s="3" t="s">
         <v>8</v>
@@ -5941,15 +5938,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="199" ht="28" spans="1:5">
+    <row r="199" spans="1:5">
       <c r="A199" s="3" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C199" s="9" t="s">
-        <v>369</v>
+        <v>336</v>
+      </c>
+      <c r="C199" s="7" t="s">
+        <v>370</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>8</v>
@@ -5958,15 +5955,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
+    <row r="200" ht="28" spans="1:5">
       <c r="A200" s="3" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B200" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C200" s="7" t="s">
-        <v>371</v>
+        <v>336</v>
+      </c>
+      <c r="C200" s="9" t="s">
+        <v>372</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>8</v>
@@ -5975,15 +5972,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="201" ht="28" spans="1:5">
+    <row r="201" spans="1:5">
       <c r="A201" s="3" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B201" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C201" s="9" t="s">
-        <v>373</v>
+        <v>336</v>
+      </c>
+      <c r="C201" s="7" t="s">
+        <v>374</v>
       </c>
       <c r="D201" s="3" t="s">
         <v>8</v>
@@ -5992,15 +5989,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
+    <row r="202" ht="28" spans="1:5">
       <c r="A202" s="3" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B202" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C202" s="7" t="s">
-        <v>375</v>
+        <v>336</v>
+      </c>
+      <c r="C202" s="9" t="s">
+        <v>376</v>
       </c>
       <c r="D202" s="3" t="s">
         <v>8</v>
@@ -6009,15 +6006,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="203" ht="28" spans="1:5">
+    <row r="203" spans="1:5">
       <c r="A203" s="3" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B203" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C203" s="9" t="s">
-        <v>377</v>
+        <v>336</v>
+      </c>
+      <c r="C203" s="7" t="s">
+        <v>378</v>
       </c>
       <c r="D203" s="3" t="s">
         <v>8</v>
@@ -6028,13 +6025,13 @@
     </row>
     <row r="204" spans="1:5">
       <c r="A204" s="3" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B204" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C204" s="7" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D204" s="3" t="s">
         <v>8</v>
@@ -6043,15 +6040,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="205" spans="1:5">
+    <row r="205" ht="28" spans="1:5">
       <c r="A205" s="3" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B205" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C205" s="7" t="s">
-        <v>381</v>
+        <v>336</v>
+      </c>
+      <c r="C205" s="9" t="s">
+        <v>382</v>
       </c>
       <c r="D205" s="3" t="s">
         <v>8</v>
@@ -6060,15 +6057,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="206" ht="28" spans="1:5">
+    <row r="206" spans="1:5">
       <c r="A206" s="3" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B206" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C206" s="9" t="s">
-        <v>383</v>
+        <v>336</v>
+      </c>
+      <c r="C206" s="7" t="s">
+        <v>384</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>8</v>
@@ -6079,13 +6076,13 @@
     </row>
     <row r="207" spans="1:5">
       <c r="A207" s="3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B207" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C207" s="7" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>8</v>
@@ -6096,13 +6093,13 @@
     </row>
     <row r="208" spans="1:5">
       <c r="A208" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B208" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C208" s="7" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>8</v>
@@ -6113,13 +6110,13 @@
     </row>
     <row r="209" spans="1:5">
       <c r="A209" s="3" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B209" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C209" s="7" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>8</v>
@@ -6130,13 +6127,13 @@
     </row>
     <row r="210" spans="1:5">
       <c r="A210" s="3" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B210" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C210" s="7" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D210" s="3" t="s">
         <v>8</v>
@@ -6147,13 +6144,13 @@
     </row>
     <row r="211" spans="1:5">
       <c r="A211" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B211" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C211" s="7" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>8</v>
@@ -6164,13 +6161,13 @@
     </row>
     <row r="212" spans="1:5">
       <c r="A212" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B212" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C212" s="7" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>8</v>
@@ -6181,13 +6178,13 @@
     </row>
     <row r="213" spans="1:5">
       <c r="A213" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B213" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C213" s="7" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>8</v>
@@ -6198,13 +6195,13 @@
     </row>
     <row r="214" spans="1:5">
       <c r="A214" s="3" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B214" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C214" s="7" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>8</v>
@@ -6215,13 +6212,13 @@
     </row>
     <row r="215" spans="1:5">
       <c r="A215" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B215" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C215" s="7" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>8</v>
@@ -6232,13 +6229,13 @@
     </row>
     <row r="216" spans="1:5">
       <c r="A216" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B216" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C216" s="7" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>8</v>
@@ -6249,13 +6246,13 @@
     </row>
     <row r="217" spans="1:5">
       <c r="A217" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B217" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C217" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D217" s="3" t="s">
         <v>8</v>
@@ -6266,13 +6263,13 @@
     </row>
     <row r="218" spans="1:5">
       <c r="A218" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B218" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C218" s="7" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D218" s="3" t="s">
         <v>8</v>
@@ -6283,13 +6280,13 @@
     </row>
     <row r="219" spans="1:5">
       <c r="A219" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B219" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C219" s="7" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D219" s="3" t="s">
         <v>8</v>
@@ -6300,13 +6297,13 @@
     </row>
     <row r="220" spans="1:5">
       <c r="A220" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B220" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C220" s="7" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D220" s="3" t="s">
         <v>8</v>
@@ -6315,15 +6312,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="221" spans="1:5">
+    <row r="221" ht="28" spans="1:5">
       <c r="A221" s="3" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B221" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C221" s="7" t="s">
-        <v>413</v>
+        <v>336</v>
+      </c>
+      <c r="C221" s="9" t="s">
+        <v>414</v>
       </c>
       <c r="D221" s="3" t="s">
         <v>8</v>
@@ -6332,15 +6329,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="222" ht="28" spans="1:5">
+    <row r="222" spans="1:5">
       <c r="A222" s="3" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B222" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C222" s="9" t="s">
-        <v>415</v>
+        <v>336</v>
+      </c>
+      <c r="C222" s="7" t="s">
+        <v>416</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>8</v>
@@ -6351,13 +6348,13 @@
     </row>
     <row r="223" spans="1:5">
       <c r="A223" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B223" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C223" s="7" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D223" s="3" t="s">
         <v>8</v>
@@ -6368,13 +6365,13 @@
     </row>
     <row r="224" spans="1:5">
       <c r="A224" s="3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B224" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C224" s="7" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D224" s="3" t="s">
         <v>8</v>
@@ -6385,13 +6382,13 @@
     </row>
     <row r="225" spans="1:5">
       <c r="A225" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B225" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C225" s="7" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D225" s="3" t="s">
         <v>8</v>
@@ -6402,13 +6399,13 @@
     </row>
     <row r="226" spans="1:5">
       <c r="A226" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B226" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C226" s="7" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D226" s="3" t="s">
         <v>8</v>
@@ -6419,13 +6416,13 @@
     </row>
     <row r="227" spans="1:5">
       <c r="A227" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B227" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C227" s="7" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D227" s="3" t="s">
         <v>8</v>
@@ -6436,13 +6433,13 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" s="3" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C228" s="7" t="s">
-        <v>427</v>
+        <v>93</v>
       </c>
       <c r="D228" s="3" t="s">
         <v>8</v>
@@ -6456,10 +6453,10 @@
         <v>428</v>
       </c>
       <c r="B229" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C229" s="7" t="s">
-        <v>93</v>
+        <v>429</v>
       </c>
       <c r="D229" s="3" t="s">
         <v>8</v>
@@ -6470,13 +6467,13 @@
     </row>
     <row r="230" spans="1:5">
       <c r="A230" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B230" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C230" s="7" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D230" s="3" t="s">
         <v>8</v>
@@ -6487,13 +6484,13 @@
     </row>
     <row r="231" spans="1:5">
       <c r="A231" s="3" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B231" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C231" s="7" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D231" s="3" t="s">
         <v>8</v>
@@ -6504,13 +6501,13 @@
     </row>
     <row r="232" spans="1:5">
       <c r="A232" s="3" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B232" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C232" s="7" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D232" s="3" t="s">
         <v>8</v>
@@ -6521,13 +6518,13 @@
     </row>
     <row r="233" spans="1:5">
       <c r="A233" s="3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B233" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C233" s="7" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D233" s="3" t="s">
         <v>8</v>
@@ -6538,35 +6535,18 @@
     </row>
     <row r="234" spans="1:5">
       <c r="A234" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B234" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C234" s="7" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D234" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E234" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5">
-      <c r="A235" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="B235" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="C235" s="7" t="s">
-        <v>440</v>
-      </c>
-      <c r="D235" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E235" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -6575,7 +6555,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E183 D1:D8 D183:D235 E2:E8 E184:E192 E193:E235 F2:F3 D9:E25 D26:E182">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D160 E160 D1:D8 D45:D75 D127:D159 E2:E8 E45:E46 E47:E75 E127:E129 E130:E131 E132:E159 F2:F3 D9:E44 D76:E126 D182:E234 D161:E181">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
works on RW failed script fixations
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -2558,8 +2558,8 @@
   <sheetPr/>
   <dimension ref="A1:F234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="C180" sqref="C180"/>
+    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
+      <selection activeCell="D237" sqref="D237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -5660,7 +5660,7 @@
         <v>58</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>8</v>
@@ -5677,7 +5677,7 @@
         <v>338</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E183" s="3" t="s">
         <v>8</v>
@@ -5694,7 +5694,7 @@
         <v>340</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E184" s="3" t="s">
         <v>8</v>
@@ -5711,7 +5711,7 @@
         <v>342</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E185" s="3" t="s">
         <v>8</v>
@@ -5728,7 +5728,7 @@
         <v>344</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E186" s="3" t="s">
         <v>8</v>
@@ -5745,7 +5745,7 @@
         <v>346</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E187" s="3" t="s">
         <v>8</v>
@@ -5762,7 +5762,7 @@
         <v>348</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>8</v>
@@ -5779,7 +5779,7 @@
         <v>350</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>8</v>
@@ -5796,7 +5796,7 @@
         <v>352</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E190" s="3" t="s">
         <v>8</v>
@@ -5813,7 +5813,7 @@
         <v>354</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E191" s="3" t="s">
         <v>8</v>
@@ -5830,7 +5830,7 @@
         <v>356</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E192" s="3" t="s">
         <v>8</v>
@@ -5847,7 +5847,7 @@
         <v>358</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E193" s="3" t="s">
         <v>8</v>
@@ -5864,7 +5864,7 @@
         <v>360</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E194" s="3" t="s">
         <v>8</v>
@@ -5881,7 +5881,7 @@
         <v>362</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E195" s="3" t="s">
         <v>8</v>
@@ -5898,7 +5898,7 @@
         <v>364</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E196" s="3" t="s">
         <v>8</v>
@@ -5915,7 +5915,7 @@
         <v>366</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E197" s="3" t="s">
         <v>8</v>
@@ -5932,7 +5932,7 @@
         <v>368</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E198" s="3" t="s">
         <v>8</v>
@@ -5949,7 +5949,7 @@
         <v>370</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E199" s="3" t="s">
         <v>8</v>
@@ -5966,7 +5966,7 @@
         <v>372</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E200" s="3" t="s">
         <v>8</v>
@@ -5983,7 +5983,7 @@
         <v>374</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>8</v>
@@ -6000,7 +6000,7 @@
         <v>376</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E202" s="3" t="s">
         <v>8</v>
@@ -6017,7 +6017,7 @@
         <v>378</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>8</v>
@@ -6034,7 +6034,7 @@
         <v>380</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E204" s="3" t="s">
         <v>8</v>
@@ -6051,7 +6051,7 @@
         <v>382</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E205" s="3" t="s">
         <v>8</v>
@@ -6068,7 +6068,7 @@
         <v>384</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E206" s="3" t="s">
         <v>8</v>
@@ -6085,7 +6085,7 @@
         <v>386</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E207" s="3" t="s">
         <v>8</v>
@@ -6102,7 +6102,7 @@
         <v>388</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E208" s="3" t="s">
         <v>8</v>
@@ -6119,7 +6119,7 @@
         <v>390</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E209" s="3" t="s">
         <v>8</v>
@@ -6136,7 +6136,7 @@
         <v>392</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E210" s="3" t="s">
         <v>8</v>
@@ -6153,7 +6153,7 @@
         <v>394</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E211" s="3" t="s">
         <v>8</v>
@@ -6170,7 +6170,7 @@
         <v>396</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E212" s="3" t="s">
         <v>8</v>
@@ -6187,7 +6187,7 @@
         <v>398</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E213" s="3" t="s">
         <v>8</v>
@@ -6204,7 +6204,7 @@
         <v>400</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E214" s="3" t="s">
         <v>8</v>
@@ -6221,7 +6221,7 @@
         <v>402</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E215" s="3" t="s">
         <v>8</v>
@@ -6238,7 +6238,7 @@
         <v>404</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E216" s="3" t="s">
         <v>8</v>
@@ -6255,7 +6255,7 @@
         <v>406</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E217" s="3" t="s">
         <v>8</v>
@@ -6272,7 +6272,7 @@
         <v>408</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E218" s="3" t="s">
         <v>8</v>
@@ -6289,7 +6289,7 @@
         <v>410</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E219" s="3" t="s">
         <v>8</v>
@@ -6306,7 +6306,7 @@
         <v>412</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E220" s="3" t="s">
         <v>8</v>
@@ -6323,7 +6323,7 @@
         <v>414</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E221" s="3" t="s">
         <v>8</v>
@@ -6340,7 +6340,7 @@
         <v>416</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E222" s="3" t="s">
         <v>8</v>
@@ -6357,7 +6357,7 @@
         <v>418</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E223" s="3" t="s">
         <v>8</v>
@@ -6374,7 +6374,7 @@
         <v>420</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E224" s="3" t="s">
         <v>8</v>
@@ -6391,7 +6391,7 @@
         <v>422</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E225" s="3" t="s">
         <v>8</v>
@@ -6408,7 +6408,7 @@
         <v>424</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E226" s="3" t="s">
         <v>8</v>
@@ -6425,7 +6425,7 @@
         <v>426</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E227" s="3" t="s">
         <v>8</v>
@@ -6442,7 +6442,7 @@
         <v>93</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E228" s="3" t="s">
         <v>8</v>
@@ -6459,7 +6459,7 @@
         <v>429</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E229" s="3" t="s">
         <v>8</v>
@@ -6476,7 +6476,7 @@
         <v>431</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E230" s="3" t="s">
         <v>8</v>
@@ -6493,7 +6493,7 @@
         <v>433</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E231" s="3" t="s">
         <v>8</v>
@@ -6510,7 +6510,7 @@
         <v>435</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E232" s="3" t="s">
         <v>8</v>
@@ -6527,7 +6527,7 @@
         <v>437</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E233" s="3" t="s">
         <v>8</v>
@@ -6544,7 +6544,7 @@
         <v>439</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E234" s="3" t="s">
         <v>8</v>
@@ -6555,7 +6555,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D181:E181 D1:D8 D176:D180 E2:E8 E176:E180 F2:F3 D182:E234 D9:E38 D39:E175">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E180 D1:D8 D176:D234 E2:E8 E176:E179 E181:E234 F2:F3 D9:E175">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
resolved issues of globalContacts, estateCreation and estateContacts
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/TestData.xlsx
+++ b/src/test/resources/test-data/TestData.xlsx
@@ -2561,8 +2561,8 @@
   <sheetPr/>
   <dimension ref="A1:F235"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="C182" sqref="C182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -3011,7 +3011,7 @@
         <v>59</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>9</v>
@@ -3027,8 +3027,8 @@
       <c r="C27" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>9</v>
+      <c r="D27" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>9</v>
@@ -3044,8 +3044,8 @@
       <c r="C28" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>9</v>
+      <c r="D28" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>9</v>
@@ -3061,8 +3061,8 @@
       <c r="C29" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>9</v>
+      <c r="D29" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>9</v>
@@ -3078,8 +3078,8 @@
       <c r="C30" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>9</v>
+      <c r="D30" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>9</v>
@@ -3095,8 +3095,8 @@
       <c r="C31" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>9</v>
+      <c r="D31" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>9</v>
@@ -3112,8 +3112,8 @@
       <c r="C32" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>9</v>
+      <c r="D32" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>9</v>
@@ -3129,8 +3129,8 @@
       <c r="C33" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>9</v>
+      <c r="D33" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>9</v>
@@ -3146,8 +3146,8 @@
       <c r="C34" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>9</v>
+      <c r="D34" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>9</v>
@@ -3163,8 +3163,8 @@
       <c r="C35" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>9</v>
+      <c r="D35" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>9</v>
@@ -3180,8 +3180,8 @@
       <c r="C36" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>9</v>
+      <c r="D36" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>9</v>
@@ -3197,8 +3197,8 @@
       <c r="C37" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>9</v>
+      <c r="D37" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>9</v>
@@ -3214,8 +3214,8 @@
       <c r="C38" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>9</v>
+      <c r="D38" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>9</v>
@@ -3231,8 +3231,8 @@
       <c r="C39" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>9</v>
+      <c r="D39" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>9</v>
@@ -3248,8 +3248,8 @@
       <c r="C40" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>9</v>
+      <c r="D40" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>9</v>
@@ -3265,8 +3265,8 @@
       <c r="C41" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>9</v>
+      <c r="D41" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>9</v>
@@ -3282,8 +3282,8 @@
       <c r="C42" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>9</v>
+      <c r="D42" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>9</v>
@@ -3299,8 +3299,8 @@
       <c r="C43" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>9</v>
+      <c r="D43" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>9</v>
@@ -3316,8 +3316,8 @@
       <c r="C44" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>9</v>
+      <c r="D44" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>9</v>
@@ -3333,8 +3333,8 @@
       <c r="C45" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>9</v>
+      <c r="D45" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>9</v>
@@ -3350,8 +3350,8 @@
       <c r="C46" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>9</v>
+      <c r="D46" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>9</v>
@@ -3367,8 +3367,8 @@
       <c r="C47" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>9</v>
+      <c r="D47" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>9</v>
@@ -3384,8 +3384,8 @@
       <c r="C48" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>9</v>
+      <c r="D48" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>9</v>
@@ -3401,8 +3401,8 @@
       <c r="C49" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>9</v>
+      <c r="D49" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>9</v>
@@ -3418,8 +3418,8 @@
       <c r="C50" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>9</v>
+      <c r="D50" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>9</v>
@@ -3435,8 +3435,8 @@
       <c r="C51" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>9</v>
+      <c r="D51" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>9</v>
@@ -3452,8 +3452,8 @@
       <c r="C52" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>9</v>
+      <c r="D52" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>9</v>
@@ -3469,8 +3469,8 @@
       <c r="C53" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>9</v>
+      <c r="D53" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>9</v>
@@ -3486,8 +3486,8 @@
       <c r="C54" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>9</v>
+      <c r="D54" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>9</v>
@@ -3503,8 +3503,8 @@
       <c r="C55" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>9</v>
+      <c r="D55" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>9</v>
@@ -3520,8 +3520,8 @@
       <c r="C56" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>9</v>
+      <c r="D56" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>9</v>
@@ -3537,8 +3537,8 @@
       <c r="C57" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>9</v>
+      <c r="D57" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>9</v>
@@ -3554,8 +3554,8 @@
       <c r="C58" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>9</v>
+      <c r="D58" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>9</v>
@@ -3571,8 +3571,8 @@
       <c r="C59" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>9</v>
+      <c r="D59" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>9</v>
@@ -3588,8 +3588,8 @@
       <c r="C60" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>9</v>
+      <c r="D60" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>9</v>
@@ -3605,8 +3605,8 @@
       <c r="C61" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>9</v>
+      <c r="D61" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>9</v>
@@ -3622,8 +3622,8 @@
       <c r="C62" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>9</v>
+      <c r="D62" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>9</v>
@@ -3639,8 +3639,8 @@
       <c r="C63" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>9</v>
+      <c r="D63" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>9</v>
@@ -3656,8 +3656,8 @@
       <c r="C64" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>9</v>
+      <c r="D64" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>9</v>
@@ -3673,8 +3673,8 @@
       <c r="C65" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>9</v>
+      <c r="D65" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>9</v>
@@ -3690,8 +3690,8 @@
       <c r="C66" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>9</v>
+      <c r="D66" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>9</v>
@@ -3707,8 +3707,8 @@
       <c r="C67" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>9</v>
+      <c r="D67" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>9</v>
@@ -3724,8 +3724,8 @@
       <c r="C68" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>9</v>
+      <c r="D68" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>9</v>
@@ -3741,8 +3741,8 @@
       <c r="C69" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>9</v>
+      <c r="D69" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>9</v>
@@ -3758,8 +3758,8 @@
       <c r="C70" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>9</v>
+      <c r="D70" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>9</v>
@@ -3775,8 +3775,8 @@
       <c r="C71" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D71" s="3" t="s">
-        <v>9</v>
+      <c r="D71" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>9</v>
@@ -3792,8 +3792,8 @@
       <c r="C72" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>9</v>
+      <c r="D72" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>9</v>
@@ -3809,8 +3809,8 @@
       <c r="C73" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="D73" s="3" t="s">
-        <v>9</v>
+      <c r="D73" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>9</v>
@@ -3826,8 +3826,8 @@
       <c r="C74" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>9</v>
+      <c r="D74" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>9</v>
@@ -3843,8 +3843,8 @@
       <c r="C75" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D75" s="3" t="s">
-        <v>9</v>
+      <c r="D75" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>9</v>
@@ -3860,8 +3860,8 @@
       <c r="C76" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D76" s="3" t="s">
-        <v>9</v>
+      <c r="D76" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>9</v>
@@ -3877,8 +3877,8 @@
       <c r="C77" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="D77" s="3" t="s">
-        <v>9</v>
+      <c r="D77" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>9</v>
@@ -3894,8 +3894,8 @@
       <c r="C78" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="D78" s="3" t="s">
-        <v>9</v>
+      <c r="D78" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>9</v>
@@ -3911,8 +3911,8 @@
       <c r="C79" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="D79" s="3" t="s">
-        <v>9</v>
+      <c r="D79" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>9</v>
@@ -3928,8 +3928,8 @@
       <c r="C80" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="D80" s="3" t="s">
-        <v>9</v>
+      <c r="D80" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>9</v>
@@ -3945,8 +3945,8 @@
       <c r="C81" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="D81" s="3" t="s">
-        <v>9</v>
+      <c r="D81" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>9</v>
@@ -3962,8 +3962,8 @@
       <c r="C82" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D82" s="3" t="s">
-        <v>9</v>
+      <c r="D82" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>9</v>
@@ -3979,8 +3979,8 @@
       <c r="C83" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="D83" s="3" t="s">
-        <v>9</v>
+      <c r="D83" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>9</v>
@@ -3996,8 +3996,8 @@
       <c r="C84" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>9</v>
+      <c r="D84" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>9</v>
@@ -4013,8 +4013,8 @@
       <c r="C85" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D85" s="3" t="s">
-        <v>9</v>
+      <c r="D85" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>9</v>
@@ -4030,8 +4030,8 @@
       <c r="C86" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>9</v>
+      <c r="D86" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>9</v>
@@ -4047,8 +4047,8 @@
       <c r="C87" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D87" s="3" t="s">
-        <v>9</v>
+      <c r="D87" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>9</v>
@@ -4064,8 +4064,8 @@
       <c r="C88" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D88" s="3" t="s">
-        <v>9</v>
+      <c r="D88" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>9</v>
@@ -4081,8 +4081,8 @@
       <c r="C89" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D89" s="3" t="s">
-        <v>9</v>
+      <c r="D89" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>9</v>
@@ -4098,8 +4098,8 @@
       <c r="C90" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D90" s="3" t="s">
-        <v>9</v>
+      <c r="D90" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>9</v>
@@ -4115,8 +4115,8 @@
       <c r="C91" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D91" s="3" t="s">
-        <v>9</v>
+      <c r="D91" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>9</v>
@@ -4132,8 +4132,8 @@
       <c r="C92" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D92" s="3" t="s">
-        <v>9</v>
+      <c r="D92" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>9</v>
@@ -4149,8 +4149,8 @@
       <c r="C93" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>9</v>
+      <c r="D93" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>9</v>
@@ -4166,8 +4166,8 @@
       <c r="C94" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D94" s="3" t="s">
-        <v>9</v>
+      <c r="D94" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>9</v>
@@ -4183,8 +4183,8 @@
       <c r="C95" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D95" s="3" t="s">
-        <v>9</v>
+      <c r="D95" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>9</v>
@@ -4200,8 +4200,8 @@
       <c r="C96" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D96" s="3" t="s">
-        <v>9</v>
+      <c r="D96" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>9</v>
@@ -4217,8 +4217,8 @@
       <c r="C97" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D97" s="3" t="s">
-        <v>9</v>
+      <c r="D97" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>9</v>
@@ -4234,8 +4234,8 @@
       <c r="C98" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D98" s="3" t="s">
-        <v>9</v>
+      <c r="D98" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>9</v>
@@ -4251,8 +4251,8 @@
       <c r="C99" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>9</v>
+      <c r="D99" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>9</v>
@@ -4268,8 +4268,8 @@
       <c r="C100" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D100" s="3" t="s">
-        <v>9</v>
+      <c r="D100" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>9</v>
@@ -4285,8 +4285,8 @@
       <c r="C101" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="D101" s="3" t="s">
-        <v>9</v>
+      <c r="D101" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E101" s="3" t="s">
         <v>9</v>
@@ -4302,8 +4302,8 @@
       <c r="C102" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="D102" s="3" t="s">
-        <v>9</v>
+      <c r="D102" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>9</v>
@@ -4319,8 +4319,8 @@
       <c r="C103" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D103" s="3" t="s">
-        <v>9</v>
+      <c r="D103" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>9</v>
@@ -4336,8 +4336,8 @@
       <c r="C104" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D104" s="3" t="s">
-        <v>9</v>
+      <c r="D104" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>9</v>
@@ -4353,8 +4353,8 @@
       <c r="C105" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D105" s="3" t="s">
-        <v>9</v>
+      <c r="D105" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>9</v>
@@ -4370,8 +4370,8 @@
       <c r="C106" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D106" s="3" t="s">
-        <v>9</v>
+      <c r="D106" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>9</v>
@@ -4387,8 +4387,8 @@
       <c r="C107" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="D107" s="3" t="s">
-        <v>9</v>
+      <c r="D107" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>9</v>
@@ -4404,8 +4404,8 @@
       <c r="C108" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D108" s="3" t="s">
-        <v>9</v>
+      <c r="D108" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>9</v>
@@ -4421,8 +4421,8 @@
       <c r="C109" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D109" s="3" t="s">
-        <v>9</v>
+      <c r="D109" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>9</v>
@@ -4438,8 +4438,8 @@
       <c r="C110" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="D110" s="3" t="s">
-        <v>9</v>
+      <c r="D110" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>9</v>
@@ -4455,8 +4455,8 @@
       <c r="C111" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D111" s="3" t="s">
-        <v>9</v>
+      <c r="D111" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>9</v>
@@ -4472,8 +4472,8 @@
       <c r="C112" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="D112" s="3" t="s">
-        <v>9</v>
+      <c r="D112" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>9</v>
@@ -4489,8 +4489,8 @@
       <c r="C113" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="D113" s="3" t="s">
-        <v>9</v>
+      <c r="D113" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>9</v>
@@ -4506,8 +4506,8 @@
       <c r="C114" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="D114" s="3" t="s">
-        <v>9</v>
+      <c r="D114" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>9</v>
@@ -4523,8 +4523,8 @@
       <c r="C115" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="D115" s="3" t="s">
-        <v>9</v>
+      <c r="D115" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>9</v>
@@ -4540,8 +4540,8 @@
       <c r="C116" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="D116" s="3" t="s">
-        <v>9</v>
+      <c r="D116" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E116" s="3" 